<commit_message>
revise NXTH in the instruction set
</commit_message>
<xml_diff>
--- a/P4E_psuedo_instruction_set.xlsx
+++ b/P4E_psuedo_instruction_set.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\P4EngineAssembler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE03CB76-C0D8-46ED-B8E3-F5E32414D262}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{509447CB-6089-4F0E-BBEF-4B18118AD40D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-3645" windowWidth="38640" windowHeight="21840" xr2:uid="{87164962-7B7D-4BAA-98E0-B9A8D7C47112}"/>
   </bookViews>
@@ -601,6 +601,56 @@
         </r>
       </text>
     </comment>
+    <comment ref="D161" authorId="0" shapeId="0" xr:uid="{D18DB5FE-3A83-491E-84D6-3985F23FC611}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t>Dianchao Wang:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+isr_len + meta_len &lt;= 40</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F162" authorId="0" shapeId="0" xr:uid="{F5C9FE6D-D006-4B70-9523-3BFBD214FD89}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>Dianchao Wang:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+isr_len + meta_len &lt;= 40</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -772,7 +822,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1181" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1187" uniqueCount="383">
   <si>
     <t>isr SHiFT</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -3945,6 +3995,14 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>COPY(L)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>COPY 4 bytes of meta data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -3953,7 +4011,7 @@
         <family val="2"/>
         <charset val="134"/>
       </rPr>
-      <t>&gt;&gt;</t>
+      <t xml:space="preserve">META [ </t>
     </r>
     <r>
       <rPr>
@@ -3964,7 +4022,7 @@
         <family val="2"/>
         <charset val="134"/>
       </rPr>
-      <t xml:space="preserve">val6 </t>
+      <t xml:space="preserve">CALC_RSLT </t>
     </r>
     <r>
       <rPr>
@@ -3974,7 +4032,7 @@
         <family val="2"/>
         <charset val="134"/>
       </rPr>
-      <t>(0-32),</t>
+      <t>] ,</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -3987,7 +4045,7 @@
         <family val="2"/>
         <charset val="134"/>
       </rPr>
-      <t>&gt;&gt;</t>
+      <t xml:space="preserve">META [ </t>
     </r>
     <r>
       <rPr>
@@ -3998,7 +4056,7 @@
         <family val="2"/>
         <charset val="134"/>
       </rPr>
-      <t xml:space="preserve">val6 </t>
+      <t>SM_DATA0</t>
     </r>
     <r>
       <rPr>
@@ -4008,16 +4066,8 @@
         <family val="2"/>
         <charset val="134"/>
       </rPr>
-      <t>(0-32) ;</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>COPY(L)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>COPY 4 bytes of meta data</t>
+      <t xml:space="preserve"> ] ,</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -4040,7 +4090,7 @@
         <family val="2"/>
         <charset val="134"/>
       </rPr>
-      <t xml:space="preserve">CALC_RSLT </t>
+      <t>SM_DATA1</t>
     </r>
     <r>
       <rPr>
@@ -4050,7 +4100,7 @@
         <family val="2"/>
         <charset val="134"/>
       </rPr>
-      <t>] ,</t>
+      <t xml:space="preserve"> ] ,</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -4074,7 +4124,7 @@
         <family val="2"/>
         <charset val="134"/>
       </rPr>
-      <t>SM_DATA0</t>
+      <t>SM_DATA2</t>
     </r>
     <r>
       <rPr>
@@ -4108,7 +4158,7 @@
         <family val="2"/>
         <charset val="134"/>
       </rPr>
-      <t>SM_DATA1</t>
+      <t>SM_DATA3</t>
     </r>
     <r>
       <rPr>
@@ -4142,7 +4192,7 @@
         <family val="2"/>
         <charset val="134"/>
       </rPr>
-      <t>SM_DATA2</t>
+      <t>SM_DATA4</t>
     </r>
     <r>
       <rPr>
@@ -4176,7 +4226,7 @@
         <family val="2"/>
         <charset val="134"/>
       </rPr>
-      <t>SM_DATA3</t>
+      <t>SM_DATA5</t>
     </r>
     <r>
       <rPr>
@@ -4210,7 +4260,7 @@
         <family val="2"/>
         <charset val="134"/>
       </rPr>
-      <t>SM_DATA4</t>
+      <t>SM_DATA6</t>
     </r>
     <r>
       <rPr>
@@ -4244,7 +4294,7 @@
         <family val="2"/>
         <charset val="134"/>
       </rPr>
-      <t>SM_DATA5</t>
+      <t>SM_DATA7</t>
     </r>
     <r>
       <rPr>
@@ -4267,7 +4317,7 @@
         <family val="2"/>
         <charset val="134"/>
       </rPr>
-      <t xml:space="preserve">META [ </t>
+      <t>&gt;&gt;</t>
     </r>
     <r>
       <rPr>
@@ -4278,7 +4328,7 @@
         <family val="2"/>
         <charset val="134"/>
       </rPr>
-      <t>SM_DATA6</t>
+      <t xml:space="preserve">val6 </t>
     </r>
     <r>
       <rPr>
@@ -4288,7 +4338,7 @@
         <family val="2"/>
         <charset val="134"/>
       </rPr>
-      <t xml:space="preserve"> ] ,</t>
+      <t>(1-32),</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -4301,7 +4351,7 @@
         <family val="2"/>
         <charset val="134"/>
       </rPr>
-      <t xml:space="preserve">META [ </t>
+      <t>&gt;&gt;</t>
     </r>
     <r>
       <rPr>
@@ -4312,7 +4362,7 @@
         <family val="2"/>
         <charset val="134"/>
       </rPr>
-      <t>SM_DATA7</t>
+      <t xml:space="preserve">val6 </t>
     </r>
     <r>
       <rPr>
@@ -4322,7 +4372,7 @@
         <family val="2"/>
         <charset val="134"/>
       </rPr>
-      <t xml:space="preserve"> ] ,</t>
+      <t>(1-32) ;</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -4851,11 +4901,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA14F7B7-5F50-4FFB-AE20-84853F321386}">
-  <dimension ref="A1:I171"/>
+  <dimension ref="A1:I173"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B47" sqref="B47"/>
+      <pane ySplit="1" topLeftCell="A134" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C172" sqref="C172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.2"/>
@@ -5839,10 +5889,10 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>23</v>
@@ -5866,7 +5916,7 @@
       </c>
       <c r="B48" s="2"/>
       <c r="C48" s="2" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>202</v>
@@ -5885,7 +5935,7 @@
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>262</v>
@@ -5904,7 +5954,7 @@
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>300</v>
@@ -5919,7 +5969,7 @@
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>202</v>
@@ -5938,7 +5988,7 @@
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>262</v>
@@ -5957,7 +6007,7 @@
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>300</v>
@@ -5972,7 +6022,7 @@
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>202</v>
@@ -5991,7 +6041,7 @@
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>262</v>
@@ -6010,7 +6060,7 @@
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>300</v>
@@ -6025,7 +6075,7 @@
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>202</v>
@@ -6044,7 +6094,7 @@
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>262</v>
@@ -6063,7 +6113,7 @@
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>300</v>
@@ -6078,7 +6128,7 @@
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>202</v>
@@ -6097,7 +6147,7 @@
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>262</v>
@@ -6116,7 +6166,7 @@
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>300</v>
@@ -6131,7 +6181,7 @@
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>202</v>
@@ -6150,7 +6200,7 @@
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>262</v>
@@ -6169,7 +6219,7 @@
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>300</v>
@@ -6184,7 +6234,7 @@
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>202</v>
@@ -6203,7 +6253,7 @@
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>262</v>
@@ -6222,7 +6272,7 @@
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>300</v>
@@ -6237,7 +6287,7 @@
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>202</v>
@@ -6256,7 +6306,7 @@
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>262</v>
@@ -6275,7 +6325,7 @@
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>300</v>
@@ -6290,7 +6340,7 @@
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>202</v>
@@ -6309,7 +6359,7 @@
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>262</v>
@@ -6328,7 +6378,7 @@
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>300</v>
@@ -7558,7 +7608,7 @@
         <v>294</v>
       </c>
       <c r="G157" s="2" t="s">
-        <v>370</v>
+        <v>381</v>
       </c>
       <c r="H157" s="14" t="s">
         <v>296</v>
@@ -7574,7 +7624,7 @@
       <c r="E158" s="2"/>
       <c r="F158" s="2"/>
       <c r="G158" s="2" t="s">
-        <v>370</v>
+        <v>381</v>
       </c>
       <c r="H158" s="14" t="s">
         <v>296</v>
@@ -7590,7 +7640,7 @@
         <v>294</v>
       </c>
       <c r="G159" s="2" t="s">
-        <v>370</v>
+        <v>381</v>
       </c>
       <c r="H159" s="14" t="s">
         <v>296</v>
@@ -7602,15 +7652,19 @@
       <c r="E160" s="2"/>
       <c r="F160" s="2"/>
       <c r="G160" s="2" t="s">
-        <v>370</v>
+        <v>381</v>
       </c>
       <c r="H160" s="14" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C161" s="2"/>
-      <c r="D161" s="2"/>
+      <c r="C161" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="D161" s="2" t="s">
+        <v>294</v>
+      </c>
       <c r="E161" s="2"/>
       <c r="F161" s="2"/>
       <c r="G161" s="2"/>
@@ -7618,81 +7672,105 @@
         <v>296</v>
       </c>
     </row>
-    <row r="162" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A162" s="8"/>
-      <c r="B162" s="13" t="s">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C162" s="2"/>
+      <c r="D162" s="2"/>
+      <c r="E162" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="F162" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="G162" s="2"/>
+      <c r="H162" s="14" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="163" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C163" s="2"/>
+      <c r="D163" s="2"/>
+      <c r="E163" s="2"/>
+      <c r="F163" s="2"/>
+      <c r="G163" s="2"/>
+      <c r="H163" s="14" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="164" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A164" s="8"/>
+      <c r="B164" s="13" t="s">
         <v>154</v>
       </c>
-      <c r="C162" s="8"/>
-      <c r="D162" s="8"/>
-      <c r="E162" s="8"/>
-      <c r="F162" s="8"/>
-      <c r="G162" s="8"/>
-      <c r="H162" s="8"/>
-      <c r="I162" s="8"/>
-    </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A163" s="2" t="s">
+      <c r="C164" s="8"/>
+      <c r="D164" s="8"/>
+      <c r="E164" s="8"/>
+      <c r="F164" s="8"/>
+      <c r="G164" s="8"/>
+      <c r="H164" s="8"/>
+      <c r="I164" s="8"/>
+    </row>
+    <row r="165" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A165" s="2" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A164" s="2" t="s">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A166" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B164" s="2" t="s">
+      <c r="B166" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="C164" s="1" t="s">
+      <c r="C166" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C165" s="2" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C166" s="1" t="s">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C167" s="2" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="168" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C168" s="1" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="167" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A167" s="8"/>
-      <c r="B167" s="13" t="s">
+    <row r="169" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A169" s="8"/>
+      <c r="B169" s="13" t="s">
         <v>153</v>
       </c>
-      <c r="C167" s="8"/>
-      <c r="D167" s="8"/>
-      <c r="E167" s="8"/>
-      <c r="F167" s="8"/>
-      <c r="G167" s="8"/>
-      <c r="H167" s="8"/>
-      <c r="I167" s="8"/>
-    </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A168" s="2" t="s">
+      <c r="C169" s="8"/>
+      <c r="D169" s="8"/>
+      <c r="E169" s="8"/>
+      <c r="F169" s="8"/>
+      <c r="G169" s="8"/>
+      <c r="H169" s="8"/>
+      <c r="I169" s="8"/>
+    </row>
+    <row r="170" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A170" s="2" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A169" s="2" t="s">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A171" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B169" s="2" t="s">
+      <c r="B171" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="C169" s="1" t="s">
+      <c r="C171" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C170" s="2" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C171" s="1" t="s">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C172" s="2" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="173" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C173" s="1" t="s">
         <v>205</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add mat related instructions
</commit_message>
<xml_diff>
--- a/P4E_psuedo_instruction_set.xlsx
+++ b/P4E_psuedo_instruction_set.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\P4EngineAssembler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E7D1ED2-4BC6-4349-86CA-4AD069455BCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{724416F4-9769-467A-9D69-2B38FE560BBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-3645" windowWidth="38640" windowHeight="21840" xr2:uid="{87164962-7B7D-4BAA-98E0-B9A8D7C47112}"/>
+    <workbookView xWindow="-24585" yWindow="4905" windowWidth="24630" windowHeight="12825" activeTab="1" xr2:uid="{87164962-7B7D-4BAA-98E0-B9A8D7C47112}"/>
   </bookViews>
   <sheets>
     <sheet name="parser" sheetId="1" r:id="rId1"/>
-    <sheet name="deparser" sheetId="2" r:id="rId2"/>
+    <sheet name="mat" sheetId="3" r:id="rId2"/>
+    <sheet name="deparser" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -661,6 +662,328 @@
     <author>Dianchao Wang</author>
   </authors>
   <commentList>
+    <comment ref="D6" authorId="0" shapeId="0" xr:uid="{FD23ABF1-9BA5-43EC-BD51-CD1D2C4163A7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>Dianchao Wang:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+boardered at nibble</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E6" authorId="0" shapeId="0" xr:uid="{A072DAF5-C9B0-4947-8A4B-34DF2F362652}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>Dianchao Wang:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+in nibble</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D9" authorId="0" shapeId="0" xr:uid="{48435A18-75AC-4A01-BDFA-9D53E3A996D4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>Dianchao Wang:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+boardered at nibble</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E9" authorId="0" shapeId="0" xr:uid="{E2857198-AF24-4C1C-9596-AE516EE637EB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>Dianchao Wang:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+in nibble</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D11" authorId="0" shapeId="0" xr:uid="{EA2363D6-F85A-42E6-8FFE-DA4AE48A21CC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>Dianchao Wang:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+boardered at nibble</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E11" authorId="0" shapeId="0" xr:uid="{F76CD282-689D-4F21-86A6-ED532F7CD372}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>Dianchao Wang:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+in nibble</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D12" authorId="0" shapeId="0" xr:uid="{185784FC-5D96-46AC-A768-2C895E7CF7F2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>Dianchao Wang:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+boardered at nibble</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E12" authorId="0" shapeId="0" xr:uid="{B826A159-F267-4848-98F5-AD093A73E5CD}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>Dianchao Wang:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+in nibble</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D16" authorId="0" shapeId="0" xr:uid="{ACD05614-D653-4576-AD66-24BC8BB78B46}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>Dianchao Wang:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+boardered at nibble</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D18" authorId="0" shapeId="0" xr:uid="{2D208463-E52D-44A0-82FB-FCF7F6E0CF94}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>Dianchao Wang:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+boardered at nibble</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D55" authorId="0" shapeId="0" xr:uid="{39D8881B-BC18-434C-A8F7-A45AD42A5267}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>Dianchao Wang:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+boardered at nibble</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D57" authorId="0" shapeId="0" xr:uid="{AD6B4964-80AF-492C-A8E5-94AAAA6F6F5F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>Dianchao Wang:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+boardered at nibble</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Dianchao Wang</author>
+  </authors>
+  <commentList>
     <comment ref="B74" authorId="0" shapeId="0" xr:uid="{04167267-17E0-4DF6-B54E-8EB3AC806BAB}">
       <text>
         <r>
@@ -822,7 +1145,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1187" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1398" uniqueCount="454">
   <si>
     <t>isr SHiFT</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -4374,6 +4697,935 @@
       </rPr>
       <t xml:space="preserve"> (1-40) } ,</t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MDF</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0b'00001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(length in byte)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(selection)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">{ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>off9</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> :</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">    to be replaced by immediate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">len </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>(1-8) } ,</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>imm32</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> ;</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">    or by AD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">    or modify metadata with mask</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(bit mask)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>mask16</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> ;</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">len </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>(1-4) } ,</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">AD [ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>idx6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ] ;</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">    the immediate or AD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0b'00010</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>COPY data between PHV &lt;---&gt; PHV</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">    or META &lt;---&gt; META</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">    or PHV &lt;---&gt; META</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">    or META &lt;---&gt; PHV</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(value to use)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">[ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>off9</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> ] ;</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">len </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>(1-16) } ,</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0b'00011</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Read Stateful Memory</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>line_offset2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> ;</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">PHV [ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>off9</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> ] ,</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>base_addr_h36</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> ,</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">AD { </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">index </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Write Stateful Memory</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>META { STM_ADDR :</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>( destination )</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> ( source )</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>left_shift3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> } ,</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0b'00100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>COUNT packet &amp; byte</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>COUNT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>counter_id24</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> ;</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">AD [ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>index</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> ] ;</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Meter packet &amp; byte</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>METER</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">META [ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>offset9</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ] ;</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>meter_id11</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> ,</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">AD [ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>index</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> ] ,</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0b'00101</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0b'00110</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LOCK / UnLoCK access to public resource</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LOCK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ULCK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>flow_id24</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ;</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>AD [</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> index</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ] ;</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MDFL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">PHV { </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>offset9</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> :</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>len</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (1-16) } ,</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>imm32</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ;</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">AD [ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>idx6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ] ;</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ADDR [ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>imm10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ] ;</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0b'10100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0b'10101</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">[ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dst_off9</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ] ;</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">[ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>src_off9</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ] ,</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">[ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>src1_off9</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ] ,</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">[ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>src2_off9</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ] ,</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(length in 8b / 4b)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0b'10110</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>COPYL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0b'10111</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RSM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WSM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RSML</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WSML</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -4503,7 +5755,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -4561,11 +5813,17 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4903,9 +6161,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA14F7B7-5F50-4FFB-AE20-84853F321386}">
   <dimension ref="A1:I173"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A134" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F162" sqref="F162"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.2"/>
@@ -4929,15 +6187,15 @@
       <c r="B1" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
     </row>
     <row r="2" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B2" s="13" t="s">
@@ -4945,7 +6203,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -4968,7 +6226,6 @@
       <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
         <v>296</v>
@@ -4987,7 +6244,6 @@
       <c r="I4" s="2"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
         <v>296</v>
@@ -5006,7 +6262,6 @@
       <c r="I5" s="2"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
         <v>296</v>
@@ -5021,7 +6276,6 @@
       <c r="I6" s="2"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -5032,7 +6286,7 @@
       <c r="I7" s="2"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>81</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -5061,7 +6315,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>82</v>
       </c>
       <c r="B9" s="2"/>
@@ -5088,7 +6342,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>83</v>
       </c>
       <c r="B10" s="2"/>
@@ -5115,7 +6369,6 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2" t="s">
         <v>296</v>
@@ -5160,7 +6413,6 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2" t="s">
         <v>296</v>
@@ -5185,7 +6437,6 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2" t="s">
         <v>296</v>
@@ -5206,7 +6457,6 @@
       <c r="I14" s="2"/>
     </row>
     <row r="15" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="8"/>
       <c r="B15" s="13" t="s">
         <v>134</v>
       </c>
@@ -5219,7 +6469,7 @@
       <c r="I15" s="8"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="1" t="s">
         <v>80</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -5246,7 +6496,6 @@
       <c r="I16" s="2"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2" t="s">
         <v>322</v>
@@ -5269,7 +6518,6 @@
       <c r="I17" s="2"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2" t="s">
         <v>322</v>
@@ -5292,7 +6540,6 @@
       <c r="I18" s="2"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2" t="s">
         <v>322</v>
@@ -5311,7 +6558,6 @@
       <c r="I19" s="2"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2" t="s">
         <v>319</v>
@@ -5334,7 +6580,6 @@
       <c r="I20" s="2"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2" t="s">
         <v>319</v>
@@ -5357,7 +6602,6 @@
       <c r="I21" s="2"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2" t="s">
         <v>319</v>
@@ -5376,7 +6620,6 @@
       <c r="I22" s="2"/>
     </row>
     <row r="23" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="8"/>
       <c r="B23" s="13" t="s">
         <v>133</v>
       </c>
@@ -5389,7 +6632,7 @@
       <c r="I23" s="8"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="1" t="s">
         <v>78</v>
       </c>
       <c r="B24" s="2" t="s">
@@ -5416,7 +6659,7 @@
       <c r="I24" s="2"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="1" t="s">
         <v>79</v>
       </c>
       <c r="B25" s="2"/>
@@ -5441,7 +6684,6 @@
       <c r="I25" s="2"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2" t="s">
         <v>322</v>
@@ -5464,7 +6706,6 @@
       <c r="I26" s="2"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2" t="s">
         <v>322</v>
@@ -5483,7 +6724,6 @@
       <c r="I27" s="2"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2" t="s">
         <v>319</v>
@@ -5506,7 +6746,6 @@
       <c r="I28" s="2"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2" t="s">
         <v>319</v>
@@ -5529,7 +6768,6 @@
       <c r="I29" s="2"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2" t="s">
         <v>319</v>
@@ -5548,7 +6786,6 @@
       <c r="I30" s="2"/>
     </row>
     <row r="31" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="8"/>
       <c r="B31" s="13" t="s">
         <v>136</v>
       </c>
@@ -5561,7 +6798,7 @@
       <c r="I31" s="8"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32" s="2" t="s">
+      <c r="A32" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B32" s="2" t="s">
@@ -5576,7 +6813,6 @@
       <c r="I32" s="2"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A33" s="2"/>
       <c r="B33" s="2" t="s">
         <v>168</v>
       </c>
@@ -5603,7 +6839,6 @@
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" s="2"/>
       <c r="C34" s="2" t="s">
         <v>322</v>
       </c>
@@ -5627,7 +6862,6 @@
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A35" s="2"/>
       <c r="C35" s="2" t="s">
         <v>322</v>
       </c>
@@ -5651,7 +6885,6 @@
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A36" s="2"/>
       <c r="C36" s="2" t="s">
         <v>322</v>
       </c>
@@ -5671,7 +6904,6 @@
       <c r="I36" s="2"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A37" s="2"/>
       <c r="C37" s="2" t="s">
         <v>319</v>
       </c>
@@ -5695,7 +6927,6 @@
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A38" s="2"/>
       <c r="C38" s="2" t="s">
         <v>319</v>
       </c>
@@ -5719,7 +6950,6 @@
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A39" s="2"/>
       <c r="C39" s="2" t="s">
         <v>319</v>
       </c>
@@ -5739,7 +6969,6 @@
       <c r="I39" s="2"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A40" s="2"/>
       <c r="C40" s="2" t="s">
         <v>322</v>
       </c>
@@ -5763,7 +6992,6 @@
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A41" s="2"/>
       <c r="C41" s="2" t="s">
         <v>322</v>
       </c>
@@ -5787,7 +7015,6 @@
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A42" s="2"/>
       <c r="C42" s="2" t="s">
         <v>322</v>
       </c>
@@ -5807,7 +7034,6 @@
       <c r="I42" s="2"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A43" s="2"/>
       <c r="C43" s="2" t="s">
         <v>319</v>
       </c>
@@ -5831,7 +7057,6 @@
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A44" s="2"/>
       <c r="C44" s="2" t="s">
         <v>319</v>
       </c>
@@ -5855,7 +7080,6 @@
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A45" s="2"/>
       <c r="C45" s="2" t="s">
         <v>319</v>
       </c>
@@ -5875,7 +7099,6 @@
       <c r="I45" s="2"/>
     </row>
     <row r="46" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="8"/>
       <c r="B46" s="13" t="s">
         <v>135</v>
       </c>
@@ -5888,7 +7111,7 @@
       <c r="I46" s="8"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A47" s="2" t="s">
+      <c r="A47" s="1" t="s">
         <v>370</v>
       </c>
       <c r="B47" s="2" t="s">
@@ -5911,7 +7134,7 @@
       <c r="I47" s="2"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A48" s="2" t="s">
+      <c r="A48" s="1" t="s">
         <v>85</v>
       </c>
       <c r="B48" s="2"/>
@@ -5931,8 +7154,7 @@
       <c r="H48" s="2"/>
       <c r="I48" s="2"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A49" s="2"/>
+    <row r="49" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B49" s="2"/>
       <c r="C49" s="2" t="s">
         <v>371</v>
@@ -5950,8 +7172,7 @@
       <c r="H49" s="2"/>
       <c r="I49" s="2"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A50" s="2"/>
+    <row r="50" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B50" s="2"/>
       <c r="C50" s="2" t="s">
         <v>371</v>
@@ -5965,8 +7186,7 @@
       <c r="H50" s="2"/>
       <c r="I50" s="2"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A51" s="2"/>
+    <row r="51" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B51" s="2"/>
       <c r="C51" s="2" t="s">
         <v>372</v>
@@ -5984,8 +7204,7 @@
       <c r="H51" s="2"/>
       <c r="I51" s="2"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A52" s="2"/>
+    <row r="52" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B52" s="2"/>
       <c r="C52" s="2" t="s">
         <v>372</v>
@@ -6003,8 +7222,7 @@
       <c r="H52" s="2"/>
       <c r="I52" s="2"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A53" s="2"/>
+    <row r="53" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B53" s="2"/>
       <c r="C53" s="2" t="s">
         <v>372</v>
@@ -6018,8 +7236,7 @@
       <c r="H53" s="2"/>
       <c r="I53" s="2"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A54" s="2"/>
+    <row r="54" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B54" s="2"/>
       <c r="C54" s="2" t="s">
         <v>373</v>
@@ -6037,8 +7254,7 @@
       <c r="H54" s="2"/>
       <c r="I54" s="2"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A55" s="2"/>
+    <row r="55" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B55" s="2"/>
       <c r="C55" s="2" t="s">
         <v>373</v>
@@ -6056,8 +7272,7 @@
       <c r="H55" s="2"/>
       <c r="I55" s="2"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A56" s="2"/>
+    <row r="56" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B56" s="2"/>
       <c r="C56" s="2" t="s">
         <v>373</v>
@@ -6071,8 +7286,7 @@
       <c r="H56" s="2"/>
       <c r="I56" s="2"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A57" s="2"/>
+    <row r="57" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B57" s="2"/>
       <c r="C57" s="2" t="s">
         <v>374</v>
@@ -6090,8 +7304,7 @@
       <c r="H57" s="2"/>
       <c r="I57" s="2"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A58" s="2"/>
+    <row r="58" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B58" s="2"/>
       <c r="C58" s="2" t="s">
         <v>374</v>
@@ -6109,8 +7322,7 @@
       <c r="H58" s="2"/>
       <c r="I58" s="2"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A59" s="2"/>
+    <row r="59" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B59" s="2"/>
       <c r="C59" s="2" t="s">
         <v>374</v>
@@ -6124,8 +7336,7 @@
       <c r="H59" s="2"/>
       <c r="I59" s="2"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A60" s="2"/>
+    <row r="60" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B60" s="2"/>
       <c r="C60" s="2" t="s">
         <v>375</v>
@@ -6143,8 +7354,7 @@
       <c r="H60" s="2"/>
       <c r="I60" s="2"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A61" s="2"/>
+    <row r="61" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B61" s="2"/>
       <c r="C61" s="2" t="s">
         <v>375</v>
@@ -6162,8 +7372,7 @@
       <c r="H61" s="2"/>
       <c r="I61" s="2"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A62" s="2"/>
+    <row r="62" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B62" s="2"/>
       <c r="C62" s="2" t="s">
         <v>375</v>
@@ -6177,8 +7386,7 @@
       <c r="H62" s="2"/>
       <c r="I62" s="2"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A63" s="2"/>
+    <row r="63" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B63" s="2"/>
       <c r="C63" s="2" t="s">
         <v>376</v>
@@ -6196,8 +7404,7 @@
       <c r="H63" s="2"/>
       <c r="I63" s="2"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A64" s="2"/>
+    <row r="64" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B64" s="2"/>
       <c r="C64" s="2" t="s">
         <v>376</v>
@@ -6216,7 +7423,6 @@
       <c r="I64" s="2"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2" t="s">
         <v>376</v>
@@ -6231,7 +7437,6 @@
       <c r="I65" s="2"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A66" s="2"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2" t="s">
         <v>377</v>
@@ -6250,7 +7455,6 @@
       <c r="I66" s="2"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A67" s="2"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2" t="s">
         <v>377</v>
@@ -6269,7 +7473,6 @@
       <c r="I67" s="2"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2" t="s">
         <v>377</v>
@@ -6284,7 +7487,6 @@
       <c r="I68" s="2"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A69" s="2"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2" t="s">
         <v>378</v>
@@ -6303,7 +7505,6 @@
       <c r="I69" s="2"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A70" s="2"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2" t="s">
         <v>378</v>
@@ -6322,7 +7523,6 @@
       <c r="I70" s="2"/>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A71" s="2"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2" t="s">
         <v>378</v>
@@ -6337,7 +7537,6 @@
       <c r="I71" s="2"/>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A72" s="2"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2" t="s">
         <v>379</v>
@@ -6356,7 +7555,6 @@
       <c r="I72" s="2"/>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2" t="s">
         <v>379</v>
@@ -6375,7 +7573,6 @@
       <c r="I73" s="2"/>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2" t="s">
         <v>379</v>
@@ -6390,7 +7587,6 @@
       <c r="I74" s="2"/>
     </row>
     <row r="75" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="8"/>
       <c r="B75" s="13" t="s">
         <v>137</v>
       </c>
@@ -6403,7 +7599,7 @@
       <c r="I75" s="8"/>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A76" s="2" t="s">
+      <c r="A76" s="1" t="s">
         <v>86</v>
       </c>
       <c r="G76" s="2"/>
@@ -6411,7 +7607,7 @@
       <c r="I76" s="2"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A77" s="2" t="s">
+      <c r="A77" s="1" t="s">
         <v>98</v>
       </c>
       <c r="B77" s="2" t="s">
@@ -6431,7 +7627,6 @@
       <c r="I77" s="2"/>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A78" s="2"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2" t="s">
         <v>302</v>
@@ -6445,7 +7640,6 @@
       <c r="I78" s="2"/>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A79" s="2"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2" t="s">
         <v>302</v>
@@ -6461,7 +7655,7 @@
       <c r="I79" s="2"/>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A80" s="2" t="s">
+      <c r="A80" s="1" t="s">
         <v>97</v>
       </c>
       <c r="B80" s="2" t="s">
@@ -6476,7 +7670,6 @@
       <c r="I80" s="2"/>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A81" s="2"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2" t="s">
         <v>302</v>
@@ -6491,7 +7684,6 @@
       <c r="I81" s="2"/>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A82" s="2"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2" t="s">
         <v>302</v>
@@ -6508,7 +7700,6 @@
       <c r="I82" s="2"/>
     </row>
     <row r="83" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="8"/>
       <c r="B83" s="13" t="s">
         <v>145</v>
       </c>
@@ -6521,7 +7712,7 @@
       <c r="I83" s="8"/>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A84" s="2" t="s">
+      <c r="A84" s="1" t="s">
         <v>138</v>
       </c>
       <c r="C84" s="2"/>
@@ -6532,7 +7723,7 @@
       <c r="I84" s="2"/>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A85" s="2" t="s">
+      <c r="A85" s="1" t="s">
         <v>158</v>
       </c>
       <c r="B85" s="2" t="s">
@@ -6546,7 +7737,6 @@
       <c r="I85" s="2"/>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A86" s="2"/>
       <c r="C86" s="1" t="s">
         <v>205</v>
       </c>
@@ -6558,7 +7748,6 @@
       <c r="I86" s="2"/>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A87" s="2"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2" t="s">
         <v>305</v>
@@ -6571,7 +7760,6 @@
       <c r="I87" s="2"/>
     </row>
     <row r="88" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="8"/>
       <c r="B88" s="13" t="s">
         <v>146</v>
       </c>
@@ -6584,7 +7772,7 @@
       <c r="I88" s="8"/>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A89" s="2" t="s">
+      <c r="A89" s="1" t="s">
         <v>138</v>
       </c>
       <c r="C89" s="2"/>
@@ -6595,7 +7783,7 @@
       <c r="I89" s="2"/>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A90" s="2" t="s">
+      <c r="A90" s="1" t="s">
         <v>87</v>
       </c>
       <c r="B90" s="2" t="s">
@@ -6609,7 +7797,6 @@
       <c r="I90" s="2"/>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A91" s="2"/>
       <c r="C91" s="1" t="s">
         <v>205</v>
       </c>
@@ -6621,7 +7808,6 @@
       <c r="I91" s="2"/>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A92" s="2"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2" t="s">
         <v>305</v>
@@ -6634,7 +7820,6 @@
       <c r="I92" s="2"/>
     </row>
     <row r="93" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="8"/>
       <c r="B93" s="13" t="s">
         <v>139</v>
       </c>
@@ -6647,7 +7832,7 @@
       <c r="I93" s="8"/>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A94" s="2" t="s">
+      <c r="A94" s="1" t="s">
         <v>88</v>
       </c>
       <c r="B94" s="2" t="s">
@@ -6662,7 +7847,6 @@
       <c r="I94" s="2"/>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A95" s="2"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2" t="s">
         <v>205</v>
@@ -6675,7 +7859,6 @@
       <c r="I95" s="2"/>
     </row>
     <row r="96" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="8"/>
       <c r="B96" s="13" t="s">
         <v>140</v>
       </c>
@@ -6688,7 +7871,7 @@
       <c r="I96" s="8"/>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A97" s="2" t="s">
+      <c r="A97" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B97" s="2" t="s">
@@ -6706,7 +7889,6 @@
       <c r="I97" s="2"/>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A98" s="2"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2" t="s">
         <v>306</v>
@@ -6718,7 +7900,6 @@
       <c r="I98" s="2"/>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A99" s="2"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2" t="s">
         <v>307</v>
@@ -6732,7 +7913,6 @@
       <c r="I99" s="2"/>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A100" s="2"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2" t="s">
         <v>307</v>
@@ -6746,7 +7926,6 @@
       <c r="I100" s="2"/>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A101" s="2"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2" t="s">
         <v>307</v>
@@ -6760,19 +7939,17 @@
       <c r="I101" s="2"/>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A102" s="2"/>
       <c r="B102" s="2"/>
-      <c r="C102" s="20" t="s">
+      <c r="C102" s="21" t="s">
         <v>205</v>
       </c>
-      <c r="D102" s="20"/>
+      <c r="D102" s="21"/>
       <c r="F102" s="2"/>
       <c r="G102" s="2"/>
       <c r="H102" s="2"/>
       <c r="I102" s="2"/>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A103" s="2"/>
       <c r="B103" s="2"/>
       <c r="D103" s="2" t="s">
         <v>308</v>
@@ -6783,7 +7960,6 @@
       <c r="I103" s="2"/>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A104" s="2"/>
       <c r="B104" s="2"/>
       <c r="D104" s="2" t="s">
         <v>309</v>
@@ -6794,7 +7970,6 @@
       <c r="I104" s="2"/>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A105" s="2"/>
       <c r="B105" s="2"/>
       <c r="D105" s="2" t="s">
         <v>310</v>
@@ -6805,7 +7980,6 @@
       <c r="I105" s="2"/>
     </row>
     <row r="106" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="8"/>
       <c r="B106" s="13" t="s">
         <v>141</v>
       </c>
@@ -6818,7 +7992,7 @@
       <c r="I106" s="8"/>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A107" s="2" t="s">
+      <c r="A107" s="1" t="s">
         <v>156</v>
       </c>
       <c r="B107" s="2" t="s">
@@ -6839,7 +8013,6 @@
       <c r="I107" s="2"/>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A108" s="2"/>
       <c r="B108" s="2"/>
       <c r="C108" s="2" t="s">
         <v>311</v>
@@ -6853,7 +8026,6 @@
       <c r="I108" s="2"/>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A109" s="2"/>
       <c r="B109" s="2"/>
       <c r="C109" s="2" t="s">
         <v>312</v>
@@ -6867,7 +8039,6 @@
       <c r="I109" s="2"/>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A110" s="2"/>
       <c r="B110" s="2"/>
       <c r="C110" s="2" t="s">
         <v>313</v>
@@ -6884,7 +8055,6 @@
       <c r="I110" s="2"/>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A111" s="2"/>
       <c r="B111" s="2"/>
       <c r="C111" s="2" t="s">
         <v>314</v>
@@ -6898,7 +8068,6 @@
       <c r="I111" s="2"/>
     </row>
     <row r="112" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A112" s="8"/>
       <c r="B112" s="13" t="s">
         <v>142</v>
       </c>
@@ -6911,7 +8080,7 @@
       <c r="I112" s="8"/>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A113" s="2" t="s">
+      <c r="A113" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B113" s="2" t="s">
@@ -6926,7 +8095,7 @@
       <c r="I113" s="2"/>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A114" s="12" t="s">
+      <c r="A114" s="3" t="s">
         <v>96</v>
       </c>
       <c r="B114" s="12" t="s">
@@ -6949,7 +8118,6 @@
       <c r="I114" s="2"/>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A115" s="2"/>
       <c r="B115" s="2"/>
       <c r="C115" s="15" t="s">
         <v>209</v>
@@ -6968,7 +8136,6 @@
       <c r="I115" s="2"/>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A116" s="2"/>
       <c r="B116" s="2"/>
       <c r="C116" s="2" t="s">
         <v>262</v>
@@ -6987,7 +8154,6 @@
       <c r="I116" s="2"/>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A117" s="2"/>
       <c r="B117" s="2"/>
       <c r="C117" s="2" t="s">
         <v>319</v>
@@ -7006,7 +8172,6 @@
       <c r="I117" s="2"/>
     </row>
     <row r="118" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="8"/>
       <c r="B118" s="13" t="s">
         <v>143</v>
       </c>
@@ -7019,7 +8184,7 @@
       <c r="I118" s="8"/>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A119" s="2" t="s">
+      <c r="A119" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B119" s="2" t="s">
@@ -7034,7 +8199,7 @@
       <c r="I119" s="2"/>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A120" s="12" t="s">
+      <c r="A120" s="3" t="s">
         <v>96</v>
       </c>
       <c r="B120" s="12" t="s">
@@ -7057,7 +8222,6 @@
       <c r="I120" s="2"/>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A121" s="2"/>
       <c r="B121" s="2"/>
       <c r="C121" s="15" t="s">
         <v>209</v>
@@ -7076,7 +8240,6 @@
       <c r="I121" s="2"/>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A122" s="2"/>
       <c r="B122" s="2"/>
       <c r="C122" s="2" t="s">
         <v>262</v>
@@ -7095,7 +8258,6 @@
       <c r="I122" s="2"/>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A123" s="2"/>
       <c r="B123" s="2"/>
       <c r="C123" s="2" t="s">
         <v>319</v>
@@ -7114,7 +8276,6 @@
       <c r="I123" s="2"/>
     </row>
     <row r="124" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A124" s="8"/>
       <c r="B124" s="13" t="s">
         <v>144</v>
       </c>
@@ -7127,7 +8288,7 @@
       <c r="I124" s="8"/>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A125" s="2" t="s">
+      <c r="A125" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B125" s="2" t="s">
@@ -7137,7 +8298,7 @@
       <c r="I125" s="2"/>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A126" s="12" t="s">
+      <c r="A126" s="3" t="s">
         <v>96</v>
       </c>
       <c r="B126" s="12" t="s">
@@ -7159,7 +8320,6 @@
       <c r="I126" s="2"/>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A127" s="2"/>
       <c r="B127" s="2"/>
       <c r="C127" s="15" t="s">
         <v>209</v>
@@ -7178,7 +8338,6 @@
       <c r="I127" s="2"/>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A128" s="2"/>
       <c r="B128" s="2"/>
       <c r="C128" s="2" t="s">
         <v>262</v>
@@ -7197,7 +8356,6 @@
       <c r="I128" s="2"/>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A129" s="2"/>
       <c r="B129" s="2"/>
       <c r="C129" s="2" t="s">
         <v>319</v>
@@ -7216,7 +8374,6 @@
       <c r="I129" s="2"/>
     </row>
     <row r="130" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A130" s="8"/>
       <c r="B130" s="13" t="s">
         <v>147</v>
       </c>
@@ -7229,7 +8386,7 @@
       <c r="I130" s="8"/>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A131" s="2" t="s">
+      <c r="A131" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B131" s="2" t="s">
@@ -7244,7 +8401,6 @@
       <c r="I131" s="2"/>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A132" s="2"/>
       <c r="B132" s="2"/>
       <c r="C132" s="1" t="s">
         <v>205</v>
@@ -7257,7 +8413,6 @@
       <c r="I132" s="2"/>
     </row>
     <row r="133" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A133" s="8"/>
       <c r="B133" s="13" t="s">
         <v>148</v>
       </c>
@@ -7269,7 +8424,7 @@
       <c r="I133" s="8"/>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A134" s="2" t="s">
+      <c r="A134" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B134" s="2" t="s">
@@ -7283,7 +8438,6 @@
       <c r="I134" s="2"/>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A135" s="2"/>
       <c r="B135" s="2"/>
       <c r="C135" s="1" t="s">
         <v>205</v>
@@ -7296,7 +8450,6 @@
       <c r="I135" s="2"/>
     </row>
     <row r="136" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A136" s="8"/>
       <c r="B136" s="13" t="s">
         <v>149</v>
       </c>
@@ -7308,7 +8461,7 @@
       <c r="I136" s="8"/>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A137" s="2" t="s">
+      <c r="A137" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B137" s="2" t="s">
@@ -7322,7 +8475,6 @@
       <c r="I137" s="2"/>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A138" s="2"/>
       <c r="B138" s="2"/>
       <c r="C138" s="1" t="s">
         <v>205</v>
@@ -7335,7 +8487,6 @@
       <c r="I138" s="2"/>
     </row>
     <row r="139" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A139" s="8"/>
       <c r="B139" s="13" t="s">
         <v>150</v>
       </c>
@@ -7361,7 +8512,7 @@
       <c r="I140" s="2"/>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A141" s="2" t="s">
+      <c r="A141" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B141" s="2" t="s">
@@ -7376,7 +8527,7 @@
       <c r="I141" s="2"/>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A142" s="2" t="s">
+      <c r="A142" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B142" s="2" t="s">
@@ -7391,7 +8542,7 @@
       <c r="I142" s="2"/>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A143" s="2" t="s">
+      <c r="A143" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B143" s="2" t="s">
@@ -7406,7 +8557,7 @@
       <c r="I143" s="2"/>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A144" s="2" t="s">
+      <c r="A144" s="1" t="s">
         <v>287</v>
       </c>
       <c r="B144" s="2" t="s">
@@ -7421,7 +8572,7 @@
       <c r="I144" s="2"/>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A145" s="2" t="s">
+      <c r="A145" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B145" s="2" t="s">
@@ -7436,7 +8587,7 @@
       <c r="I145" s="2"/>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A146" s="2" t="s">
+      <c r="A146" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B146" s="2" t="s">
@@ -7538,7 +8689,6 @@
       <c r="I152" s="2"/>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A153" s="2"/>
       <c r="B153" s="2" t="s">
         <v>195</v>
       </c>
@@ -7551,7 +8701,6 @@
       <c r="I153" s="2"/>
     </row>
     <row r="154" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A154" s="8"/>
       <c r="B154" s="13" t="s">
         <v>152</v>
       </c>
@@ -7564,12 +8713,12 @@
       <c r="I154" s="8"/>
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A155" s="2" t="s">
+      <c r="A155" s="1" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A156" s="2" t="s">
+      <c r="A156" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B156" s="2" t="s">
@@ -7697,7 +8846,6 @@
       </c>
     </row>
     <row r="164" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A164" s="8"/>
       <c r="B164" s="13" t="s">
         <v>154</v>
       </c>
@@ -7710,12 +8858,12 @@
       <c r="I164" s="8"/>
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A165" s="2" t="s">
+      <c r="A165" s="1" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A166" s="2" t="s">
+      <c r="A166" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B166" s="2" t="s">
@@ -7736,7 +8884,6 @@
       </c>
     </row>
     <row r="169" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A169" s="8"/>
       <c r="B169" s="13" t="s">
         <v>153</v>
       </c>
@@ -7749,12 +8896,12 @@
       <c r="I169" s="8"/>
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A170" s="2" t="s">
+      <c r="A170" s="1" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A171" s="2" t="s">
+      <c r="A171" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B171" s="2" t="s">
@@ -7786,12 +8933,842 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{732D935C-EC39-4DBE-84B4-44CD168E0101}">
+  <dimension ref="A1:I66"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B59" sqref="B59"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="36.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="3" customFormat="1" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+    </row>
+    <row r="2" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="16" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="G4" t="s">
+        <v>393</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" spans="1:9" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="B6" s="2"/>
+      <c r="C6" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>391</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="C8" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="C9" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>392</v>
+      </c>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>397</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="C12" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>396</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="16" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
+        <v>399</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>400</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
+        <v>401</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
+        <v>402</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="C18" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="16" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>407</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>450</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>415</v>
+      </c>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+    </row>
+    <row r="21" spans="1:7" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="B21" s="4"/>
+      <c r="C21" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="C22" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>416</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="C23" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>416</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>412</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>451</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="D24" s="22" t="s">
+        <v>414</v>
+      </c>
+      <c r="E24" s="22"/>
+      <c r="F24" s="22"/>
+    </row>
+    <row r="25" spans="1:7" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="B25" s="4"/>
+      <c r="C25" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="C26" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>416</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="C27" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>416</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B28" s="16" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>418</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="C30" s="1" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="C31" s="1" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="16" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>422</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>423</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="D33" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="C34" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="D34" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B35" s="16" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>429</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B37" s="4" t="s">
+        <v>431</v>
+      </c>
+      <c r="C37" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C38" s="5" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C39" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B41" s="16" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B42" s="4" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C43" t="s">
+        <v>435</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>436</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C44" t="s">
+        <v>435</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>436</v>
+      </c>
+      <c r="E44" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C45" t="s">
+        <v>435</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>436</v>
+      </c>
+      <c r="E45" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B46" s="16" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B47" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="B48" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="D48" t="s">
+        <v>443</v>
+      </c>
+      <c r="G48" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="H48" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="B49" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="D49" t="s">
+        <v>443</v>
+      </c>
+      <c r="G49" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="H49" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="B50" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="D50" t="s">
+        <v>444</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="F50" t="s">
+        <v>445</v>
+      </c>
+      <c r="G50" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="H50" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="B51" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="D51" t="s">
+        <v>444</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="F51" t="s">
+        <v>445</v>
+      </c>
+      <c r="G51" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="H51" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B52" s="16" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="53" spans="2:8" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="B53" s="4" t="s">
+        <v>448</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="C54" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="C55" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="56" spans="2:8" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="C56" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="C57" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="G57" s="2" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="58" spans="2:8" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B58" s="16" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="B59" s="4" t="s">
+        <v>452</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="D59" s="20" t="s">
+        <v>415</v>
+      </c>
+      <c r="E59" s="20"/>
+      <c r="F59" s="20"/>
+    </row>
+    <row r="60" spans="2:8" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="B60" s="4"/>
+      <c r="C60" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="61" spans="2:8" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="C61" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="E61" s="5" t="s">
+        <v>416</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="62" spans="2:8" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="C62" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="E62" s="5" t="s">
+        <v>416</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="63" spans="2:8" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="B63" s="4" t="s">
+        <v>453</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="D63" s="22" t="s">
+        <v>414</v>
+      </c>
+      <c r="E63" s="22"/>
+      <c r="F63" s="22"/>
+    </row>
+    <row r="64" spans="2:8" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="B64" s="4"/>
+      <c r="C64" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="65" spans="3:6" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="C65" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>416</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="66" spans="3:6" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="C66" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="E66" s="5" t="s">
+        <v>416</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>408</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="C1:I1"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="D59:F59"/>
+    <mergeCell ref="D63:F63"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{988C78EB-4E00-466C-9BD2-B10965380DEB}">
   <dimension ref="A1:I233"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E223" sqref="E223:F227"/>
+      <pane ySplit="1" topLeftCell="A192" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -7814,15 +9791,15 @@
       <c r="B1" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
     </row>
     <row r="2" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B2" s="16" t="s">
@@ -7830,12 +9807,12 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="5" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="5" t="s">
         <v>100</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -7843,7 +9820,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="5" t="s">
         <v>99</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -7851,7 +9828,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="5" t="s">
         <v>277</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -7860,13 +9837,13 @@
       <c r="C6" s="4"/>
     </row>
     <row r="7" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="6"/>
+      <c r="A7" s="19"/>
       <c r="B7" s="17" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="5" t="s">
         <v>74</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -8021,7 +9998,7 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="5" t="s">
         <v>75</v>
       </c>
       <c r="B23" s="4" t="s">
@@ -8679,7 +10656,7 @@
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A74" s="4" t="s">
+      <c r="A74" s="5" t="s">
         <v>44</v>
       </c>
       <c r="B74" s="4" t="s">
@@ -8692,7 +10669,7 @@
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A76" s="4" t="s">
+      <c r="A76" s="5" t="s">
         <v>200</v>
       </c>
       <c r="B76" s="4" t="s">
@@ -8725,12 +10702,12 @@
       </c>
     </row>
     <row r="79" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A79" s="2" t="s">
+      <c r="A79" s="1" t="s">
         <v>332</v>
       </c>
     </row>
     <row r="80" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A80" s="2" t="s">
+      <c r="A80" s="1" t="s">
         <v>102</v>
       </c>
       <c r="B80" s="2" t="s">
@@ -8744,7 +10721,7 @@
       </c>
     </row>
     <row r="81" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A81" s="2"/>
+      <c r="A81" s="1"/>
       <c r="B81" s="2"/>
       <c r="C81" s="4" t="s">
         <v>335</v>
@@ -8754,7 +10731,7 @@
       </c>
     </row>
     <row r="82" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A82" s="2"/>
+      <c r="A82" s="1"/>
       <c r="B82" s="2"/>
       <c r="C82" s="4" t="s">
         <v>336</v>
@@ -8764,7 +10741,7 @@
       </c>
     </row>
     <row r="83" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A83" s="2"/>
+      <c r="A83" s="1"/>
       <c r="B83" s="2"/>
       <c r="C83" s="4" t="s">
         <v>337</v>
@@ -8774,7 +10751,7 @@
       </c>
     </row>
     <row r="84" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A84" s="2"/>
+      <c r="A84" s="1"/>
       <c r="B84" s="2"/>
       <c r="C84" s="4" t="s">
         <v>338</v>
@@ -8784,7 +10761,7 @@
       </c>
     </row>
     <row r="85" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A85" s="2"/>
+      <c r="A85" s="1"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2" t="s">
         <v>311</v>
@@ -8805,7 +10782,7 @@
       </c>
     </row>
     <row r="87" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A87" s="2"/>
+      <c r="A87" s="1"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2" t="s">
         <v>312</v>
@@ -8815,7 +10792,7 @@
       </c>
     </row>
     <row r="88" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A88" s="2"/>
+      <c r="A88" s="1"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2" t="s">
         <v>314</v>
@@ -8825,7 +10802,7 @@
       </c>
     </row>
     <row r="89" spans="1:5" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A89" s="8"/>
+      <c r="A89" s="9"/>
       <c r="B89" s="10" t="s">
         <v>137</v>
       </c>
@@ -8833,7 +10810,7 @@
       <c r="D89" s="8"/>
     </row>
     <row r="90" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A90" s="4" t="s">
+      <c r="A90" s="5" t="s">
         <v>101</v>
       </c>
       <c r="B90" s="2" t="s">
@@ -8847,7 +10824,7 @@
       </c>
     </row>
     <row r="91" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A91" s="2"/>
+      <c r="A91" s="1"/>
       <c r="B91" s="2"/>
       <c r="C91" s="4" t="s">
         <v>335</v>
@@ -8857,7 +10834,7 @@
       </c>
     </row>
     <row r="92" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A92" s="2"/>
+      <c r="A92" s="1"/>
       <c r="B92" s="2"/>
       <c r="C92" s="4" t="s">
         <v>336</v>
@@ -8867,7 +10844,7 @@
       </c>
     </row>
     <row r="93" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A93" s="2"/>
+      <c r="A93" s="1"/>
       <c r="B93" s="2"/>
       <c r="C93" s="4" t="s">
         <v>337</v>
@@ -8925,7 +10902,7 @@
       </c>
     </row>
     <row r="100" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A100" s="4" t="s">
+      <c r="A100" s="5" t="s">
         <v>157</v>
       </c>
       <c r="B100" s="4" t="s">
@@ -8951,7 +10928,7 @@
       </c>
     </row>
     <row r="101" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A101" s="4" t="s">
+      <c r="A101" s="5" t="s">
         <v>90</v>
       </c>
       <c r="C101" s="1" t="s">
@@ -9059,7 +11036,7 @@
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A112" s="4" t="s">
+      <c r="A112" s="5" t="s">
         <v>91</v>
       </c>
       <c r="B112" s="4" t="s">
@@ -9122,7 +11099,7 @@
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A119" s="4" t="s">
+      <c r="A119" s="5" t="s">
         <v>201</v>
       </c>
       <c r="B119" s="4" t="s">
@@ -9188,49 +11165,49 @@
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A126" s="4"/>
+      <c r="A126" s="5"/>
       <c r="B126" s="4" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A127" s="4"/>
+      <c r="A127" s="5"/>
       <c r="B127" s="18" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="128" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A128" s="6"/>
+      <c r="A128" s="19"/>
       <c r="B128" s="17" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A129" s="4"/>
+      <c r="A129" s="5"/>
       <c r="B129" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A130" s="4"/>
+      <c r="A130" s="5"/>
       <c r="B130" s="18" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="131" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A131" s="6"/>
+      <c r="A131" s="19"/>
       <c r="B131" s="17" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A132" s="4"/>
+      <c r="A132" s="5"/>
       <c r="B132" s="4" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A133" s="4"/>
+      <c r="A133" s="5"/>
       <c r="B133" s="18" t="s">
         <v>229</v>
       </c>
@@ -9586,12 +11563,12 @@
       </c>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A170" s="4" t="s">
+      <c r="A170" s="5" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A171" s="4" t="s">
+      <c r="A171" s="5" t="s">
         <v>128</v>
       </c>
       <c r="B171" s="11" t="s">
@@ -9599,7 +11576,7 @@
       </c>
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A172" s="4" t="s">
+      <c r="A172" s="5" t="s">
         <v>129</v>
       </c>
       <c r="B172" s="4" t="s">
@@ -9607,7 +11584,7 @@
       </c>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A173" s="4" t="s">
+      <c r="A173" s="5" t="s">
         <v>130</v>
       </c>
       <c r="B173" s="11" t="s">
@@ -9615,7 +11592,7 @@
       </c>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A174" s="4" t="s">
+      <c r="A174" s="5" t="s">
         <v>131</v>
       </c>
       <c r="B174" s="4" t="s">
@@ -9686,7 +11663,7 @@
       <c r="G178" s="4"/>
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A179" s="4" t="s">
+      <c r="A179" s="5" t="s">
         <v>350</v>
       </c>
       <c r="B179" s="4" t="s">
@@ -9715,7 +11692,7 @@
       <c r="G181" s="4"/>
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A182" s="4"/>
+      <c r="A182" s="5"/>
       <c r="B182" s="4"/>
       <c r="C182" s="4" t="s">
         <v>347</v>
@@ -9742,7 +11719,7 @@
       </c>
     </row>
     <row r="185" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A185" s="4" t="s">
+      <c r="A185" s="5" t="s">
         <v>244</v>
       </c>
       <c r="B185" s="4" t="s">
@@ -9750,7 +11727,7 @@
       </c>
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A186" s="4" t="s">
+      <c r="A186" s="5" t="s">
         <v>245</v>
       </c>
       <c r="B186" s="4"/>
@@ -9771,7 +11748,7 @@
       </c>
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A187" s="4"/>
+      <c r="A187" s="5"/>
       <c r="B187" s="4"/>
       <c r="C187" s="4" t="s">
         <v>262</v>
@@ -9790,7 +11767,7 @@
       </c>
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A188" s="4"/>
+      <c r="A188" s="5"/>
       <c r="B188" s="4"/>
       <c r="C188" s="4" t="s">
         <v>202</v>
@@ -9831,7 +11808,7 @@
       </c>
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A191" s="4" t="s">
+      <c r="A191" s="5" t="s">
         <v>94</v>
       </c>
     </row>
@@ -9871,7 +11848,7 @@
       </c>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A196" s="4" t="s">
+      <c r="A196" s="5" t="s">
         <v>62</v>
       </c>
       <c r="B196" s="4" t="s">
@@ -9889,12 +11866,12 @@
       </c>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A199" s="4" t="s">
+      <c r="A199" s="5" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A200" s="4" t="s">
+      <c r="A200" s="5" t="s">
         <v>69</v>
       </c>
       <c r="B200" s="4" t="s">
@@ -9914,13 +11891,13 @@
       </c>
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A201" s="4"/>
+      <c r="A201" s="5"/>
       <c r="C201" s="4" t="s">
         <v>353</v>
       </c>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A202" s="4" t="s">
+      <c r="A202" s="5" t="s">
         <v>70</v>
       </c>
       <c r="B202" s="4" t="s">
@@ -9928,13 +11905,13 @@
       </c>
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A203" s="4"/>
+      <c r="A203" s="5"/>
       <c r="C203" s="4" t="s">
         <v>352</v>
       </c>
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A204" s="4" t="s">
+      <c r="A204" s="5" t="s">
         <v>120</v>
       </c>
       <c r="B204" s="4" t="s">
@@ -9942,7 +11919,7 @@
       </c>
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A205" s="4" t="s">
+      <c r="A205" s="5" t="s">
         <v>127</v>
       </c>
       <c r="C205" s="4" t="s">
@@ -10015,7 +11992,7 @@
       </c>
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A210" s="4" t="s">
+      <c r="A210" s="5" t="s">
         <v>121</v>
       </c>
       <c r="B210" s="4" t="s">
@@ -10023,7 +12000,7 @@
       </c>
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A211" s="4" t="s">
+      <c r="A211" s="5" t="s">
         <v>127</v>
       </c>
       <c r="C211" s="4" t="s">
@@ -10096,7 +12073,7 @@
       </c>
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A216" s="4" t="s">
+      <c r="A216" s="5" t="s">
         <v>120</v>
       </c>
       <c r="B216" s="4" t="s">
@@ -10104,7 +12081,7 @@
       </c>
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A217" s="4" t="s">
+      <c r="A217" s="5" t="s">
         <v>126</v>
       </c>
       <c r="C217" s="4" t="s">
@@ -10177,7 +12154,7 @@
       </c>
     </row>
     <row r="222" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A222" s="4" t="s">
+      <c r="A222" s="5" t="s">
         <v>121</v>
       </c>
       <c r="B222" s="4" t="s">
@@ -10185,7 +12162,7 @@
       </c>
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A223" s="4" t="s">
+      <c r="A223" s="5" t="s">
         <v>126</v>
       </c>
       <c r="C223" s="4" t="s">
@@ -10263,7 +12240,7 @@
       </c>
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A229" s="4" t="s">
+      <c r="A229" s="5" t="s">
         <v>162</v>
       </c>
       <c r="B229" s="4" t="s">
@@ -10271,21 +12248,21 @@
       </c>
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A230" s="4"/>
+      <c r="A230" s="5"/>
       <c r="B230" s="4"/>
       <c r="C230" s="5" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="231" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A231" s="6"/>
+      <c r="A231" s="19"/>
       <c r="B231" s="17" t="s">
         <v>241</v>
       </c>
       <c r="C231" s="6"/>
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A232" s="4" t="s">
+      <c r="A232" s="5" t="s">
         <v>72</v>
       </c>
       <c r="B232" s="4" t="s">

</xml_diff>

<commit_message>
fix a few issues of parser and deparser instructions
</commit_message>
<xml_diff>
--- a/P4E_psuedo_instruction_set.xlsx
+++ b/P4E_psuedo_instruction_set.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\P4EngineAssembler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6DE9A96-11D2-4FB8-8DDC-5655A8F18640}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B4734BE-4D2F-4466-9B68-06DA7EFDAF94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{87164962-7B7D-4BAA-98E0-B9A8D7C47112}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{87164962-7B7D-4BAA-98E0-B9A8D7C47112}"/>
   </bookViews>
   <sheets>
     <sheet name="parser" sheetId="1" r:id="rId1"/>
@@ -6208,9 +6208,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA14F7B7-5F50-4FFB-AE20-84853F321386}">
   <dimension ref="A1:I173"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C128" sqref="C128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.2"/>
@@ -8185,7 +8185,7 @@
     <row r="116" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B116" s="2"/>
       <c r="C116" s="2" t="s">
-        <v>252</v>
+        <v>312</v>
       </c>
       <c r="D116" s="2" t="s">
         <v>310</v>
@@ -8289,7 +8289,7 @@
     <row r="122" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B122" s="2"/>
       <c r="C122" s="2" t="s">
-        <v>252</v>
+        <v>312</v>
       </c>
       <c r="D122" s="2" t="s">
         <v>310</v>
@@ -8387,7 +8387,7 @@
     <row r="128" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B128" s="2"/>
       <c r="C128" s="2" t="s">
-        <v>252</v>
+        <v>312</v>
       </c>
       <c r="D128" s="2" t="s">
         <v>310</v>
@@ -9813,7 +9813,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{988C78EB-4E00-466C-9BD2-B10965380DEB}">
   <dimension ref="A1:I243"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A180" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A201" sqref="A201"/>
     </sheetView>

</xml_diff>

<commit_message>
mat add NOP(L) instructions
</commit_message>
<xml_diff>
--- a/P4E_psuedo_instruction_set.xlsx
+++ b/P4E_psuedo_instruction_set.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\P4EngineAssembler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11174EC2-5B15-4517-9D46-EFC848D39B06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AB2B8B9-AA42-4D23-9E92-C447E5FDEE41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{87164962-7B7D-4BAA-98E0-B9A8D7C47112}"/>
+    <workbookView xWindow="-38520" yWindow="-3645" windowWidth="38640" windowHeight="21840" activeTab="1" xr2:uid="{87164962-7B7D-4BAA-98E0-B9A8D7C47112}"/>
   </bookViews>
   <sheets>
     <sheet name="parser" sheetId="1" r:id="rId1"/>
@@ -928,7 +928,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C32" authorId="0" shapeId="0" xr:uid="{0C0D1569-05B5-4671-BE18-70994A53B622}">
+    <comment ref="C34" authorId="0" shapeId="0" xr:uid="{0C0D1569-05B5-4671-BE18-70994A53B622}">
       <text>
         <r>
           <rPr>
@@ -954,7 +954,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C36" authorId="0" shapeId="0" xr:uid="{B7B4802A-BD39-4EFD-8EF3-BD5110CA966B}">
+    <comment ref="C38" authorId="0" shapeId="0" xr:uid="{B7B4802A-BD39-4EFD-8EF3-BD5110CA966B}">
       <text>
         <r>
           <rPr>
@@ -980,7 +980,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G54" authorId="0" shapeId="0" xr:uid="{935D5833-A655-4765-81F8-C6C0E8C143C3}">
+    <comment ref="G56" authorId="0" shapeId="0" xr:uid="{935D5833-A655-4765-81F8-C6C0E8C143C3}">
       <text>
         <r>
           <rPr>
@@ -1006,7 +1006,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G56" authorId="0" shapeId="0" xr:uid="{28896C20-A56E-4FB2-A2DA-D4EEEF5DF3A8}">
+    <comment ref="G58" authorId="0" shapeId="0" xr:uid="{28896C20-A56E-4FB2-A2DA-D4EEEF5DF3A8}">
       <text>
         <r>
           <rPr>
@@ -1032,7 +1032,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D60" authorId="0" shapeId="0" xr:uid="{39D8881B-BC18-434C-A8F7-A45AD42A5267}">
+    <comment ref="D62" authorId="0" shapeId="0" xr:uid="{39D8881B-BC18-434C-A8F7-A45AD42A5267}">
       <text>
         <r>
           <rPr>
@@ -1058,7 +1058,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D62" authorId="0" shapeId="0" xr:uid="{AD6B4964-80AF-492C-A8E5-94AAAA6F6F5F}">
+    <comment ref="D64" authorId="0" shapeId="0" xr:uid="{AD6B4964-80AF-492C-A8E5-94AAAA6F6F5F}">
       <text>
         <r>
           <rPr>
@@ -1281,7 +1281,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1359" uniqueCount="470">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1374" uniqueCount="475">
   <si>
     <t>isr SHiFT</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -5877,6 +5877,118 @@
   </si>
   <si>
     <t xml:space="preserve">    Branch to dest, if source Equals Zero</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NOPL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">{ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>0 :</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> }</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>[</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> 0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> ];</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>[</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> 0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> ] ;</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -9158,11 +9270,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{732D935C-EC39-4DBE-84B4-44CD168E0101}">
-  <dimension ref="A1:I70"/>
+  <dimension ref="A1:I74"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A70" sqref="A70:XFD70"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -9505,260 +9617,260 @@
         <v>370</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="15" t="s">
+    <row r="20" spans="1:7" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="B20" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="B21" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="15" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+    <row r="23" spans="1:7" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>378</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B23" s="4" t="s">
         <v>379</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>437</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="C22" s="1" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="C23" s="1" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="16.5" x14ac:dyDescent="0.2">
       <c r="C24" s="1" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="C25" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="C26" s="1" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="25" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="15" t="s">
+    <row r="27" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B27" s="15" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+    <row r="28" spans="1:7" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>381</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B28" s="4" t="s">
         <v>382</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>438</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D28" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="B27" s="4"/>
-      <c r="C27" s="1" t="s">
+    <row r="29" spans="1:7" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="B29" s="4"/>
+      <c r="C29" s="1" t="s">
         <v>461</v>
-      </c>
-      <c r="D27" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="B28" s="4"/>
-      <c r="C28" s="1"/>
-      <c r="D28" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="C29" s="1" t="s">
-        <v>383</v>
       </c>
       <c r="D29" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="30" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="15" t="s">
+    <row r="30" spans="1:7" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="B30" s="4"/>
+      <c r="C30" s="1"/>
+      <c r="D30" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="C31" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="D31" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="15" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+    <row r="33" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>386</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B33" s="4" t="s">
         <v>387</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C33" s="1" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B32" s="4"/>
-      <c r="C32" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B33" s="4"/>
-      <c r="C33" s="5" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B34" s="4"/>
       <c r="C34" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B35" s="4"/>
+      <c r="C35" s="5" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B36" s="4"/>
+      <c r="C36" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B35" s="15" t="s">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B37" s="15" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B36" s="4" t="s">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B38" s="4" t="s">
         <v>388</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C38" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C37" s="5" t="s">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C39" s="5" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C38" t="s">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C40" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="39" spans="2:5" s="19" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" spans="2:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="15" t="s">
+    <row r="41" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B42" s="15" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B41" s="4" t="s">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B43" s="4" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B42" s="4"/>
-      <c r="C42" s="5" t="s">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B44" s="4"/>
+      <c r="C44" s="5" t="s">
         <v>463</v>
       </c>
-      <c r="D42" s="5"/>
-      <c r="E42" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C43" s="5" t="s">
-        <v>463</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>464</v>
-      </c>
-      <c r="E43" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C44" t="s">
-        <v>450</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>446</v>
-      </c>
+      <c r="D44" s="5"/>
       <c r="E44" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="45" spans="2:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B45" s="15" t="s">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C45" s="5" t="s">
+        <v>463</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>464</v>
+      </c>
+      <c r="E45" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C46" t="s">
+        <v>450</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>446</v>
+      </c>
+      <c r="E46" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B47" s="15" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B46" s="4" t="s">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B48" s="4" t="s">
         <v>58</v>
-      </c>
-    </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B47" s="4" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B48" s="4" t="s">
-        <v>442</v>
       </c>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B49" s="4" t="s">
-        <v>52</v>
+        <v>441</v>
       </c>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B50" s="4" t="s">
-        <v>53</v>
+        <v>442</v>
       </c>
     </row>
     <row r="51" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B51" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="52" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B52" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B53" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="54" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B54" s="4" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="53" spans="2:7" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="C53" s="1" t="s">
-        <v>445</v>
-      </c>
-      <c r="D53" s="5" t="s">
-        <v>465</v>
-      </c>
-      <c r="E53" s="5"/>
-      <c r="F53" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="G53" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="54" spans="2:7" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="C54" s="1" t="s">
-        <v>445</v>
-      </c>
-      <c r="D54" s="5" t="s">
-        <v>465</v>
-      </c>
-      <c r="E54" s="5"/>
-      <c r="F54" s="4" t="s">
-        <v>241</v>
-      </c>
-      <c r="G54" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="55" spans="2:7" ht="16.5" x14ac:dyDescent="0.2">
       <c r="C55" s="1" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>448</v>
-      </c>
-      <c r="E55" s="5" t="s">
         <v>465</v>
       </c>
+      <c r="E55" s="5"/>
       <c r="F55" s="4" t="s">
         <v>187</v>
       </c>
@@ -9768,14 +9880,12 @@
     </row>
     <row r="56" spans="2:7" ht="16.5" x14ac:dyDescent="0.2">
       <c r="C56" s="1" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>448</v>
-      </c>
-      <c r="E56" s="5" t="s">
         <v>465</v>
       </c>
+      <c r="E56" s="5"/>
       <c r="F56" s="4" t="s">
         <v>241</v>
       </c>
@@ -9783,57 +9893,57 @@
         <v>393</v>
       </c>
     </row>
-    <row r="57" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B57" s="15" t="s">
+    <row r="57" spans="2:7" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="C57" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>448</v>
+      </c>
+      <c r="E57" s="5" t="s">
+        <v>465</v>
+      </c>
+      <c r="F57" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="G57" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="58" spans="2:7" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="C58" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>448</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>465</v>
+      </c>
+      <c r="F58" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="G58" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="59" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B59" s="15" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="58" spans="2:7" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="B58" s="4" t="s">
+    <row r="60" spans="2:7" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="B60" s="4" t="s">
         <v>396</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="C60" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="D58" s="1" t="s">
+      <c r="D60" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E58" s="1" t="s">
+      <c r="E60" s="1" t="s">
         <v>361</v>
-      </c>
-    </row>
-    <row r="59" spans="2:7" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="C59" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>363</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>443</v>
-      </c>
-      <c r="F59" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="G59" s="2" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="60" spans="2:7" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="C60" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>363</v>
-      </c>
-      <c r="E60" s="2" t="s">
-        <v>444</v>
-      </c>
-      <c r="F60" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="G60" s="2" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="61" spans="2:7" ht="16.5" x14ac:dyDescent="0.2">
@@ -9844,10 +9954,10 @@
         <v>363</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>241</v>
+        <v>187</v>
       </c>
       <c r="G61" s="2" t="s">
         <v>370</v>
@@ -9861,86 +9971,100 @@
         <v>363</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>187</v>
+        <v>241</v>
       </c>
       <c r="G62" s="2" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="63" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B63" s="15" t="s">
+    <row r="63" spans="2:7" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="C63" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="G63" s="2" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="64" spans="2:7" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="C64" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="G64" s="2" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="65" spans="2:7" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="B65" s="4" t="s">
+        <v>470</v>
+      </c>
+      <c r="C65" s="2"/>
+      <c r="D65" s="2"/>
+      <c r="E65" s="2"/>
+      <c r="F65" s="2"/>
+      <c r="G65" s="2"/>
+    </row>
+    <row r="66" spans="2:7" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="B66" s="17" t="s">
+        <v>396</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="G66" s="2" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="67" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B67" s="15" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="64" spans="2:7" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="B64" s="4" t="s">
+    <row r="68" spans="2:7" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="B68" s="4" t="s">
         <v>451</v>
       </c>
-      <c r="C64" s="1" t="s">
+      <c r="C68" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="D64" s="20" t="s">
+      <c r="D68" s="20" t="s">
         <v>375</v>
       </c>
-      <c r="E64" s="20"/>
-      <c r="F64" s="20"/>
-    </row>
-    <row r="65" spans="2:6" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="B65" s="4" t="s">
+      <c r="E68" s="20"/>
+      <c r="F68" s="20"/>
+    </row>
+    <row r="69" spans="2:7" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="B69" s="4" t="s">
         <v>452</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>372</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>373</v>
-      </c>
-      <c r="F65" s="1" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="66" spans="2:6" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="C66" s="1" t="s">
-        <v>372</v>
-      </c>
-      <c r="D66" s="2" t="s">
-        <v>449</v>
-      </c>
-      <c r="E66" s="5" t="s">
-        <v>376</v>
-      </c>
-      <c r="F66" s="1" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="67" spans="2:6" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="B67" s="15" t="s">
-        <v>455</v>
-      </c>
-      <c r="C67" s="9"/>
-      <c r="D67" s="8"/>
-      <c r="E67" s="18"/>
-      <c r="F67" s="9"/>
-    </row>
-    <row r="68" spans="2:6" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="B68" s="4" t="s">
-        <v>453</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>375</v>
-      </c>
-      <c r="D68" s="22" t="s">
-        <v>374</v>
-      </c>
-      <c r="E68" s="22"/>
-      <c r="F68" s="22"/>
-    </row>
-    <row r="69" spans="2:6" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="B69" s="4" t="s">
-        <v>454</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>372</v>
@@ -9952,7 +10076,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="70" spans="2:6" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:7" ht="16.5" x14ac:dyDescent="0.2">
       <c r="C70" s="1" t="s">
         <v>372</v>
       </c>
@@ -9963,14 +10087,64 @@
         <v>376</v>
       </c>
       <c r="F70" s="1" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="71" spans="2:7" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="B71" s="15" t="s">
+        <v>455</v>
+      </c>
+      <c r="C71" s="9"/>
+      <c r="D71" s="8"/>
+      <c r="E71" s="18"/>
+      <c r="F71" s="9"/>
+    </row>
+    <row r="72" spans="2:7" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="B72" s="4" t="s">
+        <v>453</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="D72" s="22" t="s">
+        <v>374</v>
+      </c>
+      <c r="E72" s="22"/>
+      <c r="F72" s="22"/>
+    </row>
+    <row r="73" spans="2:7" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="B73" s="4" t="s">
+        <v>454</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="74" spans="2:7" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="C74" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="E74" s="5" t="s">
+        <v>376</v>
+      </c>
+      <c r="F74" s="1" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="C1:I1"/>
-    <mergeCell ref="D64:F64"/>
     <mergeCell ref="D68:F68"/>
+    <mergeCell ref="D72:F72"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9982,7 +10156,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{988C78EB-4E00-466C-9BD2-B10965380DEB}">
   <dimension ref="A1:I231"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A207" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A221" sqref="A221"/>
     </sheetView>

</xml_diff>

<commit_message>
parser SHFT adding one more parameter
</commit_message>
<xml_diff>
--- a/P4E_psuedo_instruction_set.xlsx
+++ b/P4E_psuedo_instruction_set.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\P4EngineAssembler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AB2B8B9-AA42-4D23-9E92-C447E5FDEE41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADA52403-C013-4C68-A7B9-6671DAC5CFB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-3645" windowWidth="38640" windowHeight="21840" activeTab="1" xr2:uid="{87164962-7B7D-4BAA-98E0-B9A8D7C47112}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{87164962-7B7D-4BAA-98E0-B9A8D7C47112}"/>
   </bookViews>
   <sheets>
     <sheet name="parser" sheetId="1" r:id="rId1"/>
@@ -419,7 +419,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C102" authorId="0" shapeId="0" xr:uid="{42B3C977-0E44-4FF0-87CE-41EADF029358}">
+    <comment ref="C98" authorId="0" shapeId="0" xr:uid="{5EAEF23C-593A-4A37-B755-360B9209963D}">
       <text>
         <r>
           <rPr>
@@ -441,11 +441,89 @@
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
-shift value from temp, no calculation</t>
+shift value from temp</t>
         </r>
       </text>
     </comment>
-    <comment ref="D110" authorId="0" shapeId="0" xr:uid="{B3419830-61AE-41B1-8075-0EDBC5F16888}">
+    <comment ref="C100" authorId="0" shapeId="0" xr:uid="{AD49495F-3BDD-40D6-ADD1-408F470BCB83}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>Dianchao Wang:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+shift value from temp</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C101" authorId="0" shapeId="0" xr:uid="{31ADC337-9E94-4153-8412-495E39530DEF}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>Dianchao Wang:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+shift value from temp</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C102" authorId="0" shapeId="0" xr:uid="{4B0BBC75-4AFD-4999-8471-DC753FD0455A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>Dianchao Wang:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+shift value from temp</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D114" authorId="0" shapeId="0" xr:uid="{B3419830-61AE-41B1-8075-0EDBC5F16888}">
       <text>
         <r>
           <rPr>
@@ -472,7 +550,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A140" authorId="0" shapeId="0" xr:uid="{9DF95069-D8AA-4D9B-B036-F6570707C225}">
+    <comment ref="A144" authorId="0" shapeId="0" xr:uid="{9DF95069-D8AA-4D9B-B036-F6570707C225}">
       <text>
         <r>
           <rPr>
@@ -502,7 +580,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D157" authorId="0" shapeId="0" xr:uid="{10355003-BB36-4D9F-BEF6-AC796CED51BC}">
+    <comment ref="D161" authorId="0" shapeId="0" xr:uid="{10355003-BB36-4D9F-BEF6-AC796CED51BC}">
       <text>
         <r>
           <rPr>
@@ -528,7 +606,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F157" authorId="0" shapeId="0" xr:uid="{EADD36A3-0C54-43FE-AD07-DAE0F1C398C8}">
+    <comment ref="F161" authorId="0" shapeId="0" xr:uid="{EADD36A3-0C54-43FE-AD07-DAE0F1C398C8}">
       <text>
         <r>
           <rPr>
@@ -554,7 +632,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D158" authorId="0" shapeId="0" xr:uid="{5EDDCAB0-8CF8-4E69-91EC-FCEBB8FBFB81}">
+    <comment ref="D162" authorId="0" shapeId="0" xr:uid="{5EDDCAB0-8CF8-4E69-91EC-FCEBB8FBFB81}">
       <text>
         <r>
           <rPr>
@@ -580,7 +658,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F159" authorId="0" shapeId="0" xr:uid="{E9CC35BA-90D8-4E68-A63E-1BDF886428EA}">
+    <comment ref="F163" authorId="0" shapeId="0" xr:uid="{E9CC35BA-90D8-4E68-A63E-1BDF886428EA}">
       <text>
         <r>
           <rPr>
@@ -606,7 +684,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D161" authorId="0" shapeId="0" xr:uid="{C0E77B6C-0F0F-459E-A010-D438E2938743}">
+    <comment ref="D165" authorId="0" shapeId="0" xr:uid="{C0E77B6C-0F0F-459E-A010-D438E2938743}">
       <text>
         <r>
           <rPr>
@@ -632,7 +710,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F162" authorId="0" shapeId="0" xr:uid="{149FA3A0-4084-461C-8457-384C4EC1B272}">
+    <comment ref="F166" authorId="0" shapeId="0" xr:uid="{149FA3A0-4084-461C-8457-384C4EC1B272}">
       <text>
         <r>
           <rPr>
@@ -1281,7 +1359,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1374" uniqueCount="475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1386" uniqueCount="481">
   <si>
     <t>isr SHiFT</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -5988,6 +6066,101 @@
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve"> ] ;</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>len</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> (1 - 256），</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">PHV [ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>offset9</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> ] ;</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>( store to PHV or not )</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>CRC16</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> ,</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>CRC32</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> ,</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">CSUM </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>,</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -6094,7 +6267,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -6157,9 +6330,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -6498,11 +6668,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA14F7B7-5F50-4FFB-AE20-84853F321386}">
-  <dimension ref="A1:I173"/>
+  <dimension ref="A1:I177"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D79" sqref="D79"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A106" sqref="A106:XFD106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.2"/>
@@ -8219,6 +8389,9 @@
       <c r="D97" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="E97" s="1" t="s">
+        <v>477</v>
+      </c>
       <c r="F97" s="2"/>
       <c r="G97" s="2"/>
       <c r="H97" s="2"/>
@@ -8226,10 +8399,9 @@
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B98" s="2"/>
-      <c r="C98" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="D98" s="2"/>
+      <c r="C98" s="1" t="s">
+        <v>190</v>
+      </c>
       <c r="F98" s="2"/>
       <c r="G98" s="2"/>
       <c r="H98" s="2"/>
@@ -8238,11 +8410,9 @@
     <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B99" s="2"/>
       <c r="C99" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="D99" s="2" t="s">
-        <v>286</v>
-      </c>
+        <v>284</v>
+      </c>
+      <c r="D99" s="2"/>
       <c r="F99" s="2"/>
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
@@ -8250,100 +8420,91 @@
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B100" s="2"/>
-      <c r="C100" s="2" t="s">
-        <v>285</v>
-      </c>
       <c r="D100" s="2" t="s">
-        <v>287</v>
-      </c>
-      <c r="F100" s="2"/>
+        <v>286</v>
+      </c>
       <c r="G100" s="2"/>
       <c r="H100" s="2"/>
       <c r="I100" s="2"/>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B101" s="2"/>
-      <c r="C101" s="2" t="s">
-        <v>285</v>
-      </c>
       <c r="D101" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="F101" s="2"/>
+        <v>287</v>
+      </c>
       <c r="G101" s="2"/>
       <c r="H101" s="2"/>
       <c r="I101" s="2"/>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B102" s="2"/>
-      <c r="C102" s="21" t="s">
-        <v>190</v>
-      </c>
-      <c r="D102" s="21"/>
-      <c r="F102" s="2"/>
+      <c r="D102" s="2" t="s">
+        <v>288</v>
+      </c>
       <c r="G102" s="2"/>
       <c r="H102" s="2"/>
       <c r="I102" s="2"/>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B103" s="2"/>
+      <c r="C103" s="2" t="s">
+        <v>285</v>
+      </c>
       <c r="D103" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="F103" s="2"/>
       <c r="G103" s="2"/>
       <c r="H103" s="2"/>
       <c r="I103" s="2"/>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B104" s="2"/>
+      <c r="C104" s="2" t="s">
+        <v>285</v>
+      </c>
       <c r="D104" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="F104" s="2"/>
       <c r="G104" s="2"/>
       <c r="H104" s="2"/>
       <c r="I104" s="2"/>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B105" s="2"/>
+      <c r="C105" s="2" t="s">
+        <v>285</v>
+      </c>
       <c r="D105" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="F105" s="2"/>
       <c r="G105" s="2"/>
       <c r="H105" s="2"/>
       <c r="I105" s="2"/>
     </row>
-    <row r="106" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B106" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="C106" s="8"/>
-      <c r="D106" s="8"/>
-      <c r="E106" s="8"/>
-      <c r="F106" s="8"/>
-      <c r="G106" s="8"/>
-      <c r="H106" s="8"/>
-      <c r="I106" s="8"/>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B106" s="2"/>
+      <c r="C106" s="2" t="s">
+        <v>475</v>
+      </c>
+      <c r="D106" s="2"/>
+      <c r="E106" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="G106" s="2"/>
+      <c r="H106" s="2"/>
+      <c r="I106" s="2"/>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A107" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="B107" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="C107" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D107" s="1" t="s">
-        <v>201</v>
+      <c r="B107" s="2"/>
+      <c r="C107" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="D107" s="2" t="s">
+        <v>480</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F107" s="2"/>
+        <v>476</v>
+      </c>
       <c r="G107" s="2"/>
       <c r="H107" s="2"/>
       <c r="I107" s="2"/>
@@ -8351,12 +8512,14 @@
     <row r="108" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B108" s="2"/>
       <c r="C108" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="E108" s="2" t="s">
-        <v>293</v>
-      </c>
-      <c r="F108" s="2"/>
+        <v>285</v>
+      </c>
+      <c r="D108" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>476</v>
+      </c>
       <c r="G108" s="2"/>
       <c r="H108" s="2"/>
       <c r="I108" s="2"/>
@@ -8364,91 +8527,89 @@
     <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B109" s="2"/>
       <c r="C109" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="E109" s="2" t="s">
-        <v>293</v>
-      </c>
-      <c r="F109" s="2"/>
+        <v>285</v>
+      </c>
+      <c r="D109" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>476</v>
+      </c>
       <c r="G109" s="2"/>
       <c r="H109" s="2"/>
       <c r="I109" s="2"/>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B110" s="2"/>
-      <c r="C110" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="D110" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="E110" s="2" t="s">
-        <v>293</v>
-      </c>
-      <c r="F110" s="2"/>
-      <c r="G110" s="2"/>
-      <c r="H110" s="2"/>
-      <c r="I110" s="2"/>
+    <row r="110" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B110" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="C110" s="8"/>
+      <c r="D110" s="8"/>
+      <c r="E110" s="8"/>
+      <c r="F110" s="8"/>
+      <c r="G110" s="8"/>
+      <c r="H110" s="8"/>
+      <c r="I110" s="8"/>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B111" s="2"/>
-      <c r="C111" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="E111" s="2" t="s">
-        <v>293</v>
+      <c r="A111" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="F111" s="2"/>
       <c r="G111" s="2"/>
       <c r="H111" s="2"/>
       <c r="I111" s="2"/>
     </row>
-    <row r="112" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B112" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="C112" s="8"/>
-      <c r="D112" s="8"/>
-      <c r="E112" s="8"/>
-      <c r="F112" s="8"/>
-      <c r="G112" s="8"/>
-      <c r="H112" s="8"/>
-      <c r="I112" s="8"/>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B112" s="2"/>
+      <c r="C112" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="E112" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="F112" s="2"/>
+      <c r="G112" s="2"/>
+      <c r="H112" s="2"/>
+      <c r="I112" s="2"/>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A113" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B113" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="C113" s="2"/>
-      <c r="D113" s="2"/>
-      <c r="E113" s="2"/>
+      <c r="B113" s="2"/>
+      <c r="C113" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="E113" s="2" t="s">
+        <v>293</v>
+      </c>
       <c r="F113" s="2"/>
       <c r="G113" s="2"/>
       <c r="H113" s="2"/>
       <c r="I113" s="2"/>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A114" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B114" s="12" t="s">
-        <v>163</v>
-      </c>
-      <c r="C114" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D114" s="1" t="s">
-        <v>413</v>
-      </c>
-      <c r="E114" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F114" s="1" t="s">
-        <v>194</v>
-      </c>
+      <c r="B114" s="2"/>
+      <c r="C114" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="D114" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="E114" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="F114" s="2"/>
       <c r="G114" s="2"/>
       <c r="H114" s="2"/>
       <c r="I114" s="2"/>
@@ -8456,102 +8617,97 @@
     <row r="115" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B115" s="2"/>
       <c r="C115" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="D115" s="2" t="s">
-        <v>415</v>
+        <v>292</v>
       </c>
       <c r="E115" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="F115" s="2" t="s">
-        <v>193</v>
-      </c>
+        <v>293</v>
+      </c>
+      <c r="F115" s="2"/>
       <c r="G115" s="2"/>
       <c r="H115" s="2"/>
       <c r="I115" s="2"/>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B116" s="2"/>
-      <c r="C116" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="D116" s="2" t="s">
-        <v>414</v>
-      </c>
-      <c r="E116" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="F116" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="G116" s="2"/>
-      <c r="H116" s="2"/>
-      <c r="I116" s="2"/>
+    <row r="116" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B116" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="C116" s="8"/>
+      <c r="D116" s="8"/>
+      <c r="E116" s="8"/>
+      <c r="F116" s="8"/>
+      <c r="G116" s="8"/>
+      <c r="H116" s="8"/>
+      <c r="I116" s="8"/>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B117" s="2"/>
-      <c r="C117" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="D117" s="2" t="s">
-        <v>414</v>
-      </c>
-      <c r="E117" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="F117" s="2" t="s">
-        <v>295</v>
-      </c>
+      <c r="A117" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C117" s="2"/>
+      <c r="D117" s="2"/>
+      <c r="E117" s="2"/>
+      <c r="F117" s="2"/>
       <c r="G117" s="2"/>
       <c r="H117" s="2"/>
       <c r="I117" s="2"/>
     </row>
-    <row r="118" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B118" s="13" t="s">
-        <v>129</v>
-      </c>
-      <c r="C118" s="8"/>
-      <c r="D118" s="8"/>
-      <c r="E118" s="8"/>
-      <c r="F118" s="8"/>
-      <c r="G118" s="8"/>
-      <c r="H118" s="8"/>
-      <c r="I118" s="8"/>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A118" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B118" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="E118" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F118" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="G118" s="2"/>
+      <c r="H118" s="2"/>
+      <c r="I118" s="2"/>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A119" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B119" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="C119" s="2"/>
-      <c r="D119" s="2"/>
-      <c r="E119" s="2"/>
-      <c r="F119" s="2"/>
+      <c r="B119" s="2"/>
+      <c r="C119" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D119" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="E119" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="F119" s="2" t="s">
+        <v>193</v>
+      </c>
       <c r="G119" s="2"/>
       <c r="H119" s="2"/>
       <c r="I119" s="2"/>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A120" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B120" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="C120" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D120" s="1" t="s">
-        <v>413</v>
-      </c>
-      <c r="E120" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F120" s="1" t="s">
-        <v>194</v>
+      <c r="B120" s="2"/>
+      <c r="C120" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="D120" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="E120" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="F120" s="2" t="s">
+        <v>295</v>
       </c>
       <c r="G120" s="2"/>
       <c r="H120" s="2"/>
@@ -8560,224 +8716,243 @@
     <row r="121" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B121" s="2"/>
       <c r="C121" s="2" t="s">
-        <v>187</v>
+        <v>297</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E121" s="2" t="s">
         <v>294</v>
       </c>
       <c r="F121" s="2" t="s">
-        <v>193</v>
+        <v>295</v>
       </c>
       <c r="G121" s="2"/>
       <c r="H121" s="2"/>
       <c r="I121" s="2"/>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B122" s="2"/>
-      <c r="C122" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="D122" s="2" t="s">
-        <v>414</v>
-      </c>
-      <c r="E122" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="F122" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="G122" s="2"/>
-      <c r="H122" s="2"/>
-      <c r="I122" s="2"/>
+    <row r="122" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B122" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="C122" s="8"/>
+      <c r="D122" s="8"/>
+      <c r="E122" s="8"/>
+      <c r="F122" s="8"/>
+      <c r="G122" s="8"/>
+      <c r="H122" s="8"/>
+      <c r="I122" s="8"/>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B123" s="2"/>
-      <c r="C123" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="D123" s="2" t="s">
-        <v>414</v>
-      </c>
-      <c r="E123" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="F123" s="2" t="s">
-        <v>295</v>
-      </c>
+      <c r="A123" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C123" s="2"/>
+      <c r="D123" s="2"/>
+      <c r="E123" s="2"/>
+      <c r="F123" s="2"/>
       <c r="G123" s="2"/>
       <c r="H123" s="2"/>
       <c r="I123" s="2"/>
     </row>
-    <row r="124" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B124" s="13" t="s">
-        <v>130</v>
-      </c>
-      <c r="C124" s="8"/>
-      <c r="D124" s="8"/>
-      <c r="E124" s="8"/>
-      <c r="F124" s="8"/>
-      <c r="G124" s="8"/>
-      <c r="H124" s="8"/>
-      <c r="I124" s="8"/>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A124" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B124" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D124" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="E124" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F124" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="G124" s="2"/>
+      <c r="H124" s="2"/>
+      <c r="I124" s="2"/>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A125" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B125" s="2" t="s">
-        <v>166</v>
-      </c>
+      <c r="B125" s="2"/>
+      <c r="C125" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D125" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="E125" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="F125" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="G125" s="2"/>
       <c r="H125" s="2"/>
       <c r="I125" s="2"/>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A126" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B126" s="12" t="s">
-        <v>167</v>
-      </c>
-      <c r="C126" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D126" s="1" t="s">
-        <v>413</v>
-      </c>
-      <c r="E126" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F126" s="1" t="s">
-        <v>194</v>
-      </c>
+      <c r="B126" s="2"/>
+      <c r="C126" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="D126" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="E126" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="F126" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="G126" s="2"/>
       <c r="H126" s="2"/>
       <c r="I126" s="2"/>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B127" s="2"/>
       <c r="C127" s="2" t="s">
-        <v>187</v>
+        <v>297</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E127" s="2" t="s">
         <v>294</v>
       </c>
       <c r="F127" s="2" t="s">
-        <v>193</v>
+        <v>295</v>
       </c>
       <c r="G127" s="2"/>
       <c r="H127" s="2"/>
       <c r="I127" s="2"/>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B128" s="2"/>
-      <c r="C128" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="D128" s="2" t="s">
-        <v>414</v>
-      </c>
-      <c r="E128" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="F128" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="G128" s="2"/>
-      <c r="H128" s="2"/>
-      <c r="I128" s="2"/>
+    <row r="128" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B128" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="C128" s="8"/>
+      <c r="D128" s="8"/>
+      <c r="E128" s="8"/>
+      <c r="F128" s="8"/>
+      <c r="G128" s="8"/>
+      <c r="H128" s="8"/>
+      <c r="I128" s="8"/>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B129" s="2"/>
-      <c r="C129" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="D129" s="2" t="s">
-        <v>414</v>
-      </c>
-      <c r="E129" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="F129" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="G129" s="2"/>
+      <c r="A129" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>166</v>
+      </c>
       <c r="H129" s="2"/>
       <c r="I129" s="2"/>
     </row>
-    <row r="130" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B130" s="13" t="s">
-        <v>133</v>
-      </c>
-      <c r="C130" s="8"/>
-      <c r="D130" s="8"/>
-      <c r="E130" s="8"/>
-      <c r="F130" s="8"/>
-      <c r="G130" s="8"/>
-      <c r="H130" s="8"/>
-      <c r="I130" s="8"/>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A130" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B130" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D130" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="E130" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F130" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="H130" s="2"/>
+      <c r="I130" s="2"/>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A131" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B131" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="C131" s="2"/>
-      <c r="D131" s="2"/>
-      <c r="E131" s="2"/>
-      <c r="F131" s="2"/>
+      <c r="B131" s="2"/>
+      <c r="C131" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D131" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="E131" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="F131" s="2" t="s">
+        <v>193</v>
+      </c>
       <c r="G131" s="2"/>
       <c r="H131" s="2"/>
       <c r="I131" s="2"/>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B132" s="2"/>
-      <c r="C132" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="D132" s="2"/>
-      <c r="E132" s="2"/>
-      <c r="F132" s="2"/>
+      <c r="C132" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="D132" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="E132" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="F132" s="2" t="s">
+        <v>295</v>
+      </c>
       <c r="G132" s="2"/>
       <c r="H132" s="2"/>
       <c r="I132" s="2"/>
     </row>
-    <row r="133" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B133" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="D133" s="8"/>
-      <c r="E133" s="8"/>
-      <c r="F133" s="8"/>
-      <c r="G133" s="8"/>
-      <c r="H133" s="8"/>
-      <c r="I133" s="8"/>
-    </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A134" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B134" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="D134" s="2"/>
-      <c r="E134" s="2"/>
-      <c r="F134" s="2"/>
-      <c r="G134" s="2"/>
-      <c r="H134" s="2"/>
-      <c r="I134" s="2"/>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B133" s="2"/>
+      <c r="C133" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="D133" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="E133" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="F133" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="G133" s="2"/>
+      <c r="H133" s="2"/>
+      <c r="I133" s="2"/>
+    </row>
+    <row r="134" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B134" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="C134" s="8"/>
+      <c r="D134" s="8"/>
+      <c r="E134" s="8"/>
+      <c r="F134" s="8"/>
+      <c r="G134" s="8"/>
+      <c r="H134" s="8"/>
+      <c r="I134" s="8"/>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B135" s="2"/>
-      <c r="C135" s="1" t="s">
-        <v>190</v>
-      </c>
+      <c r="A135" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C135" s="2"/>
       <c r="D135" s="2"/>
       <c r="E135" s="2"/>
       <c r="F135" s="2"/>
@@ -8785,35 +8960,35 @@
       <c r="H135" s="2"/>
       <c r="I135" s="2"/>
     </row>
-    <row r="136" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B136" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="D136" s="8"/>
-      <c r="E136" s="8"/>
-      <c r="F136" s="8"/>
-      <c r="G136" s="8"/>
-      <c r="H136" s="8"/>
-      <c r="I136" s="8"/>
-    </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A137" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B137" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="D137" s="2"/>
-      <c r="E137" s="2"/>
-      <c r="F137" s="2"/>
-      <c r="G137" s="2"/>
-      <c r="H137" s="2"/>
-      <c r="I137" s="2"/>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B136" s="2"/>
+      <c r="C136" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D136" s="2"/>
+      <c r="E136" s="2"/>
+      <c r="F136" s="2"/>
+      <c r="G136" s="2"/>
+      <c r="H136" s="2"/>
+      <c r="I136" s="2"/>
+    </row>
+    <row r="137" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B137" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="D137" s="8"/>
+      <c r="E137" s="8"/>
+      <c r="F137" s="8"/>
+      <c r="G137" s="8"/>
+      <c r="H137" s="8"/>
+      <c r="I137" s="8"/>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B138" s="2"/>
-      <c r="C138" s="1" t="s">
-        <v>190</v>
+      <c r="A138" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B138" s="2" t="s">
+        <v>169</v>
       </c>
       <c r="D138" s="2"/>
       <c r="E138" s="2"/>
@@ -8822,39 +8997,36 @@
       <c r="H138" s="2"/>
       <c r="I138" s="2"/>
     </row>
-    <row r="139" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B139" s="13" t="s">
-        <v>136</v>
-      </c>
-      <c r="C139" s="8"/>
-      <c r="D139" s="8"/>
-      <c r="E139" s="8"/>
-      <c r="F139" s="8"/>
-      <c r="G139" s="8"/>
-      <c r="H139" s="8"/>
-      <c r="I139" s="8"/>
-    </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A140" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="B140" s="2"/>
-      <c r="C140" s="2"/>
-      <c r="D140" s="2"/>
-      <c r="E140" s="2"/>
-      <c r="F140" s="2"/>
-      <c r="G140" s="2"/>
-      <c r="H140" s="2"/>
-      <c r="I140" s="2"/>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B139" s="2"/>
+      <c r="C139" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D139" s="2"/>
+      <c r="E139" s="2"/>
+      <c r="F139" s="2"/>
+      <c r="G139" s="2"/>
+      <c r="H139" s="2"/>
+      <c r="I139" s="2"/>
+    </row>
+    <row r="140" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B140" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="D140" s="8"/>
+      <c r="E140" s="8"/>
+      <c r="F140" s="8"/>
+      <c r="G140" s="8"/>
+      <c r="H140" s="8"/>
+      <c r="I140" s="8"/>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="C141" s="2"/>
+        <v>170</v>
+      </c>
       <c r="D141" s="2"/>
       <c r="E141" s="2"/>
       <c r="F141" s="2"/>
@@ -8863,13 +9035,10 @@
       <c r="I141" s="2"/>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A142" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B142" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="C142" s="2"/>
+      <c r="B142" s="2"/>
+      <c r="C142" s="1" t="s">
+        <v>190</v>
+      </c>
       <c r="D142" s="2"/>
       <c r="E142" s="2"/>
       <c r="F142" s="2"/>
@@ -8877,28 +9046,23 @@
       <c r="H142" s="2"/>
       <c r="I142" s="2"/>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A143" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B143" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="C143" s="2"/>
-      <c r="D143" s="2"/>
-      <c r="E143" s="2"/>
-      <c r="F143" s="2"/>
-      <c r="G143" s="2"/>
-      <c r="H143" s="2"/>
-      <c r="I143" s="2"/>
+    <row r="143" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B143" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="C143" s="8"/>
+      <c r="D143" s="8"/>
+      <c r="E143" s="8"/>
+      <c r="F143" s="8"/>
+      <c r="G143" s="8"/>
+      <c r="H143" s="8"/>
+      <c r="I143" s="8"/>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="B144" s="2" t="s">
-        <v>267</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="B144" s="2"/>
       <c r="C144" s="2"/>
       <c r="D144" s="2"/>
       <c r="E144" s="2"/>
@@ -8909,10 +9073,10 @@
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C145" s="2"/>
       <c r="D145" s="2"/>
@@ -8924,38 +9088,29 @@
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="C146" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D146" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="E146" s="1" t="s">
-        <v>147</v>
-      </c>
+        <v>173</v>
+      </c>
+      <c r="C146" s="2"/>
+      <c r="D146" s="2"/>
+      <c r="E146" s="2"/>
+      <c r="F146" s="2"/>
       <c r="G146" s="2"/>
       <c r="H146" s="2"/>
       <c r="I146" s="2"/>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="B147" s="2"/>
-      <c r="C147" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="D147" s="2" t="s">
-        <v>270</v>
-      </c>
-      <c r="E147" s="2" t="s">
-        <v>271</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="B147" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C147" s="2"/>
+      <c r="D147" s="2"/>
+      <c r="E147" s="2"/>
       <c r="F147" s="2"/>
       <c r="G147" s="2"/>
       <c r="H147" s="2"/>
@@ -8963,10 +9118,10 @@
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
-        <v>171</v>
+        <v>266</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>177</v>
+        <v>267</v>
       </c>
       <c r="C148" s="2"/>
       <c r="D148" s="2"/>
@@ -8977,8 +9132,11 @@
       <c r="I148" s="2"/>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A149" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="B149" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C149" s="2"/>
       <c r="D149" s="2"/>
@@ -8989,32 +9147,50 @@
       <c r="I149" s="2"/>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A150" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="B150" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="C150" s="2"/>
-      <c r="D150" s="2"/>
-      <c r="E150" s="2"/>
-      <c r="F150" s="2"/>
+        <v>176</v>
+      </c>
+      <c r="C150" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D150" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E150" s="1" t="s">
+        <v>147</v>
+      </c>
       <c r="G150" s="2"/>
       <c r="H150" s="2"/>
       <c r="I150" s="2"/>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B151" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="C151" s="2"/>
-      <c r="D151" s="2"/>
-      <c r="E151" s="2"/>
+      <c r="A151" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B151" s="2"/>
+      <c r="C151" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="D151" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="E151" s="2" t="s">
+        <v>271</v>
+      </c>
       <c r="F151" s="2"/>
       <c r="G151" s="2"/>
       <c r="H151" s="2"/>
       <c r="I151" s="2"/>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A152" s="1" t="s">
+        <v>171</v>
+      </c>
       <c r="B152" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C152" s="2"/>
       <c r="D152" s="2"/>
@@ -9026,7 +9202,7 @@
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B153" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C153" s="2"/>
       <c r="D153" s="2"/>
@@ -9036,111 +9212,95 @@
       <c r="H153" s="2"/>
       <c r="I153" s="2"/>
     </row>
-    <row r="154" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B154" s="13" t="s">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B154" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C154" s="2"/>
+      <c r="D154" s="2"/>
+      <c r="E154" s="2"/>
+      <c r="F154" s="2"/>
+      <c r="G154" s="2"/>
+      <c r="H154" s="2"/>
+      <c r="I154" s="2"/>
+    </row>
+    <row r="155" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B155" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="C155" s="2"/>
+      <c r="D155" s="2"/>
+      <c r="E155" s="2"/>
+      <c r="F155" s="2"/>
+      <c r="G155" s="2"/>
+      <c r="H155" s="2"/>
+      <c r="I155" s="2"/>
+    </row>
+    <row r="156" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B156" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C156" s="2"/>
+      <c r="D156" s="2"/>
+      <c r="E156" s="2"/>
+      <c r="F156" s="2"/>
+      <c r="G156" s="2"/>
+      <c r="H156" s="2"/>
+      <c r="I156" s="2"/>
+    </row>
+    <row r="157" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B157" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C157" s="2"/>
+      <c r="D157" s="2"/>
+      <c r="E157" s="2"/>
+      <c r="F157" s="2"/>
+      <c r="G157" s="2"/>
+      <c r="H157" s="2"/>
+      <c r="I157" s="2"/>
+    </row>
+    <row r="158" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B158" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="C154" s="8"/>
-      <c r="D154" s="8"/>
-      <c r="E154" s="8"/>
-      <c r="F154" s="8"/>
-      <c r="G154" s="8"/>
-      <c r="H154" s="8"/>
-      <c r="I154" s="8"/>
-    </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A155" s="1" t="s">
+      <c r="C158" s="8"/>
+      <c r="D158" s="8"/>
+      <c r="E158" s="8"/>
+      <c r="F158" s="8"/>
+      <c r="G158" s="8"/>
+      <c r="H158" s="8"/>
+      <c r="I158" s="8"/>
+    </row>
+    <row r="159" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A159" s="1" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A156" s="1" t="s">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A160" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B156" s="2" t="s">
+      <c r="B160" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="C156" s="1" t="s">
+      <c r="C160" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D156" s="1" t="s">
+      <c r="D160" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E156" s="1" t="s">
+      <c r="E160" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F156" s="1" t="s">
+      <c r="F160" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G156" s="1" t="s">
+      <c r="G160" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="H156" s="1" t="s">
+      <c r="H160" s="1" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C157" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="D157" s="2" t="s">
-        <v>359</v>
-      </c>
-      <c r="E157" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="F157" s="2" t="s">
-        <v>359</v>
-      </c>
-      <c r="G157" s="2" t="s">
-        <v>357</v>
-      </c>
-      <c r="H157" s="14" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C158" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="D158" s="2" t="s">
-        <v>359</v>
-      </c>
-      <c r="E158" s="2"/>
-      <c r="F158" s="2"/>
-      <c r="G158" s="2" t="s">
-        <v>357</v>
-      </c>
-      <c r="H158" s="14" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C159" s="2"/>
-      <c r="D159" s="2"/>
-      <c r="E159" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="F159" s="2" t="s">
-        <v>359</v>
-      </c>
-      <c r="G159" s="2" t="s">
-        <v>357</v>
-      </c>
-      <c r="H159" s="14" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C160" s="2"/>
-      <c r="D160" s="2"/>
-      <c r="E160" s="2"/>
-      <c r="F160" s="2"/>
-      <c r="G160" s="2" t="s">
-        <v>357</v>
-      </c>
-      <c r="H160" s="14" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.2">
@@ -9150,23 +9310,31 @@
       <c r="D161" s="2" t="s">
         <v>359</v>
       </c>
-      <c r="E161" s="2"/>
-      <c r="F161" s="2"/>
-      <c r="G161" s="2"/>
+      <c r="E161" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="F161" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="G161" s="2" t="s">
+        <v>357</v>
+      </c>
       <c r="H161" s="14" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C162" s="2"/>
-      <c r="D162" s="2"/>
-      <c r="E162" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="F162" s="2" t="s">
+      <c r="C162" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="D162" s="2" t="s">
         <v>359</v>
       </c>
-      <c r="G162" s="2"/>
+      <c r="E162" s="2"/>
+      <c r="F162" s="2"/>
+      <c r="G162" s="2" t="s">
+        <v>357</v>
+      </c>
       <c r="H162" s="14" t="s">
         <v>274</v>
       </c>
@@ -9174,93 +9342,148 @@
     <row r="163" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C163" s="2"/>
       <c r="D163" s="2"/>
-      <c r="E163" s="2"/>
-      <c r="F163" s="2"/>
-      <c r="G163" s="2"/>
+      <c r="E163" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="F163" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="G163" s="2" t="s">
+        <v>357</v>
+      </c>
       <c r="H163" s="14" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="164" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B164" s="13" t="s">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C164" s="2"/>
+      <c r="D164" s="2"/>
+      <c r="E164" s="2"/>
+      <c r="F164" s="2"/>
+      <c r="G164" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="H164" s="14" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C165" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="D165" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="E165" s="2"/>
+      <c r="F165" s="2"/>
+      <c r="G165" s="2"/>
+      <c r="H165" s="14" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="166" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C166" s="2"/>
+      <c r="D166" s="2"/>
+      <c r="E166" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="F166" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="G166" s="2"/>
+      <c r="H166" s="14" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="167" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C167" s="2"/>
+      <c r="D167" s="2"/>
+      <c r="E167" s="2"/>
+      <c r="F167" s="2"/>
+      <c r="G167" s="2"/>
+      <c r="H167" s="14" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="168" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B168" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="C164" s="8"/>
-      <c r="D164" s="8"/>
-      <c r="E164" s="8"/>
-      <c r="F164" s="8"/>
-      <c r="G164" s="8"/>
-      <c r="H164" s="8"/>
-      <c r="I164" s="8"/>
-    </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A165" s="1" t="s">
+      <c r="C168" s="8"/>
+      <c r="D168" s="8"/>
+      <c r="E168" s="8"/>
+      <c r="F168" s="8"/>
+      <c r="G168" s="8"/>
+      <c r="H168" s="8"/>
+      <c r="I168" s="8"/>
+    </row>
+    <row r="169" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A169" s="1" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A166" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B166" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="C166" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C167" s="2" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C168" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="169" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B169" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="C169" s="8"/>
-      <c r="D169" s="8"/>
-      <c r="E169" s="8"/>
-      <c r="F169" s="8"/>
-      <c r="G169" s="8"/>
-      <c r="H169" s="8"/>
-      <c r="I169" s="8"/>
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B170" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="C170" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="171" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C171" s="2" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="172" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C172" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="173" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B173" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="C173" s="8"/>
+      <c r="D173" s="8"/>
+      <c r="E173" s="8"/>
+      <c r="F173" s="8"/>
+      <c r="G173" s="8"/>
+      <c r="H173" s="8"/>
+      <c r="I173" s="8"/>
+    </row>
+    <row r="174" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A174" s="1" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A171" s="1" t="s">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A175" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B171" s="2" t="s">
+      <c r="B175" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="C171" s="1" t="s">
+      <c r="C175" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C172" s="2" t="s">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C176" s="2" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C173" s="1" t="s">
+    <row r="177" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C177" s="1" t="s">
         <v>190</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="C1:I1"/>
-    <mergeCell ref="C102:D102"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9272,7 +9495,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{732D935C-EC39-4DBE-84B4-44CD168E0101}">
   <dimension ref="A1:I74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
     </sheetView>
@@ -10106,11 +10329,11 @@
       <c r="C72" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D72" s="22" t="s">
+      <c r="D72" s="21" t="s">
         <v>374</v>
       </c>
-      <c r="E72" s="22"/>
-      <c r="F72" s="22"/>
+      <c r="E72" s="21"/>
+      <c r="F72" s="21"/>
     </row>
     <row r="73" spans="2:7" ht="16.5" x14ac:dyDescent="0.2">
       <c r="B73" s="4" t="s">

</xml_diff>

<commit_message>
add byte reversing version extract / remove instructions
</commit_message>
<xml_diff>
--- a/P4E_psuedo_instruction_set.xlsx
+++ b/P4E_psuedo_instruction_set.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\P4EngineAssembler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADA52403-C013-4C68-A7B9-6671DAC5CFB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D98A87B9-06E7-46D8-82BD-91637EE237AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{87164962-7B7D-4BAA-98E0-B9A8D7C47112}"/>
+    <workbookView xWindow="-38520" yWindow="-3645" windowWidth="38640" windowHeight="21840" xr2:uid="{87164962-7B7D-4BAA-98E0-B9A8D7C47112}"/>
   </bookViews>
   <sheets>
     <sheet name="parser" sheetId="1" r:id="rId1"/>
@@ -205,7 +205,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G24" authorId="0" shapeId="0" xr:uid="{C583D8AB-E013-4381-8744-C1A9F8AD110D}">
+    <comment ref="G28" authorId="0" shapeId="0" xr:uid="{C583D8AB-E013-4381-8744-C1A9F8AD110D}">
       <text>
         <r>
           <rPr>
@@ -232,7 +232,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H24" authorId="0" shapeId="0" xr:uid="{27BF8553-F81E-402A-9E32-1E8BF31559E7}">
+    <comment ref="H28" authorId="0" shapeId="0" xr:uid="{27BF8553-F81E-402A-9E32-1E8BF31559E7}">
       <text>
         <r>
           <rPr>
@@ -259,7 +259,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H33" authorId="0" shapeId="0" xr:uid="{D74AB13C-21EE-417A-A33E-E1DFB10E5B1A}">
+    <comment ref="H41" authorId="0" shapeId="0" xr:uid="{D74AB13C-21EE-417A-A33E-E1DFB10E5B1A}">
       <text>
         <r>
           <rPr>
@@ -286,7 +286,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I33" authorId="0" shapeId="0" xr:uid="{8DAD58C9-7FF9-4A56-9FDF-8206E60D90C1}">
+    <comment ref="I41" authorId="0" shapeId="0" xr:uid="{8DAD58C9-7FF9-4A56-9FDF-8206E60D90C1}">
       <text>
         <r>
           <rPr>
@@ -313,7 +313,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E47" authorId="0" shapeId="0" xr:uid="{70DD23D8-71AE-407E-8A53-DA5E57A5B8A3}">
+    <comment ref="E55" authorId="0" shapeId="0" xr:uid="{70DD23D8-71AE-407E-8A53-DA5E57A5B8A3}">
       <text>
         <r>
           <rPr>
@@ -340,7 +340,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F47" authorId="0" shapeId="0" xr:uid="{FFE5B977-FFE6-4DFE-A7A6-D08DD3A4A1A2}">
+    <comment ref="F55" authorId="0" shapeId="0" xr:uid="{FFE5B977-FFE6-4DFE-A7A6-D08DD3A4A1A2}">
       <text>
         <r>
           <rPr>
@@ -367,7 +367,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C86" authorId="0" shapeId="0" xr:uid="{020F32A4-8410-4792-B861-B3374DCA6F2E}">
+    <comment ref="C94" authorId="0" shapeId="0" xr:uid="{020F32A4-8410-4792-B861-B3374DCA6F2E}">
       <text>
         <r>
           <rPr>
@@ -393,7 +393,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C91" authorId="0" shapeId="0" xr:uid="{1A5CA081-D5E2-473C-BA18-38DD621C5C2B}">
+    <comment ref="C99" authorId="0" shapeId="0" xr:uid="{1A5CA081-D5E2-473C-BA18-38DD621C5C2B}">
       <text>
         <r>
           <rPr>
@@ -419,7 +419,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C98" authorId="0" shapeId="0" xr:uid="{5EAEF23C-593A-4A37-B755-360B9209963D}">
+    <comment ref="C106" authorId="0" shapeId="0" xr:uid="{5EAEF23C-593A-4A37-B755-360B9209963D}">
       <text>
         <r>
           <rPr>
@@ -445,7 +445,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C100" authorId="0" shapeId="0" xr:uid="{AD49495F-3BDD-40D6-ADD1-408F470BCB83}">
+    <comment ref="C108" authorId="0" shapeId="0" xr:uid="{AD49495F-3BDD-40D6-ADD1-408F470BCB83}">
       <text>
         <r>
           <rPr>
@@ -471,7 +471,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C101" authorId="0" shapeId="0" xr:uid="{31ADC337-9E94-4153-8412-495E39530DEF}">
+    <comment ref="C109" authorId="0" shapeId="0" xr:uid="{31ADC337-9E94-4153-8412-495E39530DEF}">
       <text>
         <r>
           <rPr>
@@ -497,7 +497,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C102" authorId="0" shapeId="0" xr:uid="{4B0BBC75-4AFD-4999-8471-DC753FD0455A}">
+    <comment ref="C110" authorId="0" shapeId="0" xr:uid="{4B0BBC75-4AFD-4999-8471-DC753FD0455A}">
       <text>
         <r>
           <rPr>
@@ -523,7 +523,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D114" authorId="0" shapeId="0" xr:uid="{B3419830-61AE-41B1-8075-0EDBC5F16888}">
+    <comment ref="D122" authorId="0" shapeId="0" xr:uid="{B3419830-61AE-41B1-8075-0EDBC5F16888}">
       <text>
         <r>
           <rPr>
@@ -550,7 +550,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A144" authorId="0" shapeId="0" xr:uid="{9DF95069-D8AA-4D9B-B036-F6570707C225}">
+    <comment ref="A152" authorId="0" shapeId="0" xr:uid="{9DF95069-D8AA-4D9B-B036-F6570707C225}">
       <text>
         <r>
           <rPr>
@@ -580,7 +580,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D161" authorId="0" shapeId="0" xr:uid="{10355003-BB36-4D9F-BEF6-AC796CED51BC}">
+    <comment ref="D169" authorId="0" shapeId="0" xr:uid="{10355003-BB36-4D9F-BEF6-AC796CED51BC}">
       <text>
         <r>
           <rPr>
@@ -606,7 +606,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F161" authorId="0" shapeId="0" xr:uid="{EADD36A3-0C54-43FE-AD07-DAE0F1C398C8}">
+    <comment ref="F169" authorId="0" shapeId="0" xr:uid="{EADD36A3-0C54-43FE-AD07-DAE0F1C398C8}">
       <text>
         <r>
           <rPr>
@@ -632,7 +632,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D162" authorId="0" shapeId="0" xr:uid="{5EDDCAB0-8CF8-4E69-91EC-FCEBB8FBFB81}">
+    <comment ref="D170" authorId="0" shapeId="0" xr:uid="{5EDDCAB0-8CF8-4E69-91EC-FCEBB8FBFB81}">
       <text>
         <r>
           <rPr>
@@ -658,7 +658,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F163" authorId="0" shapeId="0" xr:uid="{E9CC35BA-90D8-4E68-A63E-1BDF886428EA}">
+    <comment ref="F171" authorId="0" shapeId="0" xr:uid="{E9CC35BA-90D8-4E68-A63E-1BDF886428EA}">
       <text>
         <r>
           <rPr>
@@ -684,7 +684,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D165" authorId="0" shapeId="0" xr:uid="{C0E77B6C-0F0F-459E-A010-D438E2938743}">
+    <comment ref="D173" authorId="0" shapeId="0" xr:uid="{C0E77B6C-0F0F-459E-A010-D438E2938743}">
       <text>
         <r>
           <rPr>
@@ -710,7 +710,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F166" authorId="0" shapeId="0" xr:uid="{149FA3A0-4084-461C-8457-384C4EC1B272}">
+    <comment ref="F174" authorId="0" shapeId="0" xr:uid="{149FA3A0-4084-461C-8457-384C4EC1B272}">
       <text>
         <r>
           <rPr>
@@ -1359,7 +1359,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1386" uniqueCount="481">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1398" uniqueCount="490">
   <si>
     <t>isr SHiFT</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -6162,6 +6162,42 @@
       </rPr>
       <t>,</t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>parameters same as above</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R32XCT(L)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R16XCT(L)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R32RMV(L)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R16RMV(L)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>byte Reverse 32_bit then ReMoVe</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>byte Reverse two 16_bits then ReMoVe</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>byte Reverse two 16_bits then eXtraCT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>byte Reverse 32_bit then eXtraCT</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -6668,11 +6704,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA14F7B7-5F50-4FFB-AE20-84853F321386}">
-  <dimension ref="A1:I177"/>
+  <dimension ref="A1:I185"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A106" sqref="A106:XFD106"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.2"/>
@@ -7128,136 +7164,98 @@
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
     </row>
-    <row r="23" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>78</v>
+        <v>489</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>152</v>
+        <v>482</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>76</v>
+        <v>481</v>
       </c>
       <c r="I24" s="2"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>276</v>
-      </c>
+        <v>488</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>483</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
       <c r="I25" s="2"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B26" s="2"/>
-      <c r="C26" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>277</v>
-      </c>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
       <c r="I26" s="2"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B27" s="2"/>
-      <c r="C27" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
+    <row r="27" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B27" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B28" s="2"/>
-      <c r="C28" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>276</v>
+      <c r="A28" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>76</v>
       </c>
       <c r="I28" s="2"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>79</v>
+      </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>298</v>
@@ -7266,20 +7264,20 @@
         <v>279</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>241</v>
+        <v>187</v>
       </c>
       <c r="G29" s="2" t="s">
         <v>296</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="I29" s="2"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B30" s="2"/>
       <c r="C30" s="2" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>298</v>
@@ -7288,68 +7286,82 @@
         <v>279</v>
       </c>
       <c r="F30" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="I30" s="2"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B31" s="2"/>
+      <c r="C31" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="F31" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
-    </row>
-    <row r="31" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="8"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>276</v>
+      </c>
       <c r="I32" s="2"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B33" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="I33" s="1" t="s">
-        <v>76</v>
-      </c>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="I33" s="2"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B34" s="2"/>
       <c r="C34" s="2" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>298</v>
@@ -7358,169 +7370,109 @@
         <v>279</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>344</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="H34" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="I34" s="2" t="s">
-        <v>276</v>
-      </c>
+        <v>278</v>
+      </c>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C35" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>344</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="H35" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="I35" s="2" t="s">
-        <v>277</v>
-      </c>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C36" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>344</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="H36" s="2"/>
+      <c r="A36" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>484</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>481</v>
+      </c>
       <c r="I36" s="2"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C37" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>344</v>
-      </c>
-      <c r="G37" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="H37" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="I37" s="2" t="s">
-        <v>276</v>
-      </c>
+      <c r="A37" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>485</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="I37" s="2"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C38" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>344</v>
-      </c>
-      <c r="G38" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="H38" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="I38" s="2" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C39" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>344</v>
-      </c>
-      <c r="G39" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="H39" s="2"/>
-      <c r="I39" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="I38" s="2"/>
+    </row>
+    <row r="39" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B39" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
+      <c r="H39" s="8"/>
+      <c r="I39" s="8"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C40" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="G40" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="H40" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="I40" s="2" t="s">
-        <v>276</v>
-      </c>
+      <c r="A40" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C41" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="G41" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="H41" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="I41" s="2" t="s">
-        <v>277</v>
+      <c r="B41" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
@@ -7534,17 +7486,21 @@
         <v>279</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>280</v>
+        <v>344</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="H42" s="2"/>
-      <c r="I42" s="2"/>
+        <v>187</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="I42" s="2" t="s">
+        <v>276</v>
+      </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C43" s="2" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>298</v>
@@ -7553,21 +7509,21 @@
         <v>279</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>280</v>
+        <v>344</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>187</v>
+        <v>241</v>
       </c>
       <c r="H43" s="2" t="s">
         <v>296</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C44" s="2" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>298</v>
@@ -7576,17 +7532,13 @@
         <v>279</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>280</v>
+        <v>344</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="H44" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="I44" s="2" t="s">
-        <v>277</v>
-      </c>
+        <v>278</v>
+      </c>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C45" s="2" t="s">
@@ -7599,580 +7551,642 @@
         <v>279</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>280</v>
+        <v>344</v>
       </c>
       <c r="G45" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="I45" s="2" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C46" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="I46" s="2" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C47" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="G47" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="H45" s="2"/>
-      <c r="I45" s="2"/>
-    </row>
-    <row r="46" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="C46" s="8"/>
-      <c r="D46" s="8"/>
-      <c r="E46" s="8"/>
-      <c r="F46" s="8"/>
-      <c r="G46" s="8"/>
-      <c r="H46" s="8"/>
-      <c r="I46" s="8"/>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A47" s="1" t="s">
-        <v>347</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>346</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="G47" s="2"/>
       <c r="H47" s="2"/>
       <c r="I47" s="2"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A48" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B48" s="2"/>
       <c r="C48" s="2" t="s">
-        <v>348</v>
+        <v>299</v>
       </c>
       <c r="D48" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="G48" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="E48" s="2" t="s">
+      <c r="H48" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="F48" s="2" t="s">
+      <c r="I48" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="G48" s="2"/>
-      <c r="H48" s="2"/>
-      <c r="I48" s="2"/>
-    </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B49" s="2"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C49" s="2" t="s">
-        <v>348</v>
+        <v>299</v>
       </c>
       <c r="D49" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="G49" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="E49" s="2" t="s">
+      <c r="H49" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="F49" s="2" t="s">
+      <c r="I49" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="G49" s="2"/>
-      <c r="H49" s="2"/>
-      <c r="I49" s="2"/>
-    </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B50" s="2"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C50" s="2" t="s">
-        <v>348</v>
+        <v>299</v>
       </c>
       <c r="D50" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="G50" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="E50" s="2"/>
-      <c r="F50" s="2"/>
-      <c r="G50" s="2"/>
       <c r="H50" s="2"/>
       <c r="I50" s="2"/>
     </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B51" s="2"/>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C51" s="2" t="s">
-        <v>349</v>
+        <v>297</v>
       </c>
       <c r="D51" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="G51" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="E51" s="2" t="s">
+      <c r="H51" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="F51" s="2" t="s">
+      <c r="I51" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="G51" s="2"/>
-      <c r="H51" s="2"/>
-      <c r="I51" s="2"/>
-    </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B52" s="2"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C52" s="2" t="s">
-        <v>349</v>
+        <v>297</v>
       </c>
       <c r="D52" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="G52" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="E52" s="2" t="s">
+      <c r="H52" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="F52" s="2" t="s">
+      <c r="I52" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="G52" s="2"/>
-      <c r="H52" s="2"/>
-      <c r="I52" s="2"/>
-    </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B53" s="2"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C53" s="2" t="s">
-        <v>349</v>
+        <v>297</v>
       </c>
       <c r="D53" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="G53" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="E53" s="2"/>
-      <c r="F53" s="2"/>
-      <c r="G53" s="2"/>
       <c r="H53" s="2"/>
       <c r="I53" s="2"/>
     </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B54" s="2"/>
-      <c r="C54" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="F54" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="G54" s="2"/>
-      <c r="H54" s="2"/>
-      <c r="I54" s="2"/>
-    </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B55" s="2"/>
-      <c r="C55" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="F55" s="2" t="s">
-        <v>277</v>
+    <row r="54" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B54" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="C54" s="8"/>
+      <c r="D54" s="8"/>
+      <c r="E54" s="8"/>
+      <c r="F54" s="8"/>
+      <c r="G54" s="8"/>
+      <c r="H54" s="8"/>
+      <c r="I54" s="8"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>76</v>
       </c>
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
       <c r="I55" s="2"/>
     </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
+        <v>85</v>
+      </c>
       <c r="B56" s="2"/>
       <c r="C56" s="2" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="E56" s="2"/>
-      <c r="F56" s="2"/>
+        <v>187</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>276</v>
+      </c>
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
       <c r="I56" s="2"/>
     </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B57" s="2"/>
       <c r="C57" s="2" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>187</v>
+        <v>241</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>296</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
       <c r="I57" s="2"/>
     </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B58" s="2"/>
       <c r="C58" s="2" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="E58" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="F58" s="2" t="s">
-        <v>277</v>
-      </c>
+        <v>278</v>
+      </c>
+      <c r="E58" s="2"/>
+      <c r="F58" s="2"/>
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
       <c r="I58" s="2"/>
     </row>
-    <row r="59" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B59" s="2"/>
       <c r="C59" s="2" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="E59" s="2"/>
-      <c r="F59" s="2"/>
+        <v>187</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>276</v>
+      </c>
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
       <c r="I59" s="2"/>
     </row>
-    <row r="60" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B60" s="2"/>
       <c r="C60" s="2" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>187</v>
+        <v>241</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>296</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
       <c r="I60" s="2"/>
     </row>
-    <row r="61" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B61" s="2"/>
       <c r="C61" s="2" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="E61" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="F61" s="2" t="s">
-        <v>277</v>
-      </c>
+        <v>278</v>
+      </c>
+      <c r="E61" s="2"/>
+      <c r="F61" s="2"/>
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
       <c r="I61" s="2"/>
     </row>
-    <row r="62" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B62" s="2"/>
       <c r="C62" s="2" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="E62" s="2"/>
-      <c r="F62" s="2"/>
+        <v>187</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>276</v>
+      </c>
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
       <c r="I62" s="2"/>
     </row>
-    <row r="63" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B63" s="2"/>
       <c r="C63" s="2" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>187</v>
+        <v>241</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>296</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
       <c r="I63" s="2"/>
     </row>
-    <row r="64" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B64" s="2"/>
       <c r="C64" s="2" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="E64" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="F64" s="2" t="s">
-        <v>277</v>
-      </c>
+        <v>278</v>
+      </c>
+      <c r="E64" s="2"/>
+      <c r="F64" s="2"/>
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
       <c r="I64" s="2"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B65" s="2"/>
       <c r="C65" s="2" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="E65" s="2"/>
-      <c r="F65" s="2"/>
+        <v>187</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>276</v>
+      </c>
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
       <c r="I65" s="2"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B66" s="2"/>
       <c r="C66" s="2" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>187</v>
+        <v>241</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>296</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
       <c r="I66" s="2"/>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B67" s="2"/>
       <c r="C67" s="2" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="E67" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="F67" s="2" t="s">
-        <v>277</v>
-      </c>
+        <v>278</v>
+      </c>
+      <c r="E67" s="2"/>
+      <c r="F67" s="2"/>
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
       <c r="I67" s="2"/>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B68" s="2"/>
       <c r="C68" s="2" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="E68" s="2"/>
-      <c r="F68" s="2"/>
+        <v>187</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>276</v>
+      </c>
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
       <c r="I68" s="2"/>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B69" s="2"/>
       <c r="C69" s="2" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>187</v>
+        <v>241</v>
       </c>
       <c r="E69" s="2" t="s">
         <v>296</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
       <c r="I69" s="2"/>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B70" s="2"/>
       <c r="C70" s="2" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="E70" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="F70" s="2" t="s">
-        <v>277</v>
-      </c>
+        <v>278</v>
+      </c>
+      <c r="E70" s="2"/>
+      <c r="F70" s="2"/>
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
       <c r="I70" s="2"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B71" s="2"/>
       <c r="C71" s="2" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="E71" s="2"/>
-      <c r="F71" s="2"/>
+        <v>187</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>276</v>
+      </c>
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
       <c r="I71" s="2"/>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B72" s="2"/>
       <c r="C72" s="2" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>187</v>
+        <v>241</v>
       </c>
       <c r="E72" s="2" t="s">
         <v>296</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
       <c r="I72" s="2"/>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B73" s="2"/>
       <c r="C73" s="2" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="E73" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="F73" s="2" t="s">
-        <v>277</v>
-      </c>
+        <v>278</v>
+      </c>
+      <c r="E73" s="2"/>
+      <c r="F73" s="2"/>
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
       <c r="I73" s="2"/>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B74" s="2"/>
       <c r="C74" s="2" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="E74" s="2"/>
-      <c r="F74" s="2"/>
+        <v>187</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>276</v>
+      </c>
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
       <c r="I74" s="2"/>
     </row>
-    <row r="75" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B75" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="C75" s="8"/>
-      <c r="D75" s="8"/>
-      <c r="E75" s="8"/>
-      <c r="F75" s="8"/>
-      <c r="G75" s="8"/>
-      <c r="H75" s="8"/>
-      <c r="I75" s="8"/>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A76" s="1" t="s">
-        <v>86</v>
-      </c>
+    <row r="75" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B75" s="2"/>
+      <c r="C75" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="G75" s="2"/>
+      <c r="H75" s="2"/>
+      <c r="I75" s="2"/>
+    </row>
+    <row r="76" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B76" s="2"/>
+      <c r="C76" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="E76" s="2"/>
+      <c r="F76" s="2"/>
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
       <c r="I76" s="2"/>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A77" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B77" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E77" s="1" t="s">
-        <v>33</v>
+    <row r="77" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B77" s="2"/>
+      <c r="C77" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>276</v>
       </c>
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
       <c r="I77" s="2"/>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B78" s="2"/>
       <c r="C78" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="D78" s="2"/>
+        <v>355</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>241</v>
+      </c>
       <c r="E78" s="2" t="s">
-        <v>282</v>
+        <v>296</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>277</v>
       </c>
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
       <c r="I78" s="2"/>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B79" s="2"/>
       <c r="C79" s="2" t="s">
-        <v>281</v>
+        <v>355</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>466</v>
-      </c>
-      <c r="E79" s="2" t="s">
-        <v>282</v>
-      </c>
+        <v>278</v>
+      </c>
+      <c r="E79" s="2"/>
+      <c r="F79" s="2"/>
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
       <c r="I79" s="2"/>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A80" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="C80" s="2"/>
-      <c r="D80" s="2"/>
-      <c r="E80" s="2"/>
+    <row r="80" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B80" s="2"/>
+      <c r="C80" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>276</v>
+      </c>
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
       <c r="I80" s="2"/>
@@ -8180,11 +8194,16 @@
     <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B81" s="2"/>
       <c r="C81" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="D81" s="2"/>
+        <v>356</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>241</v>
+      </c>
       <c r="E81" s="2" t="s">
-        <v>282</v>
+        <v>296</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>277</v>
       </c>
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
@@ -8193,21 +8212,20 @@
     <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B82" s="2"/>
       <c r="C82" s="2" t="s">
-        <v>281</v>
+        <v>356</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>466</v>
-      </c>
-      <c r="E82" s="2" t="s">
-        <v>282</v>
-      </c>
+        <v>278</v>
+      </c>
+      <c r="E82" s="2"/>
+      <c r="F82" s="2"/>
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
       <c r="I82" s="2"/>
     </row>
     <row r="83" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B83" s="13" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="C83" s="8"/>
       <c r="D83" s="8"/>
@@ -8219,36 +8237,41 @@
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C84" s="2"/>
-      <c r="D84" s="2"/>
-      <c r="F84" s="2"/>
+        <v>86</v>
+      </c>
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
       <c r="I84" s="2"/>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>144</v>
+        <v>96</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="D85" s="2"/>
-      <c r="E85" s="2"/>
-      <c r="F85" s="2"/>
+        <v>155</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
       <c r="I85" s="2"/>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C86" s="1" t="s">
-        <v>190</v>
+      <c r="B86" s="2"/>
+      <c r="C86" s="2" t="s">
+        <v>281</v>
       </c>
       <c r="D86" s="2"/>
-      <c r="E86" s="2"/>
-      <c r="F86" s="2"/>
+      <c r="E86" s="2" t="s">
+        <v>282</v>
+      </c>
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
       <c r="I86" s="2"/>
@@ -8256,95 +8279,101 @@
     <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B87" s="2"/>
       <c r="C87" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="D87" s="2"/>
-      <c r="E87" s="2"/>
-      <c r="F87" s="2"/>
+        <v>281</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>282</v>
+      </c>
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
       <c r="I87" s="2"/>
     </row>
-    <row r="88" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B88" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="C88" s="8"/>
-      <c r="D88" s="8"/>
-      <c r="E88" s="8"/>
-      <c r="F88" s="8"/>
-      <c r="G88" s="8"/>
-      <c r="H88" s="8"/>
-      <c r="I88" s="8"/>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A88" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C88" s="2"/>
+      <c r="D88" s="2"/>
+      <c r="E88" s="2"/>
+      <c r="G88" s="2"/>
+      <c r="H88" s="2"/>
+      <c r="I88" s="2"/>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A89" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C89" s="2"/>
+      <c r="B89" s="2"/>
+      <c r="C89" s="2" t="s">
+        <v>281</v>
+      </c>
       <c r="D89" s="2"/>
-      <c r="F89" s="2"/>
+      <c r="E89" s="2" t="s">
+        <v>282</v>
+      </c>
       <c r="G89" s="2"/>
       <c r="H89" s="2"/>
       <c r="I89" s="2"/>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A90" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="D90" s="2"/>
-      <c r="E90" s="2"/>
-      <c r="F90" s="2"/>
+      <c r="B90" s="2"/>
+      <c r="C90" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>282</v>
+      </c>
       <c r="G90" s="2"/>
       <c r="H90" s="2"/>
       <c r="I90" s="2"/>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C91" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="D91" s="2"/>
-      <c r="E91" s="2"/>
-      <c r="F91" s="2"/>
-      <c r="G91" s="2"/>
-      <c r="H91" s="2"/>
-      <c r="I91" s="2"/>
+    <row r="91" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B91" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="C91" s="8"/>
+      <c r="D91" s="8"/>
+      <c r="E91" s="8"/>
+      <c r="F91" s="8"/>
+      <c r="G91" s="8"/>
+      <c r="H91" s="8"/>
+      <c r="I91" s="8"/>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B92" s="2"/>
-      <c r="C92" s="2" t="s">
-        <v>283</v>
-      </c>
+      <c r="A92" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C92" s="2"/>
       <c r="D92" s="2"/>
-      <c r="E92" s="2"/>
       <c r="F92" s="2"/>
       <c r="G92" s="2"/>
       <c r="H92" s="2"/>
       <c r="I92" s="2"/>
     </row>
-    <row r="93" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B93" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="C93" s="8"/>
-      <c r="D93" s="8"/>
-      <c r="E93" s="8"/>
-      <c r="F93" s="8"/>
-      <c r="G93" s="8"/>
-      <c r="H93" s="8"/>
-      <c r="I93" s="8"/>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A93" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D93" s="2"/>
+      <c r="E93" s="2"/>
+      <c r="F93" s="2"/>
+      <c r="G93" s="2"/>
+      <c r="H93" s="2"/>
+      <c r="I93" s="2"/>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A94" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B94" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="C94" s="2"/>
+      <c r="C94" s="1" t="s">
+        <v>190</v>
+      </c>
       <c r="D94" s="2"/>
       <c r="E94" s="2"/>
       <c r="F94" s="2"/>
@@ -8355,7 +8384,7 @@
     <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B95" s="2"/>
       <c r="C95" s="2" t="s">
-        <v>190</v>
+        <v>283</v>
       </c>
       <c r="D95" s="2"/>
       <c r="E95" s="2"/>
@@ -8366,7 +8395,7 @@
     </row>
     <row r="96" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B96" s="13" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="C96" s="8"/>
       <c r="D96" s="8"/>
@@ -8378,41 +8407,35 @@
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B97" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="C97" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D97" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E97" s="1" t="s">
-        <v>477</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="C97" s="2"/>
+      <c r="D97" s="2"/>
       <c r="F97" s="2"/>
       <c r="G97" s="2"/>
       <c r="H97" s="2"/>
       <c r="I97" s="2"/>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B98" s="2"/>
-      <c r="C98" s="1" t="s">
-        <v>190</v>
-      </c>
+      <c r="A98" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D98" s="2"/>
+      <c r="E98" s="2"/>
       <c r="F98" s="2"/>
       <c r="G98" s="2"/>
       <c r="H98" s="2"/>
       <c r="I98" s="2"/>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B99" s="2"/>
-      <c r="C99" s="2" t="s">
-        <v>284</v>
+      <c r="C99" s="1" t="s">
+        <v>190</v>
       </c>
       <c r="D99" s="2"/>
+      <c r="E99" s="2"/>
       <c r="F99" s="2"/>
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
@@ -8420,27 +8443,39 @@
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B100" s="2"/>
-      <c r="D100" s="2" t="s">
-        <v>286</v>
-      </c>
+      <c r="C100" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="D100" s="2"/>
+      <c r="E100" s="2"/>
+      <c r="F100" s="2"/>
       <c r="G100" s="2"/>
       <c r="H100" s="2"/>
       <c r="I100" s="2"/>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B101" s="2"/>
-      <c r="D101" s="2" t="s">
-        <v>287</v>
-      </c>
-      <c r="G101" s="2"/>
-      <c r="H101" s="2"/>
-      <c r="I101" s="2"/>
+    <row r="101" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B101" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="C101" s="8"/>
+      <c r="D101" s="8"/>
+      <c r="E101" s="8"/>
+      <c r="F101" s="8"/>
+      <c r="G101" s="8"/>
+      <c r="H101" s="8"/>
+      <c r="I101" s="8"/>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B102" s="2"/>
-      <c r="D102" s="2" t="s">
-        <v>288</v>
-      </c>
+      <c r="A102" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C102" s="2"/>
+      <c r="D102" s="2"/>
+      <c r="E102" s="2"/>
+      <c r="F102" s="2"/>
       <c r="G102" s="2"/>
       <c r="H102" s="2"/>
       <c r="I102" s="2"/>
@@ -8448,48 +8483,54 @@
     <row r="103" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B103" s="2"/>
       <c r="C103" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="D103" s="2" t="s">
-        <v>286</v>
-      </c>
+        <v>190</v>
+      </c>
+      <c r="D103" s="2"/>
+      <c r="E103" s="2"/>
+      <c r="F103" s="2"/>
       <c r="G103" s="2"/>
       <c r="H103" s="2"/>
       <c r="I103" s="2"/>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B104" s="2"/>
-      <c r="C104" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="D104" s="2" t="s">
-        <v>287</v>
-      </c>
-      <c r="G104" s="2"/>
-      <c r="H104" s="2"/>
-      <c r="I104" s="2"/>
+    <row r="104" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B104" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="C104" s="8"/>
+      <c r="D104" s="8"/>
+      <c r="E104" s="8"/>
+      <c r="F104" s="8"/>
+      <c r="G104" s="8"/>
+      <c r="H104" s="8"/>
+      <c r="I104" s="8"/>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B105" s="2"/>
-      <c r="C105" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="D105" s="2" t="s">
-        <v>288</v>
-      </c>
+      <c r="A105" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E105" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="F105" s="2"/>
       <c r="G105" s="2"/>
       <c r="H105" s="2"/>
       <c r="I105" s="2"/>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B106" s="2"/>
-      <c r="C106" s="2" t="s">
-        <v>475</v>
-      </c>
-      <c r="D106" s="2"/>
-      <c r="E106" s="1" t="s">
-        <v>476</v>
-      </c>
+      <c r="C106" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="F106" s="2"/>
       <c r="G106" s="2"/>
       <c r="H106" s="2"/>
       <c r="I106" s="2"/>
@@ -8497,28 +8538,18 @@
     <row r="107" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B107" s="2"/>
       <c r="C107" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="D107" s="2" t="s">
-        <v>480</v>
-      </c>
-      <c r="E107" s="1" t="s">
-        <v>476</v>
-      </c>
+        <v>284</v>
+      </c>
+      <c r="D107" s="2"/>
+      <c r="F107" s="2"/>
       <c r="G107" s="2"/>
       <c r="H107" s="2"/>
       <c r="I107" s="2"/>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B108" s="2"/>
-      <c r="C108" s="2" t="s">
-        <v>285</v>
-      </c>
       <c r="D108" s="2" t="s">
-        <v>478</v>
-      </c>
-      <c r="E108" s="1" t="s">
-        <v>476</v>
+        <v>286</v>
       </c>
       <c r="G108" s="2"/>
       <c r="H108" s="2"/>
@@ -8526,48 +8557,30 @@
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B109" s="2"/>
-      <c r="C109" s="2" t="s">
-        <v>285</v>
-      </c>
       <c r="D109" s="2" t="s">
-        <v>479</v>
-      </c>
-      <c r="E109" s="1" t="s">
-        <v>476</v>
+        <v>287</v>
       </c>
       <c r="G109" s="2"/>
       <c r="H109" s="2"/>
       <c r="I109" s="2"/>
     </row>
-    <row r="110" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B110" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="C110" s="8"/>
-      <c r="D110" s="8"/>
-      <c r="E110" s="8"/>
-      <c r="F110" s="8"/>
-      <c r="G110" s="8"/>
-      <c r="H110" s="8"/>
-      <c r="I110" s="8"/>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B110" s="2"/>
+      <c r="D110" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="G110" s="2"/>
+      <c r="H110" s="2"/>
+      <c r="I110" s="2"/>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A111" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="B111" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="C111" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D111" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="E111" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F111" s="2"/>
+      <c r="B111" s="2"/>
+      <c r="C111" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="D111" s="2" t="s">
+        <v>286</v>
+      </c>
       <c r="G111" s="2"/>
       <c r="H111" s="2"/>
       <c r="I111" s="2"/>
@@ -8575,12 +8588,11 @@
     <row r="112" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B112" s="2"/>
       <c r="C112" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="E112" s="2" t="s">
-        <v>293</v>
-      </c>
-      <c r="F112" s="2"/>
+        <v>285</v>
+      </c>
+      <c r="D112" s="2" t="s">
+        <v>287</v>
+      </c>
       <c r="G112" s="2"/>
       <c r="H112" s="2"/>
       <c r="I112" s="2"/>
@@ -8588,12 +8600,11 @@
     <row r="113" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B113" s="2"/>
       <c r="C113" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="E113" s="2" t="s">
-        <v>293</v>
-      </c>
-      <c r="F113" s="2"/>
+        <v>285</v>
+      </c>
+      <c r="D113" s="2" t="s">
+        <v>288</v>
+      </c>
       <c r="G113" s="2"/>
       <c r="H113" s="2"/>
       <c r="I113" s="2"/>
@@ -8601,15 +8612,12 @@
     <row r="114" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B114" s="2"/>
       <c r="C114" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="D114" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="E114" s="2" t="s">
-        <v>293</v>
-      </c>
-      <c r="F114" s="2"/>
+        <v>475</v>
+      </c>
+      <c r="D114" s="2"/>
+      <c r="E114" s="1" t="s">
+        <v>476</v>
+      </c>
       <c r="G114" s="2"/>
       <c r="H114" s="2"/>
       <c r="I114" s="2"/>
@@ -8617,80 +8625,77 @@
     <row r="115" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B115" s="2"/>
       <c r="C115" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="E115" s="2" t="s">
-        <v>293</v>
-      </c>
-      <c r="F115" s="2"/>
+        <v>285</v>
+      </c>
+      <c r="D115" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="E115" s="1" t="s">
+        <v>476</v>
+      </c>
       <c r="G115" s="2"/>
       <c r="H115" s="2"/>
       <c r="I115" s="2"/>
     </row>
-    <row r="116" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B116" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="C116" s="8"/>
-      <c r="D116" s="8"/>
-      <c r="E116" s="8"/>
-      <c r="F116" s="8"/>
-      <c r="G116" s="8"/>
-      <c r="H116" s="8"/>
-      <c r="I116" s="8"/>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B116" s="2"/>
+      <c r="C116" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="D116" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="E116" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="G116" s="2"/>
+      <c r="H116" s="2"/>
+      <c r="I116" s="2"/>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A117" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B117" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="C117" s="2"/>
-      <c r="D117" s="2"/>
-      <c r="E117" s="2"/>
-      <c r="F117" s="2"/>
+      <c r="B117" s="2"/>
+      <c r="C117" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="D117" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="E117" s="1" t="s">
+        <v>476</v>
+      </c>
       <c r="G117" s="2"/>
       <c r="H117" s="2"/>
       <c r="I117" s="2"/>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A118" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B118" s="12" t="s">
-        <v>163</v>
-      </c>
-      <c r="C118" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D118" s="1" t="s">
-        <v>413</v>
-      </c>
-      <c r="E118" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F118" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="G118" s="2"/>
-      <c r="H118" s="2"/>
-      <c r="I118" s="2"/>
+    <row r="118" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B118" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="C118" s="8"/>
+      <c r="D118" s="8"/>
+      <c r="E118" s="8"/>
+      <c r="F118" s="8"/>
+      <c r="G118" s="8"/>
+      <c r="H118" s="8"/>
+      <c r="I118" s="8"/>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B119" s="2"/>
-      <c r="C119" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="D119" s="2" t="s">
-        <v>415</v>
-      </c>
-      <c r="E119" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="F119" s="2" t="s">
-        <v>193</v>
-      </c>
+      <c r="A119" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="E119" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F119" s="2"/>
       <c r="G119" s="2"/>
       <c r="H119" s="2"/>
       <c r="I119" s="2"/>
@@ -8698,17 +8703,12 @@
     <row r="120" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B120" s="2"/>
       <c r="C120" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="D120" s="2" t="s">
-        <v>414</v>
+        <v>289</v>
       </c>
       <c r="E120" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="F120" s="2" t="s">
-        <v>295</v>
-      </c>
+        <v>293</v>
+      </c>
+      <c r="F120" s="2"/>
       <c r="G120" s="2"/>
       <c r="H120" s="2"/>
       <c r="I120" s="2"/>
@@ -8716,102 +8716,90 @@
     <row r="121" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B121" s="2"/>
       <c r="C121" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="D121" s="2" t="s">
-        <v>414</v>
+        <v>290</v>
       </c>
       <c r="E121" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="F121" s="2" t="s">
-        <v>295</v>
-      </c>
+        <v>293</v>
+      </c>
+      <c r="F121" s="2"/>
       <c r="G121" s="2"/>
       <c r="H121" s="2"/>
       <c r="I121" s="2"/>
     </row>
-    <row r="122" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B122" s="13" t="s">
-        <v>129</v>
-      </c>
-      <c r="C122" s="8"/>
-      <c r="D122" s="8"/>
-      <c r="E122" s="8"/>
-      <c r="F122" s="8"/>
-      <c r="G122" s="8"/>
-      <c r="H122" s="8"/>
-      <c r="I122" s="8"/>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B122" s="2"/>
+      <c r="C122" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="D122" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="E122" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="F122" s="2"/>
+      <c r="G122" s="2"/>
+      <c r="H122" s="2"/>
+      <c r="I122" s="2"/>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A123" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B123" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="C123" s="2"/>
-      <c r="D123" s="2"/>
-      <c r="E123" s="2"/>
+      <c r="B123" s="2"/>
+      <c r="C123" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="E123" s="2" t="s">
+        <v>293</v>
+      </c>
       <c r="F123" s="2"/>
       <c r="G123" s="2"/>
       <c r="H123" s="2"/>
       <c r="I123" s="2"/>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A124" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B124" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="C124" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D124" s="1" t="s">
-        <v>413</v>
-      </c>
-      <c r="E124" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F124" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="G124" s="2"/>
-      <c r="H124" s="2"/>
-      <c r="I124" s="2"/>
+    <row r="124" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B124" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="C124" s="8"/>
+      <c r="D124" s="8"/>
+      <c r="E124" s="8"/>
+      <c r="F124" s="8"/>
+      <c r="G124" s="8"/>
+      <c r="H124" s="8"/>
+      <c r="I124" s="8"/>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B125" s="2"/>
-      <c r="C125" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="D125" s="2" t="s">
-        <v>415</v>
-      </c>
-      <c r="E125" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="F125" s="2" t="s">
-        <v>193</v>
-      </c>
+      <c r="A125" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C125" s="2"/>
+      <c r="D125" s="2"/>
+      <c r="E125" s="2"/>
+      <c r="F125" s="2"/>
       <c r="G125" s="2"/>
       <c r="H125" s="2"/>
       <c r="I125" s="2"/>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B126" s="2"/>
-      <c r="C126" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="D126" s="2" t="s">
-        <v>414</v>
-      </c>
-      <c r="E126" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="F126" s="2" t="s">
-        <v>295</v>
+      <c r="A126" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B126" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D126" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="E126" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F126" s="1" t="s">
+        <v>194</v>
       </c>
       <c r="G126" s="2"/>
       <c r="H126" s="2"/>
@@ -8820,96 +8808,102 @@
     <row r="127" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B127" s="2"/>
       <c r="C127" s="2" t="s">
-        <v>297</v>
+        <v>187</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="E127" s="2" t="s">
         <v>294</v>
       </c>
       <c r="F127" s="2" t="s">
-        <v>295</v>
+        <v>193</v>
       </c>
       <c r="G127" s="2"/>
       <c r="H127" s="2"/>
       <c r="I127" s="2"/>
     </row>
-    <row r="128" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B128" s="13" t="s">
-        <v>130</v>
-      </c>
-      <c r="C128" s="8"/>
-      <c r="D128" s="8"/>
-      <c r="E128" s="8"/>
-      <c r="F128" s="8"/>
-      <c r="G128" s="8"/>
-      <c r="H128" s="8"/>
-      <c r="I128" s="8"/>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B128" s="2"/>
+      <c r="C128" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="D128" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="E128" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="F128" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="G128" s="2"/>
+      <c r="H128" s="2"/>
+      <c r="I128" s="2"/>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A129" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B129" s="2" t="s">
-        <v>166</v>
-      </c>
+      <c r="B129" s="2"/>
+      <c r="C129" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="D129" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="E129" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="F129" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="G129" s="2"/>
       <c r="H129" s="2"/>
       <c r="I129" s="2"/>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A130" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B130" s="12" t="s">
-        <v>167</v>
-      </c>
-      <c r="C130" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D130" s="1" t="s">
-        <v>413</v>
-      </c>
-      <c r="E130" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F130" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="H130" s="2"/>
-      <c r="I130" s="2"/>
+    <row r="130" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B130" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="C130" s="8"/>
+      <c r="D130" s="8"/>
+      <c r="E130" s="8"/>
+      <c r="F130" s="8"/>
+      <c r="G130" s="8"/>
+      <c r="H130" s="8"/>
+      <c r="I130" s="8"/>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B131" s="2"/>
-      <c r="C131" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="D131" s="2" t="s">
-        <v>415</v>
-      </c>
-      <c r="E131" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="F131" s="2" t="s">
-        <v>193</v>
-      </c>
+      <c r="A131" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C131" s="2"/>
+      <c r="D131" s="2"/>
+      <c r="E131" s="2"/>
+      <c r="F131" s="2"/>
       <c r="G131" s="2"/>
       <c r="H131" s="2"/>
       <c r="I131" s="2"/>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B132" s="2"/>
-      <c r="C132" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="D132" s="2" t="s">
-        <v>414</v>
-      </c>
-      <c r="E132" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="F132" s="2" t="s">
-        <v>295</v>
+      <c r="A132" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B132" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D132" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="E132" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F132" s="1" t="s">
+        <v>194</v>
       </c>
       <c r="G132" s="2"/>
       <c r="H132" s="2"/>
@@ -8918,152 +8912,187 @@
     <row r="133" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B133" s="2"/>
       <c r="C133" s="2" t="s">
-        <v>297</v>
+        <v>187</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="E133" s="2" t="s">
         <v>294</v>
       </c>
       <c r="F133" s="2" t="s">
-        <v>295</v>
+        <v>193</v>
       </c>
       <c r="G133" s="2"/>
       <c r="H133" s="2"/>
       <c r="I133" s="2"/>
     </row>
-    <row r="134" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B134" s="13" t="s">
-        <v>133</v>
-      </c>
-      <c r="C134" s="8"/>
-      <c r="D134" s="8"/>
-      <c r="E134" s="8"/>
-      <c r="F134" s="8"/>
-      <c r="G134" s="8"/>
-      <c r="H134" s="8"/>
-      <c r="I134" s="8"/>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B134" s="2"/>
+      <c r="C134" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="D134" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="E134" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="F134" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="G134" s="2"/>
+      <c r="H134" s="2"/>
+      <c r="I134" s="2"/>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A135" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B135" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="C135" s="2"/>
-      <c r="D135" s="2"/>
-      <c r="E135" s="2"/>
-      <c r="F135" s="2"/>
+      <c r="B135" s="2"/>
+      <c r="C135" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="D135" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="E135" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="F135" s="2" t="s">
+        <v>295</v>
+      </c>
       <c r="G135" s="2"/>
       <c r="H135" s="2"/>
       <c r="I135" s="2"/>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B136" s="2"/>
-      <c r="C136" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="D136" s="2"/>
-      <c r="E136" s="2"/>
-      <c r="F136" s="2"/>
-      <c r="G136" s="2"/>
-      <c r="H136" s="2"/>
-      <c r="I136" s="2"/>
-    </row>
-    <row r="137" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B137" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="D137" s="8"/>
-      <c r="E137" s="8"/>
-      <c r="F137" s="8"/>
-      <c r="G137" s="8"/>
-      <c r="H137" s="8"/>
-      <c r="I137" s="8"/>
+    <row r="136" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B136" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="C136" s="8"/>
+      <c r="D136" s="8"/>
+      <c r="E136" s="8"/>
+      <c r="F136" s="8"/>
+      <c r="G136" s="8"/>
+      <c r="H136" s="8"/>
+      <c r="I136" s="8"/>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A137" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B137" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="H137" s="2"/>
+      <c r="I137" s="2"/>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A138" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B138" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="D138" s="2"/>
-      <c r="E138" s="2"/>
-      <c r="F138" s="2"/>
-      <c r="G138" s="2"/>
+      <c r="A138" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B138" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D138" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="E138" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F138" s="1" t="s">
+        <v>194</v>
+      </c>
       <c r="H138" s="2"/>
       <c r="I138" s="2"/>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B139" s="2"/>
-      <c r="C139" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="D139" s="2"/>
-      <c r="E139" s="2"/>
-      <c r="F139" s="2"/>
+      <c r="C139" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D139" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="E139" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="F139" s="2" t="s">
+        <v>193</v>
+      </c>
       <c r="G139" s="2"/>
       <c r="H139" s="2"/>
       <c r="I139" s="2"/>
     </row>
-    <row r="140" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B140" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="D140" s="8"/>
-      <c r="E140" s="8"/>
-      <c r="F140" s="8"/>
-      <c r="G140" s="8"/>
-      <c r="H140" s="8"/>
-      <c r="I140" s="8"/>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B140" s="2"/>
+      <c r="C140" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="D140" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="E140" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="F140" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="G140" s="2"/>
+      <c r="H140" s="2"/>
+      <c r="I140" s="2"/>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A141" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B141" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="D141" s="2"/>
-      <c r="E141" s="2"/>
-      <c r="F141" s="2"/>
+      <c r="B141" s="2"/>
+      <c r="C141" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="D141" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="E141" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="F141" s="2" t="s">
+        <v>295</v>
+      </c>
       <c r="G141" s="2"/>
       <c r="H141" s="2"/>
       <c r="I141" s="2"/>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B142" s="2"/>
-      <c r="C142" s="1" t="s">
+    <row r="142" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B142" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="C142" s="8"/>
+      <c r="D142" s="8"/>
+      <c r="E142" s="8"/>
+      <c r="F142" s="8"/>
+      <c r="G142" s="8"/>
+      <c r="H142" s="8"/>
+      <c r="I142" s="8"/>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A143" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C143" s="2"/>
+      <c r="D143" s="2"/>
+      <c r="E143" s="2"/>
+      <c r="F143" s="2"/>
+      <c r="G143" s="2"/>
+      <c r="H143" s="2"/>
+      <c r="I143" s="2"/>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B144" s="2"/>
+      <c r="C144" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="D142" s="2"/>
-      <c r="E142" s="2"/>
-      <c r="F142" s="2"/>
-      <c r="G142" s="2"/>
-      <c r="H142" s="2"/>
-      <c r="I142" s="2"/>
-    </row>
-    <row r="143" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B143" s="13" t="s">
-        <v>136</v>
-      </c>
-      <c r="C143" s="8"/>
-      <c r="D143" s="8"/>
-      <c r="E143" s="8"/>
-      <c r="F143" s="8"/>
-      <c r="G143" s="8"/>
-      <c r="H143" s="8"/>
-      <c r="I143" s="8"/>
-    </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A144" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="B144" s="2"/>
-      <c r="C144" s="2"/>
       <c r="D144" s="2"/>
       <c r="E144" s="2"/>
       <c r="F144" s="2"/>
@@ -9071,29 +9100,24 @@
       <c r="H144" s="2"/>
       <c r="I144" s="2"/>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A145" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B145" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="C145" s="2"/>
-      <c r="D145" s="2"/>
-      <c r="E145" s="2"/>
-      <c r="F145" s="2"/>
-      <c r="G145" s="2"/>
-      <c r="H145" s="2"/>
-      <c r="I145" s="2"/>
+    <row r="145" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B145" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="D145" s="8"/>
+      <c r="E145" s="8"/>
+      <c r="F145" s="8"/>
+      <c r="G145" s="8"/>
+      <c r="H145" s="8"/>
+      <c r="I145" s="8"/>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="C146" s="2"/>
+        <v>169</v>
+      </c>
       <c r="D146" s="2"/>
       <c r="E146" s="2"/>
       <c r="F146" s="2"/>
@@ -9102,13 +9126,10 @@
       <c r="I146" s="2"/>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A147" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B147" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="C147" s="2"/>
+      <c r="B147" s="2"/>
+      <c r="C147" s="1" t="s">
+        <v>190</v>
+      </c>
       <c r="D147" s="2"/>
       <c r="E147" s="2"/>
       <c r="F147" s="2"/>
@@ -9116,29 +9137,24 @@
       <c r="H147" s="2"/>
       <c r="I147" s="2"/>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A148" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="B148" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="C148" s="2"/>
-      <c r="D148" s="2"/>
-      <c r="E148" s="2"/>
-      <c r="F148" s="2"/>
-      <c r="G148" s="2"/>
-      <c r="H148" s="2"/>
-      <c r="I148" s="2"/>
+    <row r="148" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B148" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="D148" s="8"/>
+      <c r="E148" s="8"/>
+      <c r="F148" s="8"/>
+      <c r="G148" s="8"/>
+      <c r="H148" s="8"/>
+      <c r="I148" s="8"/>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="C149" s="2"/>
+        <v>170</v>
+      </c>
       <c r="D149" s="2"/>
       <c r="E149" s="2"/>
       <c r="F149" s="2"/>
@@ -9147,51 +9163,34 @@
       <c r="I149" s="2"/>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A150" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B150" s="2" t="s">
-        <v>176</v>
-      </c>
+      <c r="B150" s="2"/>
       <c r="C150" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D150" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="E150" s="1" t="s">
-        <v>147</v>
-      </c>
+        <v>190</v>
+      </c>
+      <c r="D150" s="2"/>
+      <c r="E150" s="2"/>
+      <c r="F150" s="2"/>
       <c r="G150" s="2"/>
       <c r="H150" s="2"/>
       <c r="I150" s="2"/>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A151" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="B151" s="2"/>
-      <c r="C151" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="D151" s="2" t="s">
-        <v>270</v>
-      </c>
-      <c r="E151" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="F151" s="2"/>
-      <c r="G151" s="2"/>
-      <c r="H151" s="2"/>
-      <c r="I151" s="2"/>
+    <row r="151" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B151" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="C151" s="8"/>
+      <c r="D151" s="8"/>
+      <c r="E151" s="8"/>
+      <c r="F151" s="8"/>
+      <c r="G151" s="8"/>
+      <c r="H151" s="8"/>
+      <c r="I151" s="8"/>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="B152" s="2" t="s">
-        <v>177</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="B152" s="2"/>
       <c r="C152" s="2"/>
       <c r="D152" s="2"/>
       <c r="E152" s="2"/>
@@ -9201,8 +9200,11 @@
       <c r="I152" s="2"/>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A153" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="B153" s="2" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="C153" s="2"/>
       <c r="D153" s="2"/>
@@ -9213,8 +9215,11 @@
       <c r="I153" s="2"/>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A154" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="B154" s="2" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="C154" s="2"/>
       <c r="D154" s="2"/>
@@ -9225,8 +9230,11 @@
       <c r="I154" s="2"/>
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A155" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="B155" s="2" t="s">
-        <v>268</v>
+        <v>174</v>
       </c>
       <c r="C155" s="2"/>
       <c r="D155" s="2"/>
@@ -9237,8 +9245,11 @@
       <c r="I155" s="2"/>
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A156" s="1" t="s">
+        <v>266</v>
+      </c>
       <c r="B156" s="2" t="s">
-        <v>180</v>
+        <v>267</v>
       </c>
       <c r="C156" s="2"/>
       <c r="D156" s="2"/>
@@ -9249,8 +9260,11 @@
       <c r="I156" s="2"/>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A157" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="B157" s="2" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="C157" s="2"/>
       <c r="D157" s="2"/>
@@ -9260,224 +9274,338 @@
       <c r="H157" s="2"/>
       <c r="I157" s="2"/>
     </row>
-    <row r="158" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B158" s="13" t="s">
-        <v>138</v>
-      </c>
-      <c r="C158" s="8"/>
-      <c r="D158" s="8"/>
-      <c r="E158" s="8"/>
-      <c r="F158" s="8"/>
-      <c r="G158" s="8"/>
-      <c r="H158" s="8"/>
-      <c r="I158" s="8"/>
+    <row r="158" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A158" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B158" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D158" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E158" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="G158" s="2"/>
+      <c r="H158" s="2"/>
+      <c r="I158" s="2"/>
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
-        <v>137</v>
-      </c>
+        <v>146</v>
+      </c>
+      <c r="B159" s="2"/>
+      <c r="C159" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="D159" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="E159" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="F159" s="2"/>
+      <c r="G159" s="2"/>
+      <c r="H159" s="2"/>
+      <c r="I159" s="2"/>
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
-        <v>13</v>
+        <v>171</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="C160" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D160" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E160" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F160" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G160" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="H160" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>177</v>
+      </c>
+      <c r="C160" s="2"/>
+      <c r="D160" s="2"/>
+      <c r="E160" s="2"/>
+      <c r="F160" s="2"/>
+      <c r="G160" s="2"/>
+      <c r="H160" s="2"/>
+      <c r="I160" s="2"/>
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C161" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="D161" s="2" t="s">
-        <v>359</v>
-      </c>
-      <c r="E161" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="F161" s="2" t="s">
-        <v>359</v>
-      </c>
-      <c r="G161" s="2" t="s">
-        <v>357</v>
-      </c>
-      <c r="H161" s="14" t="s">
-        <v>274</v>
-      </c>
+      <c r="B161" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C161" s="2"/>
+      <c r="D161" s="2"/>
+      <c r="E161" s="2"/>
+      <c r="F161" s="2"/>
+      <c r="G161" s="2"/>
+      <c r="H161" s="2"/>
+      <c r="I161" s="2"/>
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C162" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="D162" s="2" t="s">
-        <v>359</v>
-      </c>
+      <c r="B162" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C162" s="2"/>
+      <c r="D162" s="2"/>
       <c r="E162" s="2"/>
       <c r="F162" s="2"/>
-      <c r="G162" s="2" t="s">
-        <v>357</v>
-      </c>
-      <c r="H162" s="14" t="s">
-        <v>274</v>
-      </c>
+      <c r="G162" s="2"/>
+      <c r="H162" s="2"/>
+      <c r="I162" s="2"/>
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B163" s="2" t="s">
+        <v>268</v>
+      </c>
       <c r="C163" s="2"/>
       <c r="D163" s="2"/>
-      <c r="E163" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="F163" s="2" t="s">
-        <v>359</v>
-      </c>
-      <c r="G163" s="2" t="s">
-        <v>357</v>
-      </c>
-      <c r="H163" s="14" t="s">
-        <v>274</v>
-      </c>
+      <c r="E163" s="2"/>
+      <c r="F163" s="2"/>
+      <c r="G163" s="2"/>
+      <c r="H163" s="2"/>
+      <c r="I163" s="2"/>
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B164" s="2" t="s">
+        <v>180</v>
+      </c>
       <c r="C164" s="2"/>
       <c r="D164" s="2"/>
       <c r="E164" s="2"/>
       <c r="F164" s="2"/>
-      <c r="G164" s="2" t="s">
-        <v>357</v>
-      </c>
-      <c r="H164" s="14" t="s">
-        <v>274</v>
-      </c>
+      <c r="G164" s="2"/>
+      <c r="H164" s="2"/>
+      <c r="I164" s="2"/>
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C165" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="D165" s="2" t="s">
-        <v>359</v>
-      </c>
+      <c r="B165" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C165" s="2"/>
+      <c r="D165" s="2"/>
       <c r="E165" s="2"/>
       <c r="F165" s="2"/>
       <c r="G165" s="2"/>
-      <c r="H165" s="14" t="s">
+      <c r="H165" s="2"/>
+      <c r="I165" s="2"/>
+    </row>
+    <row r="166" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B166" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="C166" s="8"/>
+      <c r="D166" s="8"/>
+      <c r="E166" s="8"/>
+      <c r="F166" s="8"/>
+      <c r="G166" s="8"/>
+      <c r="H166" s="8"/>
+      <c r="I166" s="8"/>
+    </row>
+    <row r="167" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A167" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="168" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A168" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B168" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C168" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D168" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E168" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F168" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G168" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="H168" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="169" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C169" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="D169" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="E169" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="F169" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="G169" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="H169" s="14" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C166" s="2"/>
-      <c r="D166" s="2"/>
-      <c r="E166" s="2" t="s">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C170" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="D170" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="E170" s="2"/>
+      <c r="F170" s="2"/>
+      <c r="G170" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="H170" s="14" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="171" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C171" s="2"/>
+      <c r="D171" s="2"/>
+      <c r="E171" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="F166" s="2" t="s">
+      <c r="F171" s="2" t="s">
         <v>359</v>
       </c>
-      <c r="G166" s="2"/>
-      <c r="H166" s="14" t="s">
+      <c r="G171" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="H171" s="14" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C167" s="2"/>
-      <c r="D167" s="2"/>
-      <c r="E167" s="2"/>
-      <c r="F167" s="2"/>
-      <c r="G167" s="2"/>
-      <c r="H167" s="14" t="s">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C172" s="2"/>
+      <c r="D172" s="2"/>
+      <c r="E172" s="2"/>
+      <c r="F172" s="2"/>
+      <c r="G172" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="H172" s="14" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="168" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B168" s="13" t="s">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C173" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="D173" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="E173" s="2"/>
+      <c r="F173" s="2"/>
+      <c r="G173" s="2"/>
+      <c r="H173" s="14" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="174" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C174" s="2"/>
+      <c r="D174" s="2"/>
+      <c r="E174" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="F174" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="G174" s="2"/>
+      <c r="H174" s="14" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="175" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C175" s="2"/>
+      <c r="D175" s="2"/>
+      <c r="E175" s="2"/>
+      <c r="F175" s="2"/>
+      <c r="G175" s="2"/>
+      <c r="H175" s="14" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="176" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B176" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="C168" s="8"/>
-      <c r="D168" s="8"/>
-      <c r="E168" s="8"/>
-      <c r="F168" s="8"/>
-      <c r="G168" s="8"/>
-      <c r="H168" s="8"/>
-      <c r="I168" s="8"/>
-    </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A169" s="1" t="s">
+      <c r="C176" s="8"/>
+      <c r="D176" s="8"/>
+      <c r="E176" s="8"/>
+      <c r="F176" s="8"/>
+      <c r="G176" s="8"/>
+      <c r="H176" s="8"/>
+      <c r="I176" s="8"/>
+    </row>
+    <row r="177" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A177" s="1" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A170" s="1" t="s">
+    <row r="178" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A178" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B170" s="2" t="s">
+      <c r="B178" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="C170" s="1" t="s">
+      <c r="C178" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C171" s="2" t="s">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C179" s="2" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C172" s="1" t="s">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C180" s="1" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="173" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B173" s="13" t="s">
+    <row r="181" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B181" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="C173" s="8"/>
-      <c r="D173" s="8"/>
-      <c r="E173" s="8"/>
-      <c r="F173" s="8"/>
-      <c r="G173" s="8"/>
-      <c r="H173" s="8"/>
-      <c r="I173" s="8"/>
-    </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A174" s="1" t="s">
+      <c r="C181" s="8"/>
+      <c r="D181" s="8"/>
+      <c r="E181" s="8"/>
+      <c r="F181" s="8"/>
+      <c r="G181" s="8"/>
+      <c r="H181" s="8"/>
+      <c r="I181" s="8"/>
+    </row>
+    <row r="182" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A182" s="1" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A175" s="1" t="s">
+    <row r="183" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A183" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B175" s="2" t="s">
+      <c r="B183" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="C175" s="1" t="s">
+      <c r="C183" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C176" s="2" t="s">
+    <row r="184" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C184" s="2" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="177" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C177" s="1" t="s">
+    <row r="185" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C185" s="1" t="s">
         <v>190</v>
       </c>
     </row>

</xml_diff>

<commit_message>
parser copy instruction adding intrinsic meta data as one more source selection
</commit_message>
<xml_diff>
--- a/P4E_psuedo_instruction_set.xlsx
+++ b/P4E_psuedo_instruction_set.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\P4EngineAssembler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D98A87B9-06E7-46D8-82BD-91637EE237AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E582B471-EAB5-4F77-B6C9-93011466651F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-3645" windowWidth="38640" windowHeight="21840" xr2:uid="{87164962-7B7D-4BAA-98E0-B9A8D7C47112}"/>
   </bookViews>
@@ -367,7 +367,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C94" authorId="0" shapeId="0" xr:uid="{020F32A4-8410-4792-B861-B3374DCA6F2E}">
+    <comment ref="C103" authorId="0" shapeId="0" xr:uid="{020F32A4-8410-4792-B861-B3374DCA6F2E}">
       <text>
         <r>
           <rPr>
@@ -393,7 +393,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C99" authorId="0" shapeId="0" xr:uid="{1A5CA081-D5E2-473C-BA18-38DD621C5C2B}">
+    <comment ref="C108" authorId="0" shapeId="0" xr:uid="{1A5CA081-D5E2-473C-BA18-38DD621C5C2B}">
       <text>
         <r>
           <rPr>
@@ -419,7 +419,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C106" authorId="0" shapeId="0" xr:uid="{5EAEF23C-593A-4A37-B755-360B9209963D}">
+    <comment ref="C115" authorId="0" shapeId="0" xr:uid="{5EAEF23C-593A-4A37-B755-360B9209963D}">
       <text>
         <r>
           <rPr>
@@ -445,7 +445,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C108" authorId="0" shapeId="0" xr:uid="{AD49495F-3BDD-40D6-ADD1-408F470BCB83}">
+    <comment ref="C117" authorId="0" shapeId="0" xr:uid="{AD49495F-3BDD-40D6-ADD1-408F470BCB83}">
       <text>
         <r>
           <rPr>
@@ -471,7 +471,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C109" authorId="0" shapeId="0" xr:uid="{31ADC337-9E94-4153-8412-495E39530DEF}">
+    <comment ref="C118" authorId="0" shapeId="0" xr:uid="{31ADC337-9E94-4153-8412-495E39530DEF}">
       <text>
         <r>
           <rPr>
@@ -497,7 +497,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C110" authorId="0" shapeId="0" xr:uid="{4B0BBC75-4AFD-4999-8471-DC753FD0455A}">
+    <comment ref="C119" authorId="0" shapeId="0" xr:uid="{4B0BBC75-4AFD-4999-8471-DC753FD0455A}">
       <text>
         <r>
           <rPr>
@@ -523,7 +523,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D122" authorId="0" shapeId="0" xr:uid="{B3419830-61AE-41B1-8075-0EDBC5F16888}">
+    <comment ref="D131" authorId="0" shapeId="0" xr:uid="{B3419830-61AE-41B1-8075-0EDBC5F16888}">
       <text>
         <r>
           <rPr>
@@ -550,7 +550,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A152" authorId="0" shapeId="0" xr:uid="{9DF95069-D8AA-4D9B-B036-F6570707C225}">
+    <comment ref="A161" authorId="0" shapeId="0" xr:uid="{9DF95069-D8AA-4D9B-B036-F6570707C225}">
       <text>
         <r>
           <rPr>
@@ -580,7 +580,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D169" authorId="0" shapeId="0" xr:uid="{10355003-BB36-4D9F-BEF6-AC796CED51BC}">
+    <comment ref="D178" authorId="0" shapeId="0" xr:uid="{10355003-BB36-4D9F-BEF6-AC796CED51BC}">
       <text>
         <r>
           <rPr>
@@ -606,7 +606,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F169" authorId="0" shapeId="0" xr:uid="{EADD36A3-0C54-43FE-AD07-DAE0F1C398C8}">
+    <comment ref="F178" authorId="0" shapeId="0" xr:uid="{EADD36A3-0C54-43FE-AD07-DAE0F1C398C8}">
       <text>
         <r>
           <rPr>
@@ -632,7 +632,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D170" authorId="0" shapeId="0" xr:uid="{5EDDCAB0-8CF8-4E69-91EC-FCEBB8FBFB81}">
+    <comment ref="D179" authorId="0" shapeId="0" xr:uid="{5EDDCAB0-8CF8-4E69-91EC-FCEBB8FBFB81}">
       <text>
         <r>
           <rPr>
@@ -658,7 +658,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F171" authorId="0" shapeId="0" xr:uid="{E9CC35BA-90D8-4E68-A63E-1BDF886428EA}">
+    <comment ref="F180" authorId="0" shapeId="0" xr:uid="{E9CC35BA-90D8-4E68-A63E-1BDF886428EA}">
       <text>
         <r>
           <rPr>
@@ -684,7 +684,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D173" authorId="0" shapeId="0" xr:uid="{C0E77B6C-0F0F-459E-A010-D438E2938743}">
+    <comment ref="D182" authorId="0" shapeId="0" xr:uid="{C0E77B6C-0F0F-459E-A010-D438E2938743}">
       <text>
         <r>
           <rPr>
@@ -710,7 +710,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F174" authorId="0" shapeId="0" xr:uid="{149FA3A0-4084-461C-8457-384C4EC1B272}">
+    <comment ref="F183" authorId="0" shapeId="0" xr:uid="{149FA3A0-4084-461C-8457-384C4EC1B272}">
       <text>
         <r>
           <rPr>
@@ -1359,7 +1359,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1398" uniqueCount="490">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1428" uniqueCount="493">
   <si>
     <t>isr SHiFT</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -6198,6 +6198,108 @@
   </si>
   <si>
     <t>byte Reverse 32_bit then eXtraCT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">META [ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>INTR0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> ] ,</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">META [ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>INTR1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> ] ,</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">META [ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>INTR2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> ] ,</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -6704,11 +6806,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA14F7B7-5F50-4FFB-AE20-84853F321386}">
-  <dimension ref="A1:I185"/>
+  <dimension ref="A1:I194"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D91" sqref="D91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.2"/>
@@ -8223,42 +8325,52 @@
       <c r="H82" s="2"/>
       <c r="I82" s="2"/>
     </row>
-    <row r="83" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B83" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="C83" s="8"/>
-      <c r="D83" s="8"/>
-      <c r="E83" s="8"/>
-      <c r="F83" s="8"/>
-      <c r="G83" s="8"/>
-      <c r="H83" s="8"/>
-      <c r="I83" s="8"/>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B83" s="2"/>
+      <c r="C83" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="F83" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="G83" s="2"/>
+      <c r="H83" s="2"/>
+      <c r="I83" s="2"/>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A84" s="1" t="s">
-        <v>86</v>
+      <c r="B84" s="2"/>
+      <c r="C84" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="F84" s="2" t="s">
+        <v>277</v>
       </c>
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
       <c r="I84" s="2"/>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A85" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="C85" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="D85" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E85" s="1" t="s">
-        <v>33</v>
-      </c>
+      <c r="B85" s="2"/>
+      <c r="C85" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="E85" s="2"/>
+      <c r="F85" s="2"/>
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
       <c r="I85" s="2"/>
@@ -8266,11 +8378,16 @@
     <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B86" s="2"/>
       <c r="C86" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="D86" s="2"/>
+        <v>491</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>187</v>
+      </c>
       <c r="E86" s="2" t="s">
-        <v>282</v>
+        <v>296</v>
+      </c>
+      <c r="F86" s="2" t="s">
+        <v>276</v>
       </c>
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
@@ -8279,28 +8396,31 @@
     <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B87" s="2"/>
       <c r="C87" s="2" t="s">
-        <v>281</v>
+        <v>491</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>466</v>
+        <v>241</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>282</v>
+        <v>296</v>
+      </c>
+      <c r="F87" s="2" t="s">
+        <v>277</v>
       </c>
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
       <c r="I87" s="2"/>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A88" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="C88" s="2"/>
-      <c r="D88" s="2"/>
+      <c r="B88" s="2"/>
+      <c r="C88" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>278</v>
+      </c>
       <c r="E88" s="2"/>
+      <c r="F88" s="2"/>
       <c r="G88" s="2"/>
       <c r="H88" s="2"/>
       <c r="I88" s="2"/>
@@ -8308,11 +8428,16 @@
     <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B89" s="2"/>
       <c r="C89" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="D89" s="2"/>
+        <v>492</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>187</v>
+      </c>
       <c r="E89" s="2" t="s">
-        <v>282</v>
+        <v>296</v>
+      </c>
+      <c r="F89" s="2" t="s">
+        <v>276</v>
       </c>
       <c r="G89" s="2"/>
       <c r="H89" s="2"/>
@@ -8321,62 +8446,71 @@
     <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B90" s="2"/>
       <c r="C90" s="2" t="s">
-        <v>281</v>
+        <v>492</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>466</v>
+        <v>241</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>282</v>
+        <v>296</v>
+      </c>
+      <c r="F90" s="2" t="s">
+        <v>277</v>
       </c>
       <c r="G90" s="2"/>
       <c r="H90" s="2"/>
       <c r="I90" s="2"/>
     </row>
-    <row r="91" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B91" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="C91" s="8"/>
-      <c r="D91" s="8"/>
-      <c r="E91" s="8"/>
-      <c r="F91" s="8"/>
-      <c r="G91" s="8"/>
-      <c r="H91" s="8"/>
-      <c r="I91" s="8"/>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A92" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C92" s="2"/>
-      <c r="D92" s="2"/>
-      <c r="F92" s="2"/>
-      <c r="G92" s="2"/>
-      <c r="H92" s="2"/>
-      <c r="I92" s="2"/>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B91" s="2"/>
+      <c r="C91" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="E91" s="2"/>
+      <c r="F91" s="2"/>
+      <c r="G91" s="2"/>
+      <c r="H91" s="2"/>
+      <c r="I91" s="2"/>
+    </row>
+    <row r="92" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B92" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="C92" s="8"/>
+      <c r="D92" s="8"/>
+      <c r="E92" s="8"/>
+      <c r="F92" s="8"/>
+      <c r="G92" s="8"/>
+      <c r="H92" s="8"/>
+      <c r="I92" s="8"/>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="B93" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="D93" s="2"/>
-      <c r="E93" s="2"/>
-      <c r="F93" s="2"/>
+        <v>86</v>
+      </c>
       <c r="G93" s="2"/>
       <c r="H93" s="2"/>
       <c r="I93" s="2"/>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A94" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>155</v>
+      </c>
       <c r="C94" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="D94" s="2"/>
-      <c r="E94" s="2"/>
-      <c r="F94" s="2"/>
+        <v>200</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="G94" s="2"/>
       <c r="H94" s="2"/>
       <c r="I94" s="2"/>
@@ -8384,95 +8518,103 @@
     <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B95" s="2"/>
       <c r="C95" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D95" s="2"/>
-      <c r="E95" s="2"/>
-      <c r="F95" s="2"/>
+      <c r="E95" s="2" t="s">
+        <v>282</v>
+      </c>
       <c r="G95" s="2"/>
       <c r="H95" s="2"/>
       <c r="I95" s="2"/>
     </row>
-    <row r="96" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B96" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="C96" s="8"/>
-      <c r="D96" s="8"/>
-      <c r="E96" s="8"/>
-      <c r="F96" s="8"/>
-      <c r="G96" s="8"/>
-      <c r="H96" s="8"/>
-      <c r="I96" s="8"/>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B96" s="2"/>
+      <c r="C96" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="E96" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="G96" s="2"/>
+      <c r="H96" s="2"/>
+      <c r="I96" s="2"/>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>124</v>
+        <v>95</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>156</v>
       </c>
       <c r="C97" s="2"/>
       <c r="D97" s="2"/>
-      <c r="F97" s="2"/>
+      <c r="E97" s="2"/>
       <c r="G97" s="2"/>
       <c r="H97" s="2"/>
       <c r="I97" s="2"/>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A98" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B98" s="2" t="s">
-        <v>158</v>
+      <c r="B98" s="2"/>
+      <c r="C98" s="2" t="s">
+        <v>281</v>
       </c>
       <c r="D98" s="2"/>
-      <c r="E98" s="2"/>
-      <c r="F98" s="2"/>
+      <c r="E98" s="2" t="s">
+        <v>282</v>
+      </c>
       <c r="G98" s="2"/>
       <c r="H98" s="2"/>
       <c r="I98" s="2"/>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C99" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="D99" s="2"/>
-      <c r="E99" s="2"/>
-      <c r="F99" s="2"/>
+      <c r="B99" s="2"/>
+      <c r="C99" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="E99" s="2" t="s">
+        <v>282</v>
+      </c>
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
       <c r="I99" s="2"/>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B100" s="2"/>
-      <c r="C100" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="D100" s="2"/>
-      <c r="E100" s="2"/>
-      <c r="F100" s="2"/>
-      <c r="G100" s="2"/>
-      <c r="H100" s="2"/>
-      <c r="I100" s="2"/>
-    </row>
-    <row r="101" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B101" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="C101" s="8"/>
-      <c r="D101" s="8"/>
-      <c r="E101" s="8"/>
-      <c r="F101" s="8"/>
-      <c r="G101" s="8"/>
-      <c r="H101" s="8"/>
-      <c r="I101" s="8"/>
+    <row r="100" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B100" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="C100" s="8"/>
+      <c r="D100" s="8"/>
+      <c r="E100" s="8"/>
+      <c r="F100" s="8"/>
+      <c r="G100" s="8"/>
+      <c r="H100" s="8"/>
+      <c r="I100" s="8"/>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A101" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C101" s="2"/>
+      <c r="D101" s="2"/>
+      <c r="F101" s="2"/>
+      <c r="G101" s="2"/>
+      <c r="H101" s="2"/>
+      <c r="I101" s="2"/>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
-        <v>88</v>
+        <v>144</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="C102" s="2"/>
+        <v>157</v>
+      </c>
       <c r="D102" s="2"/>
       <c r="E102" s="2"/>
       <c r="F102" s="2"/>
@@ -8481,8 +8623,7 @@
       <c r="I102" s="2"/>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B103" s="2"/>
-      <c r="C103" s="2" t="s">
+      <c r="C103" s="1" t="s">
         <v>190</v>
       </c>
       <c r="D103" s="2"/>
@@ -8492,95 +8633,101 @@
       <c r="H103" s="2"/>
       <c r="I103" s="2"/>
     </row>
-    <row r="104" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B104" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="C104" s="8"/>
-      <c r="D104" s="8"/>
-      <c r="E104" s="8"/>
-      <c r="F104" s="8"/>
-      <c r="G104" s="8"/>
-      <c r="H104" s="8"/>
-      <c r="I104" s="8"/>
-    </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A105" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B105" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="C105" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D105" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E105" s="1" t="s">
-        <v>477</v>
-      </c>
-      <c r="F105" s="2"/>
-      <c r="G105" s="2"/>
-      <c r="H105" s="2"/>
-      <c r="I105" s="2"/>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B104" s="2"/>
+      <c r="C104" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="D104" s="2"/>
+      <c r="E104" s="2"/>
+      <c r="F104" s="2"/>
+      <c r="G104" s="2"/>
+      <c r="H104" s="2"/>
+      <c r="I104" s="2"/>
+    </row>
+    <row r="105" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B105" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="C105" s="8"/>
+      <c r="D105" s="8"/>
+      <c r="E105" s="8"/>
+      <c r="F105" s="8"/>
+      <c r="G105" s="8"/>
+      <c r="H105" s="8"/>
+      <c r="I105" s="8"/>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B106" s="2"/>
-      <c r="C106" s="1" t="s">
-        <v>190</v>
-      </c>
+      <c r="A106" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C106" s="2"/>
+      <c r="D106" s="2"/>
       <c r="F106" s="2"/>
       <c r="G106" s="2"/>
       <c r="H106" s="2"/>
       <c r="I106" s="2"/>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B107" s="2"/>
-      <c r="C107" s="2" t="s">
-        <v>284</v>
+      <c r="A107" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>158</v>
       </c>
       <c r="D107" s="2"/>
+      <c r="E107" s="2"/>
       <c r="F107" s="2"/>
       <c r="G107" s="2"/>
       <c r="H107" s="2"/>
       <c r="I107" s="2"/>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B108" s="2"/>
-      <c r="D108" s="2" t="s">
-        <v>286</v>
-      </c>
+      <c r="C108" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D108" s="2"/>
+      <c r="E108" s="2"/>
+      <c r="F108" s="2"/>
       <c r="G108" s="2"/>
       <c r="H108" s="2"/>
       <c r="I108" s="2"/>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B109" s="2"/>
-      <c r="D109" s="2" t="s">
-        <v>287</v>
-      </c>
+      <c r="C109" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="D109" s="2"/>
+      <c r="E109" s="2"/>
+      <c r="F109" s="2"/>
       <c r="G109" s="2"/>
       <c r="H109" s="2"/>
       <c r="I109" s="2"/>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B110" s="2"/>
-      <c r="D110" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="G110" s="2"/>
-      <c r="H110" s="2"/>
-      <c r="I110" s="2"/>
+    <row r="110" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B110" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="C110" s="8"/>
+      <c r="D110" s="8"/>
+      <c r="E110" s="8"/>
+      <c r="F110" s="8"/>
+      <c r="G110" s="8"/>
+      <c r="H110" s="8"/>
+      <c r="I110" s="8"/>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B111" s="2"/>
-      <c r="C111" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="D111" s="2" t="s">
-        <v>286</v>
-      </c>
+      <c r="A111" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C111" s="2"/>
+      <c r="D111" s="2"/>
+      <c r="E111" s="2"/>
+      <c r="F111" s="2"/>
       <c r="G111" s="2"/>
       <c r="H111" s="2"/>
       <c r="I111" s="2"/>
@@ -8588,51 +8735,54 @@
     <row r="112" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B112" s="2"/>
       <c r="C112" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="D112" s="2" t="s">
-        <v>287</v>
-      </c>
+        <v>190</v>
+      </c>
+      <c r="D112" s="2"/>
+      <c r="E112" s="2"/>
+      <c r="F112" s="2"/>
       <c r="G112" s="2"/>
       <c r="H112" s="2"/>
       <c r="I112" s="2"/>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B113" s="2"/>
-      <c r="C113" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="D113" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="G113" s="2"/>
-      <c r="H113" s="2"/>
-      <c r="I113" s="2"/>
+    <row r="113" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B113" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="C113" s="8"/>
+      <c r="D113" s="8"/>
+      <c r="E113" s="8"/>
+      <c r="F113" s="8"/>
+      <c r="G113" s="8"/>
+      <c r="H113" s="8"/>
+      <c r="I113" s="8"/>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B114" s="2"/>
-      <c r="C114" s="2" t="s">
-        <v>475</v>
-      </c>
-      <c r="D114" s="2"/>
+      <c r="A114" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="E114" s="1" t="s">
-        <v>476</v>
-      </c>
+        <v>477</v>
+      </c>
+      <c r="F114" s="2"/>
       <c r="G114" s="2"/>
       <c r="H114" s="2"/>
       <c r="I114" s="2"/>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B115" s="2"/>
-      <c r="C115" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="D115" s="2" t="s">
-        <v>480</v>
-      </c>
-      <c r="E115" s="1" t="s">
-        <v>476</v>
-      </c>
+      <c r="C115" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="F115" s="2"/>
       <c r="G115" s="2"/>
       <c r="H115" s="2"/>
       <c r="I115" s="2"/>
@@ -8640,62 +8790,37 @@
     <row r="116" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B116" s="2"/>
       <c r="C116" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="D116" s="2" t="s">
-        <v>478</v>
-      </c>
-      <c r="E116" s="1" t="s">
-        <v>476</v>
-      </c>
+        <v>284</v>
+      </c>
+      <c r="D116" s="2"/>
+      <c r="F116" s="2"/>
       <c r="G116" s="2"/>
       <c r="H116" s="2"/>
       <c r="I116" s="2"/>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B117" s="2"/>
-      <c r="C117" s="2" t="s">
-        <v>285</v>
-      </c>
       <c r="D117" s="2" t="s">
-        <v>479</v>
-      </c>
-      <c r="E117" s="1" t="s">
-        <v>476</v>
+        <v>286</v>
       </c>
       <c r="G117" s="2"/>
       <c r="H117" s="2"/>
       <c r="I117" s="2"/>
     </row>
-    <row r="118" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B118" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="C118" s="8"/>
-      <c r="D118" s="8"/>
-      <c r="E118" s="8"/>
-      <c r="F118" s="8"/>
-      <c r="G118" s="8"/>
-      <c r="H118" s="8"/>
-      <c r="I118" s="8"/>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B118" s="2"/>
+      <c r="D118" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="G118" s="2"/>
+      <c r="H118" s="2"/>
+      <c r="I118" s="2"/>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A119" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="B119" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="C119" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D119" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="E119" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F119" s="2"/>
+      <c r="B119" s="2"/>
+      <c r="D119" s="2" t="s">
+        <v>288</v>
+      </c>
       <c r="G119" s="2"/>
       <c r="H119" s="2"/>
       <c r="I119" s="2"/>
@@ -8703,12 +8828,11 @@
     <row r="120" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B120" s="2"/>
       <c r="C120" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="E120" s="2" t="s">
-        <v>293</v>
-      </c>
-      <c r="F120" s="2"/>
+        <v>285</v>
+      </c>
+      <c r="D120" s="2" t="s">
+        <v>286</v>
+      </c>
       <c r="G120" s="2"/>
       <c r="H120" s="2"/>
       <c r="I120" s="2"/>
@@ -8716,12 +8840,11 @@
     <row r="121" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B121" s="2"/>
       <c r="C121" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="E121" s="2" t="s">
-        <v>293</v>
-      </c>
-      <c r="F121" s="2"/>
+        <v>285</v>
+      </c>
+      <c r="D121" s="2" t="s">
+        <v>287</v>
+      </c>
       <c r="G121" s="2"/>
       <c r="H121" s="2"/>
       <c r="I121" s="2"/>
@@ -8729,15 +8852,11 @@
     <row r="122" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B122" s="2"/>
       <c r="C122" s="2" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="E122" s="2" t="s">
-        <v>293</v>
-      </c>
-      <c r="F122" s="2"/>
+        <v>288</v>
+      </c>
       <c r="G122" s="2"/>
       <c r="H122" s="2"/>
       <c r="I122" s="2"/>
@@ -8745,98 +8864,90 @@
     <row r="123" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B123" s="2"/>
       <c r="C123" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="E123" s="2" t="s">
-        <v>293</v>
-      </c>
-      <c r="F123" s="2"/>
+        <v>475</v>
+      </c>
+      <c r="D123" s="2"/>
+      <c r="E123" s="1" t="s">
+        <v>476</v>
+      </c>
       <c r="G123" s="2"/>
       <c r="H123" s="2"/>
       <c r="I123" s="2"/>
     </row>
-    <row r="124" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B124" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="C124" s="8"/>
-      <c r="D124" s="8"/>
-      <c r="E124" s="8"/>
-      <c r="F124" s="8"/>
-      <c r="G124" s="8"/>
-      <c r="H124" s="8"/>
-      <c r="I124" s="8"/>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B124" s="2"/>
+      <c r="C124" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="D124" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="E124" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="G124" s="2"/>
+      <c r="H124" s="2"/>
+      <c r="I124" s="2"/>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A125" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B125" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="C125" s="2"/>
-      <c r="D125" s="2"/>
-      <c r="E125" s="2"/>
-      <c r="F125" s="2"/>
+      <c r="B125" s="2"/>
+      <c r="C125" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="D125" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="E125" s="1" t="s">
+        <v>476</v>
+      </c>
       <c r="G125" s="2"/>
       <c r="H125" s="2"/>
       <c r="I125" s="2"/>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A126" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B126" s="12" t="s">
-        <v>163</v>
-      </c>
-      <c r="C126" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D126" s="1" t="s">
-        <v>413</v>
+      <c r="B126" s="2"/>
+      <c r="C126" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="D126" s="2" t="s">
+        <v>479</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F126" s="1" t="s">
-        <v>194</v>
+        <v>476</v>
       </c>
       <c r="G126" s="2"/>
       <c r="H126" s="2"/>
       <c r="I126" s="2"/>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B127" s="2"/>
-      <c r="C127" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="D127" s="2" t="s">
-        <v>415</v>
-      </c>
-      <c r="E127" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="F127" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="G127" s="2"/>
-      <c r="H127" s="2"/>
-      <c r="I127" s="2"/>
+    <row r="127" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B127" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="C127" s="8"/>
+      <c r="D127" s="8"/>
+      <c r="E127" s="8"/>
+      <c r="F127" s="8"/>
+      <c r="G127" s="8"/>
+      <c r="H127" s="8"/>
+      <c r="I127" s="8"/>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B128" s="2"/>
-      <c r="C128" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="D128" s="2" t="s">
-        <v>414</v>
-      </c>
-      <c r="E128" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="F128" s="2" t="s">
-        <v>295</v>
-      </c>
+      <c r="A128" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D128" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="E128" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F128" s="2"/>
       <c r="G128" s="2"/>
       <c r="H128" s="2"/>
       <c r="I128" s="2"/>
@@ -8844,266 +8955,271 @@
     <row r="129" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B129" s="2"/>
       <c r="C129" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="D129" s="2" t="s">
-        <v>414</v>
+        <v>289</v>
       </c>
       <c r="E129" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="F129" s="2" t="s">
-        <v>295</v>
-      </c>
+        <v>293</v>
+      </c>
+      <c r="F129" s="2"/>
       <c r="G129" s="2"/>
       <c r="H129" s="2"/>
       <c r="I129" s="2"/>
     </row>
-    <row r="130" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B130" s="13" t="s">
-        <v>129</v>
-      </c>
-      <c r="C130" s="8"/>
-      <c r="D130" s="8"/>
-      <c r="E130" s="8"/>
-      <c r="F130" s="8"/>
-      <c r="G130" s="8"/>
-      <c r="H130" s="8"/>
-      <c r="I130" s="8"/>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B130" s="2"/>
+      <c r="C130" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="E130" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="F130" s="2"/>
+      <c r="G130" s="2"/>
+      <c r="H130" s="2"/>
+      <c r="I130" s="2"/>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A131" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B131" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="C131" s="2"/>
-      <c r="D131" s="2"/>
-      <c r="E131" s="2"/>
+      <c r="B131" s="2"/>
+      <c r="C131" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="D131" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="E131" s="2" t="s">
+        <v>293</v>
+      </c>
       <c r="F131" s="2"/>
       <c r="G131" s="2"/>
       <c r="H131" s="2"/>
       <c r="I131" s="2"/>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A132" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B132" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="C132" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D132" s="1" t="s">
-        <v>413</v>
-      </c>
-      <c r="E132" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F132" s="1" t="s">
-        <v>194</v>
-      </c>
+      <c r="B132" s="2"/>
+      <c r="C132" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="E132" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="F132" s="2"/>
       <c r="G132" s="2"/>
       <c r="H132" s="2"/>
       <c r="I132" s="2"/>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B133" s="2"/>
-      <c r="C133" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="D133" s="2" t="s">
-        <v>415</v>
-      </c>
-      <c r="E133" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="F133" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="G133" s="2"/>
-      <c r="H133" s="2"/>
-      <c r="I133" s="2"/>
+    <row r="133" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B133" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="C133" s="8"/>
+      <c r="D133" s="8"/>
+      <c r="E133" s="8"/>
+      <c r="F133" s="8"/>
+      <c r="G133" s="8"/>
+      <c r="H133" s="8"/>
+      <c r="I133" s="8"/>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B134" s="2"/>
-      <c r="C134" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="D134" s="2" t="s">
-        <v>414</v>
-      </c>
-      <c r="E134" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="F134" s="2" t="s">
-        <v>295</v>
-      </c>
+      <c r="A134" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B134" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C134" s="2"/>
+      <c r="D134" s="2"/>
+      <c r="E134" s="2"/>
+      <c r="F134" s="2"/>
       <c r="G134" s="2"/>
       <c r="H134" s="2"/>
       <c r="I134" s="2"/>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B135" s="2"/>
-      <c r="C135" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="D135" s="2" t="s">
-        <v>414</v>
-      </c>
-      <c r="E135" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="F135" s="2" t="s">
-        <v>295</v>
+      <c r="A135" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B135" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D135" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="E135" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F135" s="1" t="s">
+        <v>194</v>
       </c>
       <c r="G135" s="2"/>
       <c r="H135" s="2"/>
       <c r="I135" s="2"/>
     </row>
-    <row r="136" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B136" s="13" t="s">
-        <v>130</v>
-      </c>
-      <c r="C136" s="8"/>
-      <c r="D136" s="8"/>
-      <c r="E136" s="8"/>
-      <c r="F136" s="8"/>
-      <c r="G136" s="8"/>
-      <c r="H136" s="8"/>
-      <c r="I136" s="8"/>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B136" s="2"/>
+      <c r="C136" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D136" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="E136" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="F136" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="G136" s="2"/>
+      <c r="H136" s="2"/>
+      <c r="I136" s="2"/>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A137" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B137" s="2" t="s">
-        <v>166</v>
-      </c>
+      <c r="B137" s="2"/>
+      <c r="C137" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="D137" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="E137" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="F137" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="G137" s="2"/>
       <c r="H137" s="2"/>
       <c r="I137" s="2"/>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A138" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B138" s="12" t="s">
-        <v>167</v>
-      </c>
-      <c r="C138" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D138" s="1" t="s">
-        <v>413</v>
-      </c>
-      <c r="E138" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F138" s="1" t="s">
-        <v>194</v>
-      </c>
+      <c r="B138" s="2"/>
+      <c r="C138" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="D138" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="E138" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="F138" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="G138" s="2"/>
       <c r="H138" s="2"/>
       <c r="I138" s="2"/>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B139" s="2"/>
-      <c r="C139" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="D139" s="2" t="s">
-        <v>415</v>
-      </c>
-      <c r="E139" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="F139" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="G139" s="2"/>
-      <c r="H139" s="2"/>
-      <c r="I139" s="2"/>
+    <row r="139" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B139" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="C139" s="8"/>
+      <c r="D139" s="8"/>
+      <c r="E139" s="8"/>
+      <c r="F139" s="8"/>
+      <c r="G139" s="8"/>
+      <c r="H139" s="8"/>
+      <c r="I139" s="8"/>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B140" s="2"/>
-      <c r="C140" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="D140" s="2" t="s">
-        <v>414</v>
-      </c>
-      <c r="E140" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="F140" s="2" t="s">
-        <v>295</v>
-      </c>
+      <c r="A140" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B140" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C140" s="2"/>
+      <c r="D140" s="2"/>
+      <c r="E140" s="2"/>
+      <c r="F140" s="2"/>
       <c r="G140" s="2"/>
       <c r="H140" s="2"/>
       <c r="I140" s="2"/>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B141" s="2"/>
-      <c r="C141" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="D141" s="2" t="s">
-        <v>414</v>
-      </c>
-      <c r="E141" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="F141" s="2" t="s">
-        <v>295</v>
+      <c r="A141" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B141" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D141" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="E141" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F141" s="1" t="s">
+        <v>194</v>
       </c>
       <c r="G141" s="2"/>
       <c r="H141" s="2"/>
       <c r="I141" s="2"/>
     </row>
-    <row r="142" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B142" s="13" t="s">
-        <v>133</v>
-      </c>
-      <c r="C142" s="8"/>
-      <c r="D142" s="8"/>
-      <c r="E142" s="8"/>
-      <c r="F142" s="8"/>
-      <c r="G142" s="8"/>
-      <c r="H142" s="8"/>
-      <c r="I142" s="8"/>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B142" s="2"/>
+      <c r="C142" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D142" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="E142" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="F142" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="G142" s="2"/>
+      <c r="H142" s="2"/>
+      <c r="I142" s="2"/>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A143" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B143" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="C143" s="2"/>
-      <c r="D143" s="2"/>
-      <c r="E143" s="2"/>
-      <c r="F143" s="2"/>
+      <c r="B143" s="2"/>
+      <c r="C143" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="D143" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="E143" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="F143" s="2" t="s">
+        <v>295</v>
+      </c>
       <c r="G143" s="2"/>
       <c r="H143" s="2"/>
       <c r="I143" s="2"/>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B144" s="2"/>
-      <c r="C144" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="D144" s="2"/>
-      <c r="E144" s="2"/>
-      <c r="F144" s="2"/>
+      <c r="C144" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="D144" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="E144" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="F144" s="2" t="s">
+        <v>295</v>
+      </c>
       <c r="G144" s="2"/>
       <c r="H144" s="2"/>
       <c r="I144" s="2"/>
     </row>
     <row r="145" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B145" s="13" t="s">
-        <v>134</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="C145" s="8"/>
       <c r="D145" s="8"/>
       <c r="E145" s="8"/>
       <c r="F145" s="8"/>
@@ -9113,70 +9229,93 @@
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="D146" s="2"/>
-      <c r="E146" s="2"/>
-      <c r="F146" s="2"/>
-      <c r="G146" s="2"/>
+        <v>166</v>
+      </c>
       <c r="H146" s="2"/>
       <c r="I146" s="2"/>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B147" s="2"/>
+      <c r="A147" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B147" s="12" t="s">
+        <v>167</v>
+      </c>
       <c r="C147" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="D147" s="2"/>
-      <c r="E147" s="2"/>
-      <c r="F147" s="2"/>
-      <c r="G147" s="2"/>
+        <v>23</v>
+      </c>
+      <c r="D147" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="E147" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F147" s="1" t="s">
+        <v>194</v>
+      </c>
       <c r="H147" s="2"/>
       <c r="I147" s="2"/>
     </row>
-    <row r="148" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B148" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="D148" s="8"/>
-      <c r="E148" s="8"/>
-      <c r="F148" s="8"/>
-      <c r="G148" s="8"/>
-      <c r="H148" s="8"/>
-      <c r="I148" s="8"/>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B148" s="2"/>
+      <c r="C148" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D148" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="E148" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="F148" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="G148" s="2"/>
+      <c r="H148" s="2"/>
+      <c r="I148" s="2"/>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A149" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B149" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="D149" s="2"/>
-      <c r="E149" s="2"/>
-      <c r="F149" s="2"/>
+      <c r="B149" s="2"/>
+      <c r="C149" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="D149" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="E149" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="F149" s="2" t="s">
+        <v>295</v>
+      </c>
       <c r="G149" s="2"/>
       <c r="H149" s="2"/>
       <c r="I149" s="2"/>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B150" s="2"/>
-      <c r="C150" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="D150" s="2"/>
-      <c r="E150" s="2"/>
-      <c r="F150" s="2"/>
+      <c r="C150" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="D150" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="E150" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="F150" s="2" t="s">
+        <v>295</v>
+      </c>
       <c r="G150" s="2"/>
       <c r="H150" s="2"/>
       <c r="I150" s="2"/>
     </row>
     <row r="151" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B151" s="13" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C151" s="8"/>
       <c r="D151" s="8"/>
@@ -9188,9 +9327,11 @@
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="B152" s="2"/>
+        <v>4</v>
+      </c>
+      <c r="B152" s="2" t="s">
+        <v>168</v>
+      </c>
       <c r="C152" s="2"/>
       <c r="D152" s="2"/>
       <c r="E152" s="2"/>
@@ -9200,13 +9341,10 @@
       <c r="I152" s="2"/>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A153" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B153" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="C153" s="2"/>
+      <c r="B153" s="2"/>
+      <c r="C153" s="1" t="s">
+        <v>190</v>
+      </c>
       <c r="D153" s="2"/>
       <c r="E153" s="2"/>
       <c r="F153" s="2"/>
@@ -9214,29 +9352,24 @@
       <c r="H153" s="2"/>
       <c r="I153" s="2"/>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A154" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B154" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="C154" s="2"/>
-      <c r="D154" s="2"/>
-      <c r="E154" s="2"/>
-      <c r="F154" s="2"/>
-      <c r="G154" s="2"/>
-      <c r="H154" s="2"/>
-      <c r="I154" s="2"/>
+    <row r="154" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B154" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="D154" s="8"/>
+      <c r="E154" s="8"/>
+      <c r="F154" s="8"/>
+      <c r="G154" s="8"/>
+      <c r="H154" s="8"/>
+      <c r="I154" s="8"/>
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="C155" s="2"/>
+        <v>169</v>
+      </c>
       <c r="D155" s="2"/>
       <c r="E155" s="2"/>
       <c r="F155" s="2"/>
@@ -9245,13 +9378,10 @@
       <c r="I155" s="2"/>
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A156" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="B156" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="C156" s="2"/>
+      <c r="B156" s="2"/>
+      <c r="C156" s="1" t="s">
+        <v>190</v>
+      </c>
       <c r="D156" s="2"/>
       <c r="E156" s="2"/>
       <c r="F156" s="2"/>
@@ -9259,79 +9389,60 @@
       <c r="H156" s="2"/>
       <c r="I156" s="2"/>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A157" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B157" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="C157" s="2"/>
-      <c r="D157" s="2"/>
-      <c r="E157" s="2"/>
-      <c r="F157" s="2"/>
-      <c r="G157" s="2"/>
-      <c r="H157" s="2"/>
-      <c r="I157" s="2"/>
+    <row r="157" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B157" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="D157" s="8"/>
+      <c r="E157" s="8"/>
+      <c r="F157" s="8"/>
+      <c r="G157" s="8"/>
+      <c r="H157" s="8"/>
+      <c r="I157" s="8"/>
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="C158" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D158" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="E158" s="1" t="s">
-        <v>147</v>
-      </c>
+        <v>170</v>
+      </c>
+      <c r="D158" s="2"/>
+      <c r="E158" s="2"/>
+      <c r="F158" s="2"/>
       <c r="G158" s="2"/>
       <c r="H158" s="2"/>
       <c r="I158" s="2"/>
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A159" s="1" t="s">
-        <v>146</v>
-      </c>
       <c r="B159" s="2"/>
-      <c r="C159" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="D159" s="2" t="s">
-        <v>270</v>
-      </c>
-      <c r="E159" s="2" t="s">
-        <v>271</v>
-      </c>
+      <c r="C159" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D159" s="2"/>
+      <c r="E159" s="2"/>
       <c r="F159" s="2"/>
       <c r="G159" s="2"/>
       <c r="H159" s="2"/>
       <c r="I159" s="2"/>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A160" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="B160" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="C160" s="2"/>
-      <c r="D160" s="2"/>
-      <c r="E160" s="2"/>
-      <c r="F160" s="2"/>
-      <c r="G160" s="2"/>
-      <c r="H160" s="2"/>
-      <c r="I160" s="2"/>
+    <row r="160" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B160" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="C160" s="8"/>
+      <c r="D160" s="8"/>
+      <c r="E160" s="8"/>
+      <c r="F160" s="8"/>
+      <c r="G160" s="8"/>
+      <c r="H160" s="8"/>
+      <c r="I160" s="8"/>
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B161" s="2" t="s">
-        <v>178</v>
-      </c>
+      <c r="A161" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B161" s="2"/>
       <c r="C161" s="2"/>
       <c r="D161" s="2"/>
       <c r="E161" s="2"/>
@@ -9341,8 +9452,11 @@
       <c r="I161" s="2"/>
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A162" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="B162" s="2" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="C162" s="2"/>
       <c r="D162" s="2"/>
@@ -9353,8 +9467,11 @@
       <c r="I162" s="2"/>
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A163" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="B163" s="2" t="s">
-        <v>268</v>
+        <v>173</v>
       </c>
       <c r="C163" s="2"/>
       <c r="D163" s="2"/>
@@ -9365,8 +9482,11 @@
       <c r="I163" s="2"/>
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A164" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="B164" s="2" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="C164" s="2"/>
       <c r="D164" s="2"/>
@@ -9377,8 +9497,11 @@
       <c r="I164" s="2"/>
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A165" s="1" t="s">
+        <v>266</v>
+      </c>
       <c r="B165" s="2" t="s">
-        <v>181</v>
+        <v>267</v>
       </c>
       <c r="C165" s="2"/>
       <c r="D165" s="2"/>
@@ -9388,224 +9511,353 @@
       <c r="H165" s="2"/>
       <c r="I165" s="2"/>
     </row>
-    <row r="166" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B166" s="13" t="s">
-        <v>138</v>
-      </c>
-      <c r="C166" s="8"/>
-      <c r="D166" s="8"/>
-      <c r="E166" s="8"/>
-      <c r="F166" s="8"/>
-      <c r="G166" s="8"/>
-      <c r="H166" s="8"/>
-      <c r="I166" s="8"/>
+    <row r="166" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A166" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B166" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C166" s="2"/>
+      <c r="D166" s="2"/>
+      <c r="E166" s="2"/>
+      <c r="F166" s="2"/>
+      <c r="G166" s="2"/>
+      <c r="H166" s="2"/>
+      <c r="I166" s="2"/>
     </row>
     <row r="167" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
-        <v>137</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="B167" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C167" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D167" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E167" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="G167" s="2"/>
+      <c r="H167" s="2"/>
+      <c r="I167" s="2"/>
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B168" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="C168" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D168" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E168" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F168" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G168" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="H168" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>146</v>
+      </c>
+      <c r="B168" s="2"/>
+      <c r="C168" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="D168" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="E168" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="F168" s="2"/>
+      <c r="G168" s="2"/>
+      <c r="H168" s="2"/>
+      <c r="I168" s="2"/>
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C169" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="D169" s="2" t="s">
-        <v>359</v>
-      </c>
-      <c r="E169" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="F169" s="2" t="s">
-        <v>359</v>
-      </c>
-      <c r="G169" s="2" t="s">
-        <v>357</v>
-      </c>
-      <c r="H169" s="14" t="s">
-        <v>274</v>
-      </c>
+      <c r="A169" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B169" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C169" s="2"/>
+      <c r="D169" s="2"/>
+      <c r="E169" s="2"/>
+      <c r="F169" s="2"/>
+      <c r="G169" s="2"/>
+      <c r="H169" s="2"/>
+      <c r="I169" s="2"/>
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C170" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="D170" s="2" t="s">
-        <v>359</v>
-      </c>
+      <c r="B170" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C170" s="2"/>
+      <c r="D170" s="2"/>
       <c r="E170" s="2"/>
       <c r="F170" s="2"/>
-      <c r="G170" s="2" t="s">
-        <v>357</v>
-      </c>
-      <c r="H170" s="14" t="s">
-        <v>274</v>
-      </c>
+      <c r="G170" s="2"/>
+      <c r="H170" s="2"/>
+      <c r="I170" s="2"/>
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B171" s="2" t="s">
+        <v>179</v>
+      </c>
       <c r="C171" s="2"/>
       <c r="D171" s="2"/>
-      <c r="E171" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="F171" s="2" t="s">
-        <v>359</v>
-      </c>
-      <c r="G171" s="2" t="s">
-        <v>357</v>
-      </c>
-      <c r="H171" s="14" t="s">
-        <v>274</v>
-      </c>
+      <c r="E171" s="2"/>
+      <c r="F171" s="2"/>
+      <c r="G171" s="2"/>
+      <c r="H171" s="2"/>
+      <c r="I171" s="2"/>
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B172" s="2" t="s">
+        <v>268</v>
+      </c>
       <c r="C172" s="2"/>
       <c r="D172" s="2"/>
       <c r="E172" s="2"/>
       <c r="F172" s="2"/>
-      <c r="G172" s="2" t="s">
-        <v>357</v>
-      </c>
-      <c r="H172" s="14" t="s">
-        <v>274</v>
-      </c>
+      <c r="G172" s="2"/>
+      <c r="H172" s="2"/>
+      <c r="I172" s="2"/>
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C173" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="D173" s="2" t="s">
-        <v>359</v>
-      </c>
+      <c r="B173" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C173" s="2"/>
+      <c r="D173" s="2"/>
       <c r="E173" s="2"/>
       <c r="F173" s="2"/>
       <c r="G173" s="2"/>
-      <c r="H173" s="14" t="s">
-        <v>274</v>
-      </c>
+      <c r="H173" s="2"/>
+      <c r="I173" s="2"/>
     </row>
     <row r="174" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B174" s="2" t="s">
+        <v>181</v>
+      </c>
       <c r="C174" s="2"/>
       <c r="D174" s="2"/>
-      <c r="E174" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="F174" s="2" t="s">
-        <v>359</v>
-      </c>
+      <c r="E174" s="2"/>
+      <c r="F174" s="2"/>
       <c r="G174" s="2"/>
-      <c r="H174" s="14" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C175" s="2"/>
-      <c r="D175" s="2"/>
-      <c r="E175" s="2"/>
-      <c r="F175" s="2"/>
-      <c r="G175" s="2"/>
-      <c r="H175" s="14" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="176" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B176" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="C176" s="8"/>
-      <c r="D176" s="8"/>
-      <c r="E176" s="8"/>
-      <c r="F176" s="8"/>
-      <c r="G176" s="8"/>
-      <c r="H176" s="8"/>
-      <c r="I176" s="8"/>
+      <c r="H174" s="2"/>
+      <c r="I174" s="2"/>
+    </row>
+    <row r="175" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B175" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="C175" s="8"/>
+      <c r="D175" s="8"/>
+      <c r="E175" s="8"/>
+      <c r="F175" s="8"/>
+      <c r="G175" s="8"/>
+      <c r="H175" s="8"/>
+      <c r="I175" s="8"/>
+    </row>
+    <row r="176" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A176" s="1" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A177" s="1" t="s">
-        <v>137</v>
+        <v>13</v>
+      </c>
+      <c r="B177" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C177" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D177" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E177" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F177" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G177" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="H177" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="178" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A178" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B178" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="C178" s="1" t="s">
-        <v>21</v>
+      <c r="C178" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="D178" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="E178" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="F178" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="G178" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="H178" s="14" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="179" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C179" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="D179" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="E179" s="2"/>
+      <c r="F179" s="2"/>
+      <c r="G179" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="H179" s="14" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="180" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C180" s="2"/>
+      <c r="D180" s="2"/>
+      <c r="E180" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="F180" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="G180" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="H180" s="14" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="181" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C181" s="2"/>
+      <c r="D181" s="2"/>
+      <c r="E181" s="2"/>
+      <c r="F181" s="2"/>
+      <c r="G181" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="H181" s="14" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="182" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C182" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="D182" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="E182" s="2"/>
+      <c r="F182" s="2"/>
+      <c r="G182" s="2"/>
+      <c r="H182" s="14" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="183" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C183" s="2"/>
+      <c r="D183" s="2"/>
+      <c r="E183" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="F183" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="G183" s="2"/>
+      <c r="H183" s="14" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="184" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C184" s="2"/>
+      <c r="D184" s="2"/>
+      <c r="E184" s="2"/>
+      <c r="F184" s="2"/>
+      <c r="G184" s="2"/>
+      <c r="H184" s="14" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="185" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B185" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="C185" s="8"/>
+      <c r="D185" s="8"/>
+      <c r="E185" s="8"/>
+      <c r="F185" s="8"/>
+      <c r="G185" s="8"/>
+      <c r="H185" s="8"/>
+      <c r="I185" s="8"/>
+    </row>
+    <row r="186" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A186" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="187" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A187" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B187" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="C187" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="188" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C188" s="2" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C180" s="1" t="s">
+    <row r="189" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C189" s="1" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="181" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B181" s="13" t="s">
+    <row r="190" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B190" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="C181" s="8"/>
-      <c r="D181" s="8"/>
-      <c r="E181" s="8"/>
-      <c r="F181" s="8"/>
-      <c r="G181" s="8"/>
-      <c r="H181" s="8"/>
-      <c r="I181" s="8"/>
-    </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A182" s="1" t="s">
+      <c r="C190" s="8"/>
+      <c r="D190" s="8"/>
+      <c r="E190" s="8"/>
+      <c r="F190" s="8"/>
+      <c r="G190" s="8"/>
+      <c r="H190" s="8"/>
+      <c r="I190" s="8"/>
+    </row>
+    <row r="191" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A191" s="1" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A183" s="1" t="s">
+    <row r="192" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A192" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B183" s="2" t="s">
+      <c r="B192" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="C183" s="1" t="s">
+      <c r="C192" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C184" s="2" t="s">
+    <row r="193" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C193" s="2" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C185" s="1" t="s">
+    <row r="194" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C194" s="1" t="s">
         <v>190</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix a problem in parser NXTH(L) instruction
</commit_message>
<xml_diff>
--- a/P4E_psuedo_instruction_set.xlsx
+++ b/P4E_psuedo_instruction_set.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\P4EngineAssembler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E582B471-EAB5-4F77-B6C9-93011466651F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49368393-F412-4A9B-95CE-B73D594322BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-3645" windowWidth="38640" windowHeight="21840" xr2:uid="{87164962-7B7D-4BAA-98E0-B9A8D7C47112}"/>
   </bookViews>
@@ -632,7 +632,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D179" authorId="0" shapeId="0" xr:uid="{5EDDCAB0-8CF8-4E69-91EC-FCEBB8FBFB81}">
+    <comment ref="D179" authorId="0" shapeId="0" xr:uid="{AD2C89F3-2621-4DC3-B2F0-4EEE583A6F75}">
       <text>
         <r>
           <rPr>
@@ -684,7 +684,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D182" authorId="0" shapeId="0" xr:uid="{C0E77B6C-0F0F-459E-A010-D438E2938743}">
+    <comment ref="D182" authorId="0" shapeId="0" xr:uid="{50FC7ECC-28FD-4D49-9E10-DC3BCC6B4269}">
       <text>
         <r>
           <rPr>
@@ -2990,40 +2990,6 @@
         <family val="2"/>
         <charset val="134"/>
       </rPr>
-      <t xml:space="preserve">ISR { </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Microsoft YaHei Light"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>off6</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Microsoft YaHei Light"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve"> :</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Microsoft YaHei Light"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
       <t xml:space="preserve">META { </t>
     </r>
     <r>
@@ -6299,6 +6265,40 @@
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve"> ] ,</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">ISR { </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>off5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei Light"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> :</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -6809,8 +6809,8 @@
   <dimension ref="A1:I194"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D91" sqref="D91"/>
+      <pane ySplit="1" topLeftCell="A158" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D178" sqref="D178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.2"/>
@@ -6857,7 +6857,7 @@
         <v>149</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>25</v>
@@ -6875,16 +6875,16 @@
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>187</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
@@ -6893,16 +6893,16 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>241</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
@@ -6911,10 +6911,10 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -6940,7 +6940,7 @@
         <v>150</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>26</v>
@@ -6967,25 +6967,25 @@
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>187</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -6994,43 +6994,43 @@
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>241</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B11" s="2"/>
       <c r="C11" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
@@ -7038,67 +7038,67 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B12" s="2"/>
       <c r="C12" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D12" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>298</v>
-      </c>
       <c r="F12" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>187</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B13" s="2"/>
       <c r="C13" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D13" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="E13" s="2" t="s">
-        <v>298</v>
-      </c>
       <c r="F13" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>241</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B14" s="2"/>
       <c r="C14" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D14" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>298</v>
-      </c>
       <c r="F14" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
@@ -7145,60 +7145,60 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B17" s="2"/>
       <c r="C17" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>187</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="I17" s="2"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B18" s="2"/>
       <c r="C18" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>241</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="I18" s="2"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B19" s="2"/>
       <c r="C19" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
@@ -7207,60 +7207,60 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B20" s="2"/>
       <c r="C20" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>298</v>
-      </c>
       <c r="E20" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>187</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="I20" s="2"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B21" s="2"/>
       <c r="C21" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>298</v>
-      </c>
       <c r="E21" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>241</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="I21" s="2"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B22" s="2"/>
       <c r="C22" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>298</v>
-      </c>
       <c r="E22" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
@@ -7278,25 +7278,25 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="I24" s="2"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
@@ -7357,60 +7357,60 @@
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>187</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="I29" s="2"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B30" s="2"/>
       <c r="C30" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>241</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="I30" s="2"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B31" s="2"/>
       <c r="C31" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
@@ -7419,60 +7419,60 @@
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B32" s="2"/>
       <c r="C32" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="D32" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="D32" s="2" t="s">
-        <v>298</v>
-      </c>
       <c r="E32" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>187</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="I32" s="2"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B33" s="2"/>
       <c r="C33" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="D33" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="D33" s="2" t="s">
-        <v>298</v>
-      </c>
       <c r="E33" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>241</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="I33" s="2"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B34" s="2"/>
       <c r="C34" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="D34" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="D34" s="2" t="s">
-        <v>298</v>
-      </c>
       <c r="E34" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
@@ -7490,25 +7490,25 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="I36" s="2"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
@@ -7579,260 +7579,260 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C42" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="G42" s="2" t="s">
         <v>187</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C43" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="G43" s="2" t="s">
         <v>241</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C44" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C45" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="D45" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="D45" s="2" t="s">
-        <v>298</v>
-      </c>
       <c r="E45" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="G45" s="2" t="s">
         <v>187</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C46" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="D46" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="D46" s="2" t="s">
-        <v>298</v>
-      </c>
       <c r="E46" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="G46" s="2" t="s">
         <v>241</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C47" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="D47" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="D47" s="2" t="s">
-        <v>298</v>
-      </c>
       <c r="E47" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="H47" s="2"/>
       <c r="I47" s="2"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C48" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E48" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="F48" s="2" t="s">
         <v>279</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>280</v>
       </c>
       <c r="G48" s="2" t="s">
         <v>187</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C49" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E49" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="F49" s="2" t="s">
         <v>279</v>
-      </c>
-      <c r="F49" s="2" t="s">
-        <v>280</v>
       </c>
       <c r="G49" s="2" t="s">
         <v>241</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C50" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E50" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="F50" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="F50" s="2" t="s">
-        <v>280</v>
-      </c>
       <c r="G50" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="H50" s="2"/>
       <c r="I50" s="2"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C51" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="D51" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="D51" s="2" t="s">
-        <v>298</v>
-      </c>
       <c r="E51" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="F51" s="2" t="s">
         <v>279</v>
-      </c>
-      <c r="F51" s="2" t="s">
-        <v>280</v>
       </c>
       <c r="G51" s="2" t="s">
         <v>187</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C52" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="D52" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="D52" s="2" t="s">
-        <v>298</v>
-      </c>
       <c r="E52" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="F52" s="2" t="s">
         <v>279</v>
-      </c>
-      <c r="F52" s="2" t="s">
-        <v>280</v>
       </c>
       <c r="G52" s="2" t="s">
         <v>241</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C53" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="D53" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="D53" s="2" t="s">
-        <v>298</v>
-      </c>
       <c r="E53" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="F53" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="F53" s="2" t="s">
-        <v>280</v>
-      </c>
       <c r="G53" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="H53" s="2"/>
       <c r="I53" s="2"/>
@@ -7851,10 +7851,10 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>23</v>
@@ -7878,16 +7878,16 @@
       </c>
       <c r="B56" s="2"/>
       <c r="C56" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>187</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
@@ -7896,16 +7896,16 @@
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B57" s="2"/>
       <c r="C57" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>241</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
@@ -7914,10 +7914,10 @@
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B58" s="2"/>
       <c r="C58" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E58" s="2"/>
       <c r="F58" s="2"/>
@@ -7928,16 +7928,16 @@
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B59" s="2"/>
       <c r="C59" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>187</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
@@ -7946,16 +7946,16 @@
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B60" s="2"/>
       <c r="C60" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>241</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
@@ -7964,10 +7964,10 @@
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B61" s="2"/>
       <c r="C61" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E61" s="2"/>
       <c r="F61" s="2"/>
@@ -7978,16 +7978,16 @@
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B62" s="2"/>
       <c r="C62" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>187</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
@@ -7996,16 +7996,16 @@
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B63" s="2"/>
       <c r="C63" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>241</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
@@ -8014,10 +8014,10 @@
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B64" s="2"/>
       <c r="C64" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E64" s="2"/>
       <c r="F64" s="2"/>
@@ -8028,16 +8028,16 @@
     <row r="65" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B65" s="2"/>
       <c r="C65" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>187</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
@@ -8046,16 +8046,16 @@
     <row r="66" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B66" s="2"/>
       <c r="C66" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>241</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
@@ -8064,10 +8064,10 @@
     <row r="67" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B67" s="2"/>
       <c r="C67" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E67" s="2"/>
       <c r="F67" s="2"/>
@@ -8078,16 +8078,16 @@
     <row r="68" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B68" s="2"/>
       <c r="C68" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>187</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
@@ -8096,16 +8096,16 @@
     <row r="69" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B69" s="2"/>
       <c r="C69" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>241</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
@@ -8114,10 +8114,10 @@
     <row r="70" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B70" s="2"/>
       <c r="C70" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E70" s="2"/>
       <c r="F70" s="2"/>
@@ -8128,16 +8128,16 @@
     <row r="71" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B71" s="2"/>
       <c r="C71" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>187</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
@@ -8146,16 +8146,16 @@
     <row r="72" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B72" s="2"/>
       <c r="C72" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>241</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
@@ -8164,10 +8164,10 @@
     <row r="73" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B73" s="2"/>
       <c r="C73" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E73" s="2"/>
       <c r="F73" s="2"/>
@@ -8178,16 +8178,16 @@
     <row r="74" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B74" s="2"/>
       <c r="C74" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>187</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
@@ -8196,16 +8196,16 @@
     <row r="75" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B75" s="2"/>
       <c r="C75" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>241</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
@@ -8214,10 +8214,10 @@
     <row r="76" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B76" s="2"/>
       <c r="C76" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E76" s="2"/>
       <c r="F76" s="2"/>
@@ -8228,16 +8228,16 @@
     <row r="77" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B77" s="2"/>
       <c r="C77" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>187</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
@@ -8246,16 +8246,16 @@
     <row r="78" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B78" s="2"/>
       <c r="C78" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D78" s="2" t="s">
         <v>241</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
@@ -8264,10 +8264,10 @@
     <row r="79" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B79" s="2"/>
       <c r="C79" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E79" s="2"/>
       <c r="F79" s="2"/>
@@ -8278,16 +8278,16 @@
     <row r="80" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B80" s="2"/>
       <c r="C80" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D80" s="2" t="s">
         <v>187</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
@@ -8296,16 +8296,16 @@
     <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B81" s="2"/>
       <c r="C81" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>241</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
@@ -8314,10 +8314,10 @@
     <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B82" s="2"/>
       <c r="C82" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E82" s="2"/>
       <c r="F82" s="2"/>
@@ -8328,16 +8328,16 @@
     <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B83" s="2"/>
       <c r="C83" s="2" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="D83" s="2" t="s">
         <v>187</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
@@ -8346,16 +8346,16 @@
     <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B84" s="2"/>
       <c r="C84" s="2" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="D84" s="2" t="s">
         <v>241</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
@@ -8364,10 +8364,10 @@
     <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B85" s="2"/>
       <c r="C85" s="2" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E85" s="2"/>
       <c r="F85" s="2"/>
@@ -8378,16 +8378,16 @@
     <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B86" s="2"/>
       <c r="C86" s="2" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="D86" s="2" t="s">
         <v>187</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
@@ -8396,16 +8396,16 @@
     <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B87" s="2"/>
       <c r="C87" s="2" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="D87" s="2" t="s">
         <v>241</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
@@ -8414,10 +8414,10 @@
     <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B88" s="2"/>
       <c r="C88" s="2" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E88" s="2"/>
       <c r="F88" s="2"/>
@@ -8428,16 +8428,16 @@
     <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B89" s="2"/>
       <c r="C89" s="2" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="D89" s="2" t="s">
         <v>187</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G89" s="2"/>
       <c r="H89" s="2"/>
@@ -8446,16 +8446,16 @@
     <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B90" s="2"/>
       <c r="C90" s="2" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="D90" s="2" t="s">
         <v>241</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G90" s="2"/>
       <c r="H90" s="2"/>
@@ -8464,10 +8464,10 @@
     <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B91" s="2"/>
       <c r="C91" s="2" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E91" s="2"/>
       <c r="F91" s="2"/>
@@ -8518,11 +8518,11 @@
     <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B95" s="2"/>
       <c r="C95" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D95" s="2"/>
       <c r="E95" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G95" s="2"/>
       <c r="H95" s="2"/>
@@ -8531,13 +8531,13 @@
     <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B96" s="2"/>
       <c r="C96" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="E96" s="2" t="s">
         <v>281</v>
-      </c>
-      <c r="D96" s="2" t="s">
-        <v>466</v>
-      </c>
-      <c r="E96" s="2" t="s">
-        <v>282</v>
       </c>
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
@@ -8560,11 +8560,11 @@
     <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B98" s="2"/>
       <c r="C98" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D98" s="2"/>
       <c r="E98" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G98" s="2"/>
       <c r="H98" s="2"/>
@@ -8573,13 +8573,13 @@
     <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B99" s="2"/>
       <c r="C99" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="E99" s="2" t="s">
         <v>281</v>
-      </c>
-      <c r="D99" s="2" t="s">
-        <v>466</v>
-      </c>
-      <c r="E99" s="2" t="s">
-        <v>282</v>
       </c>
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
@@ -8636,7 +8636,7 @@
     <row r="104" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B104" s="2"/>
       <c r="C104" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D104" s="2"/>
       <c r="E104" s="2"/>
@@ -8696,7 +8696,7 @@
     <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B109" s="2"/>
       <c r="C109" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D109" s="2"/>
       <c r="E109" s="2"/>
@@ -8770,7 +8770,7 @@
         <v>34</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="F114" s="2"/>
       <c r="G114" s="2"/>
@@ -8790,7 +8790,7 @@
     <row r="116" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B116" s="2"/>
       <c r="C116" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D116" s="2"/>
       <c r="F116" s="2"/>
@@ -8801,7 +8801,7 @@
     <row r="117" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B117" s="2"/>
       <c r="D117" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="G117" s="2"/>
       <c r="H117" s="2"/>
@@ -8810,7 +8810,7 @@
     <row r="118" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B118" s="2"/>
       <c r="D118" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G118" s="2"/>
       <c r="H118" s="2"/>
@@ -8819,7 +8819,7 @@
     <row r="119" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B119" s="2"/>
       <c r="D119" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G119" s="2"/>
       <c r="H119" s="2"/>
@@ -8828,10 +8828,10 @@
     <row r="120" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B120" s="2"/>
       <c r="C120" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="D120" s="2" t="s">
         <v>285</v>
-      </c>
-      <c r="D120" s="2" t="s">
-        <v>286</v>
       </c>
       <c r="G120" s="2"/>
       <c r="H120" s="2"/>
@@ -8840,10 +8840,10 @@
     <row r="121" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B121" s="2"/>
       <c r="C121" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G121" s="2"/>
       <c r="H121" s="2"/>
@@ -8852,10 +8852,10 @@
     <row r="122" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B122" s="2"/>
       <c r="C122" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G122" s="2"/>
       <c r="H122" s="2"/>
@@ -8864,11 +8864,11 @@
     <row r="123" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B123" s="2"/>
       <c r="C123" s="2" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D123" s="2"/>
       <c r="E123" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="G123" s="2"/>
       <c r="H123" s="2"/>
@@ -8877,13 +8877,13 @@
     <row r="124" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B124" s="2"/>
       <c r="C124" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="G124" s="2"/>
       <c r="H124" s="2"/>
@@ -8892,13 +8892,13 @@
     <row r="125" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B125" s="2"/>
       <c r="C125" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="G125" s="2"/>
       <c r="H125" s="2"/>
@@ -8907,13 +8907,13 @@
     <row r="126" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B126" s="2"/>
       <c r="C126" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="G126" s="2"/>
       <c r="H126" s="2"/>
@@ -8955,10 +8955,10 @@
     <row r="129" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B129" s="2"/>
       <c r="C129" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E129" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F129" s="2"/>
       <c r="G129" s="2"/>
@@ -8968,10 +8968,10 @@
     <row r="130" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B130" s="2"/>
       <c r="C130" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E130" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F130" s="2"/>
       <c r="G130" s="2"/>
@@ -8981,13 +8981,13 @@
     <row r="131" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B131" s="2"/>
       <c r="C131" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D131" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E131" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F131" s="2"/>
       <c r="G131" s="2"/>
@@ -8997,10 +8997,10 @@
     <row r="132" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B132" s="2"/>
       <c r="C132" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="E132" s="2" t="s">
         <v>292</v>
-      </c>
-      <c r="E132" s="2" t="s">
-        <v>293</v>
       </c>
       <c r="F132" s="2"/>
       <c r="G132" s="2"/>
@@ -9045,7 +9045,7 @@
         <v>23</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E135" s="1" t="s">
         <v>24</v>
@@ -9063,10 +9063,10 @@
         <v>187</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E136" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F136" s="2" t="s">
         <v>193</v>
@@ -9078,16 +9078,16 @@
     <row r="137" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B137" s="2"/>
       <c r="C137" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E137" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="F137" s="2" t="s">
         <v>294</v>
-      </c>
-      <c r="F137" s="2" t="s">
-        <v>295</v>
       </c>
       <c r="G137" s="2"/>
       <c r="H137" s="2"/>
@@ -9096,16 +9096,16 @@
     <row r="138" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B138" s="2"/>
       <c r="C138" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E138" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="F138" s="2" t="s">
         <v>294</v>
-      </c>
-      <c r="F138" s="2" t="s">
-        <v>295</v>
       </c>
       <c r="G138" s="2"/>
       <c r="H138" s="2"/>
@@ -9149,7 +9149,7 @@
         <v>23</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E141" s="1" t="s">
         <v>24</v>
@@ -9167,10 +9167,10 @@
         <v>187</v>
       </c>
       <c r="D142" s="2" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E142" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F142" s="2" t="s">
         <v>193</v>
@@ -9182,16 +9182,16 @@
     <row r="143" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B143" s="2"/>
       <c r="C143" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D143" s="2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E143" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="F143" s="2" t="s">
         <v>294</v>
-      </c>
-      <c r="F143" s="2" t="s">
-        <v>295</v>
       </c>
       <c r="G143" s="2"/>
       <c r="H143" s="2"/>
@@ -9200,16 +9200,16 @@
     <row r="144" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B144" s="2"/>
       <c r="C144" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D144" s="2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E144" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="F144" s="2" t="s">
         <v>294</v>
-      </c>
-      <c r="F144" s="2" t="s">
-        <v>295</v>
       </c>
       <c r="G144" s="2"/>
       <c r="H144" s="2"/>
@@ -9248,7 +9248,7 @@
         <v>23</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E147" s="1" t="s">
         <v>24</v>
@@ -9265,10 +9265,10 @@
         <v>187</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E148" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F148" s="2" t="s">
         <v>193</v>
@@ -9280,16 +9280,16 @@
     <row r="149" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B149" s="2"/>
       <c r="C149" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D149" s="2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E149" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="F149" s="2" t="s">
         <v>294</v>
-      </c>
-      <c r="F149" s="2" t="s">
-        <v>295</v>
       </c>
       <c r="G149" s="2"/>
       <c r="H149" s="2"/>
@@ -9298,16 +9298,16 @@
     <row r="150" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B150" s="2"/>
       <c r="C150" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D150" s="2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E150" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="F150" s="2" t="s">
         <v>294</v>
-      </c>
-      <c r="F150" s="2" t="s">
-        <v>295</v>
       </c>
       <c r="G150" s="2"/>
       <c r="H150" s="2"/>
@@ -9685,54 +9685,54 @@
     </row>
     <row r="178" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C178" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="D178" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="E178" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="D178" s="2" t="s">
-        <v>359</v>
-      </c>
-      <c r="E178" s="2" t="s">
+      <c r="F178" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="G178" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="H178" s="14" t="s">
         <v>273</v>
-      </c>
-      <c r="F178" s="2" t="s">
-        <v>359</v>
-      </c>
-      <c r="G178" s="2" t="s">
-        <v>357</v>
-      </c>
-      <c r="H178" s="14" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="179" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C179" s="2" t="s">
-        <v>272</v>
+        <v>492</v>
       </c>
       <c r="D179" s="2" t="s">
-        <v>359</v>
+        <v>293</v>
       </c>
       <c r="E179" s="2"/>
       <c r="F179" s="2"/>
       <c r="G179" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="H179" s="14" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="180" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C180" s="2"/>
       <c r="D180" s="2"/>
       <c r="E180" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F180" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="G180" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="H180" s="14" t="s">
         <v>273</v>
-      </c>
-      <c r="F180" s="2" t="s">
-        <v>359</v>
-      </c>
-      <c r="G180" s="2" t="s">
-        <v>357</v>
-      </c>
-      <c r="H180" s="14" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="181" spans="1:9" x14ac:dyDescent="0.2">
@@ -9741,38 +9741,38 @@
       <c r="E181" s="2"/>
       <c r="F181" s="2"/>
       <c r="G181" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="H181" s="14" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="182" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C182" s="2" t="s">
-        <v>272</v>
+        <v>492</v>
       </c>
       <c r="D182" s="2" t="s">
-        <v>359</v>
+        <v>293</v>
       </c>
       <c r="E182" s="2"/>
       <c r="F182" s="2"/>
       <c r="G182" s="2"/>
       <c r="H182" s="14" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="183" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C183" s="2"/>
       <c r="D183" s="2"/>
       <c r="E183" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F183" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="G183" s="2"/>
       <c r="H183" s="14" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="184" spans="1:9" x14ac:dyDescent="0.2">
@@ -9782,7 +9782,7 @@
       <c r="F184" s="2"/>
       <c r="G184" s="2"/>
       <c r="H184" s="14" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="185" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -9815,7 +9815,7 @@
     </row>
     <row r="188" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C188" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="189" spans="1:9" x14ac:dyDescent="0.2">
@@ -9853,7 +9853,7 @@
     </row>
     <row r="193" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C193" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="194" spans="3:3" x14ac:dyDescent="0.2">
@@ -9911,27 +9911,27 @@
     </row>
     <row r="2" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B2" s="15" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -9939,19 +9939,19 @@
     </row>
     <row r="4" spans="1:9" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>187</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
@@ -9959,55 +9959,55 @@
     <row r="5" spans="1:9" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="C5" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>241</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>187</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>241</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="8" spans="1:9" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.2">
       <c r="B8" s="15" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
@@ -10016,191 +10016,191 @@
     </row>
     <row r="9" spans="1:9" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D9" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>187</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="16.5" x14ac:dyDescent="0.2">
       <c r="C11" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>241</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C12" s="4" t="s">
+        <v>456</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>457</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>458</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>187</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C13" s="4" t="s">
+        <v>456</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>457</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>458</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>241</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B14" s="15" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>225</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>420</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>421</v>
-      </c>
       <c r="E15" s="1" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="F15" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>418</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>419</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>187</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>187</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>241</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>241</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>187</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>241</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="16.5" x14ac:dyDescent="0.2">
@@ -10208,16 +10208,16 @@
         <v>241</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>187</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="16.5" x14ac:dyDescent="0.2">
@@ -10240,37 +10240,37 @@
         <v>187</v>
       </c>
       <c r="D21" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>471</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>472</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>187</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="22" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B22" s="15" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>377</v>
+      </c>
+      <c r="B23" s="4" t="s">
         <v>378</v>
       </c>
-      <c r="B23" s="4" t="s">
-        <v>379</v>
-      </c>
       <c r="C23" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="16.5" x14ac:dyDescent="0.2">
       <c r="C24" s="1" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="16.5" x14ac:dyDescent="0.2">
@@ -10280,23 +10280,23 @@
     </row>
     <row r="26" spans="1:7" ht="16.5" x14ac:dyDescent="0.2">
       <c r="C26" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="27" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B27" s="15" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>380</v>
+      </c>
+      <c r="B28" s="4" t="s">
         <v>381</v>
       </c>
-      <c r="B28" s="4" t="s">
-        <v>382</v>
-      </c>
       <c r="C28" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D28" t="s">
         <v>65</v>
@@ -10305,41 +10305,41 @@
     <row r="29" spans="1:7" ht="16.5" x14ac:dyDescent="0.2">
       <c r="B29" s="4"/>
       <c r="C29" s="1" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="D29" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="16.5" x14ac:dyDescent="0.2">
       <c r="B30" s="4"/>
       <c r="C30" s="1"/>
       <c r="D30" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="16.5" x14ac:dyDescent="0.2">
       <c r="C31" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D31" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="32" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B32" s="15" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>385</v>
+      </c>
+      <c r="B33" s="4" t="s">
         <v>386</v>
       </c>
-      <c r="B33" s="4" t="s">
-        <v>387</v>
-      </c>
       <c r="C33" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
@@ -10351,23 +10351,23 @@
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B35" s="4"/>
       <c r="C35" s="5" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B36" s="4"/>
       <c r="C36" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B37" s="15" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B38" s="4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C38" t="s">
         <v>190</v>
@@ -10375,60 +10375,60 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C39" s="5" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C40" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="41" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="42" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B42" s="15" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B43" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B44" s="4"/>
       <c r="C44" s="5" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D44" s="5"/>
       <c r="E44" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C45" s="5" t="s">
+        <v>462</v>
+      </c>
+      <c r="D45" s="5" t="s">
         <v>463</v>
       </c>
-      <c r="D45" s="5" t="s">
-        <v>464</v>
-      </c>
       <c r="E45" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C46" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E46" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="47" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B47" s="15" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
@@ -10438,12 +10438,12 @@
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B49" s="4" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B50" s="4" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="51" spans="2:7" x14ac:dyDescent="0.2">
@@ -10468,85 +10468,85 @@
     </row>
     <row r="55" spans="2:7" ht="16.5" x14ac:dyDescent="0.2">
       <c r="C55" s="1" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="E55" s="5"/>
       <c r="F55" s="4" t="s">
         <v>187</v>
       </c>
       <c r="G55" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="56" spans="2:7" ht="16.5" x14ac:dyDescent="0.2">
       <c r="C56" s="1" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="E56" s="5"/>
       <c r="F56" s="4" t="s">
         <v>241</v>
       </c>
       <c r="G56" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="57" spans="2:7" ht="16.5" x14ac:dyDescent="0.2">
       <c r="C57" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="D57" s="5" t="s">
         <v>447</v>
       </c>
-      <c r="D57" s="5" t="s">
-        <v>448</v>
-      </c>
       <c r="E57" s="5" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="F57" s="4" t="s">
         <v>187</v>
       </c>
       <c r="G57" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="58" spans="2:7" ht="16.5" x14ac:dyDescent="0.2">
       <c r="C58" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="D58" s="5" t="s">
         <v>447</v>
       </c>
-      <c r="D58" s="5" t="s">
-        <v>448</v>
-      </c>
       <c r="E58" s="5" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="F58" s="4" t="s">
         <v>241</v>
       </c>
       <c r="G58" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="59" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B59" s="15" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="60" spans="2:7" ht="16.5" x14ac:dyDescent="0.2">
       <c r="B60" s="4" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>36</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="61" spans="2:7" ht="16.5" x14ac:dyDescent="0.2">
@@ -10554,16 +10554,16 @@
         <v>187</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="F61" s="2" t="s">
         <v>187</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="62" spans="2:7" ht="16.5" x14ac:dyDescent="0.2">
@@ -10571,16 +10571,16 @@
         <v>241</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="F62" s="2" t="s">
         <v>241</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="63" spans="2:7" ht="16.5" x14ac:dyDescent="0.2">
@@ -10588,16 +10588,16 @@
         <v>187</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="F63" s="2" t="s">
         <v>241</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="64" spans="2:7" ht="16.5" x14ac:dyDescent="0.2">
@@ -10605,21 +10605,21 @@
         <v>241</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="F64" s="2" t="s">
         <v>187</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="65" spans="2:7" ht="16.5" x14ac:dyDescent="0.2">
       <c r="B65" s="4" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
@@ -10629,73 +10629,73 @@
     </row>
     <row r="66" spans="2:7" ht="16.5" x14ac:dyDescent="0.2">
       <c r="B66" s="17" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>187</v>
       </c>
       <c r="D66" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="E66" s="2" t="s">
         <v>471</v>
-      </c>
-      <c r="E66" s="2" t="s">
-        <v>472</v>
       </c>
       <c r="F66" s="2" t="s">
         <v>187</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="67" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B67" s="15" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="68" spans="2:7" ht="16.5" x14ac:dyDescent="0.2">
       <c r="B68" s="4" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C68" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="D68" s="20" t="s">
         <v>374</v>
-      </c>
-      <c r="D68" s="20" t="s">
-        <v>375</v>
       </c>
       <c r="E68" s="20"/>
       <c r="F68" s="20"/>
     </row>
     <row r="69" spans="2:7" ht="16.5" x14ac:dyDescent="0.2">
       <c r="B69" s="4" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C69" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="D69" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="D69" s="1" t="s">
-        <v>373</v>
-      </c>
       <c r="F69" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="70" spans="2:7" ht="16.5" x14ac:dyDescent="0.2">
       <c r="C70" s="1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="E70" s="5" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="71" spans="2:7" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.2">
       <c r="B71" s="15" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C71" s="9"/>
       <c r="D71" s="8"/>
@@ -10704,43 +10704,43 @@
     </row>
     <row r="72" spans="2:7" ht="16.5" x14ac:dyDescent="0.2">
       <c r="B72" s="4" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D72" s="21" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E72" s="21"/>
       <c r="F72" s="21"/>
     </row>
     <row r="73" spans="2:7" ht="16.5" x14ac:dyDescent="0.2">
       <c r="B73" s="4" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C73" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="D73" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="D73" s="1" t="s">
-        <v>373</v>
-      </c>
       <c r="F73" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="74" spans="2:7" ht="16.5" x14ac:dyDescent="0.2">
       <c r="C74" s="1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="E74" s="5" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
   </sheetData>
@@ -10809,7 +10809,7 @@
         <v>98</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -10817,7 +10817,7 @@
         <v>97</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -10825,7 +10825,7 @@
         <v>256</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C6" s="4"/>
     </row>
@@ -11015,7 +11015,7 @@
         <v>187</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>261</v>
@@ -11029,7 +11029,7 @@
         <v>188</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>261</v>
@@ -11043,7 +11043,7 @@
         <v>189</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>261</v>
@@ -11057,7 +11057,7 @@
         <v>187</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>261</v>
@@ -11071,7 +11071,7 @@
         <v>188</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>261</v>
@@ -11085,7 +11085,7 @@
         <v>189</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>261</v>
@@ -11099,7 +11099,7 @@
         <v>187</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>261</v>
@@ -11113,7 +11113,7 @@
         <v>188</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>261</v>
@@ -11127,7 +11127,7 @@
         <v>189</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>261</v>
@@ -11141,7 +11141,7 @@
         <v>187</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>264</v>
@@ -11155,7 +11155,7 @@
         <v>188</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E34" s="4" t="s">
         <v>264</v>
@@ -11169,7 +11169,7 @@
         <v>189</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>264</v>
@@ -11183,7 +11183,7 @@
         <v>187</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E36" s="5" t="s">
         <v>198</v>
@@ -11197,7 +11197,7 @@
         <v>188</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E37" s="5" t="s">
         <v>198</v>
@@ -11211,7 +11211,7 @@
         <v>189</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E38" s="5" t="s">
         <v>198</v>
@@ -11225,7 +11225,7 @@
         <v>187</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E39" s="5" t="s">
         <v>198</v>
@@ -11239,7 +11239,7 @@
         <v>188</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E40" s="5" t="s">
         <v>198</v>
@@ -11253,7 +11253,7 @@
         <v>189</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E41" s="5" t="s">
         <v>198</v>
@@ -11267,7 +11267,7 @@
         <v>187</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E42" s="5" t="s">
         <v>198</v>
@@ -11281,7 +11281,7 @@
         <v>188</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E43" s="5" t="s">
         <v>198</v>
@@ -11295,7 +11295,7 @@
         <v>189</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E44" s="5" t="s">
         <v>198</v>
@@ -11309,7 +11309,7 @@
         <v>187</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E45" s="5" t="s">
         <v>195</v>
@@ -11323,7 +11323,7 @@
         <v>188</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E46" s="5" t="s">
         <v>195</v>
@@ -11337,7 +11337,7 @@
         <v>189</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E47" s="5" t="s">
         <v>195</v>
@@ -11696,7 +11696,7 @@
     </row>
     <row r="79" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="80" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
@@ -11704,94 +11704,94 @@
         <v>100</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>57</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A81" s="1"/>
       <c r="B81" s="2"/>
       <c r="C81" s="4" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A82" s="1"/>
       <c r="B82" s="2"/>
       <c r="C82" s="4" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A83" s="1"/>
       <c r="B83" s="2"/>
       <c r="C83" s="4" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A84" s="1"/>
       <c r="B84" s="2"/>
       <c r="C84" s="4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A85" s="1"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="C86" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D86" s="4" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A87" s="1"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A88" s="1"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="89" spans="1:5" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.2">
@@ -11807,86 +11807,86 @@
         <v>99</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>89</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A91" s="1"/>
       <c r="B91" s="2"/>
       <c r="C91" s="4" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A92" s="1"/>
       <c r="B92" s="2"/>
       <c r="C92" s="4" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A93" s="1"/>
       <c r="B93" s="2"/>
       <c r="C93" s="4" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="C94" s="4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="C95" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="C96" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="97" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
       <c r="C97" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D97" s="4" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="98" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
       <c r="C98" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="99" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -11931,16 +11931,16 @@
         <v>187</v>
       </c>
       <c r="E101" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="F101" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="G101" s="4" t="s">
         <v>301</v>
       </c>
-      <c r="F101" s="4" t="s">
-        <v>300</v>
-      </c>
-      <c r="G101" s="4" t="s">
+      <c r="H101" s="4" t="s">
         <v>302</v>
-      </c>
-      <c r="H101" s="4" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="102" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
@@ -11948,7 +11948,7 @@
         <v>192</v>
       </c>
       <c r="D102" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="103" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
@@ -11956,7 +11956,7 @@
         <v>192</v>
       </c>
       <c r="D103" s="4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="104" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
@@ -11964,7 +11964,7 @@
         <v>192</v>
       </c>
       <c r="D104" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="105" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -11987,16 +11987,16 @@
         <v>187</v>
       </c>
       <c r="E107" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="F107" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="G107" s="4" t="s">
         <v>301</v>
       </c>
-      <c r="F107" s="4" t="s">
-        <v>300</v>
-      </c>
-      <c r="G107" s="4" t="s">
+      <c r="H107" s="4" t="s">
         <v>302</v>
-      </c>
-      <c r="H107" s="4" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="108" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
@@ -12004,7 +12004,7 @@
         <v>192</v>
       </c>
       <c r="D108" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="109" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
@@ -12012,7 +12012,7 @@
         <v>192</v>
       </c>
       <c r="D109" s="4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="110" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
@@ -12020,7 +12020,7 @@
         <v>192</v>
       </c>
       <c r="D110" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="111" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -12094,7 +12094,7 @@
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" s="5"/>
       <c r="B119" s="4" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C119" s="5" t="s">
         <v>245</v>
@@ -12127,7 +12127,7 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B122" s="4" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C122" s="4"/>
       <c r="D122" s="4"/>
@@ -12149,13 +12149,13 @@
     </row>
     <row r="125" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B125" s="15" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126" s="5"/>
       <c r="B126" s="4" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C126" s="5" t="s">
         <v>245</v>
@@ -12180,7 +12180,7 @@
     </row>
     <row r="128" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B128" s="15" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C128" s="6"/>
       <c r="D128" s="6"/>
@@ -12188,7 +12188,7 @@
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B129" s="4" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C129" s="4"/>
       <c r="D129" s="4"/>
@@ -12222,13 +12222,13 @@
     <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A134" s="5"/>
       <c r="B134" s="17" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135" s="5"/>
       <c r="B135" s="17" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="136" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -12246,13 +12246,13 @@
     <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138" s="5"/>
       <c r="B138" s="17" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139" s="5"/>
       <c r="B139" s="17" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="140" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -12270,19 +12270,19 @@
     <row r="142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A142" s="5"/>
       <c r="B142" s="17" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143" s="5"/>
       <c r="B143" s="17" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C143" s="4" t="s">
         <v>187</v>
       </c>
       <c r="D143" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E143" s="4" t="s">
         <v>238</v>
@@ -12293,7 +12293,7 @@
         <v>188</v>
       </c>
       <c r="D144" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E144" s="4" t="s">
         <v>238</v>
@@ -12304,7 +12304,7 @@
         <v>189</v>
       </c>
       <c r="D145" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E145" s="4" t="s">
         <v>238</v>
@@ -12316,7 +12316,7 @@
         <v>187</v>
       </c>
       <c r="D146" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E146" s="5" t="s">
         <v>197</v>
@@ -12328,7 +12328,7 @@
         <v>188</v>
       </c>
       <c r="D147" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E147" s="5" t="s">
         <v>197</v>
@@ -12340,7 +12340,7 @@
         <v>189</v>
       </c>
       <c r="D148" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E148" s="5" t="s">
         <v>197</v>
@@ -12680,41 +12680,41 @@
     </row>
     <row r="185" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C185" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D185" s="4" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E185" s="4" t="s">
         <v>252</v>
       </c>
       <c r="F185" s="4" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G185" s="4"/>
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D186" s="4" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E186" s="4" t="s">
         <v>252</v>
       </c>
       <c r="F186" s="4" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G186" s="4"/>
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C187" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D187" s="4"/>
       <c r="E187" s="4" t="s">
         <v>252</v>
       </c>
       <c r="F187" s="4" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G187" s="4"/>
     </row>
@@ -12725,27 +12725,27 @@
         <v>252</v>
       </c>
       <c r="F188" s="4" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G188" s="4"/>
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A189" s="5" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B189" s="4" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C190" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D190" s="4" t="s">
         <v>252</v>
       </c>
       <c r="F190" s="4" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G190" s="4"/>
     </row>
@@ -12754,7 +12754,7 @@
         <v>252</v>
       </c>
       <c r="F191" s="4" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G191" s="4"/>
     </row>
@@ -12762,13 +12762,13 @@
       <c r="A192" s="5"/>
       <c r="B192" s="4"/>
       <c r="C192" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D192" s="5" t="s">
         <v>192</v>
       </c>
       <c r="F192" s="4" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="193" spans="1:7" x14ac:dyDescent="0.2">
@@ -12776,7 +12776,7 @@
         <v>192</v>
       </c>
       <c r="F193" s="4" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G193" s="4"/>
     </row>
@@ -12876,7 +12876,7 @@
     </row>
     <row r="201" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A201" s="5" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="202" spans="1:7" x14ac:dyDescent="0.2">
@@ -12884,7 +12884,7 @@
         <v>101</v>
       </c>
       <c r="B202" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C202" s="5" t="s">
         <v>190</v>
@@ -12895,10 +12895,10 @@
         <v>102</v>
       </c>
       <c r="B203" s="4" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C203" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="204" spans="1:7" x14ac:dyDescent="0.2">
@@ -12960,7 +12960,7 @@
     <row r="211" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A211" s="5"/>
       <c r="C211" s="4" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.2">
@@ -12974,15 +12974,15 @@
     <row r="213" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A213" s="5"/>
       <c r="C213" s="4" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A214" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B214" s="4" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.2">
@@ -12990,13 +12990,13 @@
         <v>113</v>
       </c>
       <c r="C215" s="4" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D215" s="4" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E215" s="4" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.2">
@@ -13004,66 +13004,66 @@
         <v>110</v>
       </c>
       <c r="C216" s="4" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D216" s="4" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E216" s="4" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="F216" s="4" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C217" s="4" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D217" s="4" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E217" s="4" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="F217" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C218" s="4" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D218" s="4" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E218" s="4" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F218" s="4" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C219" s="4" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D219" s="4" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E219" s="4" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="F219" s="4" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A220" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B220" s="4" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.2">
@@ -13071,13 +13071,13 @@
         <v>112</v>
       </c>
       <c r="C221" s="4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D221" s="4" t="s">
+        <v>333</v>
+      </c>
+      <c r="E221" s="4" t="s">
         <v>334</v>
-      </c>
-      <c r="E221" s="4" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="222" spans="1:6" x14ac:dyDescent="0.2">
@@ -13085,58 +13085,58 @@
         <v>111</v>
       </c>
       <c r="C222" s="4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D222" s="4" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E222" s="4" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="F222" s="4" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C223" s="4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D223" s="4" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E223" s="4" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="F223" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C224" s="4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D224" s="4" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E224" s="4" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F224" s="4" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C225" s="4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D225" s="4" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E225" s="4" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="F225" s="4" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="226" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
fix SNDP(C) no calculation when source selection mode 3
</commit_message>
<xml_diff>
--- a/P4E_psuedo_instruction_set.xlsx
+++ b/P4E_psuedo_instruction_set.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\P4EngineAssembler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36A68664-E0AF-4D1B-9108-8829FCA38343}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4503A0C-774C-405C-80EE-67258B6BE83F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-3645" windowWidth="38640" windowHeight="21840" activeTab="1" xr2:uid="{87164962-7B7D-4BAA-98E0-B9A8D7C47112}"/>
+    <workbookView xWindow="-9290" yWindow="-21710" windowWidth="38620" windowHeight="21820" activeTab="2" xr2:uid="{87164962-7B7D-4BAA-98E0-B9A8D7C47112}"/>
   </bookViews>
   <sheets>
     <sheet name="parser" sheetId="1" r:id="rId1"/>
@@ -1224,7 +1224,7 @@
     <author>Dianchao Wang</author>
   </authors>
   <commentList>
-    <comment ref="B74" authorId="0" shapeId="0" xr:uid="{04167267-17E0-4DF6-B54E-8EB3AC806BAB}">
+    <comment ref="B77" authorId="0" shapeId="0" xr:uid="{04167267-17E0-4DF6-B54E-8EB3AC806BAB}">
       <text>
         <r>
           <rPr>
@@ -1250,7 +1250,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H101" authorId="0" shapeId="0" xr:uid="{7B59C6D1-C763-425C-8F6C-E1635B5F267C}">
+    <comment ref="H104" authorId="0" shapeId="0" xr:uid="{7B59C6D1-C763-425C-8F6C-E1635B5F267C}">
       <text>
         <r>
           <rPr>
@@ -1276,7 +1276,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H107" authorId="0" shapeId="0" xr:uid="{6766D2B6-4F7C-4D98-ABB1-B500845D4104}">
+    <comment ref="H110" authorId="0" shapeId="0" xr:uid="{6766D2B6-4F7C-4D98-ABB1-B500845D4104}">
       <text>
         <r>
           <rPr>
@@ -1302,7 +1302,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D113" authorId="0" shapeId="0" xr:uid="{1232E5F3-A694-45DA-83F2-6A0D1C7503DB}">
+    <comment ref="D116" authorId="0" shapeId="0" xr:uid="{1232E5F3-A694-45DA-83F2-6A0D1C7503DB}">
       <text>
         <r>
           <rPr>
@@ -1328,7 +1328,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D120" authorId="0" shapeId="0" xr:uid="{4C4353DC-270D-4DC9-A5D4-1860084DFD51}">
+    <comment ref="D123" authorId="0" shapeId="0" xr:uid="{4C4353DC-270D-4DC9-A5D4-1860084DFD51}">
       <text>
         <r>
           <rPr>
@@ -1354,7 +1354,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D127" authorId="0" shapeId="0" xr:uid="{A3BBB9B6-6FEE-4677-8A3B-DB59F1F7A659}">
+    <comment ref="D130" authorId="0" shapeId="0" xr:uid="{A3BBB9B6-6FEE-4677-8A3B-DB59F1F7A659}">
       <text>
         <r>
           <rPr>
@@ -1380,7 +1380,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C204" authorId="0" shapeId="0" xr:uid="{DFB4FAA4-43F6-4B75-ABE8-01CB5D2DA0F6}">
+    <comment ref="C207" authorId="0" shapeId="0" xr:uid="{DFB4FAA4-43F6-4B75-ABE8-01CB5D2DA0F6}">
       <text>
         <r>
           <rPr>
@@ -1411,7 +1411,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1442" uniqueCount="488">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1445" uniqueCount="488">
   <si>
     <t>isr SHiFT</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -6496,13 +6496,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -6867,18 +6867,18 @@
       <c r="B1" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
     </row>
     <row r="2" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>118</v>
       </c>
     </row>
@@ -7137,7 +7137,7 @@
       <c r="I14" s="1"/>
     </row>
     <row r="15" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="10" t="s">
         <v>120</v>
       </c>
       <c r="C15" s="3"/>
@@ -7346,7 +7346,7 @@
       <c r="I26" s="1"/>
     </row>
     <row r="27" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="10" t="s">
         <v>119</v>
       </c>
       <c r="C27" s="3"/>
@@ -7558,7 +7558,7 @@
       <c r="I38" s="1"/>
     </row>
     <row r="39" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B39" s="11" t="s">
+      <c r="B39" s="10" t="s">
         <v>122</v>
       </c>
       <c r="C39" s="3"/>
@@ -7871,7 +7871,7 @@
       <c r="I53" s="1"/>
     </row>
     <row r="54" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B54" s="11" t="s">
+      <c r="B54" s="10" t="s">
         <v>121</v>
       </c>
       <c r="C54" s="3"/>
@@ -8509,7 +8509,7 @@
       <c r="I91" s="1"/>
     </row>
     <row r="92" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B92" s="11" t="s">
+      <c r="B92" s="10" t="s">
         <v>123</v>
       </c>
       <c r="C92" s="3"/>
@@ -8619,7 +8619,7 @@
       <c r="I99" s="1"/>
     </row>
     <row r="100" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B100" s="11" t="s">
+      <c r="B100" s="10" t="s">
         <v>131</v>
       </c>
       <c r="C100" s="3"/>
@@ -8679,7 +8679,7 @@
       <c r="I104" s="1"/>
     </row>
     <row r="105" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B105" s="11" t="s">
+      <c r="B105" s="10" t="s">
         <v>132</v>
       </c>
       <c r="C105" s="3"/>
@@ -8739,7 +8739,7 @@
       <c r="I109" s="1"/>
     </row>
     <row r="110" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B110" s="11" t="s">
+      <c r="B110" s="10" t="s">
         <v>125</v>
       </c>
       <c r="C110" s="3"/>
@@ -8778,7 +8778,7 @@
       <c r="I112" s="1"/>
     </row>
     <row r="113" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B113" s="11" t="s">
+      <c r="B113" s="10" t="s">
         <v>126</v>
       </c>
       <c r="C113" s="3"/>
@@ -8953,7 +8953,7 @@
       <c r="I126" s="1"/>
     </row>
     <row r="127" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B127" s="11" t="s">
+      <c r="B127" s="10" t="s">
         <v>127</v>
       </c>
       <c r="C127" s="3"/>
@@ -9041,7 +9041,7 @@
       <c r="I132" s="1"/>
     </row>
     <row r="133" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B133" s="11" t="s">
+      <c r="B133" s="10" t="s">
         <v>128</v>
       </c>
       <c r="C133" s="3"/>
@@ -9145,7 +9145,7 @@
       <c r="I138" s="1"/>
     </row>
     <row r="139" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B139" s="11" t="s">
+      <c r="B139" s="10" t="s">
         <v>129</v>
       </c>
       <c r="C139" s="3"/>
@@ -9249,7 +9249,7 @@
       <c r="I144" s="1"/>
     </row>
     <row r="145" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B145" s="11" t="s">
+      <c r="B145" s="10" t="s">
         <v>130</v>
       </c>
       <c r="C145" s="3"/>
@@ -9347,7 +9347,7 @@
       <c r="I150" s="1"/>
     </row>
     <row r="151" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B151" s="11" t="s">
+      <c r="B151" s="10" t="s">
         <v>133</v>
       </c>
       <c r="C151" s="3"/>
@@ -9386,7 +9386,7 @@
       <c r="I153" s="1"/>
     </row>
     <row r="154" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B154" s="11" t="s">
+      <c r="B154" s="10" t="s">
         <v>134</v>
       </c>
       <c r="D154" s="3"/>
@@ -9423,7 +9423,7 @@
       <c r="I156" s="1"/>
     </row>
     <row r="157" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B157" s="11" t="s">
+      <c r="B157" s="10" t="s">
         <v>135</v>
       </c>
       <c r="D157" s="3"/>
@@ -9460,7 +9460,7 @@
       <c r="I159" s="1"/>
     </row>
     <row r="160" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B160" s="11" t="s">
+      <c r="B160" s="10" t="s">
         <v>136</v>
       </c>
       <c r="C160" s="3"/>
@@ -9674,7 +9674,7 @@
       <c r="I174" s="1"/>
     </row>
     <row r="175" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B175" s="11" t="s">
+      <c r="B175" s="10" t="s">
         <v>138</v>
       </c>
       <c r="C175" s="3"/>
@@ -9819,7 +9819,7 @@
       </c>
     </row>
     <row r="185" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B185" s="11" t="s">
+      <c r="B185" s="10" t="s">
         <v>140</v>
       </c>
       <c r="C185" s="3"/>
@@ -9857,7 +9857,7 @@
       </c>
     </row>
     <row r="190" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B190" s="11" t="s">
+      <c r="B190" s="10" t="s">
         <v>139</v>
       </c>
       <c r="C190" s="3"/>
@@ -9908,7 +9908,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{732D935C-EC39-4DBE-84B4-44CD168E0101}">
   <dimension ref="A1:I78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B47" sqref="B47"/>
     </sheetView>
@@ -9933,15 +9933,15 @@
       <c r="B1" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
     </row>
     <row r="2" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B2" s="5" t="s">
@@ -10412,7 +10412,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="41" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="42" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B42" s="5" t="s">
         <v>336</v>
@@ -10739,11 +10739,11 @@
       <c r="C72" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="D72" s="9" t="s">
+      <c r="D72" s="11" t="s">
         <v>325</v>
       </c>
-      <c r="E72" s="9"/>
-      <c r="F72" s="9"/>
+      <c r="E72" s="11"/>
+      <c r="F72" s="11"/>
     </row>
     <row r="73" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B73" s="1" t="s">
@@ -10786,11 +10786,11 @@
       <c r="C76" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="D76" s="9" t="s">
+      <c r="D76" s="11" t="s">
         <v>324</v>
       </c>
-      <c r="E76" s="9"/>
-      <c r="F76" s="9"/>
+      <c r="E76" s="11"/>
+      <c r="F76" s="11"/>
     </row>
     <row r="77" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B77" s="1" t="s">
@@ -10834,11 +10834,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{988C78EB-4E00-466C-9BD2-B10965380DEB}">
-  <dimension ref="A1:I231"/>
+  <dimension ref="A1:I234"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A168" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A173" sqref="A173"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C72" sqref="C72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -10862,15 +10862,15 @@
       <c r="B1" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
     </row>
     <row r="2" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B2" s="5" t="s">
@@ -11697,6 +11697,7 @@
       <c r="D69" s="2" t="s">
         <v>190</v>
       </c>
+      <c r="F69" s="1"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C70" s="1" t="s">
@@ -11705,6 +11706,7 @@
       <c r="D70" s="2" t="s">
         <v>190</v>
       </c>
+      <c r="F70" s="1"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C71" s="1" t="s">
@@ -11713,114 +11715,103 @@
       <c r="D71" s="2" t="s">
         <v>190</v>
       </c>
+      <c r="F71" s="1"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C72" s="2" t="s">
+      <c r="F72" s="1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F73" s="1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F74" s="1" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C75" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="D72" s="1"/>
-    </row>
-    <row r="73" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B73" s="5" t="s">
+      <c r="D75" s="1"/>
+    </row>
+    <row r="76" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B76" s="5" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A74" s="2" t="s">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A77" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B74" s="1" t="s">
+      <c r="B77" s="1" t="s">
         <v>199</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B75" s="5" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A76" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="C76" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D76" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E76" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C77" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="E77" s="1" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="78" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B78" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C80" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B81" s="5" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A82" s="2" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A80" s="2" t="s">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A83" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B80" s="1" t="s">
+      <c r="B83" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="C80" s="2" t="s">
+      <c r="C83" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E80" s="2" t="s">
+      <c r="E83" s="2" t="s">
         <v>291</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B81" s="1"/>
-      <c r="C81" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="E81" s="1" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B82" s="1"/>
-      <c r="C82" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="E82" s="1" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B83" s="1"/>
-      <c r="C83" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="E83" s="1" t="s">
-        <v>440</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B84" s="1"/>
       <c r="C84" s="1" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="E84" s="1" t="s">
         <v>440</v>
@@ -11829,18 +11820,16 @@
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B85" s="1"/>
       <c r="C85" s="1" t="s">
-        <v>441</v>
+        <v>282</v>
       </c>
       <c r="E85" s="1" t="s">
         <v>440</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B86" s="1"/>
       <c r="C86" s="1" t="s">
-        <v>442</v>
-      </c>
-      <c r="D86" s="1" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="E86" s="1" t="s">
         <v>440</v>
@@ -11849,7 +11838,7 @@
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B87" s="1"/>
       <c r="C87" s="1" t="s">
-        <v>443</v>
+        <v>284</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>440</v>
@@ -11858,79 +11847,84 @@
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B88" s="1"/>
       <c r="C88" s="1" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="E88" s="1" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="89" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B89" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="C89" s="3"/>
-      <c r="D89" s="3"/>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C89" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>440</v>
+      </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A90" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="B90" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="C90" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E90" s="2" t="s">
-        <v>291</v>
+      <c r="B90" s="1"/>
+      <c r="C90" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>440</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B91" s="1"/>
       <c r="C91" s="1" t="s">
-        <v>281</v>
+        <v>444</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B92" s="1"/>
-      <c r="C92" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="E92" s="1" t="s">
-        <v>440</v>
-      </c>
+    <row r="92" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B92" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="C92" s="3"/>
+      <c r="D92" s="3"/>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B93" s="1"/>
-      <c r="C93" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="E93" s="1" t="s">
-        <v>440</v>
+      <c r="A93" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E93" s="2" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B94" s="1"/>
       <c r="C94" s="1" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="E94" s="1" t="s">
         <v>440</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B95" s="1"/>
       <c r="C95" s="1" t="s">
-        <v>441</v>
+        <v>282</v>
       </c>
       <c r="E95" s="1" t="s">
         <v>440</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B96" s="1"/>
       <c r="C96" s="1" t="s">
-        <v>443</v>
+        <v>283</v>
       </c>
       <c r="E96" s="1" t="s">
         <v>440</v>
@@ -11938,10 +11932,7 @@
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C97" s="1" t="s">
-        <v>442</v>
-      </c>
-      <c r="D97" s="1" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="E97" s="1" t="s">
         <v>440</v>
@@ -11949,432 +11940,424 @@
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C98" s="1" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="E98" s="1" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="99" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B99" s="5" t="s">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C99" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C100" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C101" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B102" s="5" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A100" s="2" t="s">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A103" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="B100" s="1" t="s">
+      <c r="B103" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="C100" s="2" t="s">
+      <c r="C103" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="D100" s="2" t="s">
+      <c r="D103" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="E100" s="2" t="s">
+      <c r="E103" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="F100" s="2" t="s">
+      <c r="F103" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="G100" s="2" t="s">
+      <c r="G103" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="H100" s="2" t="s">
+      <c r="H103" s="2" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A101" s="2" t="s">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A104" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C101" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="D101" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="E101" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="F101" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="G101" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="H101" s="1" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C102" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="D102" s="1" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C103" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="D103" s="1" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C104" s="2" t="s">
         <v>192</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="105" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B105" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="D105" s="3"/>
+        <v>187</v>
+      </c>
+      <c r="E104" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="F104" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="G104" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="H104" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C105" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B106" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="D106" s="1"/>
+      <c r="C106" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C107" s="2" t="s">
         <v>192</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="E107" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="F107" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="G107" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="H107" s="1" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C108" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="D108" s="1" t="s">
-        <v>274</v>
-      </c>
+        <v>276</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B108" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="D108" s="3"/>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C109" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="D109" s="1" t="s">
-        <v>275</v>
-      </c>
+      <c r="B109" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="D109" s="1"/>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C110" s="2" t="s">
         <v>192</v>
       </c>
       <c r="D110" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="F110" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="G110" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="H110" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C111" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C112" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C113" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="D113" s="1" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="111" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B111" s="5" t="s">
+    <row r="114" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B114" s="5" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A112" s="2" t="s">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A115" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B112" s="1" t="s">
+      <c r="B115" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C112" s="2" t="s">
+      <c r="C115" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="D112" s="2" t="s">
+      <c r="D115" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="E112" s="2" t="s">
+      <c r="E115" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="113" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C113" s="1" t="s">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C116" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="D113" s="1" t="s">
+      <c r="D116" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="E113" s="1" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="114" spans="2:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B114" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="C114" s="3"/>
-      <c r="D114" s="3"/>
-      <c r="E114" s="3"/>
-    </row>
-    <row r="115" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B115" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="C115" s="1"/>
-      <c r="D115" s="1"/>
-      <c r="E115" s="1"/>
-    </row>
-    <row r="116" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C116" s="1"/>
-      <c r="D116" s="1"/>
       <c r="E116" s="1" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="117" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C117" s="2" t="s">
+    <row r="117" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B117" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="C117" s="3"/>
+      <c r="D117" s="3"/>
+      <c r="E117" s="3"/>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B118" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C118" s="1"/>
+      <c r="D118" s="1"/>
+      <c r="E118" s="1"/>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C119" s="1"/>
+      <c r="D119" s="1"/>
+      <c r="E119" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C120" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="D117" s="1"/>
-      <c r="E117" s="1"/>
-    </row>
-    <row r="118" spans="2:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B118" s="5" t="s">
+      <c r="D120" s="1"/>
+      <c r="E120" s="1"/>
+    </row>
+    <row r="121" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B121" s="5" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="119" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B119" s="1" t="s">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B122" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="C119" s="2" t="s">
+      <c r="C122" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="D119" s="2" t="s">
+      <c r="D122" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="E119" s="2" t="s">
+      <c r="E122" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="120" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C120" s="1" t="s">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C123" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="D120" s="1" t="s">
+      <c r="D123" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="E120" s="1" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="121" spans="2:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B121" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="C121" s="3"/>
-      <c r="D121" s="3"/>
-      <c r="E121" s="3"/>
-    </row>
-    <row r="122" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B122" s="1" t="s">
-        <v>345</v>
-      </c>
-      <c r="C122" s="1"/>
-      <c r="D122" s="1"/>
-      <c r="E122" s="1"/>
-    </row>
-    <row r="123" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C123" s="1"/>
-      <c r="D123" s="1"/>
       <c r="E123" s="1" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="124" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C124" s="2" t="s">
+    <row r="124" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B124" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C124" s="3"/>
+      <c r="D124" s="3"/>
+      <c r="E124" s="3"/>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B125" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="C125" s="1"/>
+      <c r="D125" s="1"/>
+      <c r="E125" s="1"/>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C126" s="1"/>
+      <c r="D126" s="1"/>
+      <c r="E126" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C127" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="D124" s="1"/>
-      <c r="E124" s="1"/>
-    </row>
-    <row r="125" spans="2:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B125" s="5" t="s">
+      <c r="D127" s="1"/>
+      <c r="E127" s="1"/>
+    </row>
+    <row r="128" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B128" s="5" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="126" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B126" s="1" t="s">
-        <v>346</v>
-      </c>
-      <c r="C126" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="D126" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="E126" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="127" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C127" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="D127" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="E127" s="1" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="128" spans="2:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B128" s="5" t="s">
-        <v>343</v>
-      </c>
-      <c r="C128" s="3"/>
-      <c r="D128" s="3"/>
-      <c r="E128" s="3"/>
     </row>
     <row r="129" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B129" s="1" t="s">
-        <v>347</v>
-      </c>
-      <c r="C129" s="1"/>
-      <c r="D129" s="1"/>
-      <c r="E129" s="1"/>
+        <v>346</v>
+      </c>
+      <c r="C129" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="D129" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="E129" s="2" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="130" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C130" s="1"/>
-      <c r="D130" s="1"/>
+      <c r="C130" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="D130" s="1" t="s">
+        <v>236</v>
+      </c>
       <c r="E130" s="1" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="131" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C131" s="2" t="s">
+    <row r="131" spans="2:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B131" s="5" t="s">
+        <v>343</v>
+      </c>
+      <c r="C131" s="3"/>
+      <c r="D131" s="3"/>
+      <c r="E131" s="3"/>
+    </row>
+    <row r="132" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B132" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="C132" s="1"/>
+      <c r="D132" s="1"/>
+      <c r="E132" s="1"/>
+    </row>
+    <row r="133" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C133" s="1"/>
+      <c r="D133" s="1"/>
+      <c r="E133" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="134" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C134" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="D131" s="1"/>
-      <c r="E131" s="1"/>
-    </row>
-    <row r="132" spans="2:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B132" s="5" t="s">
+      <c r="D134" s="1"/>
+      <c r="E134" s="1"/>
+    </row>
+    <row r="135" spans="2:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B135" s="5" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="133" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B133" s="1" t="s">
+    <row r="136" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B136" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="134" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B134" s="6" t="s">
+    <row r="137" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B137" s="6" t="s">
         <v>349</v>
-      </c>
-    </row>
-    <row r="135" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B135" s="6" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="136" spans="2:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B136" s="5" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="137" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B137" s="1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="138" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B138" s="6" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="139" spans="2:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B139" s="5" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="140" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B140" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="141" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B141" s="6" t="s">
         <v>351</v>
-      </c>
-    </row>
-    <row r="139" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B139" s="6" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="140" spans="2:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B140" s="5" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="141" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B141" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="142" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B142" s="6" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="143" spans="2:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B143" s="5" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="144" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B144" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="145" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B145" s="6" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="143" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B143" s="6" t="s">
+    <row r="146" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B146" s="6" t="s">
         <v>352</v>
       </c>
-      <c r="C143" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="D143" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="E143" s="1" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="144" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C144" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="D144" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="E144" s="1" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="145" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C145" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="D145" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="E145" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="F145" s="1"/>
-    </row>
-    <row r="146" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C146" s="1" t="s">
         <v>187</v>
       </c>
       <c r="D146" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="E146" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="F146" s="1"/>
+      <c r="E146" s="1" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="147" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C147" s="1" t="s">
@@ -12383,10 +12366,9 @@
       <c r="D147" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="E147" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="F147" s="1"/>
+      <c r="E147" s="1" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="148" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C148" s="1" t="s">
@@ -12395,8 +12377,8 @@
       <c r="D148" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="E148" s="2" t="s">
-        <v>197</v>
+      <c r="E148" s="1" t="s">
+        <v>238</v>
       </c>
       <c r="F148" s="1"/>
     </row>
@@ -12404,11 +12386,11 @@
       <c r="C149" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="D149" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="E149" s="1" t="s">
-        <v>238</v>
+      <c r="D149" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="E149" s="2" t="s">
+        <v>197</v>
       </c>
       <c r="F149" s="1"/>
     </row>
@@ -12416,11 +12398,11 @@
       <c r="C150" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="D150" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="E150" s="1" t="s">
-        <v>238</v>
+      <c r="D150" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="E150" s="2" t="s">
+        <v>197</v>
       </c>
       <c r="F150" s="1"/>
     </row>
@@ -12428,11 +12410,11 @@
       <c r="C151" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="D151" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="E151" s="1" t="s">
-        <v>238</v>
+      <c r="D151" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="E151" s="2" t="s">
+        <v>197</v>
       </c>
       <c r="F151" s="1"/>
     </row>
@@ -12441,9 +12423,11 @@
         <v>187</v>
       </c>
       <c r="D152" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="E152" s="1"/>
+        <v>259</v>
+      </c>
+      <c r="E152" s="1" t="s">
+        <v>238</v>
+      </c>
       <c r="F152" s="1"/>
     </row>
     <row r="153" spans="2:6" x14ac:dyDescent="0.2">
@@ -12451,9 +12435,11 @@
         <v>188</v>
       </c>
       <c r="D153" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="E153" s="1"/>
+        <v>259</v>
+      </c>
+      <c r="E153" s="1" t="s">
+        <v>238</v>
+      </c>
       <c r="F153" s="1"/>
     </row>
     <row r="154" spans="2:6" x14ac:dyDescent="0.2">
@@ -12461,14 +12447,16 @@
         <v>189</v>
       </c>
       <c r="D154" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="E154" s="1"/>
+        <v>259</v>
+      </c>
+      <c r="E154" s="1" t="s">
+        <v>238</v>
+      </c>
       <c r="F154" s="1"/>
     </row>
     <row r="155" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C155" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D155" s="2" t="s">
         <v>190</v>
@@ -12476,304 +12464,298 @@
       <c r="E155" s="1"/>
       <c r="F155" s="1"/>
     </row>
-    <row r="156" spans="2:6" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B156" s="5" t="s">
+    <row r="156" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C156" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="D156" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="E156" s="1"/>
+      <c r="F156" s="1"/>
+    </row>
+    <row r="157" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C157" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D157" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="E157" s="1"/>
+      <c r="F157" s="1"/>
+    </row>
+    <row r="158" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C158" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D158" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="E158" s="1"/>
+      <c r="F158" s="1"/>
+    </row>
+    <row r="159" spans="2:6" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B159" s="5" t="s">
         <v>213</v>
-      </c>
-    </row>
-    <row r="157" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B157" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="158" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B158" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="159" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B159" s="1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="160" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B160" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="161" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B161" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="162" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B162" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="163" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B163" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C160" s="2" t="s">
+      <c r="C163" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D160" s="2" t="s">
+      <c r="D163" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="E160" s="2" t="s">
+      <c r="E163" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="F160" s="2" t="s">
+      <c r="F163" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="161" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B161" s="1"/>
-      <c r="C161" s="1" t="s">
+    <row r="164" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B164" s="1"/>
+      <c r="C164" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="D161" s="1" t="s">
+      <c r="D164" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="E161" s="1" t="s">
+      <c r="E164" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="F161" s="1" t="s">
+      <c r="F164" s="1" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="162" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C162" s="1" t="s">
+    <row r="165" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C165" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="D162" s="1" t="s">
+      <c r="D165" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="E162" s="1" t="s">
+      <c r="E165" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="F162" s="1" t="s">
+      <c r="F165" s="1" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="163" spans="2:6" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B163" s="5" t="s">
+    <row r="166" spans="2:6" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B166" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="C163" s="3"/>
-      <c r="D163" s="3"/>
-      <c r="E163" s="3"/>
-      <c r="F163" s="3"/>
-    </row>
-    <row r="164" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B164" s="1" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="165" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B165" s="1" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="166" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B166" s="1" t="s">
-        <v>249</v>
-      </c>
+      <c r="C166" s="3"/>
+      <c r="D166" s="3"/>
+      <c r="E166" s="3"/>
+      <c r="F166" s="3"/>
     </row>
     <row r="167" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B167" s="1" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="168" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B168" s="1" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="169" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B169" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="170" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B170" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="C167" s="1"/>
-      <c r="D167" s="1"/>
-    </row>
-    <row r="168" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="E168" s="1" t="s">
+      <c r="C170" s="1"/>
+      <c r="D170" s="1"/>
+    </row>
+    <row r="171" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E171" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="F168" s="1" t="s">
+      <c r="F171" s="1" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="169" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C169" s="1"/>
-      <c r="D169" s="1"/>
-      <c r="E169" s="1" t="s">
+    <row r="172" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C172" s="1"/>
+      <c r="D172" s="1"/>
+      <c r="E172" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="F169" s="1" t="s">
+      <c r="F172" s="1" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="170" spans="2:6" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B170" s="5" t="s">
+    <row r="173" spans="2:6" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B173" s="5" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="171" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B171" s="1" t="s">
+    <row r="174" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B174" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="172" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C172" s="2" t="s">
+    <row r="175" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C175" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D172" s="2" t="s">
+      <c r="D175" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="E172" s="2" t="s">
+      <c r="E175" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="F172" s="2" t="s">
+      <c r="F175" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="173" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C173" s="1" t="s">
+    <row r="176" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C176" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="D173" s="1" t="s">
+      <c r="D176" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="E173" s="1" t="s">
+      <c r="E176" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="F173" s="1" t="s">
+      <c r="F176" s="1" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="174" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C174" s="1" t="s">
+    <row r="177" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C177" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="D174" s="1" t="s">
+      <c r="D177" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="E174" s="1" t="s">
+      <c r="E177" s="1" t="s">
         <v>241</v>
-      </c>
-      <c r="F174" s="1" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="175" spans="2:6" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B175" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="C175" s="3"/>
-      <c r="D175" s="3"/>
-      <c r="E175" s="3"/>
-      <c r="F175" s="3"/>
-    </row>
-    <row r="176" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B176" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="C176" s="1"/>
-      <c r="D176" s="1"/>
-    </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E177" s="1" t="s">
-        <v>187</v>
       </c>
       <c r="F177" s="1" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C178" s="1"/>
-      <c r="D178" s="1"/>
-      <c r="E178" s="1" t="s">
+    <row r="178" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B178" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="C178" s="3"/>
+      <c r="D178" s="3"/>
+      <c r="E178" s="3"/>
+      <c r="F178" s="3"/>
+    </row>
+    <row r="179" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B179" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C179" s="1"/>
+      <c r="D179" s="1"/>
+    </row>
+    <row r="180" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E180" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="F180" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="181" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C181" s="1"/>
+      <c r="D181" s="1"/>
+      <c r="E181" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="F178" s="1" t="s">
+      <c r="F181" s="1" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="179" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B179" s="5" t="s">
+    <row r="182" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B182" s="5" t="s">
         <v>122</v>
-      </c>
-    </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A180" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A181" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="B181" s="4" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A182" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B182" s="1" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A183" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="B183" s="4" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A184" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B184" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="185" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A185" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B185" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="186" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A186" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B186" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="187" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A187" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B184" s="1" t="s">
+      <c r="B187" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="C184" s="2" t="s">
+      <c r="C187" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D184" s="2" t="s">
+      <c r="D187" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="E184" s="2" t="s">
+      <c r="E187" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="F184" s="2" t="s">
+      <c r="F187" s="2" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C185" s="1" t="s">
+    <row r="188" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C188" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="D185" s="1" t="s">
+      <c r="D188" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="E185" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="F185" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="G185" s="1"/>
-    </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D186" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="E186" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="F186" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="G186" s="1"/>
-    </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C187" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="D187" s="1"/>
-      <c r="E187" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="F187" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="G187" s="1"/>
-    </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C188" s="1"/>
-      <c r="D188" s="1"/>
       <c r="E188" s="1" t="s">
         <v>252</v>
       </c>
@@ -12783,18 +12765,23 @@
       <c r="G188" s="1"/>
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A189" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="B189" s="1" t="s">
-        <v>294</v>
-      </c>
+      <c r="D189" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="E189" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="F189" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="G189" s="1"/>
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C190" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="D190" s="1" t="s">
+      <c r="D190" s="1"/>
+      <c r="E190" s="1" t="s">
         <v>252</v>
       </c>
       <c r="F190" s="1" t="s">
@@ -12803,7 +12790,9 @@
       <c r="G190" s="1"/>
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D191" s="1" t="s">
+      <c r="C191" s="1"/>
+      <c r="D191" s="1"/>
+      <c r="E191" s="1" t="s">
         <v>252</v>
       </c>
       <c r="F191" s="1" t="s">
@@ -12812,99 +12801,75 @@
       <c r="G191" s="1"/>
     </row>
     <row r="192" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B192" s="1"/>
-      <c r="C192" s="1" t="s">
+      <c r="A192" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="B192" s="1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="193" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C193" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="D192" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="F192" s="1" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D193" s="2" t="s">
-        <v>192</v>
+      <c r="D193" s="1" t="s">
+        <v>252</v>
       </c>
       <c r="F193" s="1" t="s">
         <v>293</v>
       </c>
       <c r="G193" s="1"/>
     </row>
-    <row r="194" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B194" s="5" t="s">
+    <row r="194" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D194" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="F194" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="G194" s="1"/>
+    </row>
+    <row r="195" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B195" s="1"/>
+      <c r="C195" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="D195" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="F195" s="1" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="196" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D196" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="F196" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="G196" s="1"/>
+    </row>
+    <row r="197" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B197" s="5" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A195" s="2" t="s">
+    <row r="198" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A198" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="B195" s="1" t="s">
+      <c r="B198" s="1" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A196" s="2" t="s">
+    <row r="199" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A199" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="B196" s="1"/>
-      <c r="C196" s="1" t="s">
+      <c r="B199" s="1"/>
+      <c r="C199" s="1" t="s">
         <v>241</v>
-      </c>
-      <c r="D196" s="2" t="s">
-        <v>445</v>
-      </c>
-      <c r="E196" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="F196" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="G196" s="2" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B197" s="1"/>
-      <c r="C197" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="D197" s="2" t="s">
-        <v>445</v>
-      </c>
-      <c r="E197" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="F197" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="G197" s="2" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B198" s="1"/>
-      <c r="C198" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="D198" s="2" t="s">
-        <v>445</v>
-      </c>
-      <c r="E198" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="F198" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="G198" s="2" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C199" s="1" t="s">
-        <v>187</v>
       </c>
       <c r="D199" s="2" t="s">
         <v>445</v>
@@ -12913,172 +12878,183 @@
         <v>253</v>
       </c>
       <c r="F199" s="1" t="s">
-        <v>241</v>
+        <v>187</v>
       </c>
       <c r="G199" s="2" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="200" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B200" s="5" t="s">
+    <row r="200" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B200" s="1"/>
+      <c r="C200" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="D200" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="E200" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="F200" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="G200" s="2" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="201" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B201" s="1"/>
+      <c r="C201" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D201" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="E201" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="F201" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="G201" s="2" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="202" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C202" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D202" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="E202" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="F202" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="G202" s="2" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="203" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B203" s="5" t="s">
         <v>218</v>
-      </c>
-    </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A201" s="2" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A202" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B202" s="1" t="s">
-        <v>354</v>
-      </c>
-      <c r="C202" s="2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A203" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B203" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="C203" s="1" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="204" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A204" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C204" s="2" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="205" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A205" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B205" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="C205" s="2" t="s">
         <v>190</v>
-      </c>
-    </row>
-    <row r="205" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B205" s="5" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="206" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A206" s="2" t="s">
-        <v>62</v>
+        <v>102</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>61</v>
+        <v>355</v>
+      </c>
+      <c r="C206" s="1" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="207" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A207" s="2" t="s">
+        <v>103</v>
+      </c>
       <c r="C207" s="2" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="208" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B208" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A209" s="2" t="s">
-        <v>68</v>
+        <v>62</v>
+      </c>
+      <c r="B209" s="1" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A210" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B210" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="C210" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D210" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E210" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F210" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C211" s="1" t="s">
-        <v>298</v>
+        <v>190</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B211" s="5" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A212" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B212" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C213" s="1" t="s">
-        <v>297</v>
+      <c r="A213" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B213" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C213" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D213" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E213" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F213" s="2" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A214" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="B214" s="1" t="s">
-        <v>389</v>
+      <c r="C214" s="1" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A215" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B215" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="216" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C216" s="1" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="217" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A217" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="B217" s="1" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="218" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A218" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C215" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="D215" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="E215" s="1" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A216" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C216" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="D216" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="E216" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="F216" s="1" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C217" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="D217" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="E217" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="F217" s="1" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="218" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C218" s="1" t="s">
         <v>299</v>
       </c>
@@ -13086,13 +13062,13 @@
         <v>301</v>
       </c>
       <c r="E218" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="F218" s="1" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A219" s="2" t="s">
+        <v>110</v>
+      </c>
       <c r="C219" s="1" t="s">
         <v>299</v>
       </c>
@@ -13100,66 +13076,66 @@
         <v>301</v>
       </c>
       <c r="E219" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="F219" s="1" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="220" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C220" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="D220" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="E220" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="F220" s="1" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="221" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C221" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="D221" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="E221" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="F221" s="1" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="222" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C222" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="D222" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="E222" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="F219" s="1" t="s">
+      <c r="F222" s="1" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="220" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A220" s="2" t="s">
+    <row r="223" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A223" s="2" t="s">
         <v>391</v>
       </c>
-      <c r="B220" s="1" t="s">
+      <c r="B223" s="1" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="221" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A221" s="2" t="s">
+    <row r="224" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A224" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="C221" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="D221" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="E221" s="1" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="222" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A222" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C222" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="D222" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="E222" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="F222" s="1" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="223" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C223" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="D223" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="E223" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="F223" s="1" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="224" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C224" s="1" t="s">
         <v>300</v>
       </c>
@@ -13167,13 +13143,13 @@
         <v>302</v>
       </c>
       <c r="E224" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="F224" s="1" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A225" s="2" t="s">
+        <v>111</v>
+      </c>
       <c r="C225" s="1" t="s">
         <v>300</v>
       </c>
@@ -13181,47 +13157,89 @@
         <v>302</v>
       </c>
       <c r="E225" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="F225" s="1" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="226" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C226" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="D226" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="E226" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="F226" s="1" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="227" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C227" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="D227" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="E227" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="F227" s="1" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="228" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C228" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="D228" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="E228" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="F225" s="1" t="s">
+      <c r="F228" s="1" t="s">
         <v>311</v>
-      </c>
-    </row>
-    <row r="226" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B226" s="5" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="227" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A227" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="B227" s="1" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="228" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B228" s="1"/>
-      <c r="C228" s="2" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="229" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B229" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="C229" s="3"/>
+        <v>221</v>
+      </c>
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A230" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B230" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="231" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B231" s="1"/>
+      <c r="C231" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="232" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B232" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="C232" s="3"/>
+    </row>
+    <row r="233" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A233" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B230" s="1" t="s">
+      <c r="B233" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="231" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C231" s="2" t="s">
+    <row r="234" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C234" s="2" t="s">
         <v>190</v>
       </c>
     </row>

</xml_diff>

<commit_message>
parser header calculation instructions change
</commit_message>
<xml_diff>
--- a/P4E_psuedo_instruction_set.xlsx
+++ b/P4E_psuedo_instruction_set.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\P4EngineAssembler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4503A0C-774C-405C-80EE-67258B6BE83F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{055754AD-D662-4616-A8F9-7B86428A82FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9290" yWindow="-21710" windowWidth="38620" windowHeight="21820" activeTab="2" xr2:uid="{87164962-7B7D-4BAA-98E0-B9A8D7C47112}"/>
+    <workbookView xWindow="-9290" yWindow="-21710" windowWidth="38620" windowHeight="21820" xr2:uid="{87164962-7B7D-4BAA-98E0-B9A8D7C47112}"/>
   </bookViews>
   <sheets>
     <sheet name="parser" sheetId="1" r:id="rId1"/>
@@ -1411,7 +1411,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1445" uniqueCount="488">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1445" uniqueCount="491">
   <si>
     <t>isr SHiFT</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -3934,10 +3934,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>(offset)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>0b'00010</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -6009,6 +6005,310 @@
   </si>
   <si>
     <r>
+      <t>len</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (1-32) } ,</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>mask32</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ;</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">TCAM_KEY { </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">offset5 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>len</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (1-10) } ,</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">imm40 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(hex) ;</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">ISR { </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>off5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> :</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">META { </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">off9 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>len</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (1-40) } ,</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&gt;&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">val6 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(1-32),</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">-&gt;nxt_state8 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&gt;&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">val6 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(1-32) ;</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>len</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (8 | 16 | 24 | 32) } ,</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
@@ -6040,7 +6340,21 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> (in byte) </t>
+      <t xml:space="preserve"> (0 | 8 | 16 | 24) :</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">{ </t>
     </r>
     <r>
       <rPr>
@@ -6052,8 +6366,40 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>:</t>
-    </r>
+      <t>offset9</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (0-511) :</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">mask32 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(offset in bit, in byte for PHV)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -6069,314 +6415,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> (1-32) } ,</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">{ </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>offset5</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (in bit) :</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>mask32</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> ;</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">TCAM_KEY { </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">offset5 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>:</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>len</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (1-10) } ,</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">imm40 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(hex) ;</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">ISR { </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>off5</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> :</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">META { </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">off9 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>:</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>len</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (1-40) } ,</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&gt;&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">val6 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(1-32),</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">-&gt;nxt_state8 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>;</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&gt;&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">val6 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(1-32) ;</t>
+      <t xml:space="preserve"> (16 | 32) } ,</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -6841,9 +6880,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA14F7B7-5F50-4FFB-AE20-84853F321386}">
   <dimension ref="A1:I194"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D137" sqref="D137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6908,16 +6947,16 @@
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>187</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -6926,16 +6965,16 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>241</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
@@ -6944,10 +6983,10 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -7000,25 +7039,25 @@
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>269</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>448</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>449</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>187</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -7027,43 +7066,43 @@
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>269</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>448</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>449</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>241</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>269</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>448</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>449</v>
-      </c>
       <c r="G11" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
@@ -7071,67 +7110,67 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>268</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>448</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>449</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>187</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>268</v>
       </c>
       <c r="E13" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>448</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>449</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>241</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>268</v>
       </c>
       <c r="E14" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>448</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>449</v>
-      </c>
       <c r="G14" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
@@ -7181,19 +7220,19 @@
         <v>269</v>
       </c>
       <c r="D17" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>448</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>449</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>187</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="I17" s="1"/>
     </row>
@@ -7203,19 +7242,19 @@
         <v>269</v>
       </c>
       <c r="D18" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>448</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>449</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>241</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="I18" s="1"/>
     </row>
@@ -7225,13 +7264,13 @@
         <v>269</v>
       </c>
       <c r="D19" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>448</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>449</v>
-      </c>
       <c r="F19" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
@@ -7243,19 +7282,19 @@
         <v>268</v>
       </c>
       <c r="D20" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>448</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>449</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>187</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="I20" s="1"/>
     </row>
@@ -7265,19 +7304,19 @@
         <v>268</v>
       </c>
       <c r="D21" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>448</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>449</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>241</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="I21" s="1"/>
     </row>
@@ -7287,13 +7326,13 @@
         <v>268</v>
       </c>
       <c r="D22" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>448</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>449</v>
-      </c>
       <c r="F22" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
@@ -7311,25 +7350,25 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="I24" s="1"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
@@ -7393,19 +7432,19 @@
         <v>269</v>
       </c>
       <c r="D29" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>448</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>449</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>187</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="I29" s="1"/>
     </row>
@@ -7415,19 +7454,19 @@
         <v>269</v>
       </c>
       <c r="D30" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="E30" s="1" t="s">
         <v>448</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>449</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>241</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="I30" s="1"/>
     </row>
@@ -7437,13 +7476,13 @@
         <v>269</v>
       </c>
       <c r="D31" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="E31" s="1" t="s">
         <v>448</v>
       </c>
-      <c r="E31" s="1" t="s">
-        <v>449</v>
-      </c>
       <c r="F31" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
@@ -7455,19 +7494,19 @@
         <v>268</v>
       </c>
       <c r="D32" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="E32" s="1" t="s">
         <v>448</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>449</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>187</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="I32" s="1"/>
     </row>
@@ -7477,19 +7516,19 @@
         <v>268</v>
       </c>
       <c r="D33" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="E33" s="1" t="s">
         <v>448</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>449</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>241</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="I33" s="1"/>
     </row>
@@ -7499,13 +7538,13 @@
         <v>268</v>
       </c>
       <c r="D34" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="E34" s="1" t="s">
         <v>448</v>
       </c>
-      <c r="E34" s="1" t="s">
-        <v>449</v>
-      </c>
       <c r="F34" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
@@ -7523,25 +7562,25 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="I36" s="1"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
@@ -7615,22 +7654,22 @@
         <v>269</v>
       </c>
       <c r="D42" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="E42" s="1" t="s">
         <v>448</v>
       </c>
-      <c r="E42" s="1" t="s">
-        <v>449</v>
-      </c>
       <c r="F42" s="1" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>187</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
@@ -7638,22 +7677,22 @@
         <v>269</v>
       </c>
       <c r="D43" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="E43" s="1" t="s">
         <v>448</v>
       </c>
-      <c r="E43" s="1" t="s">
-        <v>449</v>
-      </c>
       <c r="F43" s="1" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>241</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
@@ -7661,16 +7700,16 @@
         <v>269</v>
       </c>
       <c r="D44" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="E44" s="1" t="s">
         <v>448</v>
       </c>
-      <c r="E44" s="1" t="s">
-        <v>449</v>
-      </c>
       <c r="F44" s="1" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
@@ -7680,22 +7719,22 @@
         <v>268</v>
       </c>
       <c r="D45" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="E45" s="1" t="s">
         <v>448</v>
       </c>
-      <c r="E45" s="1" t="s">
-        <v>449</v>
-      </c>
       <c r="F45" s="1" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="G45" s="1" t="s">
         <v>187</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
@@ -7703,22 +7742,22 @@
         <v>268</v>
       </c>
       <c r="D46" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="E46" s="1" t="s">
         <v>448</v>
       </c>
-      <c r="E46" s="1" t="s">
-        <v>449</v>
-      </c>
       <c r="F46" s="1" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>241</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
@@ -7726,16 +7765,16 @@
         <v>268</v>
       </c>
       <c r="D47" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="E47" s="1" t="s">
         <v>448</v>
       </c>
-      <c r="E47" s="1" t="s">
-        <v>449</v>
-      </c>
       <c r="F47" s="1" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
@@ -7745,10 +7784,10 @@
         <v>269</v>
       </c>
       <c r="D48" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="E48" s="1" t="s">
         <v>448</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>449</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>281</v>
@@ -7757,10 +7796,10 @@
         <v>187</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
@@ -7768,10 +7807,10 @@
         <v>269</v>
       </c>
       <c r="D49" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="E49" s="1" t="s">
         <v>448</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>449</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>281</v>
@@ -7780,10 +7819,10 @@
         <v>241</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
@@ -7791,16 +7830,16 @@
         <v>269</v>
       </c>
       <c r="D50" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="E50" s="1" t="s">
         <v>448</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>449</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>281</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
@@ -7810,10 +7849,10 @@
         <v>268</v>
       </c>
       <c r="D51" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="E51" s="1" t="s">
         <v>448</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>449</v>
       </c>
       <c r="F51" s="1" t="s">
         <v>281</v>
@@ -7822,10 +7861,10 @@
         <v>187</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
@@ -7833,10 +7872,10 @@
         <v>268</v>
       </c>
       <c r="D52" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="E52" s="1" t="s">
         <v>448</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>449</v>
       </c>
       <c r="F52" s="1" t="s">
         <v>281</v>
@@ -7845,10 +7884,10 @@
         <v>241</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
@@ -7856,16 +7895,16 @@
         <v>268</v>
       </c>
       <c r="D53" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="E53" s="1" t="s">
         <v>448</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>449</v>
       </c>
       <c r="F53" s="1" t="s">
         <v>281</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
@@ -7911,16 +7950,16 @@
       </c>
       <c r="B56" s="1"/>
       <c r="C56" s="1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>187</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="G56" s="1"/>
       <c r="H56" s="1"/>
@@ -7929,16 +7968,16 @@
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B57" s="1"/>
       <c r="C57" s="1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>241</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="G57" s="1"/>
       <c r="H57" s="1"/>
@@ -7947,10 +7986,10 @@
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B58" s="1"/>
       <c r="C58" s="1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
@@ -7961,16 +8000,16 @@
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B59" s="1"/>
       <c r="C59" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>187</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="G59" s="1"/>
       <c r="H59" s="1"/>
@@ -7979,16 +8018,16 @@
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B60" s="1"/>
       <c r="C60" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>241</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="G60" s="1"/>
       <c r="H60" s="1"/>
@@ -7997,10 +8036,10 @@
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B61" s="1"/>
       <c r="C61" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>
@@ -8011,16 +8050,16 @@
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B62" s="1"/>
       <c r="C62" s="1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>187</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="G62" s="1"/>
       <c r="H62" s="1"/>
@@ -8029,16 +8068,16 @@
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B63" s="1"/>
       <c r="C63" s="1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>241</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="G63" s="1"/>
       <c r="H63" s="1"/>
@@ -8047,10 +8086,10 @@
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B64" s="1"/>
       <c r="C64" s="1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E64" s="1"/>
       <c r="F64" s="1"/>
@@ -8061,16 +8100,16 @@
     <row r="65" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B65" s="1"/>
       <c r="C65" s="1" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>187</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="G65" s="1"/>
       <c r="H65" s="1"/>
@@ -8079,16 +8118,16 @@
     <row r="66" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B66" s="1"/>
       <c r="C66" s="1" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>241</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="G66" s="1"/>
       <c r="H66" s="1"/>
@@ -8097,10 +8136,10 @@
     <row r="67" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B67" s="1"/>
       <c r="C67" s="1" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E67" s="1"/>
       <c r="F67" s="1"/>
@@ -8111,16 +8150,16 @@
     <row r="68" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B68" s="1"/>
       <c r="C68" s="1" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>187</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="G68" s="1"/>
       <c r="H68" s="1"/>
@@ -8129,16 +8168,16 @@
     <row r="69" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B69" s="1"/>
       <c r="C69" s="1" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>241</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="G69" s="1"/>
       <c r="H69" s="1"/>
@@ -8147,10 +8186,10 @@
     <row r="70" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B70" s="1"/>
       <c r="C70" s="1" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E70" s="1"/>
       <c r="F70" s="1"/>
@@ -8161,16 +8200,16 @@
     <row r="71" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B71" s="1"/>
       <c r="C71" s="1" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>187</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="G71" s="1"/>
       <c r="H71" s="1"/>
@@ -8179,16 +8218,16 @@
     <row r="72" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B72" s="1"/>
       <c r="C72" s="1" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>241</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="G72" s="1"/>
       <c r="H72" s="1"/>
@@ -8197,10 +8236,10 @@
     <row r="73" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B73" s="1"/>
       <c r="C73" s="1" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E73" s="1"/>
       <c r="F73" s="1"/>
@@ -8211,16 +8250,16 @@
     <row r="74" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B74" s="1"/>
       <c r="C74" s="1" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>187</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="G74" s="1"/>
       <c r="H74" s="1"/>
@@ -8229,16 +8268,16 @@
     <row r="75" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B75" s="1"/>
       <c r="C75" s="1" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>241</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="G75" s="1"/>
       <c r="H75" s="1"/>
@@ -8247,10 +8286,10 @@
     <row r="76" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B76" s="1"/>
       <c r="C76" s="1" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E76" s="1"/>
       <c r="F76" s="1"/>
@@ -8261,16 +8300,16 @@
     <row r="77" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B77" s="1"/>
       <c r="C77" s="1" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>187</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="G77" s="1"/>
       <c r="H77" s="1"/>
@@ -8279,16 +8318,16 @@
     <row r="78" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B78" s="1"/>
       <c r="C78" s="1" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>241</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="G78" s="1"/>
       <c r="H78" s="1"/>
@@ -8297,10 +8336,10 @@
     <row r="79" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B79" s="1"/>
       <c r="C79" s="1" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E79" s="1"/>
       <c r="F79" s="1"/>
@@ -8311,16 +8350,16 @@
     <row r="80" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B80" s="1"/>
       <c r="C80" s="1" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>187</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="G80" s="1"/>
       <c r="H80" s="1"/>
@@ -8329,16 +8368,16 @@
     <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B81" s="1"/>
       <c r="C81" s="1" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>241</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="G81" s="1"/>
       <c r="H81" s="1"/>
@@ -8347,10 +8386,10 @@
     <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B82" s="1"/>
       <c r="C82" s="1" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E82" s="1"/>
       <c r="F82" s="1"/>
@@ -8361,16 +8400,16 @@
     <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B83" s="1"/>
       <c r="C83" s="1" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>187</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="G83" s="1"/>
       <c r="H83" s="1"/>
@@ -8379,16 +8418,16 @@
     <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B84" s="1"/>
       <c r="C84" s="1" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>241</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="G84" s="1"/>
       <c r="H84" s="1"/>
@@ -8397,10 +8436,10 @@
     <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B85" s="1"/>
       <c r="C85" s="1" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E85" s="1"/>
       <c r="F85" s="1"/>
@@ -8411,16 +8450,16 @@
     <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B86" s="1"/>
       <c r="C86" s="1" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>187</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="G86" s="1"/>
       <c r="H86" s="1"/>
@@ -8429,16 +8468,16 @@
     <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B87" s="1"/>
       <c r="C87" s="1" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>241</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="G87" s="1"/>
       <c r="H87" s="1"/>
@@ -8447,10 +8486,10 @@
     <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B88" s="1"/>
       <c r="C88" s="1" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E88" s="1"/>
       <c r="F88" s="1"/>
@@ -8461,16 +8500,16 @@
     <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B89" s="1"/>
       <c r="C89" s="1" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="D89" s="1" t="s">
         <v>187</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="G89" s="1"/>
       <c r="H89" s="1"/>
@@ -8479,16 +8518,16 @@
     <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B90" s="1"/>
       <c r="C90" s="1" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>241</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="G90" s="1"/>
       <c r="H90" s="1"/>
@@ -8497,10 +8536,10 @@
     <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B91" s="1"/>
       <c r="C91" s="1" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E91" s="1"/>
       <c r="F91" s="1"/>
@@ -8551,11 +8590,11 @@
     <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B95" s="1"/>
       <c r="C95" s="1" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="D95" s="1"/>
       <c r="E95" s="1" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="G95" s="1"/>
       <c r="H95" s="1"/>
@@ -8564,13 +8603,13 @@
     <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B96" s="1"/>
       <c r="C96" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="E96" s="1" t="s">
         <v>462</v>
-      </c>
-      <c r="D96" s="1" t="s">
-        <v>464</v>
-      </c>
-      <c r="E96" s="1" t="s">
-        <v>463</v>
       </c>
       <c r="G96" s="1"/>
       <c r="H96" s="1"/>
@@ -8593,11 +8632,11 @@
     <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B98" s="1"/>
       <c r="C98" s="1" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="D98" s="1"/>
       <c r="E98" s="1" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="G98" s="1"/>
       <c r="H98" s="1"/>
@@ -8606,13 +8645,13 @@
     <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B99" s="1"/>
       <c r="C99" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="E99" s="1" t="s">
         <v>462</v>
-      </c>
-      <c r="D99" s="1" t="s">
-        <v>464</v>
-      </c>
-      <c r="E99" s="1" t="s">
-        <v>463</v>
       </c>
       <c r="G99" s="1"/>
       <c r="H99" s="1"/>
@@ -8669,7 +8708,7 @@
     <row r="104" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B104" s="1"/>
       <c r="C104" s="1" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D104" s="1"/>
       <c r="E104" s="1"/>
@@ -8729,7 +8768,7 @@
     <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B109" s="1"/>
       <c r="C109" s="1" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D109" s="1"/>
       <c r="E109" s="1"/>
@@ -8803,7 +8842,7 @@
         <v>34</v>
       </c>
       <c r="E114" s="2" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="F114" s="1"/>
       <c r="G114" s="1"/>
@@ -8823,7 +8862,7 @@
     <row r="116" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B116" s="1"/>
       <c r="C116" s="1" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="D116" s="1"/>
       <c r="F116" s="1"/>
@@ -8834,7 +8873,7 @@
     <row r="117" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B117" s="1"/>
       <c r="D117" s="1" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G117" s="1"/>
       <c r="H117" s="1"/>
@@ -8861,10 +8900,10 @@
     <row r="120" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B120" s="1"/>
       <c r="C120" s="1" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G120" s="1"/>
       <c r="H120" s="1"/>
@@ -8873,7 +8912,7 @@
     <row r="121" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B121" s="1"/>
       <c r="C121" s="1" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="D121" s="1" t="s">
         <v>262</v>
@@ -8885,7 +8924,7 @@
     <row r="122" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B122" s="1"/>
       <c r="C122" s="1" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="D122" s="1" t="s">
         <v>264</v>
@@ -8897,11 +8936,11 @@
     <row r="123" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B123" s="1"/>
       <c r="C123" s="1" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="D123" s="1"/>
       <c r="E123" s="2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="G123" s="1"/>
       <c r="H123" s="1"/>
@@ -8910,13 +8949,13 @@
     <row r="124" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B124" s="1"/>
       <c r="C124" s="1" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="E124" s="2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="G124" s="1"/>
       <c r="H124" s="1"/>
@@ -8925,13 +8964,13 @@
     <row r="125" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B125" s="1"/>
       <c r="C125" s="1" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="E125" s="2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="G125" s="1"/>
       <c r="H125" s="1"/>
@@ -8940,13 +8979,13 @@
     <row r="126" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B126" s="1"/>
       <c r="C126" s="1" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="E126" s="2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="G126" s="1"/>
       <c r="H126" s="1"/>
@@ -8988,10 +9027,10 @@
     <row r="129" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B129" s="1"/>
       <c r="C129" s="1" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="F129" s="1"/>
       <c r="G129" s="1"/>
@@ -9001,10 +9040,10 @@
     <row r="130" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B130" s="1"/>
       <c r="C130" s="1" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="F130" s="1"/>
       <c r="G130" s="1"/>
@@ -9014,13 +9053,13 @@
     <row r="131" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B131" s="1"/>
       <c r="C131" s="1" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="F131" s="1"/>
       <c r="G131" s="1"/>
@@ -9030,10 +9069,10 @@
     <row r="132" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B132" s="1"/>
       <c r="C132" s="1" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="F132" s="1"/>
       <c r="G132" s="1"/>
@@ -9078,7 +9117,7 @@
         <v>23</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>357</v>
+        <v>489</v>
       </c>
       <c r="E135" s="2" t="s">
         <v>24</v>
@@ -9096,13 +9135,13 @@
         <v>187</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>475</v>
+        <v>487</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>476</v>
+        <v>490</v>
       </c>
       <c r="F136" s="1" t="s">
-        <v>193</v>
+        <v>488</v>
       </c>
       <c r="G136" s="1"/>
       <c r="H136" s="1"/>
@@ -9114,13 +9153,13 @@
         <v>269</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>477</v>
+        <v>486</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>476</v>
+        <v>490</v>
       </c>
       <c r="F137" s="1" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="G137" s="1"/>
       <c r="H137" s="1"/>
@@ -9132,13 +9171,13 @@
         <v>268</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>477</v>
+        <v>486</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>476</v>
+        <v>490</v>
       </c>
       <c r="F138" s="1" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="G138" s="1"/>
       <c r="H138" s="1"/>
@@ -9182,7 +9221,7 @@
         <v>23</v>
       </c>
       <c r="D141" s="2" t="s">
-        <v>357</v>
+        <v>489</v>
       </c>
       <c r="E141" s="2" t="s">
         <v>24</v>
@@ -9200,10 +9239,10 @@
         <v>187</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>475</v>
+        <v>487</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>476</v>
+        <v>485</v>
       </c>
       <c r="F142" s="1" t="s">
         <v>193</v>
@@ -9218,13 +9257,13 @@
         <v>269</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>477</v>
+        <v>486</v>
       </c>
       <c r="E143" s="1" t="s">
-        <v>476</v>
+        <v>485</v>
       </c>
       <c r="F143" s="1" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="G143" s="1"/>
       <c r="H143" s="1"/>
@@ -9236,13 +9275,13 @@
         <v>268</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>477</v>
+        <v>486</v>
       </c>
       <c r="E144" s="1" t="s">
-        <v>476</v>
+        <v>485</v>
       </c>
       <c r="F144" s="1" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="G144" s="1"/>
       <c r="H144" s="1"/>
@@ -9281,7 +9320,7 @@
         <v>23</v>
       </c>
       <c r="D147" s="2" t="s">
-        <v>357</v>
+        <v>489</v>
       </c>
       <c r="E147" s="2" t="s">
         <v>24</v>
@@ -9298,13 +9337,13 @@
         <v>187</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>475</v>
+        <v>487</v>
       </c>
       <c r="E148" s="1" t="s">
-        <v>476</v>
+        <v>485</v>
       </c>
       <c r="F148" s="1" t="s">
-        <v>193</v>
+        <v>488</v>
       </c>
       <c r="G148" s="1"/>
       <c r="H148" s="1"/>
@@ -9316,13 +9355,13 @@
         <v>269</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>477</v>
+        <v>486</v>
       </c>
       <c r="E149" s="1" t="s">
-        <v>476</v>
+        <v>485</v>
       </c>
       <c r="F149" s="1" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="G149" s="1"/>
       <c r="H149" s="1"/>
@@ -9334,13 +9373,13 @@
         <v>268</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>477</v>
+        <v>486</v>
       </c>
       <c r="E150" s="1" t="s">
-        <v>476</v>
+        <v>485</v>
       </c>
       <c r="F150" s="1" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="G150" s="1"/>
       <c r="H150" s="1"/>
@@ -9585,13 +9624,13 @@
       </c>
       <c r="B168" s="1"/>
       <c r="C168" s="1" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="E168" s="1" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="F168" s="1"/>
       <c r="G168" s="1"/>
@@ -9718,54 +9757,54 @@
     </row>
     <row r="178" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C178" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="D178" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="E178" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="F178" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="G178" s="1" t="s">
         <v>482</v>
       </c>
-      <c r="D178" s="1" t="s">
-        <v>476</v>
-      </c>
-      <c r="E178" s="1" t="s">
+      <c r="H178" s="4" t="s">
         <v>483</v>
-      </c>
-      <c r="F178" s="1" t="s">
-        <v>484</v>
-      </c>
-      <c r="G178" s="1" t="s">
-        <v>485</v>
-      </c>
-      <c r="H178" s="4" t="s">
-        <v>486</v>
       </c>
     </row>
     <row r="179" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C179" s="1" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="D179" s="1" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="E179" s="1"/>
       <c r="F179" s="1"/>
       <c r="G179" s="1" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="H179" s="4" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
     </row>
     <row r="180" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C180" s="1"/>
       <c r="D180" s="1"/>
       <c r="E180" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="F180" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="G180" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="H180" s="4" t="s">
         <v>483</v>
-      </c>
-      <c r="F180" s="1" t="s">
-        <v>484</v>
-      </c>
-      <c r="G180" s="1" t="s">
-        <v>485</v>
-      </c>
-      <c r="H180" s="4" t="s">
-        <v>486</v>
       </c>
     </row>
     <row r="181" spans="1:9" x14ac:dyDescent="0.2">
@@ -9774,38 +9813,38 @@
       <c r="E181" s="1"/>
       <c r="F181" s="1"/>
       <c r="G181" s="1" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="H181" s="4" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
     </row>
     <row r="182" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C182" s="1" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="D182" s="1" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="E182" s="1"/>
       <c r="F182" s="1"/>
       <c r="G182" s="1"/>
       <c r="H182" s="4" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
     </row>
     <row r="183" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C183" s="1"/>
       <c r="D183" s="1"/>
       <c r="E183" s="1" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="F183" s="1" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="G183" s="1"/>
       <c r="H183" s="4" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
     </row>
     <row r="184" spans="1:9" x14ac:dyDescent="0.2">
@@ -9815,7 +9854,7 @@
       <c r="F184" s="1"/>
       <c r="G184" s="1"/>
       <c r="H184" s="4" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
     </row>
     <row r="185" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -9848,7 +9887,7 @@
     </row>
     <row r="188" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C188" s="1" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
     </row>
     <row r="189" spans="1:9" x14ac:dyDescent="0.2">
@@ -9886,7 +9925,7 @@
     </row>
     <row r="193" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C193" s="1" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
     </row>
     <row r="194" spans="3:3" x14ac:dyDescent="0.2">
@@ -9950,19 +9989,19 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>323</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>338</v>
@@ -9970,74 +10009,74 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>187</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>405</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>406</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C5" s="1" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>241</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>187</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>405</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>241</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="8" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B8" s="5" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -10046,10 +10085,10 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>323</v>
@@ -10058,10 +10097,10 @@
         <v>318</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>338</v>
@@ -10069,85 +10108,85 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>408</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>409</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>187</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C11" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>408</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>409</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>241</v>
       </c>
       <c r="F11" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>405</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>187</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>241</v>
       </c>
       <c r="F13" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>405</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B14" s="5" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -10158,19 +10197,19 @@
         <v>225</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>364</v>
-      </c>
       <c r="F15" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="G15" s="2" t="s">
         <v>360</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -10181,16 +10220,16 @@
         <v>187</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>187</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -10201,16 +10240,16 @@
         <v>241</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>241</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -10221,16 +10260,16 @@
         <v>187</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>241</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -10238,16 +10277,16 @@
         <v>241</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>187</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -10270,16 +10309,16 @@
         <v>187</v>
       </c>
       <c r="D21" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>414</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>415</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>187</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="22" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -10295,12 +10334,12 @@
         <v>328</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C24" s="2" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -10310,7 +10349,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C26" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="27" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -10326,7 +10365,7 @@
         <v>330</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>65</v>
@@ -10335,24 +10374,24 @@
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B29" s="1"/>
       <c r="C29" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>419</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B30" s="1"/>
       <c r="D30" s="2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C31" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="32" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -10368,7 +10407,7 @@
         <v>334</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
@@ -10380,18 +10419,18 @@
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B35" s="1"/>
       <c r="C35" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B36" s="1"/>
       <c r="C36" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B37" s="5" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
@@ -10404,12 +10443,12 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C39" s="2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C40" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="41" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
@@ -10420,38 +10459,38 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B43" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B44" s="1"/>
       <c r="C44" s="2" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C45" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="D45" s="2" t="s">
         <v>425</v>
       </c>
-      <c r="D45" s="2" t="s">
-        <v>426</v>
-      </c>
       <c r="E45" s="2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C46" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="D46" s="2" t="s">
         <v>427</v>
       </c>
-      <c r="D46" s="2" t="s">
-        <v>428</v>
-      </c>
       <c r="E46" s="2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="47" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -10467,77 +10506,77 @@
     <row r="49" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B49" s="1"/>
       <c r="C49" s="2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>187</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B50" s="1"/>
       <c r="C50" s="2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>241</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="51" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B51" s="1"/>
       <c r="C51" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F51" s="1" t="s">
         <v>187</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="52" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B52" s="1"/>
       <c r="C52" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F52" s="1" t="s">
         <v>241</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B53" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="54" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B54" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="55" spans="2:7" x14ac:dyDescent="0.2">
@@ -10562,52 +10601,52 @@
     </row>
     <row r="59" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C59" s="2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>187</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="60" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C60" s="2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>241</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="61" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C61" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>187</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="62" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C62" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>241</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="63" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -10634,16 +10673,16 @@
         <v>187</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F65" s="1" t="s">
         <v>187</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="66" spans="2:7" x14ac:dyDescent="0.2">
@@ -10651,16 +10690,16 @@
         <v>241</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F66" s="1" t="s">
         <v>241</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="67" spans="2:7" x14ac:dyDescent="0.2">
@@ -10668,16 +10707,16 @@
         <v>187</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F67" s="1" t="s">
         <v>241</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="68" spans="2:7" x14ac:dyDescent="0.2">
@@ -10685,21 +10724,21 @@
         <v>241</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F68" s="1" t="s">
         <v>187</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="69" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B69" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
@@ -10715,16 +10754,16 @@
         <v>187</v>
       </c>
       <c r="D70" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="E70" s="1" t="s">
         <v>414</v>
-      </c>
-      <c r="E70" s="1" t="s">
-        <v>415</v>
       </c>
       <c r="F70" s="1" t="s">
         <v>187</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="71" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -10734,7 +10773,7 @@
     </row>
     <row r="72" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B72" s="1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>324</v>
@@ -10747,41 +10786,41 @@
     </row>
     <row r="73" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B73" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C73" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="D73" s="2" t="s">
         <v>435</v>
       </c>
-      <c r="D73" s="2" t="s">
+      <c r="F73" s="2" t="s">
         <v>436</v>
-      </c>
-      <c r="F73" s="2" t="s">
-        <v>437</v>
       </c>
     </row>
     <row r="74" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C74" s="2" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D74" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="E74" s="2" t="s">
         <v>438</v>
       </c>
-      <c r="E74" s="2" t="s">
-        <v>439</v>
-      </c>
       <c r="F74" s="2" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="75" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B75" s="5" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D75" s="3"/>
     </row>
     <row r="76" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B76" s="1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>325</v>
@@ -10794,30 +10833,30 @@
     </row>
     <row r="77" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B77" s="1" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C77" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="D77" s="2" t="s">
         <v>435</v>
       </c>
-      <c r="D77" s="2" t="s">
+      <c r="F77" s="2" t="s">
         <v>436</v>
-      </c>
-      <c r="F77" s="2" t="s">
-        <v>437</v>
       </c>
     </row>
     <row r="78" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C78" s="2" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D78" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="E78" s="2" t="s">
         <v>438</v>
       </c>
-      <c r="E78" s="2" t="s">
-        <v>439</v>
-      </c>
       <c r="F78" s="2" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
   </sheetData>
@@ -10836,8 +10875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{988C78EB-4E00-466C-9BD2-B10965380DEB}">
   <dimension ref="A1:I234"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C72" sqref="C72"/>
     </sheetView>
   </sheetViews>
@@ -11814,7 +11853,7 @@
         <v>281</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
@@ -11823,7 +11862,7 @@
         <v>282</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
@@ -11832,7 +11871,7 @@
         <v>283</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
@@ -11841,45 +11880,45 @@
         <v>284</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B88" s="1"/>
       <c r="C88" s="1" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C89" s="1" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="D89" s="1" t="s">
         <v>280</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B90" s="1"/>
       <c r="C90" s="1" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B91" s="1"/>
       <c r="C91" s="1" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="92" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -11909,7 +11948,7 @@
         <v>281</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
@@ -11918,7 +11957,7 @@
         <v>282</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
@@ -11927,7 +11966,7 @@
         <v>283</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.2">
@@ -11935,42 +11974,42 @@
         <v>284</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C98" s="1" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C99" s="1" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C100" s="1" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="D100" s="1" t="s">
         <v>280</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C101" s="1" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="102" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -12872,7 +12911,7 @@
         <v>241</v>
       </c>
       <c r="D199" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E199" s="1" t="s">
         <v>253</v>
@@ -12890,7 +12929,7 @@
         <v>241</v>
       </c>
       <c r="D200" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E200" s="1" t="s">
         <v>253</v>
@@ -12908,7 +12947,7 @@
         <v>187</v>
       </c>
       <c r="D201" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E201" s="1" t="s">
         <v>253</v>
@@ -12925,7 +12964,7 @@
         <v>187</v>
       </c>
       <c r="D202" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E202" s="1" t="s">
         <v>253</v>
@@ -13045,10 +13084,10 @@
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A217" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.2">
@@ -13126,10 +13165,10 @@
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A223" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
mat COPY(L) added one more parameter of swap mode
</commit_message>
<xml_diff>
--- a/P4E_psuedo_instruction_set.xlsx
+++ b/P4E_psuedo_instruction_set.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\P4EngineAssembler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{055754AD-D662-4616-A8F9-7B86428A82FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F022380-F54D-483A-94E6-4A2F1B867676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9290" yWindow="-21710" windowWidth="38620" windowHeight="21820" xr2:uid="{87164962-7B7D-4BAA-98E0-B9A8D7C47112}"/>
+    <workbookView xWindow="-9290" yWindow="-21710" windowWidth="38620" windowHeight="21820" activeTab="1" xr2:uid="{87164962-7B7D-4BAA-98E0-B9A8D7C47112}"/>
   </bookViews>
   <sheets>
     <sheet name="parser" sheetId="1" r:id="rId1"/>
@@ -1006,7 +1006,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C34" authorId="0" shapeId="0" xr:uid="{0C0D1569-05B5-4671-BE18-70994A53B622}">
+    <comment ref="C37" authorId="0" shapeId="0" xr:uid="{0C0D1569-05B5-4671-BE18-70994A53B622}">
       <text>
         <r>
           <rPr>
@@ -1032,7 +1032,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C38" authorId="0" shapeId="0" xr:uid="{B7B4802A-BD39-4EFD-8EF3-BD5110CA966B}">
+    <comment ref="C41" authorId="0" shapeId="0" xr:uid="{B7B4802A-BD39-4EFD-8EF3-BD5110CA966B}">
       <text>
         <r>
           <rPr>
@@ -1058,7 +1058,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G50" authorId="0" shapeId="0" xr:uid="{FFBF8204-87BF-49D9-8007-D8E49DA90F04}">
+    <comment ref="G53" authorId="0" shapeId="0" xr:uid="{FFBF8204-87BF-49D9-8007-D8E49DA90F04}">
       <text>
         <r>
           <rPr>
@@ -1084,7 +1084,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G52" authorId="0" shapeId="0" xr:uid="{DDFC8BEF-8AA7-4999-A858-0492C4F1E09D}">
+    <comment ref="G55" authorId="0" shapeId="0" xr:uid="{DDFC8BEF-8AA7-4999-A858-0492C4F1E09D}">
       <text>
         <r>
           <rPr>
@@ -1110,7 +1110,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F60" authorId="0" shapeId="0" xr:uid="{935D5833-A655-4765-81F8-C6C0E8C143C3}">
+    <comment ref="F63" authorId="0" shapeId="0" xr:uid="{935D5833-A655-4765-81F8-C6C0E8C143C3}">
       <text>
         <r>
           <rPr>
@@ -1136,7 +1136,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F62" authorId="0" shapeId="0" xr:uid="{28896C20-A56E-4FB2-A2DA-D4EEEF5DF3A8}">
+    <comment ref="F65" authorId="0" shapeId="0" xr:uid="{28896C20-A56E-4FB2-A2DA-D4EEEF5DF3A8}">
       <text>
         <r>
           <rPr>
@@ -1162,7 +1162,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D66" authorId="0" shapeId="0" xr:uid="{39D8881B-BC18-434C-A8F7-A45AD42A5267}">
+    <comment ref="D69" authorId="0" shapeId="0" xr:uid="{39D8881B-BC18-434C-A8F7-A45AD42A5267}">
       <text>
         <r>
           <rPr>
@@ -1188,7 +1188,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D68" authorId="0" shapeId="0" xr:uid="{AD6B4964-80AF-492C-A8E5-94AAAA6F6F5F}">
+    <comment ref="D71" authorId="0" shapeId="0" xr:uid="{AD6B4964-80AF-492C-A8E5-94AAAA6F6F5F}">
       <text>
         <r>
           <rPr>
@@ -1411,7 +1411,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1445" uniqueCount="491">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1452" uniqueCount="498">
   <si>
     <t>isr SHiFT</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -6417,6 +6417,34 @@
       </rPr>
       <t xml:space="preserve"> (16 | 32) } ,</t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R16COPYL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R32COPYL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R64COPYL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R16COPY</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R32COPY</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R64COPY</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R128COPYL</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -6880,8 +6908,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA14F7B7-5F50-4FFB-AE20-84853F321386}">
   <dimension ref="A1:I194"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D137" sqref="D137"/>
     </sheetView>
   </sheetViews>
@@ -9945,11 +9973,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{732D935C-EC39-4DBE-84B4-44CD168E0101}">
-  <dimension ref="A1:I78"/>
+  <dimension ref="A1:I85"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B47" sqref="B47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -10291,437 +10319,416 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>61</v>
+        <v>494</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
-      <c r="G20" s="2" t="s">
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B21" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B22" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B23" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="2" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B21" s="6" t="s">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B24" s="6" t="s">
         <v>225</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C24" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D24" s="1" t="s">
         <v>413</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>414</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="F24" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="G21" s="1" t="s">
+      <c r="G24" s="1" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="5" t="s">
+    <row r="25" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="5" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B26" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C26" s="2" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C24" s="2" t="s">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C27" s="2" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C25" s="2" t="s">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C28" s="2" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C26" s="2" t="s">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C29" s="2" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="27" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="5" t="s">
+    <row r="30" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B30" s="5" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B31" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D31" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B29" s="1"/>
-      <c r="C29" s="2" t="s">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B32" s="1"/>
+      <c r="C32" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="D32" s="2" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B30" s="1"/>
-      <c r="D30" s="2" t="s">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B33" s="1"/>
+      <c r="D33" s="2" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C31" s="2" t="s">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C34" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D34" s="2" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="32" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="5" t="s">
+    <row r="35" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B35" s="5" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="2" t="s">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B36" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C36" s="2" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B34" s="1"/>
-      <c r="C34" s="2" t="s">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B37" s="1"/>
+      <c r="C37" s="2" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B35" s="1"/>
-      <c r="C35" s="2" t="s">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B38" s="1"/>
+      <c r="C38" s="2" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B36" s="1"/>
-      <c r="C36" s="2" t="s">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B39" s="1"/>
+      <c r="C39" s="2" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B37" s="5" t="s">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B40" s="5" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B38" s="1" t="s">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B41" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C41" s="2" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C39" s="2" t="s">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C42" s="2" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C40" s="2" t="s">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C43" s="2" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="41" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B42" s="5" t="s">
+    <row r="44" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B45" s="5" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B43" s="1" t="s">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B46" s="1" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B44" s="1"/>
-      <c r="C44" s="2" t="s">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B47" s="1"/>
+      <c r="C47" s="2" t="s">
         <v>424</v>
       </c>
-      <c r="E44" s="2" t="s">
+      <c r="E47" s="2" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C45" s="2" t="s">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C48" s="2" t="s">
         <v>424</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="D48" s="2" t="s">
         <v>425</v>
       </c>
-      <c r="E45" s="2" t="s">
+      <c r="E48" s="2" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C46" s="2" t="s">
+    <row r="49" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C49" s="2" t="s">
         <v>426</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="D49" s="2" t="s">
         <v>427</v>
       </c>
-      <c r="E46" s="2" t="s">
+      <c r="E49" s="2" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="47" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B47" s="5" t="s">
+    <row r="50" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B50" s="5" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B48" s="1" t="s">
+    <row r="51" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B51" s="1" t="s">
         <v>58</v>
-      </c>
-    </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B49" s="1"/>
-      <c r="C49" s="2" t="s">
-        <v>428</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>420</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="G49" s="2" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B50" s="1"/>
-      <c r="C50" s="2" t="s">
-        <v>428</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>420</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="G50" s="2" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B51" s="1"/>
-      <c r="C51" s="2" t="s">
-        <v>430</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>402</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>420</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="G51" s="2" t="s">
-        <v>429</v>
       </c>
     </row>
     <row r="52" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B52" s="1"/>
       <c r="C52" s="2" t="s">
-        <v>430</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>402</v>
+        <v>428</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>420</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>241</v>
+        <v>187</v>
       </c>
       <c r="G52" s="2" t="s">
         <v>429</v>
       </c>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B53" s="1" t="s">
-        <v>379</v>
+      <c r="B53" s="1"/>
+      <c r="C53" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="54" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B54" s="1" t="s">
-        <v>380</v>
+      <c r="B54" s="1"/>
+      <c r="C54" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="55" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B55" s="1" t="s">
-        <v>52</v>
+      <c r="B55" s="1"/>
+      <c r="C55" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="56" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B56" s="1" t="s">
-        <v>53</v>
+        <v>379</v>
       </c>
     </row>
     <row r="57" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B57" s="1" t="s">
-        <v>54</v>
+        <v>380</v>
       </c>
     </row>
     <row r="58" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B58" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="59" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B59" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="60" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B60" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="61" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B61" s="1" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C59" s="2" t="s">
-        <v>428</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="F59" s="2" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C60" s="2" t="s">
-        <v>428</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="F60" s="2" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C61" s="2" t="s">
-        <v>430</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>402</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="F61" s="2" t="s">
-        <v>429</v>
       </c>
     </row>
     <row r="62" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C62" s="2" t="s">
-        <v>430</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>402</v>
+        <v>428</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>241</v>
+        <v>187</v>
       </c>
       <c r="F62" s="2" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="63" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B63" s="5" t="s">
+    <row r="63" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C63" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="64" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C64" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="65" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C65" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="66" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B66" s="5" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="64" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B64" s="1" t="s">
+    <row r="67" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B67" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="C64" s="2" t="s">
+      <c r="C67" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="D64" s="2" t="s">
+      <c r="D67" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E64" s="2" t="s">
+      <c r="E67" s="2" t="s">
         <v>316</v>
-      </c>
-    </row>
-    <row r="65" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C65" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>404</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>431</v>
-      </c>
-      <c r="F65" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="G65" s="1" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="66" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C66" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>404</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>432</v>
-      </c>
-      <c r="F66" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="G66" s="1" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="67" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C67" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>404</v>
-      </c>
-      <c r="E67" s="1" t="s">
-        <v>432</v>
-      </c>
-      <c r="F67" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="G67" s="1" t="s">
-        <v>411</v>
       </c>
     </row>
     <row r="68" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C68" s="1" t="s">
-        <v>241</v>
+        <v>187</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>404</v>
@@ -10737,133 +10744,224 @@
       </c>
     </row>
     <row r="69" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B69" s="1" t="s">
-        <v>391</v>
-      </c>
-      <c r="C69" s="1"/>
-      <c r="D69" s="1"/>
-      <c r="E69" s="1"/>
-      <c r="F69" s="1"/>
-      <c r="G69" s="1"/>
+      <c r="C69" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>411</v>
+      </c>
     </row>
     <row r="70" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B70" s="6" t="s">
-        <v>340</v>
-      </c>
       <c r="C70" s="1" t="s">
         <v>187</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>413</v>
+        <v>404</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>414</v>
+        <v>432</v>
       </c>
       <c r="F70" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="71" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C71" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="F71" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="G70" s="1" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="71" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B71" s="5" t="s">
-        <v>341</v>
+      <c r="G71" s="1" t="s">
+        <v>411</v>
       </c>
     </row>
     <row r="72" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B72" s="1" t="s">
-        <v>381</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="D72" s="11" t="s">
-        <v>325</v>
-      </c>
-      <c r="E72" s="11"/>
-      <c r="F72" s="11"/>
+        <v>491</v>
+      </c>
+      <c r="C72" s="1"/>
+      <c r="D72" s="1"/>
+      <c r="E72" s="1"/>
+      <c r="F72" s="1"/>
+      <c r="G72" s="1"/>
     </row>
     <row r="73" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B73" s="1" t="s">
-        <v>382</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>434</v>
-      </c>
-      <c r="D73" s="2" t="s">
-        <v>435</v>
-      </c>
-      <c r="F73" s="2" t="s">
-        <v>436</v>
-      </c>
+        <v>492</v>
+      </c>
+      <c r="C73" s="1"/>
+      <c r="D73" s="1"/>
+      <c r="E73" s="1"/>
+      <c r="F73" s="1"/>
+      <c r="G73" s="1"/>
     </row>
     <row r="74" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C74" s="2" t="s">
-        <v>434</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>437</v>
-      </c>
-      <c r="E74" s="2" t="s">
-        <v>438</v>
-      </c>
-      <c r="F74" s="2" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="75" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B75" s="5" t="s">
-        <v>385</v>
-      </c>
-      <c r="D75" s="3"/>
+      <c r="B74" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="C74" s="1"/>
+      <c r="D74" s="1"/>
+      <c r="E74" s="1"/>
+      <c r="F74" s="1"/>
+      <c r="G74" s="1"/>
+    </row>
+    <row r="75" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B75" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="C75" s="1"/>
+      <c r="D75" s="1"/>
+      <c r="E75" s="1"/>
+      <c r="F75" s="1"/>
+      <c r="G75" s="1"/>
     </row>
     <row r="76" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B76" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="C76" s="1"/>
+      <c r="D76" s="1"/>
+      <c r="E76" s="1"/>
+      <c r="F76" s="1"/>
+      <c r="G76" s="1"/>
+    </row>
+    <row r="77" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B77" s="6" t="s">
+        <v>340</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="G77" s="1" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="78" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B78" s="5" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="79" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B79" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="D79" s="11" t="s">
+        <v>325</v>
+      </c>
+      <c r="E79" s="11"/>
+      <c r="F79" s="11"/>
+    </row>
+    <row r="80" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B80" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="81" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C81" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="82" spans="2:6" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B82" s="5" t="s">
+        <v>385</v>
+      </c>
+      <c r="D82" s="3"/>
+    </row>
+    <row r="83" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B83" s="1" t="s">
         <v>383</v>
       </c>
-      <c r="C76" s="2" t="s">
+      <c r="C83" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="D76" s="11" t="s">
+      <c r="D83" s="11" t="s">
         <v>324</v>
       </c>
-      <c r="E76" s="11"/>
-      <c r="F76" s="11"/>
-    </row>
-    <row r="77" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B77" s="1" t="s">
+      <c r="E83" s="11"/>
+      <c r="F83" s="11"/>
+    </row>
+    <row r="84" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B84" s="1" t="s">
         <v>384</v>
       </c>
-      <c r="C77" s="2" t="s">
+      <c r="C84" s="2" t="s">
         <v>434</v>
       </c>
-      <c r="D77" s="2" t="s">
+      <c r="D84" s="2" t="s">
         <v>435</v>
       </c>
-      <c r="F77" s="2" t="s">
+      <c r="F84" s="2" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="78" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C78" s="2" t="s">
+    <row r="85" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C85" s="2" t="s">
         <v>434</v>
       </c>
-      <c r="D78" s="1" t="s">
+      <c r="D85" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="E78" s="2" t="s">
+      <c r="E85" s="2" t="s">
         <v>438</v>
       </c>
-      <c r="F78" s="2" t="s">
+      <c r="F85" s="2" t="s">
         <v>436</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="C1:I1"/>
-    <mergeCell ref="D72:F72"/>
-    <mergeCell ref="D76:F76"/>
+    <mergeCell ref="D79:F79"/>
+    <mergeCell ref="D83:F83"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
NXTP(L) added more parameters to accelerate payload calculation
</commit_message>
<xml_diff>
--- a/P4E_psuedo_instruction_set.xlsx
+++ b/P4E_psuedo_instruction_set.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\P4EngineAssembler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F022380-F54D-483A-94E6-4A2F1B867676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0448C6EF-423D-4B2A-B77A-A3C68EB6D1D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9290" yWindow="-21710" windowWidth="38620" windowHeight="21820" activeTab="1" xr2:uid="{87164962-7B7D-4BAA-98E0-B9A8D7C47112}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{87164962-7B7D-4BAA-98E0-B9A8D7C47112}"/>
   </bookViews>
   <sheets>
     <sheet name="parser" sheetId="1" r:id="rId1"/>
@@ -1411,7 +1411,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1452" uniqueCount="498">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1459" uniqueCount="501">
   <si>
     <t>isr SHiFT</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -6445,6 +6445,65 @@
   </si>
   <si>
     <t>R128COPYL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(dest phv to hold igored tail)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">PHV { </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>offset9</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : </t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>len</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (1-4) } </t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -6906,18 +6965,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA14F7B7-5F50-4FFB-AE20-84853F321386}">
-  <dimension ref="A1:I194"/>
+  <dimension ref="A1:I196"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D137" sqref="D137"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A161" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E187" sqref="E187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="37" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.375" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.375" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.625" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21" style="2" bestFit="1" customWidth="1"/>
@@ -9909,61 +9968,89 @@
       <c r="B187" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="C187" s="2" t="s">
+      <c r="C187" s="11" t="s">
+        <v>498</v>
+      </c>
+      <c r="D187" s="11"/>
+      <c r="E187" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="188" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C188" s="1" t="s">
+      <c r="E188" s="1" t="s">
         <v>484</v>
       </c>
     </row>
     <row r="189" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C189" s="2" t="s">
+      <c r="E189" s="2" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="190" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B190" s="10" t="s">
+    <row r="190" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C190" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="D190" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="E190" s="1" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="191" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B191" s="1"/>
+      <c r="C191" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="D191" s="2" t="s">
+        <v>500</v>
+      </c>
+      <c r="E191" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="192" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B192" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="C190" s="3"/>
-      <c r="D190" s="3"/>
-      <c r="E190" s="3"/>
-      <c r="F190" s="3"/>
-      <c r="G190" s="3"/>
-      <c r="H190" s="3"/>
-      <c r="I190" s="3"/>
-    </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A191" s="2" t="s">
+      <c r="C192" s="3"/>
+      <c r="D192" s="3"/>
+      <c r="E192" s="3"/>
+      <c r="F192" s="3"/>
+      <c r="G192" s="3"/>
+      <c r="H192" s="3"/>
+      <c r="I192" s="3"/>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A193" s="2" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A192" s="2" t="s">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A194" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B192" s="1" t="s">
+      <c r="B194" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="C192" s="2" t="s">
+      <c r="C194" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="193" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C193" s="1" t="s">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C195" s="1" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="194" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C194" s="2" t="s">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C196" s="2" t="s">
         <v>190</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="C1:I1"/>
+    <mergeCell ref="C187:D187"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9975,7 +10062,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{732D935C-EC39-4DBE-84B4-44CD168E0101}">
   <dimension ref="A1:I85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B74" sqref="B74"/>
     </sheetView>

</xml_diff>

<commit_message>
deparser counter operating instructions revised
</commit_message>
<xml_diff>
--- a/P4E_psuedo_instruction_set.xlsx
+++ b/P4E_psuedo_instruction_set.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\P4EngineAssembler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B41CBF48-DD4E-4471-ACAB-9CA456BE7088}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B8A8585-1851-4070-9EAD-2C65FE4D6831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-2475" windowWidth="38640" windowHeight="21840" activeTab="2" xr2:uid="{87164962-7B7D-4BAA-98E0-B9A8D7C47112}"/>
   </bookViews>
@@ -1380,7 +1380,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C217" authorId="0" shapeId="0" xr:uid="{DFB4FAA4-43F6-4B75-ABE8-01CB5D2DA0F6}">
+    <comment ref="C225" authorId="0" shapeId="0" xr:uid="{DFB4FAA4-43F6-4B75-ABE8-01CB5D2DA0F6}">
       <text>
         <r>
           <rPr>
@@ -1411,7 +1411,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1487" uniqueCount="505">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1501" uniqueCount="507">
   <si>
     <t>isr SHiFT</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -6520,6 +6520,70 @@
   </si>
   <si>
     <t>ADD data from phv / cond / poff / plen with temp register ( Unsigned )</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PHV {</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> off9 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 32 / 64 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>} ;</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TMP ;</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -11074,11 +11138,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{988C78EB-4E00-466C-9BD2-B10965380DEB}">
-  <dimension ref="A1:I244"/>
+  <dimension ref="A1:I252"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A114" sqref="A114"/>
+      <pane ySplit="1" topLeftCell="A173" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B192" sqref="B192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -13151,445 +13215,518 @@
       <c r="G201" s="1"/>
     </row>
     <row r="202" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A202" s="2" t="s">
+      <c r="C202" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="D202" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="E202" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="F202" s="1"/>
+      <c r="G202" s="1"/>
+    </row>
+    <row r="203" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D203" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="E203" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="F203" s="1"/>
+      <c r="G203" s="1"/>
+    </row>
+    <row r="204" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C204" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="D204" s="1"/>
+      <c r="E204" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="F204" s="1"/>
+      <c r="G204" s="1"/>
+    </row>
+    <row r="205" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C205" s="1"/>
+      <c r="D205" s="1"/>
+      <c r="E205" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="F205" s="1"/>
+      <c r="G205" s="1"/>
+    </row>
+    <row r="206" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A206" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="B202" s="1" t="s">
+      <c r="B206" s="1" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C203" s="1" t="s">
+      <c r="G206" s="1"/>
+    </row>
+    <row r="207" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C207" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="D203" s="1" t="s">
+      <c r="D207" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="F203" s="1" t="s">
+      <c r="F207" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="G203" s="1"/>
-    </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D204" s="1" t="s">
+    </row>
+    <row r="208" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D208" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="F204" s="1" t="s">
+      <c r="F208" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="G204" s="1"/>
-    </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B205" s="1"/>
-      <c r="C205" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="D205" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="F205" s="1" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D206" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="F206" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="G206" s="1"/>
-    </row>
-    <row r="207" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B207" s="5" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A208" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="B208" s="1" t="s">
-        <v>223</v>
-      </c>
+      <c r="G208" s="1"/>
     </row>
     <row r="209" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A209" s="2" t="s">
-        <v>224</v>
-      </c>
       <c r="B209" s="1"/>
       <c r="C209" s="1" t="s">
-        <v>239</v>
+        <v>289</v>
       </c>
       <c r="D209" s="2" t="s">
-        <v>441</v>
-      </c>
-      <c r="E209" s="1" t="s">
-        <v>251</v>
+        <v>190</v>
       </c>
       <c r="F209" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="G209" s="2" t="s">
-        <v>252</v>
-      </c>
+        <v>290</v>
+      </c>
+      <c r="G209" s="1"/>
     </row>
     <row r="210" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B210" s="1"/>
-      <c r="C210" s="1" t="s">
-        <v>239</v>
-      </c>
       <c r="D210" s="2" t="s">
-        <v>441</v>
-      </c>
-      <c r="E210" s="1" t="s">
-        <v>251</v>
+        <v>190</v>
       </c>
       <c r="F210" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="G210" s="2" t="s">
-        <v>252</v>
+        <v>290</v>
       </c>
     </row>
     <row r="211" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B211" s="1"/>
       <c r="C211" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="D211" s="2" t="s">
-        <v>441</v>
-      </c>
-      <c r="E211" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="F211" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="G211" s="2" t="s">
-        <v>252</v>
-      </c>
+        <v>289</v>
+      </c>
+      <c r="D211" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="F211" s="1"/>
     </row>
     <row r="212" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C212" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="D212" s="2" t="s">
-        <v>441</v>
-      </c>
-      <c r="E212" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="F212" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="G212" s="2" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="213" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B213" s="5" t="s">
-        <v>216</v>
-      </c>
+      <c r="D212" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="F212" s="1"/>
+    </row>
+    <row r="213" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C213" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="D213" s="2" t="s">
+        <v>506</v>
+      </c>
+      <c r="F213" s="1"/>
     </row>
     <row r="214" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A214" s="2" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="215" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A215" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="B215" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="C215" s="2" t="s">
-        <v>188</v>
+      <c r="D214" s="2" t="s">
+        <v>506</v>
+      </c>
+      <c r="G214" s="1"/>
+    </row>
+    <row r="215" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B215" s="5" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="216" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A216" s="2" t="s">
-        <v>101</v>
+        <v>223</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>352</v>
-      </c>
-      <c r="C216" s="1" t="s">
-        <v>287</v>
+        <v>223</v>
       </c>
     </row>
     <row r="217" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A217" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="C217" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="218" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B218" s="5" t="s">
-        <v>217</v>
+        <v>224</v>
+      </c>
+      <c r="B217" s="1"/>
+      <c r="C217" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D217" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="E217" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="F217" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="G217" s="2" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="218" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B218" s="1"/>
+      <c r="C218" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D218" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="E218" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="F218" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="G218" s="2" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="219" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A219" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B219" s="1" t="s">
-        <v>61</v>
+      <c r="B219" s="1"/>
+      <c r="C219" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D219" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="E219" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="F219" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="G219" s="2" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="220" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C220" s="2" t="s">
-        <v>188</v>
+      <c r="C220" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D220" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="E220" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="F220" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="G220" s="2" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="221" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B221" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="222" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A222" s="2" t="s">
-        <v>68</v>
+        <v>353</v>
       </c>
     </row>
     <row r="223" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A223" s="2" t="s">
-        <v>69</v>
+        <v>100</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>63</v>
+        <v>351</v>
       </c>
       <c r="C223" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D223" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E223" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F223" s="2" t="s">
-        <v>67</v>
+        <v>188</v>
       </c>
     </row>
     <row r="224" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A224" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B224" s="1" t="s">
+        <v>352</v>
+      </c>
       <c r="C224" s="1" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A225" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B225" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="226" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C226" s="1" t="s">
-        <v>294</v>
+        <v>102</v>
+      </c>
+      <c r="C225" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="226" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B226" s="5" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A227" s="2" t="s">
-        <v>387</v>
+        <v>62</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>385</v>
+        <v>61</v>
       </c>
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A228" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C228" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="D228" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="E228" s="1" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="229" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A229" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="C229" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="D229" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="E229" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="F229" s="1" t="s">
-        <v>305</v>
+      <c r="C228" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="229" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B229" s="5" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C230" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="D230" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="E230" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="F230" s="1" t="s">
-        <v>306</v>
+      <c r="A230" s="2" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C231" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="D231" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="E231" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="F231" s="1" t="s">
-        <v>307</v>
+      <c r="A231" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B231" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C231" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D231" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E231" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F231" s="2" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C232" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="D232" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="E232" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="F232" s="1" t="s">
-        <v>308</v>
+        <v>295</v>
       </c>
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A233" s="2" t="s">
-        <v>387</v>
+        <v>70</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>386</v>
+        <v>64</v>
       </c>
     </row>
     <row r="234" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A234" s="2" t="s">
-        <v>111</v>
-      </c>
       <c r="C234" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="D234" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="E234" s="1" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
     </row>
     <row r="235" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A235" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C235" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="D235" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="E235" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="B235" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="236" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A236" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C236" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="D236" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="E236" s="1" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="237" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A237" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C237" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="D237" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="E237" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="F235" s="1" t="s">
+      <c r="F237" s="1" t="s">
         <v>305</v>
-      </c>
-    </row>
-    <row r="236" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C236" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="D236" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="E236" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="F236" s="1" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="237" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C237" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="D237" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="E237" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="F237" s="1" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="238" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C238" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="D238" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="E238" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="F238" s="1" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="239" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C239" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="D239" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="E239" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="F239" s="1" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="240" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C240" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="D240" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="E240" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="F240" s="1" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="241" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A241" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="B241" s="1" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="242" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A242" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C242" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="D238" s="1" t="s">
+      <c r="D242" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="E238" s="1" t="s">
+      <c r="E242" s="1" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="243" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A243" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C243" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="D243" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="E243" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="F243" s="1" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="244" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C244" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="D244" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="E244" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="F244" s="1" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="245" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C245" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="D245" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="E245" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="F245" s="1" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="246" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C246" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="D246" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="E246" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="F238" s="1" t="s">
+      <c r="F246" s="1" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="239" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B239" s="5" t="s">
+    <row r="247" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B247" s="5" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="240" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A240" s="2" t="s">
+    <row r="248" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A248" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="B240" s="1" t="s">
+      <c r="B248" s="1" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B241" s="1"/>
-      <c r="C241" s="2" t="s">
+    <row r="249" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B249" s="1"/>
+      <c r="C249" s="2" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="242" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B242" s="5" t="s">
+    <row r="250" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B250" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="C242" s="3"/>
-    </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A243" s="2" t="s">
+      <c r="C250" s="3"/>
+    </row>
+    <row r="251" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A251" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B243" s="1" t="s">
+      <c r="B251" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C244" s="2" t="s">
+    <row r="252" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C252" s="2" t="s">
         <v>188</v>
       </c>
     </row>

</xml_diff>

<commit_message>
deparser aligning machine code per source file and code block added
</commit_message>
<xml_diff>
--- a/P4E_psuedo_instruction_set.xlsx
+++ b/P4E_psuedo_instruction_set.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\P4EngineAssembler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B8A8585-1851-4070-9EAD-2C65FE4D6831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4396100-8556-47C9-85DB-DEC240B92611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-2475" windowWidth="38640" windowHeight="21840" activeTab="2" xr2:uid="{87164962-7B7D-4BAA-98E0-B9A8D7C47112}"/>
   </bookViews>
@@ -1411,7 +1411,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1501" uniqueCount="507">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1501" uniqueCount="508">
   <si>
     <t>isr SHiFT</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -6584,6 +6584,23 @@
   </si>
   <si>
     <t>TMP ;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>src_len</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (1-8) } ；</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -11141,8 +11158,8 @@
   <dimension ref="A1:I252"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A173" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B192" sqref="B192"/>
+      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B113" sqref="B113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -12378,7 +12395,7 @@
         <v>269</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>268</v>
+        <v>507</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.2">
@@ -12494,7 +12511,7 @@
         <v>269</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>268</v>
+        <v>507</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
change J/B instructions' CONDR to CNDR
</commit_message>
<xml_diff>
--- a/P4E_psuedo_instruction_set.xlsx
+++ b/P4E_psuedo_instruction_set.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\P4EngineAssembler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8562FDC0-E265-4859-8CF6-6B576BFEF63C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2146E050-9297-44A6-A4DE-C1ADB32A6B60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{87164962-7B7D-4BAA-98E0-B9A8D7C47112}"/>
   </bookViews>
@@ -1359,7 +1359,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1494" uniqueCount="498">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1494" uniqueCount="497">
   <si>
     <t>isr SHiFT</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -3301,23 +3301,6 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> (signed) ,</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>CONDR</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> ;</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -6982,7 +6965,7 @@
         <v>144</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>23</v>
@@ -7000,16 +6983,16 @@
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>169</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -7018,16 +7001,16 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>223</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
@@ -7036,10 +7019,10 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -7065,7 +7048,7 @@
         <v>145</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>24</v>
@@ -7092,25 +7075,25 @@
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>249</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>419</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>420</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>169</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -7119,43 +7102,43 @@
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>249</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>419</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>420</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>223</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>249</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>420</v>
-      </c>
       <c r="G11" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
@@ -7163,67 +7146,67 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>248</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>419</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>420</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>169</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>248</v>
       </c>
       <c r="E13" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>419</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>420</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>223</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>248</v>
       </c>
       <c r="E14" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>420</v>
-      </c>
       <c r="G14" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
@@ -7273,19 +7256,19 @@
         <v>249</v>
       </c>
       <c r="D17" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>419</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>420</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>169</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="I17" s="1"/>
     </row>
@@ -7295,19 +7278,19 @@
         <v>249</v>
       </c>
       <c r="D18" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>419</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>420</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>223</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="I18" s="1"/>
     </row>
@@ -7317,13 +7300,13 @@
         <v>249</v>
       </c>
       <c r="D19" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>420</v>
-      </c>
       <c r="F19" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
@@ -7335,19 +7318,19 @@
         <v>248</v>
       </c>
       <c r="D20" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>419</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>420</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>169</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="I20" s="1"/>
     </row>
@@ -7357,19 +7340,19 @@
         <v>248</v>
       </c>
       <c r="D21" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>419</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>420</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>223</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="I21" s="1"/>
     </row>
@@ -7379,13 +7362,13 @@
         <v>248</v>
       </c>
       <c r="D22" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>420</v>
-      </c>
       <c r="F22" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
@@ -7403,25 +7386,25 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="I24" s="1"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
@@ -7485,19 +7468,19 @@
         <v>249</v>
       </c>
       <c r="D29" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>419</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>420</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>169</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="I29" s="1"/>
     </row>
@@ -7507,19 +7490,19 @@
         <v>249</v>
       </c>
       <c r="D30" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="E30" s="1" t="s">
         <v>419</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>420</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>223</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="I30" s="1"/>
     </row>
@@ -7529,13 +7512,13 @@
         <v>249</v>
       </c>
       <c r="D31" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="E31" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="E31" s="1" t="s">
-        <v>420</v>
-      </c>
       <c r="F31" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
@@ -7547,19 +7530,19 @@
         <v>248</v>
       </c>
       <c r="D32" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="E32" s="1" t="s">
         <v>419</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>420</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>169</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="I32" s="1"/>
     </row>
@@ -7569,19 +7552,19 @@
         <v>248</v>
       </c>
       <c r="D33" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="E33" s="1" t="s">
         <v>419</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>420</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>223</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="I33" s="1"/>
     </row>
@@ -7591,13 +7574,13 @@
         <v>248</v>
       </c>
       <c r="D34" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="E34" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="E34" s="1" t="s">
-        <v>420</v>
-      </c>
       <c r="F34" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
@@ -7615,25 +7598,25 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="I36" s="1"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
@@ -7707,22 +7690,22 @@
         <v>249</v>
       </c>
       <c r="D42" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="E42" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="E42" s="1" t="s">
-        <v>420</v>
-      </c>
       <c r="F42" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>169</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
@@ -7730,22 +7713,22 @@
         <v>249</v>
       </c>
       <c r="D43" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="E43" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="E43" s="1" t="s">
-        <v>420</v>
-      </c>
       <c r="F43" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>223</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
@@ -7753,16 +7736,16 @@
         <v>249</v>
       </c>
       <c r="D44" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="E44" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="E44" s="1" t="s">
-        <v>420</v>
-      </c>
       <c r="F44" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
@@ -7772,22 +7755,22 @@
         <v>248</v>
       </c>
       <c r="D45" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="E45" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="E45" s="1" t="s">
-        <v>420</v>
-      </c>
       <c r="F45" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="G45" s="1" t="s">
         <v>169</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
@@ -7795,22 +7778,22 @@
         <v>248</v>
       </c>
       <c r="D46" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="E46" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="E46" s="1" t="s">
-        <v>420</v>
-      </c>
       <c r="F46" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>223</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
@@ -7818,16 +7801,16 @@
         <v>248</v>
       </c>
       <c r="D47" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="E47" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="E47" s="1" t="s">
-        <v>420</v>
-      </c>
       <c r="F47" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
@@ -7837,10 +7820,10 @@
         <v>249</v>
       </c>
       <c r="D48" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="E48" s="1" t="s">
         <v>419</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>420</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>256</v>
@@ -7849,10 +7832,10 @@
         <v>169</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
@@ -7860,10 +7843,10 @@
         <v>249</v>
       </c>
       <c r="D49" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="E49" s="1" t="s">
         <v>419</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>420</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>256</v>
@@ -7872,10 +7855,10 @@
         <v>223</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
@@ -7883,16 +7866,16 @@
         <v>249</v>
       </c>
       <c r="D50" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="E50" s="1" t="s">
         <v>419</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>420</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>256</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
@@ -7902,10 +7885,10 @@
         <v>248</v>
       </c>
       <c r="D51" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="E51" s="1" t="s">
         <v>419</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>420</v>
       </c>
       <c r="F51" s="1" t="s">
         <v>256</v>
@@ -7914,10 +7897,10 @@
         <v>169</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
@@ -7925,10 +7908,10 @@
         <v>248</v>
       </c>
       <c r="D52" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="E52" s="1" t="s">
         <v>419</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>420</v>
       </c>
       <c r="F52" s="1" t="s">
         <v>256</v>
@@ -7937,10 +7920,10 @@
         <v>223</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
@@ -7948,16 +7931,16 @@
         <v>248</v>
       </c>
       <c r="D53" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="E53" s="1" t="s">
         <v>419</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>420</v>
       </c>
       <c r="F53" s="1" t="s">
         <v>256</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
@@ -7976,10 +7959,10 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>21</v>
@@ -8003,16 +7986,16 @@
       </c>
       <c r="B56" s="1"/>
       <c r="C56" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>169</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="G56" s="1"/>
       <c r="H56" s="1"/>
@@ -8021,16 +8004,16 @@
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B57" s="1"/>
       <c r="C57" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>223</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G57" s="1"/>
       <c r="H57" s="1"/>
@@ -8039,10 +8022,10 @@
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B58" s="1"/>
       <c r="C58" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
@@ -8053,16 +8036,16 @@
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B59" s="1"/>
       <c r="C59" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>169</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="G59" s="1"/>
       <c r="H59" s="1"/>
@@ -8071,16 +8054,16 @@
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B60" s="1"/>
       <c r="C60" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>223</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G60" s="1"/>
       <c r="H60" s="1"/>
@@ -8089,10 +8072,10 @@
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B61" s="1"/>
       <c r="C61" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>
@@ -8103,16 +8086,16 @@
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B62" s="1"/>
       <c r="C62" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>169</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="G62" s="1"/>
       <c r="H62" s="1"/>
@@ -8121,16 +8104,16 @@
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B63" s="1"/>
       <c r="C63" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>223</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G63" s="1"/>
       <c r="H63" s="1"/>
@@ -8139,10 +8122,10 @@
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B64" s="1"/>
       <c r="C64" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E64" s="1"/>
       <c r="F64" s="1"/>
@@ -8153,16 +8136,16 @@
     <row r="65" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B65" s="1"/>
       <c r="C65" s="1" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>169</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="G65" s="1"/>
       <c r="H65" s="1"/>
@@ -8171,16 +8154,16 @@
     <row r="66" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B66" s="1"/>
       <c r="C66" s="1" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>223</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G66" s="1"/>
       <c r="H66" s="1"/>
@@ -8189,10 +8172,10 @@
     <row r="67" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B67" s="1"/>
       <c r="C67" s="1" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E67" s="1"/>
       <c r="F67" s="1"/>
@@ -8203,16 +8186,16 @@
     <row r="68" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B68" s="1"/>
       <c r="C68" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>169</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="G68" s="1"/>
       <c r="H68" s="1"/>
@@ -8221,16 +8204,16 @@
     <row r="69" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B69" s="1"/>
       <c r="C69" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>223</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G69" s="1"/>
       <c r="H69" s="1"/>
@@ -8239,10 +8222,10 @@
     <row r="70" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B70" s="1"/>
       <c r="C70" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E70" s="1"/>
       <c r="F70" s="1"/>
@@ -8253,16 +8236,16 @@
     <row r="71" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B71" s="1"/>
       <c r="C71" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>169</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="G71" s="1"/>
       <c r="H71" s="1"/>
@@ -8271,16 +8254,16 @@
     <row r="72" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B72" s="1"/>
       <c r="C72" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>223</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G72" s="1"/>
       <c r="H72" s="1"/>
@@ -8289,10 +8272,10 @@
     <row r="73" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B73" s="1"/>
       <c r="C73" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E73" s="1"/>
       <c r="F73" s="1"/>
@@ -8303,16 +8286,16 @@
     <row r="74" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B74" s="1"/>
       <c r="C74" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>169</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="G74" s="1"/>
       <c r="H74" s="1"/>
@@ -8321,16 +8304,16 @@
     <row r="75" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B75" s="1"/>
       <c r="C75" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>223</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G75" s="1"/>
       <c r="H75" s="1"/>
@@ -8339,10 +8322,10 @@
     <row r="76" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B76" s="1"/>
       <c r="C76" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E76" s="1"/>
       <c r="F76" s="1"/>
@@ -8353,16 +8336,16 @@
     <row r="77" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B77" s="1"/>
       <c r="C77" s="1" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>169</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="G77" s="1"/>
       <c r="H77" s="1"/>
@@ -8371,16 +8354,16 @@
     <row r="78" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B78" s="1"/>
       <c r="C78" s="1" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>223</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G78" s="1"/>
       <c r="H78" s="1"/>
@@ -8389,10 +8372,10 @@
     <row r="79" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B79" s="1"/>
       <c r="C79" s="1" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E79" s="1"/>
       <c r="F79" s="1"/>
@@ -8403,16 +8386,16 @@
     <row r="80" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B80" s="1"/>
       <c r="C80" s="1" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>169</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="G80" s="1"/>
       <c r="H80" s="1"/>
@@ -8421,16 +8404,16 @@
     <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B81" s="1"/>
       <c r="C81" s="1" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>223</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G81" s="1"/>
       <c r="H81" s="1"/>
@@ -8439,10 +8422,10 @@
     <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B82" s="1"/>
       <c r="C82" s="1" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E82" s="1"/>
       <c r="F82" s="1"/>
@@ -8453,16 +8436,16 @@
     <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B83" s="1"/>
       <c r="C83" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>169</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="G83" s="1"/>
       <c r="H83" s="1"/>
@@ -8471,16 +8454,16 @@
     <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B84" s="1"/>
       <c r="C84" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>223</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G84" s="1"/>
       <c r="H84" s="1"/>
@@ -8489,10 +8472,10 @@
     <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B85" s="1"/>
       <c r="C85" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E85" s="1"/>
       <c r="F85" s="1"/>
@@ -8503,16 +8486,16 @@
     <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B86" s="1"/>
       <c r="C86" s="1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>169</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="G86" s="1"/>
       <c r="H86" s="1"/>
@@ -8521,16 +8504,16 @@
     <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B87" s="1"/>
       <c r="C87" s="1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>223</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G87" s="1"/>
       <c r="H87" s="1"/>
@@ -8539,10 +8522,10 @@
     <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B88" s="1"/>
       <c r="C88" s="1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E88" s="1"/>
       <c r="F88" s="1"/>
@@ -8553,16 +8536,16 @@
     <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B89" s="1"/>
       <c r="C89" s="1" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D89" s="1" t="s">
         <v>169</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="G89" s="1"/>
       <c r="H89" s="1"/>
@@ -8571,16 +8554,16 @@
     <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B90" s="1"/>
       <c r="C90" s="1" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>223</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G90" s="1"/>
       <c r="H90" s="1"/>
@@ -8589,10 +8572,10 @@
     <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B91" s="1"/>
       <c r="C91" s="1" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E91" s="1"/>
       <c r="F91" s="1"/>
@@ -8643,11 +8626,11 @@
     <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B95" s="1"/>
       <c r="C95" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D95" s="1"/>
       <c r="E95" s="1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="G95" s="1"/>
       <c r="H95" s="1"/>
@@ -8656,13 +8639,13 @@
     <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B96" s="1"/>
       <c r="C96" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="E96" s="1" t="s">
         <v>433</v>
-      </c>
-      <c r="D96" s="1" t="s">
-        <v>435</v>
-      </c>
-      <c r="E96" s="1" t="s">
-        <v>434</v>
       </c>
       <c r="G96" s="1"/>
       <c r="H96" s="1"/>
@@ -8685,11 +8668,11 @@
     <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B98" s="1"/>
       <c r="C98" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D98" s="1"/>
       <c r="E98" s="1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="G98" s="1"/>
       <c r="H98" s="1"/>
@@ -8698,13 +8681,13 @@
     <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B99" s="1"/>
       <c r="C99" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="E99" s="1" t="s">
         <v>433</v>
-      </c>
-      <c r="D99" s="1" t="s">
-        <v>435</v>
-      </c>
-      <c r="E99" s="1" t="s">
-        <v>434</v>
       </c>
       <c r="G99" s="1"/>
       <c r="H99" s="1"/>
@@ -8761,7 +8744,7 @@
     <row r="104" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B104" s="1"/>
       <c r="C104" s="1" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D104" s="1"/>
       <c r="E104" s="1"/>
@@ -8821,7 +8804,7 @@
     <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B109" s="1"/>
       <c r="C109" s="1" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D109" s="1"/>
       <c r="E109" s="1"/>
@@ -8895,7 +8878,7 @@
         <v>32</v>
       </c>
       <c r="E114" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="F114" s="1"/>
       <c r="G114" s="1"/>
@@ -8915,7 +8898,7 @@
     <row r="116" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B116" s="1"/>
       <c r="C116" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D116" s="1"/>
       <c r="F116" s="1"/>
@@ -8926,7 +8909,7 @@
     <row r="117" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B117" s="1"/>
       <c r="D117" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G117" s="1"/>
       <c r="H117" s="1"/>
@@ -8953,10 +8936,10 @@
     <row r="120" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B120" s="1"/>
       <c r="C120" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G120" s="1"/>
       <c r="H120" s="1"/>
@@ -8965,7 +8948,7 @@
     <row r="121" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B121" s="1"/>
       <c r="C121" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="D121" s="1" t="s">
         <v>244</v>
@@ -8977,7 +8960,7 @@
     <row r="122" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B122" s="1"/>
       <c r="C122" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="D122" s="1" t="s">
         <v>246</v>
@@ -8989,11 +8972,11 @@
     <row r="123" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B123" s="1"/>
       <c r="C123" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D123" s="1"/>
       <c r="E123" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G123" s="1"/>
       <c r="H123" s="1"/>
@@ -9002,13 +8985,13 @@
     <row r="124" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B124" s="1"/>
       <c r="C124" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="E124" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G124" s="1"/>
       <c r="H124" s="1"/>
@@ -9017,13 +9000,13 @@
     <row r="125" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B125" s="1"/>
       <c r="C125" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E125" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G125" s="1"/>
       <c r="H125" s="1"/>
@@ -9032,13 +9015,13 @@
     <row r="126" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B126" s="1"/>
       <c r="C126" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="E126" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G126" s="1"/>
       <c r="H126" s="1"/>
@@ -9080,10 +9063,10 @@
     <row r="129" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B129" s="1"/>
       <c r="C129" s="1" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="F129" s="1"/>
       <c r="G129" s="1"/>
@@ -9093,10 +9076,10 @@
     <row r="130" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B130" s="1"/>
       <c r="C130" s="1" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="F130" s="1"/>
       <c r="G130" s="1"/>
@@ -9106,13 +9089,13 @@
     <row r="131" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B131" s="1"/>
       <c r="C131" s="1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="F131" s="1"/>
       <c r="G131" s="1"/>
@@ -9122,10 +9105,10 @@
     <row r="132" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B132" s="1"/>
       <c r="C132" s="1" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="F132" s="1"/>
       <c r="G132" s="1"/>
@@ -9170,7 +9153,7 @@
         <v>21</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="E135" s="2" t="s">
         <v>22</v>
@@ -9188,13 +9171,13 @@
         <v>169</v>
       </c>
       <c r="D136" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="E136" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="F136" s="1" t="s">
         <v>458</v>
-      </c>
-      <c r="E136" s="1" t="s">
-        <v>461</v>
-      </c>
-      <c r="F136" s="1" t="s">
-        <v>459</v>
       </c>
       <c r="G136" s="1"/>
       <c r="H136" s="1"/>
@@ -9206,13 +9189,13 @@
         <v>249</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="F137" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="G137" s="1"/>
       <c r="H137" s="1"/>
@@ -9224,13 +9207,13 @@
         <v>248</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="F138" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="G138" s="1"/>
       <c r="H138" s="1"/>
@@ -9274,7 +9257,7 @@
         <v>21</v>
       </c>
       <c r="D141" s="2" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="E141" s="2" t="s">
         <v>22</v>
@@ -9292,10 +9275,10 @@
         <v>169</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="F142" s="1" t="s">
         <v>175</v>
@@ -9310,13 +9293,13 @@
         <v>249</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="E143" s="1" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="F143" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="G143" s="1"/>
       <c r="H143" s="1"/>
@@ -9328,13 +9311,13 @@
         <v>248</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="E144" s="1" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="F144" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="G144" s="1"/>
       <c r="H144" s="1"/>
@@ -9373,7 +9356,7 @@
         <v>21</v>
       </c>
       <c r="D147" s="2" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="E147" s="2" t="s">
         <v>22</v>
@@ -9390,13 +9373,13 @@
         <v>169</v>
       </c>
       <c r="D148" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="E148" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="F148" s="1" t="s">
         <v>458</v>
-      </c>
-      <c r="E148" s="1" t="s">
-        <v>456</v>
-      </c>
-      <c r="F148" s="1" t="s">
-        <v>459</v>
       </c>
       <c r="G148" s="1"/>
       <c r="H148" s="1"/>
@@ -9408,13 +9391,13 @@
         <v>249</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="E149" s="1" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="F149" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="G149" s="1"/>
       <c r="H149" s="1"/>
@@ -9426,13 +9409,13 @@
         <v>248</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="E150" s="1" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="F150" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="G150" s="1"/>
       <c r="H150" s="1"/>
@@ -9581,7 +9564,7 @@
         <v>7</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C162" s="1"/>
       <c r="D162" s="1"/>
@@ -9596,7 +9579,7 @@
         <v>8</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="C163" s="1"/>
       <c r="D163" s="1"/>
@@ -9611,7 +9594,7 @@
         <v>9</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C164" s="1"/>
       <c r="D164" s="1"/>
@@ -9626,7 +9609,7 @@
         <v>247</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C165" s="1"/>
       <c r="D165" s="1"/>
@@ -9641,7 +9624,7 @@
         <v>10</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C166" s="1"/>
       <c r="D166" s="1"/>
@@ -9656,7 +9639,7 @@
         <v>11</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="C167" s="2" t="s">
         <v>35</v>
@@ -9673,17 +9656,17 @@
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A168" s="2" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B168" s="1"/>
       <c r="C168" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="D168" s="1" t="s">
         <v>447</v>
       </c>
-      <c r="D168" s="1" t="s">
+      <c r="E168" s="1" t="s">
         <v>448</v>
-      </c>
-      <c r="E168" s="1" t="s">
-        <v>449</v>
       </c>
       <c r="F168" s="1"/>
       <c r="G168" s="1"/>
@@ -9735,54 +9718,54 @@
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C172" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="D172" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="E172" s="1" t="s">
         <v>450</v>
       </c>
-      <c r="D172" s="1" t="s">
-        <v>445</v>
-      </c>
-      <c r="E172" s="1" t="s">
+      <c r="F172" s="1" t="s">
         <v>451</v>
       </c>
-      <c r="F172" s="1" t="s">
+      <c r="G172" s="1" t="s">
         <v>452</v>
       </c>
-      <c r="G172" s="1" t="s">
+      <c r="H172" s="4" t="s">
         <v>453</v>
-      </c>
-      <c r="H172" s="4" t="s">
-        <v>454</v>
       </c>
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C173" s="1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E173" s="1"/>
       <c r="F173" s="1"/>
       <c r="G173" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="H173" s="4" t="s">
         <v>453</v>
-      </c>
-      <c r="H173" s="4" t="s">
-        <v>454</v>
       </c>
     </row>
     <row r="174" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C174" s="1"/>
       <c r="D174" s="1"/>
       <c r="E174" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="F174" s="1" t="s">
         <v>451</v>
       </c>
-      <c r="F174" s="1" t="s">
+      <c r="G174" s="1" t="s">
         <v>452</v>
       </c>
-      <c r="G174" s="1" t="s">
+      <c r="H174" s="4" t="s">
         <v>453</v>
-      </c>
-      <c r="H174" s="4" t="s">
-        <v>454</v>
       </c>
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.2">
@@ -9791,38 +9774,38 @@
       <c r="E175" s="1"/>
       <c r="F175" s="1"/>
       <c r="G175" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="H175" s="4" t="s">
         <v>453</v>
-      </c>
-      <c r="H175" s="4" t="s">
-        <v>454</v>
       </c>
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C176" s="1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E176" s="1"/>
       <c r="F176" s="1"/>
       <c r="G176" s="1"/>
       <c r="H176" s="4" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C177" s="1"/>
       <c r="D177" s="1"/>
       <c r="E177" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="F177" s="1" t="s">
         <v>451</v>
-      </c>
-      <c r="F177" s="1" t="s">
-        <v>452</v>
       </c>
       <c r="G177" s="1"/>
       <c r="H177" s="4" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="178" spans="1:9" x14ac:dyDescent="0.2">
@@ -9832,7 +9815,7 @@
       <c r="F178" s="1"/>
       <c r="G178" s="1"/>
       <c r="H178" s="4" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="179" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -9854,13 +9837,13 @@
     </row>
     <row r="181" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A181" s="2" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="C181" s="11" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="D181" s="11"/>
       <c r="E181" s="2" t="s">
@@ -9869,7 +9852,7 @@
     </row>
     <row r="182" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E182" s="1" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="183" spans="1:9" x14ac:dyDescent="0.2">
@@ -9879,22 +9862,22 @@
     </row>
     <row r="184" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C184" s="2" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="D184" s="2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="E184" s="1" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="185" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B185" s="1"/>
       <c r="C185" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="D185" s="2" t="s">
         <v>470</v>
-      </c>
-      <c r="D185" s="2" t="s">
-        <v>471</v>
       </c>
       <c r="E185" s="2" t="s">
         <v>172</v>
@@ -9919,10 +9902,10 @@
     </row>
     <row r="188" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A188" s="2" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="C188" s="2" t="s">
         <v>19</v>
@@ -9930,7 +9913,7 @@
     </row>
     <row r="189" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C189" s="1" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="190" spans="1:9" x14ac:dyDescent="0.2">
@@ -9990,99 +9973,99 @@
     </row>
     <row r="2" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B2" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>169</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>376</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>377</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C5" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>223</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>169</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>376</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>223</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="8" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B8" s="5" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -10091,191 +10074,191 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>379</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>380</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>169</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C11" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>379</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>380</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>223</v>
       </c>
       <c r="F11" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>376</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>169</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>223</v>
       </c>
       <c r="F13" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>376</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B14" s="5" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>207</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>335</v>
-      </c>
       <c r="F15" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="G15" s="2" t="s">
         <v>331</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>169</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>169</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>223</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>223</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>169</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>223</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -10283,21 +10266,21 @@
         <v>223</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>169</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -10307,7 +10290,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -10317,7 +10300,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -10345,37 +10328,37 @@
         <v>169</v>
       </c>
       <c r="D24" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>385</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>386</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>169</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="25" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B25" s="5" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>300</v>
-      </c>
       <c r="C26" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C27" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -10385,23 +10368,23 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C29" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="30" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B30" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>302</v>
-      </c>
       <c r="C31" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>63</v>
@@ -10410,40 +10393,40 @@
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B32" s="1"/>
       <c r="C32" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="D32" s="2" t="s">
         <v>390</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>391</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B33" s="1"/>
       <c r="D33" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C34" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="35" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B35" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>306</v>
-      </c>
       <c r="C36" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
@@ -10455,23 +10438,23 @@
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B38" s="1"/>
       <c r="C38" s="2" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B39" s="1"/>
       <c r="C39" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B40" s="5" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B41" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>172</v>
@@ -10479,59 +10462,59 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C42" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C43" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="44" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="45" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B45" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B46" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B47" s="1"/>
       <c r="C47" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C48" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="D48" s="2" t="s">
         <v>396</v>
       </c>
-      <c r="D48" s="2" t="s">
-        <v>397</v>
-      </c>
       <c r="E48" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C49" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="D49" s="2" t="s">
         <v>398</v>
       </c>
-      <c r="D49" s="2" t="s">
-        <v>399</v>
-      </c>
       <c r="E49" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="50" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B50" s="5" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="51" spans="2:7" x14ac:dyDescent="0.2">
@@ -10542,77 +10525,77 @@
     <row r="52" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B52" s="1"/>
       <c r="C52" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F52" s="1" t="s">
         <v>169</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B53" s="1"/>
       <c r="C53" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F53" s="1" t="s">
         <v>223</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="54" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B54" s="1"/>
       <c r="C54" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F54" s="1" t="s">
         <v>169</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="55" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B55" s="1"/>
       <c r="C55" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>223</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="56" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B56" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="57" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B57" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="58" spans="2:7" x14ac:dyDescent="0.2">
@@ -10637,71 +10620,71 @@
     </row>
     <row r="62" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C62" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>169</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="63" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C63" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>223</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="64" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C64" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>169</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="65" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C65" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>223</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="66" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B66" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="67" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B67" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>34</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="68" spans="2:7" x14ac:dyDescent="0.2">
@@ -10709,16 +10692,16 @@
         <v>169</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="F68" s="1" t="s">
         <v>169</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="69" spans="2:7" x14ac:dyDescent="0.2">
@@ -10726,16 +10709,16 @@
         <v>223</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="F69" s="1" t="s">
         <v>223</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="70" spans="2:7" x14ac:dyDescent="0.2">
@@ -10743,16 +10726,16 @@
         <v>169</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="F70" s="1" t="s">
         <v>223</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="71" spans="2:7" x14ac:dyDescent="0.2">
@@ -10760,21 +10743,21 @@
         <v>223</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="F71" s="1" t="s">
         <v>169</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="72" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B72" s="1" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
@@ -10784,7 +10767,7 @@
     </row>
     <row r="73" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B73" s="1" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
@@ -10794,7 +10777,7 @@
     </row>
     <row r="74" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B74" s="1" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
@@ -10804,7 +10787,7 @@
     </row>
     <row r="75" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B75" s="1" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
@@ -10814,7 +10797,7 @@
     </row>
     <row r="76" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B76" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
@@ -10824,115 +10807,115 @@
     </row>
     <row r="77" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B77" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>169</v>
       </c>
       <c r="D77" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="E77" s="1" t="s">
         <v>385</v>
-      </c>
-      <c r="E77" s="1" t="s">
-        <v>386</v>
       </c>
       <c r="F77" s="1" t="s">
         <v>169</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="78" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B78" s="5" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="79" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B79" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C79" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="D79" s="11" t="s">
         <v>296</v>
-      </c>
-      <c r="D79" s="11" t="s">
-        <v>297</v>
       </c>
       <c r="E79" s="11"/>
       <c r="F79" s="11"/>
     </row>
     <row r="80" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B80" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C80" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="D80" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="D80" s="2" t="s">
+      <c r="F80" s="2" t="s">
         <v>407</v>
-      </c>
-      <c r="F80" s="2" t="s">
-        <v>408</v>
       </c>
     </row>
     <row r="81" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C81" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D81" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="E81" s="2" t="s">
         <v>409</v>
       </c>
-      <c r="E81" s="2" t="s">
-        <v>410</v>
-      </c>
       <c r="F81" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="82" spans="2:6" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B82" s="5" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D82" s="3"/>
     </row>
     <row r="83" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B83" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D83" s="11" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E83" s="11"/>
       <c r="F83" s="11"/>
     </row>
     <row r="84" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B84" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C84" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="D84" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="D84" s="2" t="s">
+      <c r="F84" s="2" t="s">
         <v>407</v>
-      </c>
-      <c r="F84" s="2" t="s">
-        <v>408</v>
       </c>
     </row>
     <row r="85" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C85" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D85" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="E85" s="2" t="s">
         <v>409</v>
       </c>
-      <c r="E85" s="2" t="s">
-        <v>410</v>
-      </c>
       <c r="F85" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
   </sheetData>
@@ -10952,8 +10935,8 @@
   <dimension ref="A1:I252"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D112" sqref="D112"/>
+      <pane ySplit="1" topLeftCell="A221" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E236" sqref="E236"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -11929,72 +11912,72 @@
         <v>256</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B85" s="1"/>
       <c r="C85" s="1" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B86" s="1"/>
       <c r="C86" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B87" s="1"/>
       <c r="C87" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B88" s="1"/>
       <c r="C88" s="1" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C89" s="1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B90" s="1"/>
       <c r="C90" s="1" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B91" s="1"/>
       <c r="C91" s="1" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="92" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -12024,68 +12007,68 @@
         <v>256</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B95" s="1"/>
       <c r="C95" s="1" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B96" s="1"/>
       <c r="C96" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C97" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C98" s="1" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C99" s="1" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C100" s="1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C101" s="1" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="102" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -12095,7 +12078,7 @@
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>209</v>
@@ -12121,7 +12104,7 @@
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="C104" s="2" t="s">
         <v>174</v>
@@ -12139,7 +12122,7 @@
         <v>252</v>
       </c>
       <c r="H104" s="1" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.2">
@@ -12147,7 +12130,7 @@
         <v>174</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.2">
@@ -12155,7 +12138,7 @@
         <v>174</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.2">
@@ -12163,21 +12146,21 @@
         <v>174</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="D108" s="1"/>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="C109" s="2" t="s">
         <v>174</v>
@@ -12189,7 +12172,7 @@
         <v>251</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.2">
@@ -12197,7 +12180,7 @@
         <v>174</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.2">
@@ -12205,7 +12188,7 @@
         <v>174</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.2">
@@ -12213,7 +12196,7 @@
         <v>174</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="113" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -12224,7 +12207,7 @@
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>210</v>
@@ -12233,7 +12216,7 @@
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B115" s="1"/>
       <c r="C115" s="2" t="s">
@@ -12252,7 +12235,7 @@
         <v>252</v>
       </c>
       <c r="H115" s="1" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.2">
@@ -12261,7 +12244,7 @@
         <v>174</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.2">
@@ -12270,7 +12253,7 @@
         <v>174</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.2">
@@ -12279,21 +12262,21 @@
         <v>174</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A119" s="2" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="D119" s="1"/>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="C120" s="2" t="s">
         <v>174</v>
@@ -12305,7 +12288,7 @@
         <v>251</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.2">
@@ -12313,7 +12296,7 @@
         <v>174</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.2">
@@ -12321,7 +12304,7 @@
         <v>174</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.2">
@@ -12329,7 +12312,7 @@
         <v>174</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="124" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -12402,7 +12385,7 @@
     </row>
     <row r="132" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B132" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C132" s="2" t="s">
         <v>227</v>
@@ -12435,7 +12418,7 @@
     </row>
     <row r="135" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B135" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C135" s="1"/>
       <c r="D135" s="1"/>
@@ -12457,12 +12440,12 @@
     </row>
     <row r="138" spans="2:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B138" s="5" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="139" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B139" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C139" s="2" t="s">
         <v>227</v>
@@ -12487,7 +12470,7 @@
     </row>
     <row r="141" spans="2:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B141" s="5" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C141" s="3"/>
       <c r="D141" s="3"/>
@@ -12495,7 +12478,7 @@
     </row>
     <row r="142" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B142" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C142" s="1"/>
       <c r="D142" s="1"/>
@@ -12527,12 +12510,12 @@
     </row>
     <row r="147" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B147" s="6" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="148" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B148" s="6" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="149" spans="2:6" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -12547,12 +12530,12 @@
     </row>
     <row r="151" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B151" s="6" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="152" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B152" s="6" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="153" spans="2:6" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -12567,12 +12550,12 @@
     </row>
     <row r="155" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B155" s="6" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="156" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B156" s="6" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C156" s="1" t="s">
         <v>169</v>
@@ -13033,7 +13016,7 @@
         <v>268</v>
       </c>
       <c r="E202" s="1" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="F202" s="1"/>
       <c r="G202" s="1"/>
@@ -13043,7 +13026,7 @@
         <v>268</v>
       </c>
       <c r="E203" s="1" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="F203" s="1"/>
       <c r="G203" s="1"/>
@@ -13054,7 +13037,7 @@
       </c>
       <c r="D204" s="1"/>
       <c r="E204" s="1" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="F204" s="1"/>
       <c r="G204" s="1"/>
@@ -13063,7 +13046,7 @@
       <c r="C205" s="1"/>
       <c r="D205" s="1"/>
       <c r="E205" s="1" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="F205" s="1"/>
       <c r="G205" s="1"/>
@@ -13123,13 +13106,13 @@
         <v>264</v>
       </c>
       <c r="D211" s="1" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="F211" s="1"/>
     </row>
     <row r="212" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D212" s="1" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="F212" s="1"/>
     </row>
@@ -13138,13 +13121,13 @@
         <v>264</v>
       </c>
       <c r="D213" s="2" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="F213" s="1"/>
     </row>
     <row r="214" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D214" s="2" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G214" s="1"/>
     </row>
@@ -13170,7 +13153,7 @@
         <v>223</v>
       </c>
       <c r="D217" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E217" s="1" t="s">
         <v>235</v>
@@ -13188,7 +13171,7 @@
         <v>223</v>
       </c>
       <c r="D218" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E218" s="1" t="s">
         <v>235</v>
@@ -13206,7 +13189,7 @@
         <v>169</v>
       </c>
       <c r="D219" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E219" s="1" t="s">
         <v>235</v>
@@ -13223,7 +13206,7 @@
         <v>169</v>
       </c>
       <c r="D220" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E220" s="1" t="s">
         <v>235</v>
@@ -13242,7 +13225,7 @@
     </row>
     <row r="222" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A222" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="223" spans="1:7" x14ac:dyDescent="0.2">
@@ -13250,7 +13233,7 @@
         <v>98</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C223" s="2" t="s">
         <v>172</v>
@@ -13261,7 +13244,7 @@
         <v>99</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C224" s="1" t="s">
         <v>262</v>
@@ -13343,10 +13326,10 @@
     </row>
     <row r="235" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A235" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="236" spans="1:6" x14ac:dyDescent="0.2">
@@ -13360,7 +13343,7 @@
         <v>273</v>
       </c>
       <c r="E236" s="1" t="s">
-        <v>275</v>
+        <v>496</v>
       </c>
     </row>
     <row r="237" spans="1:6" x14ac:dyDescent="0.2">
@@ -13374,10 +13357,10 @@
         <v>273</v>
       </c>
       <c r="E237" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F237" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="238" spans="1:6" x14ac:dyDescent="0.2">
@@ -13388,10 +13371,10 @@
         <v>273</v>
       </c>
       <c r="E238" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F238" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="239" spans="1:6" x14ac:dyDescent="0.2">
@@ -13402,10 +13385,10 @@
         <v>273</v>
       </c>
       <c r="E239" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F239" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="240" spans="1:6" x14ac:dyDescent="0.2">
@@ -13416,18 +13399,18 @@
         <v>273</v>
       </c>
       <c r="E240" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F240" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="241" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A241" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B241" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="242" spans="1:6" x14ac:dyDescent="0.2">
@@ -13441,7 +13424,7 @@
         <v>274</v>
       </c>
       <c r="E242" s="1" t="s">
-        <v>275</v>
+        <v>496</v>
       </c>
     </row>
     <row r="243" spans="1:6" x14ac:dyDescent="0.2">
@@ -13455,10 +13438,10 @@
         <v>274</v>
       </c>
       <c r="E243" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F243" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="244" spans="1:6" x14ac:dyDescent="0.2">
@@ -13469,10 +13452,10 @@
         <v>274</v>
       </c>
       <c r="E244" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F244" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="245" spans="1:6" x14ac:dyDescent="0.2">
@@ -13483,10 +13466,10 @@
         <v>274</v>
       </c>
       <c r="E245" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F245" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="246" spans="1:6" x14ac:dyDescent="0.2">
@@ -13497,10 +13480,10 @@
         <v>274</v>
       </c>
       <c r="E246" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F246" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="247" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
added NXTPNFL instruction for setting not_final flag
</commit_message>
<xml_diff>
--- a/P4E_psuedo_instruction_set.xlsx
+++ b/P4E_psuedo_instruction_set.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\P4EngineAssembler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{568F4A66-2214-4EAE-9697-EB6A709F1810}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7529F553-9F64-441F-96C2-14A3D6235ACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{87164962-7B7D-4BAA-98E0-B9A8D7C47112}"/>
+    <workbookView xWindow="28680" yWindow="-2475" windowWidth="38640" windowHeight="21840" xr2:uid="{87164962-7B7D-4BAA-98E0-B9A8D7C47112}"/>
   </bookViews>
   <sheets>
     <sheet name="parser" sheetId="1" r:id="rId1"/>
@@ -1697,7 +1697,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1792" uniqueCount="509">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1793" uniqueCount="509">
   <si>
     <t>isr SHiFT</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -6495,6 +6495,20 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">0b00xxxxxx </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(x = 0/1)</t>
+    </r>
+    <r>
       <rPr>
         <b/>
         <sz val="11"/>
@@ -6504,35 +6518,73 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>len</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (1-4) } </t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">0b00xxxxxx </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(x = 0/1)</t>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>0b00xxxxxx</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (x = 0/1) ,</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADDTU</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">    result put back to  phv / cond / poff / plen</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">    result put back to temp register</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADDT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADD data from phv / cond / poff / plen with temp register</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADD data from phv / cond / poff / plen with temp register ( Unsigned )</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PHV {</t>
     </r>
     <r>
       <rPr>
@@ -6544,73 +6596,18 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>,</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>0b00xxxxxx</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (x = 0/1) ,</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ADDTU</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">    result put back to  phv / cond / poff / plen</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">    result put back to temp register</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ADDT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ADD data from phv / cond / poff / plen with temp register</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ADD data from phv / cond / poff / plen with temp register ( Unsigned )</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>PHV {</t>
+      <t xml:space="preserve"> off9 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:</t>
     </r>
     <r>
       <rPr>
@@ -6622,29 +6619,6 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> off9 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
       <t xml:space="preserve"> 32 / 64 </t>
     </r>
     <r>
@@ -6839,6 +6813,10 @@
   </si>
   <si>
     <t>delay [ 1 ] ,</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NXTPNFL</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -6978,7 +6956,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -7012,27 +6990,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -7056,6 +7013,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7391,11 +7351,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA14F7B7-5F50-4FFB-AE20-84853F321386}">
-  <dimension ref="A1:I210"/>
+  <dimension ref="A1:I211"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A171" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F114" sqref="F114:F123"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A158" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B206" sqref="B206"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -7419,15 +7379,15 @@
       <c r="B1" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
     </row>
     <row r="2" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B2" s="10" t="s">
@@ -9358,7 +9318,7 @@
         <v>363</v>
       </c>
       <c r="F114" s="2" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="G114" s="1"/>
       <c r="H114" s="1"/>
@@ -9379,7 +9339,7 @@
         <v>172</v>
       </c>
       <c r="F116" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="G116" s="1"/>
       <c r="H116" s="1"/>
@@ -9432,7 +9392,7 @@
         <v>437</v>
       </c>
       <c r="F121" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="G121" s="1"/>
       <c r="H121" s="1"/>
@@ -9444,7 +9404,7 @@
         <v>244</v>
       </c>
       <c r="F122" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="G122" s="1"/>
       <c r="H122" s="1"/>
@@ -9456,7 +9416,7 @@
         <v>246</v>
       </c>
       <c r="F123" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="G123" s="1"/>
       <c r="H123" s="1"/>
@@ -9621,7 +9581,7 @@
         <v>412</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="E135" s="1" t="s">
         <v>443</v>
@@ -9691,10 +9651,10 @@
         <v>176</v>
       </c>
       <c r="G139" s="2" t="s">
+        <v>496</v>
+      </c>
+      <c r="H139" s="2" t="s">
         <v>497</v>
-      </c>
-      <c r="H139" s="2" t="s">
-        <v>498</v>
       </c>
       <c r="I139" s="1"/>
     </row>
@@ -9764,10 +9724,10 @@
         <v>458</v>
       </c>
       <c r="G143" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="H143" s="2" t="s">
         <v>500</v>
-      </c>
-      <c r="H143" s="2" t="s">
-        <v>501</v>
       </c>
       <c r="I143" s="1"/>
     </row>
@@ -9786,10 +9746,10 @@
         <v>445</v>
       </c>
       <c r="G144" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="H144" s="2" t="s">
         <v>500</v>
-      </c>
-      <c r="H144" s="2" t="s">
-        <v>501</v>
       </c>
       <c r="I144" s="1"/>
     </row>
@@ -9808,10 +9768,10 @@
         <v>445</v>
       </c>
       <c r="G145" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="H145" s="2" t="s">
         <v>500</v>
-      </c>
-      <c r="H145" s="2" t="s">
-        <v>501</v>
       </c>
       <c r="I145" s="1"/>
     </row>
@@ -9862,10 +9822,10 @@
         <v>176</v>
       </c>
       <c r="G148" s="2" t="s">
+        <v>496</v>
+      </c>
+      <c r="H148" s="2" t="s">
         <v>497</v>
-      </c>
-      <c r="H148" s="2" t="s">
-        <v>498</v>
       </c>
       <c r="I148" s="1"/>
     </row>
@@ -9935,10 +9895,10 @@
         <v>175</v>
       </c>
       <c r="G152" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="H152" s="2" t="s">
         <v>500</v>
-      </c>
-      <c r="H152" s="2" t="s">
-        <v>501</v>
       </c>
       <c r="I152" s="1"/>
     </row>
@@ -9957,10 +9917,10 @@
         <v>445</v>
       </c>
       <c r="G153" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="H153" s="2" t="s">
         <v>500</v>
-      </c>
-      <c r="H153" s="2" t="s">
-        <v>501</v>
       </c>
       <c r="I153" s="1"/>
     </row>
@@ -9979,10 +9939,10 @@
         <v>445</v>
       </c>
       <c r="G154" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="H154" s="2" t="s">
         <v>500</v>
-      </c>
-      <c r="H154" s="2" t="s">
-        <v>501</v>
       </c>
       <c r="I154" s="1"/>
     </row>
@@ -10028,10 +9988,10 @@
         <v>176</v>
       </c>
       <c r="G157" s="2" t="s">
+        <v>496</v>
+      </c>
+      <c r="H157" s="2" t="s">
         <v>497</v>
-      </c>
-      <c r="H157" s="2" t="s">
-        <v>498</v>
       </c>
       <c r="I157" s="1"/>
     </row>
@@ -10101,10 +10061,10 @@
         <v>458</v>
       </c>
       <c r="G161" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="H161" s="2" t="s">
         <v>500</v>
-      </c>
-      <c r="H161" s="2" t="s">
-        <v>501</v>
       </c>
       <c r="I161" s="1"/>
     </row>
@@ -10123,10 +10083,10 @@
         <v>445</v>
       </c>
       <c r="G162" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="H162" s="2" t="s">
         <v>500</v>
-      </c>
-      <c r="H162" s="2" t="s">
-        <v>501</v>
       </c>
       <c r="I162" s="1"/>
     </row>
@@ -10145,10 +10105,10 @@
         <v>445</v>
       </c>
       <c r="G163" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="H163" s="2" t="s">
         <v>500</v>
-      </c>
-      <c r="H163" s="2" t="s">
-        <v>501</v>
       </c>
       <c r="I163" s="1"/>
     </row>
@@ -10295,7 +10255,7 @@
         <v>7</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C175" s="1"/>
       <c r="D175" s="1"/>
@@ -10310,7 +10270,7 @@
         <v>8</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C176" s="1"/>
       <c r="D176" s="1"/>
@@ -10325,7 +10285,7 @@
         <v>9</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="C177" s="1"/>
       <c r="D177" s="1"/>
@@ -10340,7 +10300,7 @@
         <v>247</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C178" s="1"/>
       <c r="D178" s="1"/>
@@ -10355,7 +10315,7 @@
         <v>10</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C179" s="1"/>
       <c r="D179" s="1"/>
@@ -10370,7 +10330,7 @@
         <v>11</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C180" s="2" t="s">
         <v>35</v>
@@ -10387,7 +10347,7 @@
     </row>
     <row r="181" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A181" s="2" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B181" s="1"/>
       <c r="C181" s="1" t="s">
@@ -10447,7 +10407,7 @@
         <v>14</v>
       </c>
       <c r="I184" s="2" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="185" spans="1:9" x14ac:dyDescent="0.2">
@@ -10579,7 +10539,7 @@
         <v>453</v>
       </c>
       <c r="I192" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="193" spans="1:9" x14ac:dyDescent="0.2">
@@ -10598,7 +10558,7 @@
         <v>453</v>
       </c>
       <c r="I193" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="194" spans="1:9" x14ac:dyDescent="0.2">
@@ -10617,7 +10577,7 @@
         <v>453</v>
       </c>
       <c r="I194" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="195" spans="1:9" x14ac:dyDescent="0.2">
@@ -10632,7 +10592,7 @@
         <v>453</v>
       </c>
       <c r="I195" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="196" spans="1:9" x14ac:dyDescent="0.2">
@@ -10649,7 +10609,7 @@
         <v>453</v>
       </c>
       <c r="I196" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="197" spans="1:9" x14ac:dyDescent="0.2">
@@ -10666,7 +10626,7 @@
         <v>453</v>
       </c>
       <c r="I197" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="198" spans="1:9" x14ac:dyDescent="0.2">
@@ -10679,7 +10639,7 @@
         <v>453</v>
       </c>
       <c r="I198" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="199" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -10701,15 +10661,15 @@
     </row>
     <row r="201" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A201" s="2" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>489</v>
-      </c>
-      <c r="C201" s="11" t="s">
+        <v>488</v>
+      </c>
+      <c r="C201" s="19" t="s">
         <v>468</v>
       </c>
-      <c r="D201" s="11"/>
+      <c r="D201" s="19"/>
       <c r="E201" s="2" t="s">
         <v>19</v>
       </c>
@@ -10741,47 +10701,52 @@
         <v>469</v>
       </c>
       <c r="D205" s="2" t="s">
-        <v>470</v>
+        <v>398</v>
       </c>
       <c r="E205" s="2" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="206" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B206" s="10" t="s">
+    <row r="206" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B206" s="1" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="207" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B207" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="C206" s="3"/>
-      <c r="D206" s="3"/>
-      <c r="E206" s="3"/>
-      <c r="F206" s="3"/>
-      <c r="G206" s="3"/>
-      <c r="H206" s="3"/>
-      <c r="I206" s="3"/>
-    </row>
-    <row r="207" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A207" s="2" t="s">
-        <v>134</v>
-      </c>
+      <c r="C207" s="3"/>
+      <c r="D207" s="3"/>
+      <c r="E207" s="3"/>
+      <c r="F207" s="3"/>
+      <c r="G207" s="3"/>
+      <c r="H207" s="3"/>
+      <c r="I207" s="3"/>
     </row>
     <row r="208" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A208" s="2" t="s">
-        <v>492</v>
-      </c>
-      <c r="B208" s="1" t="s">
-        <v>490</v>
-      </c>
-      <c r="C208" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A209" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="B209" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="C209" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="209" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C209" s="1" t="s">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C210" s="1" t="s">
         <v>454</v>
       </c>
     </row>
-    <row r="210" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C210" s="2" t="s">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C211" s="2" t="s">
         <v>172</v>
       </c>
     </row>
@@ -10801,7 +10766,7 @@
   <dimension ref="A1:I85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
@@ -10825,15 +10790,15 @@
       <c r="B1" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
     </row>
     <row r="2" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B2" s="5" t="s">
@@ -11701,11 +11666,11 @@
       <c r="C79" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="D79" s="11" t="s">
+      <c r="D79" s="19" t="s">
         <v>296</v>
       </c>
-      <c r="E79" s="11"/>
-      <c r="F79" s="11"/>
+      <c r="E79" s="19"/>
+      <c r="F79" s="19"/>
     </row>
     <row r="80" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B80" s="1" t="s">
@@ -11748,11 +11713,11 @@
       <c r="C83" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="D83" s="11" t="s">
+      <c r="D83" s="19" t="s">
         <v>295</v>
       </c>
-      <c r="E83" s="11"/>
-      <c r="F83" s="11"/>
+      <c r="E83" s="19"/>
+      <c r="F83" s="19"/>
     </row>
     <row r="84" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B84" s="1" t="s">
@@ -11798,8 +11763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{988C78EB-4E00-466C-9BD2-B10965380DEB}">
   <dimension ref="A1:I296"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A187" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A256" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G219" sqref="G219"/>
     </sheetView>
   </sheetViews>
@@ -11824,15 +11789,15 @@
       <c r="B1" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
     </row>
     <row r="2" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B2" s="5" t="s">
@@ -12770,7 +12735,7 @@
         <v>263</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
@@ -12785,7 +12750,7 @@
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B85" s="1"/>
       <c r="C85" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E85" s="1" t="s">
         <v>410</v>
@@ -12794,7 +12759,7 @@
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B86" s="1"/>
       <c r="C86" s="1" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E86" s="1" t="s">
         <v>410</v>
@@ -12803,19 +12768,19 @@
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B87" s="1"/>
       <c r="C87" s="1" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>410</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B88" s="1"/>
       <c r="C88" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="E88" s="1" t="s">
         <v>410</v>
@@ -12824,13 +12789,13 @@
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B89" s="1"/>
       <c r="C89" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="E89" s="1" t="s">
         <v>410</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
@@ -12847,7 +12812,7 @@
         <v>412</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>410</v>
@@ -12904,7 +12869,7 @@
     <row r="97" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B97" s="1"/>
       <c r="C97" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E97" s="1" t="s">
         <v>410</v>
@@ -12913,7 +12878,7 @@
     <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B98" s="1"/>
       <c r="C98" s="1" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E98" s="1" t="s">
         <v>410</v>
@@ -12922,19 +12887,19 @@
     <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B99" s="1"/>
       <c r="C99" s="1" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E99" s="1" t="s">
         <v>410</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B100" s="1"/>
       <c r="C100" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="E100" s="1" t="s">
         <v>410</v>
@@ -12942,13 +12907,13 @@
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C101" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="E101" s="1" t="s">
         <v>410</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.2">
@@ -12972,7 +12937,7 @@
         <v>412</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="E104" s="1" t="s">
         <v>410</v>
@@ -12993,7 +12958,7 @@
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>209</v>
@@ -13017,12 +12982,12 @@
         <v>222</v>
       </c>
       <c r="I107" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C108" s="2" t="s">
         <v>174</v>
@@ -13040,7 +13005,7 @@
         <v>252</v>
       </c>
       <c r="H108" s="1" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.2">
@@ -13048,7 +13013,7 @@
         <v>174</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.2">
@@ -13056,7 +13021,7 @@
         <v>174</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.2">
@@ -13064,7 +13029,7 @@
         <v>174</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.2">
@@ -13072,10 +13037,10 @@
         <v>174</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="I112" s="2" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.2">
@@ -13083,24 +13048,24 @@
         <v>174</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="I113" s="2" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="D114" s="1"/>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="C115" s="2" t="s">
         <v>174</v>
@@ -13112,7 +13077,7 @@
         <v>251</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.2">
@@ -13120,7 +13085,7 @@
         <v>174</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.2">
@@ -13128,7 +13093,7 @@
         <v>174</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.2">
@@ -13136,7 +13101,7 @@
         <v>174</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="119" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -13147,19 +13112,19 @@
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>210</v>
       </c>
       <c r="D120" s="1"/>
       <c r="I120" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A121" s="2" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B121" s="1"/>
       <c r="C121" s="2" t="s">
@@ -13178,7 +13143,7 @@
         <v>252</v>
       </c>
       <c r="H121" s="1" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.2">
@@ -13187,7 +13152,7 @@
         <v>174</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.2">
@@ -13196,7 +13161,7 @@
         <v>174</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.2">
@@ -13205,7 +13170,7 @@
         <v>174</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.2">
@@ -13214,10 +13179,10 @@
         <v>174</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="I125" s="2" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.2">
@@ -13226,24 +13191,24 @@
         <v>174</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="I126" s="2" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A127" s="2" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="D127" s="1"/>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A128" s="2" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="C128" s="2" t="s">
         <v>174</v>
@@ -13255,7 +13220,7 @@
         <v>251</v>
       </c>
       <c r="F128" s="1" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.2">
@@ -13263,7 +13228,7 @@
         <v>174</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.2">
@@ -13271,7 +13236,7 @@
         <v>174</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.2">
@@ -13279,7 +13244,7 @@
         <v>174</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="132" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -13304,7 +13269,7 @@
         <v>54</v>
       </c>
       <c r="F133" s="2" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.2">
@@ -13330,7 +13295,7 @@
         <v>219</v>
       </c>
       <c r="F135" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="136" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -13365,7 +13330,7 @@
         <v>219</v>
       </c>
       <c r="F139" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="140" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -13387,7 +13352,7 @@
         <v>54</v>
       </c>
       <c r="F141" s="2" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.2">
@@ -13413,7 +13378,7 @@
         <v>219</v>
       </c>
       <c r="F143" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="144" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -13424,7 +13389,7 @@
       <c r="D144" s="3"/>
       <c r="E144" s="3"/>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B145" s="1" t="s">
         <v>316</v>
       </c>
@@ -13432,14 +13397,14 @@
       <c r="D145" s="1"/>
       <c r="E145" s="1"/>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C146" s="1"/>
       <c r="D146" s="1"/>
       <c r="E146" s="1" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C147" s="2" t="s">
         <v>172</v>
       </c>
@@ -13448,15 +13413,15 @@
         <v>219</v>
       </c>
       <c r="F147" s="2" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="148" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.2">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B148" s="5" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B149" s="1" t="s">
         <v>317</v>
       </c>
@@ -13470,10 +13435,10 @@
         <v>54</v>
       </c>
       <c r="F149" s="2" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.2">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B150" s="1"/>
       <c r="C150" s="1" t="s">
         <v>217</v>
@@ -13485,7 +13450,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C151" s="1" t="s">
         <v>217</v>
       </c>
@@ -13496,10 +13461,10 @@
         <v>219</v>
       </c>
       <c r="F151" s="2" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="152" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.2">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B152" s="5" t="s">
         <v>314</v>
       </c>
@@ -13507,7 +13472,7 @@
       <c r="D152" s="3"/>
       <c r="E152" s="3"/>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B153" s="1" t="s">
         <v>318</v>
       </c>
@@ -13515,14 +13480,14 @@
       <c r="D153" s="1"/>
       <c r="E153" s="1"/>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C154" s="1"/>
       <c r="D154" s="1"/>
       <c r="E154" s="1" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="155" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C155" s="2" t="s">
         <v>172</v>
       </c>
@@ -13531,568 +13496,446 @@
         <v>219</v>
       </c>
       <c r="F155" s="2" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="156" spans="1:8" s="7" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A156" s="22"/>
-      <c r="B156" s="19" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" s="7" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A156" s="15"/>
+      <c r="B156" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="C156" s="18"/>
-      <c r="D156" s="18"/>
-      <c r="E156" s="18"/>
-      <c r="F156" s="18"/>
-      <c r="G156" s="18"/>
-      <c r="H156" s="16"/>
-    </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A157" s="23"/>
-      <c r="B157" s="12" t="s">
+      <c r="C156" s="11"/>
+      <c r="D156" s="11"/>
+      <c r="E156" s="11"/>
+      <c r="F156" s="11"/>
+      <c r="G156" s="11"/>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A157" s="16"/>
+      <c r="B157" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C157" s="13"/>
-      <c r="D157" s="13"/>
-      <c r="E157" s="13"/>
-      <c r="F157" s="13"/>
-      <c r="G157" s="13"/>
-      <c r="H157" s="13"/>
-    </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A158" s="23"/>
-      <c r="B158" s="14" t="s">
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A158" s="16"/>
+      <c r="B158" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="C158" s="13"/>
-      <c r="D158" s="13"/>
-      <c r="E158" s="13"/>
-      <c r="F158" s="13"/>
-      <c r="G158" s="13"/>
-      <c r="H158" s="13"/>
-    </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A159" s="23"/>
-      <c r="B159" s="14" t="s">
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A159" s="16"/>
+      <c r="B159" s="6" t="s">
         <v>319</v>
       </c>
-      <c r="C159" s="13"/>
-      <c r="D159" s="13"/>
-      <c r="E159" s="13"/>
-      <c r="F159" s="13"/>
-      <c r="G159" s="13"/>
-      <c r="H159" s="13"/>
-    </row>
-    <row r="160" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A160" s="24"/>
-      <c r="B160" s="15" t="s">
+    </row>
+    <row r="160" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A160" s="17"/>
+      <c r="B160" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="C160" s="16"/>
-      <c r="D160" s="16"/>
-      <c r="E160" s="16"/>
-      <c r="F160" s="16"/>
-      <c r="G160" s="16"/>
-      <c r="H160" s="16"/>
-    </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A161" s="23"/>
-      <c r="B161" s="12" t="s">
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A161" s="16"/>
+      <c r="B161" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C161" s="13"/>
-      <c r="D161" s="13"/>
-      <c r="E161" s="13"/>
-      <c r="F161" s="13"/>
-      <c r="G161" s="13"/>
-      <c r="H161" s="13"/>
-    </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A162" s="23"/>
-      <c r="B162" s="14" t="s">
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A162" s="16"/>
+      <c r="B162" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="C162" s="13"/>
-      <c r="D162" s="13"/>
-      <c r="E162" s="13"/>
-      <c r="F162" s="13"/>
-      <c r="G162" s="13"/>
-      <c r="H162" s="13"/>
-    </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A163" s="23"/>
-      <c r="B163" s="14" t="s">
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A163" s="16"/>
+      <c r="B163" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="C163" s="13"/>
-      <c r="D163" s="13"/>
-      <c r="E163" s="13"/>
-      <c r="F163" s="13"/>
-      <c r="G163" s="13"/>
-      <c r="H163" s="13"/>
-    </row>
-    <row r="164" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A164" s="24"/>
-      <c r="B164" s="15" t="s">
+    </row>
+    <row r="164" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A164" s="17"/>
+      <c r="B164" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="C164" s="16"/>
-      <c r="D164" s="16"/>
-      <c r="E164" s="16"/>
-      <c r="F164" s="16"/>
-      <c r="G164" s="16"/>
-      <c r="H164" s="16"/>
-    </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A165" s="23"/>
-      <c r="B165" s="12" t="s">
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A165" s="16"/>
+      <c r="B165" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C165" s="13"/>
-      <c r="D165" s="13"/>
-      <c r="E165" s="13"/>
-      <c r="F165" s="13"/>
-      <c r="G165" s="13"/>
-      <c r="H165" s="13"/>
-    </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A166" s="23"/>
-      <c r="B166" s="14" t="s">
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A166" s="16"/>
+      <c r="B166" s="6" t="s">
         <v>324</v>
       </c>
-      <c r="C166" s="13"/>
-      <c r="D166" s="13"/>
-      <c r="E166" s="13"/>
-      <c r="F166" s="13"/>
-      <c r="G166" s="13"/>
-      <c r="H166" s="13"/>
-    </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A167" s="23"/>
-      <c r="B167" s="14" t="s">
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A167" s="16"/>
+      <c r="B167" s="6" t="s">
         <v>323</v>
       </c>
-      <c r="C167" s="13" t="s">
-        <v>504</v>
-      </c>
-      <c r="D167" s="13" t="s">
+      <c r="C167" s="2" t="s">
+        <v>503</v>
+      </c>
+      <c r="D167" s="2" t="s">
+        <v>506</v>
+      </c>
+      <c r="E167" s="2" t="s">
+        <v>505</v>
+      </c>
+      <c r="F167" s="2" t="s">
+        <v>496</v>
+      </c>
+      <c r="G167" s="2" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A168" s="16"/>
+      <c r="B168" s="6"/>
+      <c r="C168" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D168" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="E168" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A169" s="16"/>
+      <c r="B169" s="6"/>
+      <c r="C169" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D169" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="E169" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A170" s="16"/>
+      <c r="B170" s="6"/>
+      <c r="C170" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D170" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="E170" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A171" s="16"/>
+      <c r="B171" s="6"/>
+      <c r="C171" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D171" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="E171" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A172" s="16"/>
+      <c r="B172" s="6"/>
+      <c r="C172" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D172" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="E172" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A173" s="16"/>
+      <c r="B173" s="6"/>
+      <c r="C173" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D173" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="E173" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A174" s="16"/>
+      <c r="B174" s="6"/>
+      <c r="C174" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D174" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="E174" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A175" s="16"/>
+      <c r="B175" s="6"/>
+      <c r="C175" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D175" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="E175" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A176" s="16"/>
+      <c r="B176" s="6"/>
+      <c r="C176" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D176" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="E176" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A177" s="16"/>
+      <c r="B177" s="6"/>
+      <c r="C177" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D177" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E177" s="1"/>
+    </row>
+    <row r="178" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A178" s="16"/>
+      <c r="B178" s="6"/>
+      <c r="C178" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D178" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E178" s="1"/>
+    </row>
+    <row r="179" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A179" s="16"/>
+      <c r="B179" s="6"/>
+      <c r="C179" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D179" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E179" s="1"/>
+    </row>
+    <row r="180" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A180" s="16"/>
+      <c r="C180" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D180" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="E180" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="F180" s="2" t="s">
         <v>507</v>
       </c>
-      <c r="E167" s="17" t="s">
-        <v>506</v>
-      </c>
-      <c r="F167" s="17" t="s">
-        <v>497</v>
-      </c>
-      <c r="G167" s="13" t="s">
-        <v>498</v>
-      </c>
-      <c r="H167" s="13"/>
-    </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A168" s="23"/>
-      <c r="B168" s="14"/>
-      <c r="C168" s="12" t="s">
+      <c r="G180" s="2" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="181" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A181" s="16"/>
+      <c r="C181" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D181" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="E181" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="G181" s="2" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="182" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A182" s="16"/>
+      <c r="C182" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D182" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="E182" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="F182" s="1"/>
+      <c r="G182" s="2" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A183" s="16"/>
+      <c r="C183" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="D168" s="12" t="s">
+      <c r="D183" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="E168" s="12" t="s">
+      <c r="E183" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="F183" s="2" t="s">
+        <v>507</v>
+      </c>
+      <c r="G183" s="2" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A184" s="16"/>
+      <c r="C184" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D184" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="E184" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="F184" s="1"/>
+      <c r="G184" s="2" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="185" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A185" s="16"/>
+      <c r="C185" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D185" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="E185" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="F185" s="1"/>
+      <c r="G185" s="2" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="186" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A186" s="16"/>
+      <c r="C186" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D186" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="E186" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="F168" s="17"/>
-      <c r="G168" s="13"/>
-      <c r="H168" s="13"/>
-    </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A169" s="23"/>
-      <c r="B169" s="14"/>
-      <c r="C169" s="12" t="s">
+      <c r="F186" s="2" t="s">
+        <v>507</v>
+      </c>
+      <c r="G186" s="2" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="187" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A187" s="16"/>
+      <c r="C187" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="D169" s="12" t="s">
-        <v>261</v>
-      </c>
-      <c r="E169" s="12" t="s">
+      <c r="D187" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="E187" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="F169" s="17"/>
-      <c r="G169" s="13"/>
-      <c r="H169" s="13"/>
-    </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A170" s="23"/>
-      <c r="B170" s="14"/>
-      <c r="C170" s="12" t="s">
+      <c r="F187" s="1"/>
+      <c r="G187" s="2" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="188" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A188" s="16"/>
+      <c r="C188" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="D170" s="12" t="s">
-        <v>261</v>
-      </c>
-      <c r="E170" s="12" t="s">
+      <c r="D188" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="E188" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="F170" s="17"/>
-      <c r="G170" s="13"/>
-      <c r="H170" s="13"/>
-    </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A171" s="23"/>
-      <c r="B171" s="14"/>
-      <c r="C171" s="12" t="s">
+      <c r="F188" s="1"/>
+      <c r="G188" s="2" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="189" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A189" s="16"/>
+      <c r="C189" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="D171" s="12" t="s">
-        <v>261</v>
-      </c>
-      <c r="E171" s="13" t="s">
-        <v>179</v>
-      </c>
-      <c r="F171" s="17"/>
-      <c r="G171" s="13"/>
-      <c r="H171" s="13"/>
-    </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A172" s="23"/>
-      <c r="B172" s="14"/>
-      <c r="C172" s="12" t="s">
+      <c r="D189" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E189" s="1"/>
+      <c r="F189" s="2" t="s">
+        <v>507</v>
+      </c>
+      <c r="G189" s="2" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="190" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A190" s="16"/>
+      <c r="C190" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="D172" s="12" t="s">
-        <v>261</v>
-      </c>
-      <c r="E172" s="13" t="s">
-        <v>179</v>
-      </c>
-      <c r="F172" s="17"/>
-      <c r="G172" s="13"/>
-      <c r="H172" s="13"/>
-    </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A173" s="23"/>
-      <c r="B173" s="14"/>
-      <c r="C173" s="12" t="s">
+      <c r="D190" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E190" s="1"/>
+      <c r="F190" s="1"/>
+      <c r="G190" s="2" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="191" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A191" s="18"/>
+      <c r="B191" s="13"/>
+      <c r="C191" s="14" t="s">
         <v>171</v>
       </c>
-      <c r="D173" s="12" t="s">
-        <v>261</v>
-      </c>
-      <c r="E173" s="13" t="s">
-        <v>179</v>
-      </c>
-      <c r="F173" s="17"/>
-      <c r="G173" s="13"/>
-      <c r="H173" s="13"/>
-    </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A174" s="23"/>
-      <c r="B174" s="14"/>
-      <c r="C174" s="12" t="s">
-        <v>169</v>
-      </c>
-      <c r="D174" s="13" t="s">
-        <v>241</v>
-      </c>
-      <c r="E174" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="F174" s="17"/>
-      <c r="G174" s="13"/>
-      <c r="H174" s="13"/>
-    </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A175" s="23"/>
-      <c r="B175" s="14"/>
-      <c r="C175" s="12" t="s">
-        <v>170</v>
-      </c>
-      <c r="D175" s="13" t="s">
-        <v>241</v>
-      </c>
-      <c r="E175" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="F175" s="17"/>
-      <c r="G175" s="13"/>
-      <c r="H175" s="13"/>
-    </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A176" s="23"/>
-      <c r="B176" s="14"/>
-      <c r="C176" s="12" t="s">
-        <v>171</v>
-      </c>
-      <c r="D176" s="13" t="s">
-        <v>241</v>
-      </c>
-      <c r="E176" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="F176" s="17"/>
-      <c r="G176" s="13"/>
-      <c r="H176" s="13"/>
-    </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A177" s="23"/>
-      <c r="B177" s="14"/>
-      <c r="C177" s="12" t="s">
-        <v>169</v>
-      </c>
-      <c r="D177" s="13" t="s">
+      <c r="D191" s="13" t="s">
         <v>172</v>
       </c>
-      <c r="E177" s="12"/>
-      <c r="F177" s="17"/>
-      <c r="G177" s="13"/>
-      <c r="H177" s="13"/>
-    </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A178" s="23"/>
-      <c r="B178" s="14"/>
-      <c r="C178" s="12" t="s">
-        <v>170</v>
-      </c>
-      <c r="D178" s="13" t="s">
-        <v>172</v>
-      </c>
-      <c r="E178" s="12"/>
-      <c r="F178" s="17"/>
-      <c r="G178" s="13"/>
-      <c r="H178" s="13"/>
-    </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A179" s="23"/>
-      <c r="B179" s="14"/>
-      <c r="C179" s="12" t="s">
-        <v>171</v>
-      </c>
-      <c r="D179" s="13" t="s">
-        <v>172</v>
-      </c>
-      <c r="E179" s="12"/>
-      <c r="F179" s="17"/>
-      <c r="G179" s="13"/>
-      <c r="H179" s="13"/>
-    </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A180" s="23"/>
-      <c r="B180" s="13"/>
-      <c r="C180" s="12" t="s">
-        <v>169</v>
-      </c>
-      <c r="D180" s="12" t="s">
-        <v>261</v>
-      </c>
-      <c r="E180" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="F180" s="17" t="s">
-        <v>508</v>
-      </c>
-      <c r="G180" s="13" t="s">
-        <v>501</v>
-      </c>
-      <c r="H180" s="13"/>
-    </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A181" s="23"/>
-      <c r="B181" s="13"/>
-      <c r="C181" s="12" t="s">
-        <v>170</v>
-      </c>
-      <c r="D181" s="12" t="s">
-        <v>261</v>
-      </c>
-      <c r="E181" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="F181" s="13"/>
-      <c r="G181" s="13" t="s">
-        <v>501</v>
-      </c>
-      <c r="H181" s="13"/>
-    </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A182" s="23"/>
-      <c r="B182" s="13"/>
-      <c r="C182" s="12" t="s">
-        <v>171</v>
-      </c>
-      <c r="D182" s="12" t="s">
-        <v>261</v>
-      </c>
-      <c r="E182" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="F182" s="12"/>
-      <c r="G182" s="13" t="s">
-        <v>501</v>
-      </c>
-      <c r="H182" s="13"/>
-    </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A183" s="23"/>
-      <c r="B183" s="13"/>
-      <c r="C183" s="12" t="s">
-        <v>169</v>
-      </c>
-      <c r="D183" s="12" t="s">
-        <v>261</v>
-      </c>
-      <c r="E183" s="13" t="s">
-        <v>179</v>
-      </c>
-      <c r="F183" s="17" t="s">
-        <v>508</v>
-      </c>
-      <c r="G183" s="13" t="s">
-        <v>501</v>
-      </c>
-      <c r="H183" s="13"/>
-    </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A184" s="23"/>
-      <c r="B184" s="13"/>
-      <c r="C184" s="12" t="s">
-        <v>170</v>
-      </c>
-      <c r="D184" s="12" t="s">
-        <v>261</v>
-      </c>
-      <c r="E184" s="13" t="s">
-        <v>179</v>
-      </c>
-      <c r="F184" s="12"/>
-      <c r="G184" s="13" t="s">
-        <v>501</v>
-      </c>
-      <c r="H184" s="13"/>
-    </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A185" s="23"/>
-      <c r="B185" s="13"/>
-      <c r="C185" s="12" t="s">
-        <v>171</v>
-      </c>
-      <c r="D185" s="12" t="s">
-        <v>261</v>
-      </c>
-      <c r="E185" s="13" t="s">
-        <v>179</v>
-      </c>
-      <c r="F185" s="12"/>
-      <c r="G185" s="13" t="s">
-        <v>501</v>
-      </c>
-      <c r="H185" s="13"/>
-    </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A186" s="23"/>
-      <c r="B186" s="13"/>
-      <c r="C186" s="12" t="s">
-        <v>169</v>
-      </c>
-      <c r="D186" s="13" t="s">
-        <v>241</v>
-      </c>
-      <c r="E186" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="F186" s="17" t="s">
-        <v>508</v>
-      </c>
-      <c r="G186" s="13" t="s">
-        <v>501</v>
-      </c>
-      <c r="H186" s="13"/>
-    </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A187" s="23"/>
-      <c r="B187" s="13"/>
-      <c r="C187" s="12" t="s">
-        <v>170</v>
-      </c>
-      <c r="D187" s="13" t="s">
-        <v>241</v>
-      </c>
-      <c r="E187" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="F187" s="12"/>
-      <c r="G187" s="13" t="s">
-        <v>501</v>
-      </c>
-      <c r="H187" s="13"/>
-    </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A188" s="23"/>
-      <c r="B188" s="13"/>
-      <c r="C188" s="12" t="s">
-        <v>171</v>
-      </c>
-      <c r="D188" s="13" t="s">
-        <v>241</v>
-      </c>
-      <c r="E188" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="F188" s="12"/>
-      <c r="G188" s="13" t="s">
-        <v>501</v>
-      </c>
-      <c r="H188" s="13"/>
-    </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A189" s="23"/>
-      <c r="B189" s="13"/>
-      <c r="C189" s="12" t="s">
-        <v>169</v>
-      </c>
-      <c r="D189" s="13" t="s">
-        <v>172</v>
-      </c>
-      <c r="E189" s="12"/>
-      <c r="F189" s="17" t="s">
-        <v>508</v>
-      </c>
-      <c r="G189" s="13" t="s">
-        <v>501</v>
-      </c>
-      <c r="H189" s="13"/>
-    </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A190" s="23"/>
-      <c r="B190" s="13"/>
-      <c r="C190" s="12" t="s">
-        <v>170</v>
-      </c>
-      <c r="D190" s="13" t="s">
-        <v>172</v>
-      </c>
-      <c r="E190" s="12"/>
-      <c r="F190" s="12"/>
-      <c r="G190" s="13" t="s">
-        <v>501</v>
-      </c>
-      <c r="H190" s="13"/>
-    </row>
-    <row r="191" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A191" s="25"/>
-      <c r="B191" s="20"/>
-      <c r="C191" s="21" t="s">
-        <v>171</v>
-      </c>
-      <c r="D191" s="20" t="s">
-        <v>172</v>
-      </c>
-      <c r="E191" s="21"/>
-      <c r="F191" s="21"/>
-      <c r="G191" s="20" t="s">
-        <v>501</v>
-      </c>
-      <c r="H191" s="13"/>
-    </row>
-    <row r="192" spans="1:8" s="7" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="E191" s="14"/>
+      <c r="F191" s="14"/>
+      <c r="G191" s="13" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="192" spans="1:7" s="7" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B192" s="5" t="s">
         <v>195</v>
       </c>
@@ -14128,8 +13971,8 @@
       <c r="F196" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="G196" s="17" t="s">
-        <v>497</v>
+      <c r="G196" s="2" t="s">
+        <v>496</v>
       </c>
     </row>
     <row r="197" spans="2:7" x14ac:dyDescent="0.2">
@@ -14146,7 +13989,6 @@
       <c r="F197" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="G197" s="17"/>
     </row>
     <row r="198" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B198" s="1"/>
@@ -14162,7 +14004,6 @@
       <c r="F198" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="G198" s="17"/>
     </row>
     <row r="199" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B199" s="1"/>
@@ -14178,8 +14019,8 @@
       <c r="F199" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="G199" s="17" t="s">
-        <v>499</v>
+      <c r="G199" s="2" t="s">
+        <v>498</v>
       </c>
     </row>
     <row r="200" spans="2:7" x14ac:dyDescent="0.2">
@@ -14195,8 +14036,8 @@
       <c r="F200" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="G200" s="17" t="s">
-        <v>499</v>
+      <c r="G200" s="2" t="s">
+        <v>498</v>
       </c>
     </row>
     <row r="201" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -14259,8 +14100,8 @@
       <c r="F208" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="G208" s="17" t="s">
-        <v>499</v>
+      <c r="G208" s="2" t="s">
+        <v>498</v>
       </c>
     </row>
     <row r="209" spans="1:7" x14ac:dyDescent="0.2">
@@ -14272,8 +14113,8 @@
       <c r="F209" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="G209" s="17" t="s">
-        <v>499</v>
+      <c r="G209" s="2" t="s">
+        <v>498</v>
       </c>
     </row>
     <row r="210" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -14299,8 +14140,8 @@
       <c r="F212" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="G212" s="17" t="s">
-        <v>497</v>
+      <c r="G212" s="2" t="s">
+        <v>496</v>
       </c>
     </row>
     <row r="213" spans="1:7" x14ac:dyDescent="0.2">
@@ -14316,7 +14157,6 @@
       <c r="F213" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="G213" s="17"/>
     </row>
     <row r="214" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C214" s="1" t="s">
@@ -14331,7 +14171,6 @@
       <c r="F214" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="G214" s="17"/>
     </row>
     <row r="215" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C215" s="1" t="s">
@@ -14346,8 +14185,8 @@
       <c r="F215" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="G215" s="17" t="s">
-        <v>499</v>
+      <c r="G215" s="2" t="s">
+        <v>498</v>
       </c>
     </row>
     <row r="216" spans="1:7" x14ac:dyDescent="0.2">
@@ -14363,8 +14202,8 @@
       <c r="F216" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="G216" s="17" t="s">
-        <v>499</v>
+      <c r="G216" s="2" t="s">
+        <v>498</v>
       </c>
     </row>
     <row r="217" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -14412,8 +14251,8 @@
       <c r="F221" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="G221" s="17" t="s">
-        <v>499</v>
+      <c r="G221" s="2" t="s">
+        <v>498</v>
       </c>
     </row>
     <row r="222" spans="1:7" x14ac:dyDescent="0.2">
@@ -14425,8 +14264,8 @@
       <c r="F222" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="G222" s="17" t="s">
-        <v>499</v>
+      <c r="G222" s="2" t="s">
+        <v>498</v>
       </c>
     </row>
     <row r="223" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -14542,7 +14381,7 @@
         <v>268</v>
       </c>
       <c r="E233" s="1" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="F233" s="1"/>
       <c r="G233" s="1"/>
@@ -14552,7 +14391,7 @@
         <v>268</v>
       </c>
       <c r="E234" s="1" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="F234" s="1"/>
       <c r="G234" s="1"/>
@@ -14563,7 +14402,7 @@
       </c>
       <c r="D235" s="1"/>
       <c r="E235" s="1" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="F235" s="1"/>
       <c r="G235" s="1"/>
@@ -14572,7 +14411,7 @@
       <c r="C236" s="1"/>
       <c r="D236" s="1"/>
       <c r="E236" s="1" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="F236" s="1"/>
       <c r="G236" s="1"/>
@@ -14632,13 +14471,13 @@
         <v>264</v>
       </c>
       <c r="D242" s="1" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="F242" s="1"/>
     </row>
     <row r="243" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D243" s="1" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="F243" s="1"/>
     </row>
@@ -14647,13 +14486,13 @@
         <v>264</v>
       </c>
       <c r="D244" s="2" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="F244" s="1"/>
     </row>
     <row r="245" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D245" s="2" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="G245" s="1"/>
     </row>
@@ -14676,13 +14515,13 @@
       </c>
       <c r="B248" s="1"/>
       <c r="C248" s="2" t="s">
+        <v>503</v>
+      </c>
+      <c r="F248" s="2" t="s">
         <v>504</v>
       </c>
-      <c r="F248" s="2" t="s">
-        <v>505</v>
-      </c>
       <c r="H248" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="249" spans="1:8" x14ac:dyDescent="0.2">
@@ -14739,7 +14578,7 @@
         <v>236</v>
       </c>
       <c r="H251" s="2" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="252" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -14795,7 +14634,7 @@
         <v>236</v>
       </c>
       <c r="H254" s="2" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="255" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -14886,7 +14725,7 @@
         <v>65</v>
       </c>
       <c r="G265" s="2" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="266" spans="1:7" x14ac:dyDescent="0.2">
@@ -14927,7 +14766,7 @@
         <v>273</v>
       </c>
       <c r="E270" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="271" spans="1:7" x14ac:dyDescent="0.2">
@@ -15001,10 +14840,10 @@
         <v>273</v>
       </c>
       <c r="E275" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="G275" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="276" spans="1:7" x14ac:dyDescent="0.2">
@@ -15021,7 +14860,7 @@
         <v>279</v>
       </c>
       <c r="G276" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="277" spans="1:7" x14ac:dyDescent="0.2">
@@ -15038,7 +14877,7 @@
         <v>280</v>
       </c>
       <c r="G277" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="278" spans="1:7" x14ac:dyDescent="0.2">
@@ -15055,7 +14894,7 @@
         <v>281</v>
       </c>
       <c r="G278" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="279" spans="1:7" x14ac:dyDescent="0.2">
@@ -15072,7 +14911,7 @@
         <v>282</v>
       </c>
       <c r="G279" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="280" spans="1:7" x14ac:dyDescent="0.2">
@@ -15095,7 +14934,7 @@
         <v>274</v>
       </c>
       <c r="E281" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="282" spans="1:7" x14ac:dyDescent="0.2">
@@ -15169,10 +15008,10 @@
         <v>274</v>
       </c>
       <c r="E286" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="G286" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="287" spans="1:7" x14ac:dyDescent="0.2">
@@ -15189,7 +15028,7 @@
         <v>279</v>
       </c>
       <c r="G287" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="288" spans="1:7" x14ac:dyDescent="0.2">
@@ -15206,7 +15045,7 @@
         <v>280</v>
       </c>
       <c r="G288" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="289" spans="1:7" x14ac:dyDescent="0.2">
@@ -15223,7 +15062,7 @@
         <v>281</v>
       </c>
       <c r="G289" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="290" spans="1:7" x14ac:dyDescent="0.2">
@@ -15240,7 +15079,7 @@
         <v>282</v>
       </c>
       <c r="G290" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="291" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
revise soft hint of delay and / or defer for ADD(T)(U) instructions
</commit_message>
<xml_diff>
--- a/P4E_psuedo_instruction_set.xlsx
+++ b/P4E_psuedo_instruction_set.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\P4EngineAssembler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7529F553-9F64-441F-96C2-14A3D6235ACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2CD4DCF-FC69-4658-9C7F-6DBFED34FEB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-2475" windowWidth="38640" windowHeight="21840" xr2:uid="{87164962-7B7D-4BAA-98E0-B9A8D7C47112}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{87164962-7B7D-4BAA-98E0-B9A8D7C47112}"/>
   </bookViews>
   <sheets>
     <sheet name="parser" sheetId="1" r:id="rId1"/>
@@ -1510,7 +1510,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D134" authorId="0" shapeId="0" xr:uid="{E63EC469-582C-47E9-B724-9ADEF3800F1E}">
+    <comment ref="D138" authorId="0" shapeId="0" xr:uid="{E63EC469-582C-47E9-B724-9ADEF3800F1E}">
       <text>
         <r>
           <rPr>
@@ -1536,7 +1536,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D135" authorId="0" shapeId="0" xr:uid="{1232E5F3-A694-45DA-83F2-6A0D1C7503DB}">
+    <comment ref="D139" authorId="0" shapeId="0" xr:uid="{1232E5F3-A694-45DA-83F2-6A0D1C7503DB}">
       <text>
         <r>
           <rPr>
@@ -1562,7 +1562,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D142" authorId="0" shapeId="0" xr:uid="{39506270-CD44-456C-A43B-11D24D8E9899}">
+    <comment ref="D146" authorId="0" shapeId="0" xr:uid="{39506270-CD44-456C-A43B-11D24D8E9899}">
       <text>
         <r>
           <rPr>
@@ -1588,7 +1588,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D143" authorId="0" shapeId="0" xr:uid="{4C4353DC-270D-4DC9-A5D4-1860084DFD51}">
+    <comment ref="D147" authorId="0" shapeId="0" xr:uid="{4C4353DC-270D-4DC9-A5D4-1860084DFD51}">
       <text>
         <r>
           <rPr>
@@ -1614,7 +1614,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D150" authorId="0" shapeId="0" xr:uid="{5F1A8F02-AE77-49EE-89BE-BF2CACFE2BF8}">
+    <comment ref="D154" authorId="0" shapeId="0" xr:uid="{5F1A8F02-AE77-49EE-89BE-BF2CACFE2BF8}">
       <text>
         <r>
           <rPr>
@@ -1640,7 +1640,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D151" authorId="0" shapeId="0" xr:uid="{A3BBB9B6-6FEE-4677-8A3B-DB59F1F7A659}">
+    <comment ref="D155" authorId="0" shapeId="0" xr:uid="{A3BBB9B6-6FEE-4677-8A3B-DB59F1F7A659}">
       <text>
         <r>
           <rPr>
@@ -1666,7 +1666,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C259" authorId="0" shapeId="0" xr:uid="{DFB4FAA4-43F6-4B75-ABE8-01CB5D2DA0F6}">
+    <comment ref="C263" authorId="0" shapeId="0" xr:uid="{DFB4FAA4-43F6-4B75-ABE8-01CB5D2DA0F6}">
       <text>
         <r>
           <rPr>
@@ -1697,7 +1697,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1793" uniqueCount="509">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1819" uniqueCount="512">
   <si>
     <t>isr SHiFT</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -6817,6 +6817,18 @@
   </si>
   <si>
     <t>NXTPNFL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">    NeXT Payload with Not_Final and  Last flags set</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>delay hint</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>delay [ 1 ] ;</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -7353,9 +7365,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA14F7B7-5F50-4FFB-AE20-84853F321386}">
   <dimension ref="A1:I211"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A158" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B206" sqref="B206"/>
+      <selection pane="bottomLeft" activeCell="A202" sqref="A202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -10666,33 +10678,30 @@
       <c r="B201" s="1" t="s">
         <v>488</v>
       </c>
-      <c r="C201" s="19" t="s">
+    </row>
+    <row r="202" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A202" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="B202" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="C202" s="19" t="s">
         <v>468</v>
       </c>
-      <c r="D201" s="19"/>
-      <c r="E201" s="2" t="s">
+      <c r="D202" s="19"/>
+      <c r="E202" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="E202" s="1" t="s">
+    <row r="203" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E203" s="1" t="s">
         <v>454</v>
       </c>
     </row>
-    <row r="203" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="E203" s="2" t="s">
+    <row r="204" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E204" s="2" t="s">
         <v>172</v>
-      </c>
-    </row>
-    <row r="204" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C204" s="2" t="s">
-        <v>469</v>
-      </c>
-      <c r="D204" s="2" t="s">
-        <v>398</v>
-      </c>
-      <c r="E204" s="1" t="s">
-        <v>454</v>
       </c>
     </row>
     <row r="205" spans="1:9" x14ac:dyDescent="0.2">
@@ -10703,13 +10712,19 @@
       <c r="D205" s="2" t="s">
         <v>398</v>
       </c>
-      <c r="E205" s="2" t="s">
+      <c r="E205" s="1" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="206" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C206" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="D206" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="E206" s="2" t="s">
         <v>172</v>
-      </c>
-    </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B206" s="1" t="s">
-        <v>508</v>
       </c>
     </row>
     <row r="207" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -10753,7 +10768,7 @@
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="C1:I1"/>
-    <mergeCell ref="C201:D201"/>
+    <mergeCell ref="C202:D202"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11761,11 +11776,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{988C78EB-4E00-466C-9BD2-B10965380DEB}">
-  <dimension ref="A1:I296"/>
+  <dimension ref="A1:J300"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A256" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G219" sqref="G219"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A94" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J127" sqref="J127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -11779,7 +11794,8 @@
     <col min="7" max="7" width="14.625" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.375" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.25" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9" style="2"/>
+    <col min="10" max="10" width="10.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
@@ -12866,7 +12882,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B97" s="1"/>
       <c r="C97" s="1" t="s">
         <v>495</v>
@@ -12875,7 +12891,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B98" s="1"/>
       <c r="C98" s="1" t="s">
         <v>493</v>
@@ -12884,7 +12900,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B99" s="1"/>
       <c r="C99" s="1" t="s">
         <v>493</v>
@@ -12896,7 +12912,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B100" s="1"/>
       <c r="C100" s="1" t="s">
         <v>494</v>
@@ -12905,7 +12921,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C101" s="1" t="s">
         <v>494</v>
       </c>
@@ -12916,7 +12932,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C102" s="1" t="s">
         <v>411</v>
       </c>
@@ -12924,7 +12940,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C103" s="1" t="s">
         <v>413</v>
       </c>
@@ -12932,7 +12948,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C104" s="1" t="s">
         <v>412</v>
       </c>
@@ -12943,7 +12959,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C105" s="1" t="s">
         <v>414</v>
       </c>
@@ -12951,12 +12967,12 @@
         <v>410</v>
       </c>
     </row>
-    <row r="106" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B106" s="5" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
         <v>477</v>
       </c>
@@ -12982,10 +12998,13 @@
         <v>222</v>
       </c>
       <c r="I107" s="2" t="s">
+        <v>510</v>
+      </c>
+      <c r="J107" s="2" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
         <v>473</v>
       </c>
@@ -13008,324 +13027,370 @@
         <v>492</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C109" s="2" t="s">
         <v>174</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
+        <v>169</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="F109" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="G109" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="H109" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="I109" s="2" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C110" s="2" t="s">
         <v>174</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C111" s="2" t="s">
         <v>174</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C112" s="2" t="s">
         <v>174</v>
       </c>
       <c r="D112" s="1" t="s">
         <v>493</v>
       </c>
-      <c r="I112" s="2" t="s">
+      <c r="J112" s="2" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C113" s="2" t="s">
         <v>174</v>
       </c>
       <c r="D113" s="1" t="s">
         <v>494</v>
       </c>
-      <c r="I113" s="2" t="s">
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C114" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="J114" s="2" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A114" s="2" t="s">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A115" s="2" t="s">
         <v>477</v>
       </c>
-      <c r="B114" s="1" t="s">
+      <c r="B115" s="1" t="s">
         <v>472</v>
       </c>
-      <c r="D114" s="1"/>
-    </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A115" s="2" t="s">
+      <c r="D115" s="1"/>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A116" s="2" t="s">
         <v>474</v>
       </c>
-      <c r="C115" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="D115" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="E115" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="F115" s="1" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C116" s="2" t="s">
         <v>174</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.2">
+        <v>169</v>
+      </c>
+      <c r="E116" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="F116" s="1" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C117" s="2" t="s">
         <v>174</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.2">
+        <v>169</v>
+      </c>
+      <c r="E117" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="F117" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="I117" s="2" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C118" s="2" t="s">
         <v>174</v>
       </c>
       <c r="D118" s="1" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C119" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C120" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D120" s="1" t="s">
         <v>494</v>
       </c>
     </row>
-    <row r="119" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B119" s="5" t="s">
+    <row r="121" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B121" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="D119" s="3"/>
-    </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A120" s="2" t="s">
+      <c r="D121" s="3"/>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A122" s="2" t="s">
         <v>476</v>
       </c>
-      <c r="B120" s="1" t="s">
+      <c r="B122" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="D120" s="1"/>
-      <c r="I120" s="2" t="s">
+      <c r="D122" s="1"/>
+      <c r="J122" s="2" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A121" s="2" t="s">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A123" s="2" t="s">
         <v>473</v>
       </c>
-      <c r="B121" s="1"/>
-      <c r="C121" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="D121" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="E121" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="F121" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="G121" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="H121" s="1" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B122" s="1"/>
-      <c r="C122" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="D122" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B123" s="1"/>
       <c r="C123" s="2" t="s">
         <v>174</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
+        <v>169</v>
+      </c>
+      <c r="E123" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="F123" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="G123" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="H123" s="1" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B124" s="1"/>
       <c r="C124" s="2" t="s">
         <v>174</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.2">
+        <v>169</v>
+      </c>
+      <c r="E124" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="F124" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="G124" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="H124" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="I124" s="2" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B125" s="1"/>
       <c r="C125" s="2" t="s">
         <v>174</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>493</v>
-      </c>
-      <c r="I125" s="2" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.2">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B126" s="1"/>
       <c r="C126" s="2" t="s">
         <v>174</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>494</v>
-      </c>
-      <c r="I126" s="2" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B127" s="1"/>
+      <c r="C127" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D127" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="J127" s="2" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A127" s="2" t="s">
-        <v>476</v>
-      </c>
-      <c r="B127" s="1" t="s">
-        <v>475</v>
-      </c>
-      <c r="D127" s="1"/>
-    </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A128" s="2" t="s">
-        <v>474</v>
-      </c>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B128" s="1"/>
       <c r="C128" s="2" t="s">
         <v>174</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="E128" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="F128" s="1" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B129" s="1"/>
       <c r="C129" s="2" t="s">
         <v>174</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C130" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="D130" s="1" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
+        <v>494</v>
+      </c>
+      <c r="J129" s="2" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A130" s="2" t="s">
+        <v>476</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="D130" s="1"/>
+    </row>
+    <row r="131" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A131" s="2" t="s">
+        <v>474</v>
+      </c>
       <c r="C131" s="2" t="s">
         <v>174</v>
       </c>
       <c r="D131" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E131" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="F131" s="1" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C132" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D132" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E132" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="F132" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="I132" s="2" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C133" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D133" s="1" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C134" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D134" s="1" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C135" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D135" s="1" t="s">
         <v>494</v>
       </c>
     </row>
-    <row r="132" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B132" s="5" t="s">
+    <row r="136" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B136" s="5" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A133" s="2" t="s">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A137" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B133" s="1" t="s">
+      <c r="B137" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C133" s="2" t="s">
+      <c r="C137" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="D133" s="2" t="s">
+      <c r="D137" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="E133" s="2" t="s">
+      <c r="E137" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="F133" s="2" t="s">
+      <c r="F137" s="2" t="s">
         <v>496</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B134" s="1"/>
-      <c r="C134" s="1" t="s">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B138" s="1"/>
+      <c r="C138" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="D134" s="1" t="s">
+      <c r="D138" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="E134" s="1" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C135" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="D135" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="E135" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="F135" s="2" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="136" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B136" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="C136" s="3"/>
-      <c r="D136" s="3"/>
-      <c r="E136" s="3"/>
-    </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B137" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="C137" s="1"/>
-      <c r="D137" s="1"/>
-      <c r="E137" s="1"/>
-    </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C138" s="1"/>
-      <c r="D138" s="1"/>
       <c r="E138" s="1" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C139" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="D139" s="1"/>
+    <row r="139" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C139" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D139" s="1" t="s">
+        <v>218</v>
+      </c>
       <c r="E139" s="1" t="s">
         <v>219</v>
       </c>
@@ -13333,47 +13398,34 @@
         <v>498</v>
       </c>
     </row>
-    <row r="140" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B140" s="5" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
+        <v>191</v>
+      </c>
+      <c r="C140" s="3"/>
+      <c r="D140" s="3"/>
+      <c r="E140" s="3"/>
+    </row>
+    <row r="141" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B141" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="C141" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="D141" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="E141" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F141" s="2" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B142" s="1"/>
-      <c r="C142" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="D142" s="1" t="s">
-        <v>218</v>
-      </c>
+        <v>190</v>
+      </c>
+      <c r="C141" s="1"/>
+      <c r="D141" s="1"/>
+      <c r="E141" s="1"/>
+    </row>
+    <row r="142" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C142" s="1"/>
+      <c r="D142" s="1"/>
       <c r="E142" s="1" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C143" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="D143" s="1" t="s">
-        <v>218</v>
-      </c>
+    <row r="143" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C143" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D143" s="1"/>
       <c r="E143" s="1" t="s">
         <v>219</v>
       </c>
@@ -13381,34 +13433,47 @@
         <v>498</v>
       </c>
     </row>
-    <row r="144" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B144" s="5" t="s">
-        <v>192</v>
-      </c>
-      <c r="C144" s="3"/>
-      <c r="D144" s="3"/>
-      <c r="E144" s="3"/>
+        <v>125</v>
+      </c>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B145" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="C145" s="1"/>
-      <c r="D145" s="1"/>
-      <c r="E145" s="1"/>
+        <v>315</v>
+      </c>
+      <c r="C145" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="D145" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="E145" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F145" s="2" t="s">
+        <v>496</v>
+      </c>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C146" s="1"/>
-      <c r="D146" s="1"/>
+      <c r="B146" s="1"/>
+      <c r="C146" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D146" s="1" t="s">
+        <v>218</v>
+      </c>
       <c r="E146" s="1" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C147" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="D147" s="1"/>
+      <c r="C147" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D147" s="1" t="s">
+        <v>218</v>
+      </c>
       <c r="E147" s="1" t="s">
         <v>219</v>
       </c>
@@ -13418,45 +13483,32 @@
     </row>
     <row r="148" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B148" s="5" t="s">
-        <v>313</v>
-      </c>
+        <v>192</v>
+      </c>
+      <c r="C148" s="3"/>
+      <c r="D148" s="3"/>
+      <c r="E148" s="3"/>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B149" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="C149" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="D149" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="E149" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F149" s="2" t="s">
-        <v>496</v>
-      </c>
+        <v>316</v>
+      </c>
+      <c r="C149" s="1"/>
+      <c r="D149" s="1"/>
+      <c r="E149" s="1"/>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B150" s="1"/>
-      <c r="C150" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="D150" s="1" t="s">
-        <v>218</v>
-      </c>
+      <c r="C150" s="1"/>
+      <c r="D150" s="1"/>
       <c r="E150" s="1" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C151" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="D151" s="1" t="s">
-        <v>218</v>
-      </c>
+      <c r="C151" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D151" s="1"/>
       <c r="E151" s="1" t="s">
         <v>219</v>
       </c>
@@ -13466,32 +13518,45 @@
     </row>
     <row r="152" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B152" s="5" t="s">
-        <v>314</v>
-      </c>
-      <c r="C152" s="3"/>
-      <c r="D152" s="3"/>
-      <c r="E152" s="3"/>
+        <v>313</v>
+      </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B153" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="C153" s="1"/>
-      <c r="D153" s="1"/>
-      <c r="E153" s="1"/>
+        <v>317</v>
+      </c>
+      <c r="C153" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="D153" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="E153" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F153" s="2" t="s">
+        <v>496</v>
+      </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C154" s="1"/>
-      <c r="D154" s="1"/>
+      <c r="B154" s="1"/>
+      <c r="C154" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D154" s="1" t="s">
+        <v>218</v>
+      </c>
       <c r="E154" s="1" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="155" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C155" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="D155" s="1"/>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C155" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D155" s="1" t="s">
+        <v>218</v>
+      </c>
       <c r="E155" s="1" t="s">
         <v>219</v>
       </c>
@@ -13499,184 +13564,167 @@
         <v>498</v>
       </c>
     </row>
-    <row r="156" spans="1:7" s="7" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A156" s="15"/>
-      <c r="B156" s="12" t="s">
+    <row r="156" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B156" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="C156" s="3"/>
+      <c r="D156" s="3"/>
+      <c r="E156" s="3"/>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B157" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="C157" s="1"/>
+      <c r="D157" s="1"/>
+      <c r="E157" s="1"/>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C158" s="1"/>
+      <c r="D158" s="1"/>
+      <c r="E158" s="1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C159" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D159" s="1"/>
+      <c r="E159" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="F159" s="2" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" s="7" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A160" s="15"/>
+      <c r="B160" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="C156" s="11"/>
-      <c r="D156" s="11"/>
-      <c r="E156" s="11"/>
-      <c r="F156" s="11"/>
-      <c r="G156" s="11"/>
-    </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A157" s="16"/>
-      <c r="B157" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A158" s="16"/>
-      <c r="B158" s="6" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A159" s="16"/>
-      <c r="B159" s="6" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="160" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A160" s="17"/>
-      <c r="B160" s="5" t="s">
-        <v>193</v>
-      </c>
+      <c r="C160" s="11"/>
+      <c r="D160" s="11"/>
+      <c r="E160" s="11"/>
+      <c r="F160" s="11"/>
+      <c r="G160" s="11"/>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A161" s="16"/>
       <c r="B161" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A162" s="16"/>
       <c r="B162" s="6" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A163" s="16"/>
       <c r="B163" s="6" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="164" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A164" s="17"/>
       <c r="B164" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A165" s="16"/>
       <c r="B165" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A166" s="16"/>
       <c r="B166" s="6" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A167" s="16"/>
       <c r="B167" s="6" t="s">
-        <v>323</v>
-      </c>
-      <c r="C167" s="2" t="s">
-        <v>503</v>
-      </c>
-      <c r="D167" s="2" t="s">
-        <v>506</v>
-      </c>
-      <c r="E167" s="2" t="s">
-        <v>505</v>
-      </c>
-      <c r="F167" s="2" t="s">
-        <v>496</v>
-      </c>
-      <c r="G167" s="2" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A168" s="16"/>
-      <c r="B168" s="6"/>
-      <c r="C168" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="D168" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="E168" s="1" t="s">
-        <v>220</v>
+        <v>321</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A168" s="17"/>
+      <c r="B168" s="5" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A169" s="16"/>
-      <c r="B169" s="6"/>
-      <c r="C169" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="D169" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="E169" s="1" t="s">
-        <v>220</v>
+      <c r="B169" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A170" s="16"/>
-      <c r="B170" s="6"/>
-      <c r="C170" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="D170" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="E170" s="1" t="s">
-        <v>220</v>
+      <c r="B170" s="6" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A171" s="16"/>
-      <c r="B171" s="6"/>
-      <c r="C171" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="D171" s="1" t="s">
-        <v>261</v>
+      <c r="B171" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="C171" s="2" t="s">
+        <v>503</v>
+      </c>
+      <c r="D171" s="2" t="s">
+        <v>506</v>
       </c>
       <c r="E171" s="2" t="s">
-        <v>179</v>
+        <v>505</v>
+      </c>
+      <c r="F171" s="2" t="s">
+        <v>496</v>
+      </c>
+      <c r="G171" s="2" t="s">
+        <v>497</v>
       </c>
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A172" s="16"/>
       <c r="B172" s="6"/>
       <c r="C172" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D172" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="E172" s="2" t="s">
-        <v>179</v>
+      <c r="E172" s="1" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A173" s="16"/>
       <c r="B173" s="6"/>
       <c r="C173" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D173" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="E173" s="2" t="s">
-        <v>179</v>
+      <c r="E173" s="1" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A174" s="16"/>
       <c r="B174" s="6"/>
       <c r="C174" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="D174" s="2" t="s">
-        <v>241</v>
+        <v>171</v>
+      </c>
+      <c r="D174" s="1" t="s">
+        <v>261</v>
       </c>
       <c r="E174" s="1" t="s">
         <v>220</v>
@@ -13686,140 +13734,127 @@
       <c r="A175" s="16"/>
       <c r="B175" s="6"/>
       <c r="C175" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="D175" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="E175" s="1" t="s">
-        <v>220</v>
+        <v>169</v>
+      </c>
+      <c r="D175" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="E175" s="2" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A176" s="16"/>
       <c r="B176" s="6"/>
       <c r="C176" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="D176" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="E176" s="1" t="s">
-        <v>220</v>
+        <v>170</v>
+      </c>
+      <c r="D176" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="E176" s="2" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A177" s="16"/>
       <c r="B177" s="6"/>
       <c r="C177" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="D177" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="E177" s="1"/>
+        <v>171</v>
+      </c>
+      <c r="D177" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="E177" s="2" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A178" s="16"/>
       <c r="B178" s="6"/>
       <c r="C178" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D178" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="E178" s="1"/>
+        <v>241</v>
+      </c>
+      <c r="E178" s="1" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A179" s="16"/>
       <c r="B179" s="6"/>
       <c r="C179" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D179" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="E179" s="1"/>
+        <v>241</v>
+      </c>
+      <c r="E179" s="1" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A180" s="16"/>
+      <c r="B180" s="6"/>
       <c r="C180" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="D180" s="1" t="s">
-        <v>261</v>
+        <v>171</v>
+      </c>
+      <c r="D180" s="2" t="s">
+        <v>241</v>
       </c>
       <c r="E180" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="F180" s="2" t="s">
-        <v>507</v>
-      </c>
-      <c r="G180" s="2" t="s">
-        <v>500</v>
-      </c>
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A181" s="16"/>
+      <c r="B181" s="6"/>
       <c r="C181" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="D181" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="E181" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="G181" s="2" t="s">
-        <v>500</v>
-      </c>
+        <v>169</v>
+      </c>
+      <c r="D181" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E181" s="1"/>
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A182" s="16"/>
+      <c r="B182" s="6"/>
       <c r="C182" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="D182" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="E182" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="F182" s="1"/>
-      <c r="G182" s="2" t="s">
-        <v>500</v>
-      </c>
+        <v>170</v>
+      </c>
+      <c r="D182" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E182" s="1"/>
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A183" s="16"/>
+      <c r="B183" s="6"/>
       <c r="C183" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="D183" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="E183" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="F183" s="2" t="s">
-        <v>507</v>
-      </c>
-      <c r="G183" s="2" t="s">
-        <v>500</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="D183" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E183" s="1"/>
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A184" s="16"/>
       <c r="C184" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D184" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="E184" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="F184" s="1"/>
+      <c r="E184" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="F184" s="2" t="s">
+        <v>507</v>
+      </c>
       <c r="G184" s="2" t="s">
         <v>500</v>
       </c>
@@ -13827,15 +13862,14 @@
     <row r="185" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A185" s="16"/>
       <c r="C185" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D185" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="E185" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="F185" s="1"/>
+      <c r="E185" s="1" t="s">
+        <v>220</v>
+      </c>
       <c r="G185" s="2" t="s">
         <v>500</v>
       </c>
@@ -13843,17 +13877,15 @@
     <row r="186" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A186" s="16"/>
       <c r="C186" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="D186" s="2" t="s">
-        <v>241</v>
+        <v>171</v>
+      </c>
+      <c r="D186" s="1" t="s">
+        <v>261</v>
       </c>
       <c r="E186" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="F186" s="2" t="s">
-        <v>507</v>
-      </c>
+      <c r="F186" s="1"/>
       <c r="G186" s="2" t="s">
         <v>500</v>
       </c>
@@ -13861,15 +13893,17 @@
     <row r="187" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A187" s="16"/>
       <c r="C187" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="D187" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="E187" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="F187" s="1"/>
+        <v>169</v>
+      </c>
+      <c r="D187" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="E187" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="F187" s="2" t="s">
+        <v>507</v>
+      </c>
       <c r="G187" s="2" t="s">
         <v>500</v>
       </c>
@@ -13877,13 +13911,13 @@
     <row r="188" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A188" s="16"/>
       <c r="C188" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="D188" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="E188" s="1" t="s">
-        <v>220</v>
+        <v>170</v>
+      </c>
+      <c r="D188" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="E188" s="2" t="s">
+        <v>179</v>
       </c>
       <c r="F188" s="1"/>
       <c r="G188" s="2" t="s">
@@ -13893,15 +13927,15 @@
     <row r="189" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A189" s="16"/>
       <c r="C189" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="D189" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="E189" s="1"/>
-      <c r="F189" s="2" t="s">
-        <v>507</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="D189" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="E189" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="F189" s="1"/>
       <c r="G189" s="2" t="s">
         <v>500</v>
       </c>
@@ -13909,469 +13943,484 @@
     <row r="190" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A190" s="16"/>
       <c r="C190" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D190" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="E190" s="1"/>
-      <c r="F190" s="1"/>
+        <v>241</v>
+      </c>
+      <c r="E190" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="F190" s="2" t="s">
+        <v>507</v>
+      </c>
       <c r="G190" s="2" t="s">
         <v>500</v>
       </c>
     </row>
-    <row r="191" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A191" s="18"/>
-      <c r="B191" s="13"/>
-      <c r="C191" s="14" t="s">
+    <row r="191" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A191" s="16"/>
+      <c r="C191" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D191" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="E191" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="F191" s="1"/>
+      <c r="G191" s="2" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="192" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A192" s="16"/>
+      <c r="C192" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="D191" s="13" t="s">
+      <c r="D192" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="E192" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="F192" s="1"/>
+      <c r="G192" s="2" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="193" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A193" s="16"/>
+      <c r="C193" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D193" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="E191" s="14"/>
-      <c r="F191" s="14"/>
-      <c r="G191" s="13" t="s">
+      <c r="E193" s="1"/>
+      <c r="F193" s="2" t="s">
+        <v>507</v>
+      </c>
+      <c r="G193" s="2" t="s">
         <v>500</v>
       </c>
     </row>
-    <row r="192" spans="1:7" s="7" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B192" s="5" t="s">
+    <row r="194" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A194" s="16"/>
+      <c r="C194" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D194" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E194" s="1"/>
+      <c r="F194" s="1"/>
+      <c r="G194" s="2" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="195" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A195" s="18"/>
+      <c r="B195" s="13"/>
+      <c r="C195" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="D195" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="E195" s="14"/>
+      <c r="F195" s="14"/>
+      <c r="G195" s="13" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="196" spans="1:7" s="7" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B196" s="5" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="193" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B193" s="1" t="s">
+    <row r="197" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B197" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="194" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B194" s="1" t="s">
+    <row r="198" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B198" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="195" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B195" s="1" t="s">
+    <row r="199" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B199" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="196" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B196" s="1" t="s">
+    <row r="200" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B200" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C196" s="2" t="s">
+      <c r="C200" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D196" s="2" t="s">
+      <c r="D200" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="E196" s="2" t="s">
+      <c r="E200" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F196" s="2" t="s">
+      <c r="F200" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="G196" s="2" t="s">
+      <c r="G200" s="2" t="s">
         <v>496</v>
       </c>
     </row>
-    <row r="197" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B197" s="1"/>
-      <c r="C197" s="1" t="s">
+    <row r="201" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B201" s="1"/>
+      <c r="C201" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="D197" s="1" t="s">
+      <c r="D201" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="E197" s="1" t="s">
+      <c r="E201" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="F197" s="1" t="s">
+      <c r="F201" s="1" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="198" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B198" s="1"/>
-      <c r="C198" s="1" t="s">
+    <row r="202" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B202" s="1"/>
+      <c r="C202" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="D198" s="1" t="s">
+      <c r="D202" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="E198" s="1" t="s">
+      <c r="E202" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="F198" s="1" t="s">
+      <c r="F202" s="1" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="199" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B199" s="1"/>
-      <c r="C199" s="1" t="s">
+    <row r="203" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B203" s="1"/>
+      <c r="C203" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="D199" s="1" t="s">
+      <c r="D203" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="E199" s="1" t="s">
+      <c r="E203" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="F199" s="1" t="s">
+      <c r="F203" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="G199" s="2" t="s">
+      <c r="G203" s="2" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="200" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C200" s="1" t="s">
+    <row r="204" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C204" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="D200" s="1" t="s">
+      <c r="D204" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="E200" s="1" t="s">
+      <c r="E204" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="F200" s="1" t="s">
+      <c r="F204" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="G200" s="2" t="s">
+      <c r="G204" s="2" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="201" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B201" s="5" t="s">
+    <row r="205" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B205" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="C201" s="3"/>
-      <c r="D201" s="3"/>
-      <c r="E201" s="3"/>
-      <c r="F201" s="3"/>
-    </row>
-    <row r="202" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B202" s="1" t="s">
+      <c r="C205" s="3"/>
+      <c r="D205" s="3"/>
+      <c r="E205" s="3"/>
+      <c r="F205" s="3"/>
+    </row>
+    <row r="206" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B206" s="1" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="203" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B203" s="1" t="s">
+    <row r="207" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B207" s="1" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="204" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B204" s="1" t="s">
+    <row r="208" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B208" s="1" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="205" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B205" s="1" t="s">
+    <row r="209" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B209" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="C205" s="1"/>
-      <c r="D205" s="1"/>
-    </row>
-    <row r="206" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B206" s="1"/>
-      <c r="C206" s="1"/>
-      <c r="D206" s="1"/>
-      <c r="E206" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="F206" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="207" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B207" s="1"/>
-      <c r="C207" s="1"/>
-      <c r="D207" s="1"/>
-      <c r="E207" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="F207" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="208" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E208" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="F208" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="G208" s="2" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C209" s="1"/>
       <c r="D209" s="1"/>
-      <c r="E209" s="1" t="s">
+    </row>
+    <row r="210" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B210" s="1"/>
+      <c r="C210" s="1"/>
+      <c r="D210" s="1"/>
+      <c r="E210" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F210" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="211" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B211" s="1"/>
+      <c r="C211" s="1"/>
+      <c r="D211" s="1"/>
+      <c r="E211" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="F209" s="1" t="s">
+      <c r="F211" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="G209" s="2" t="s">
+    </row>
+    <row r="212" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E212" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F212" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="G212" s="2" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="210" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B210" s="5" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B211" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C212" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D212" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="E212" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="F212" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="G212" s="2" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C213" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="D213" s="1" t="s">
-        <v>226</v>
-      </c>
+    <row r="213" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C213" s="1"/>
+      <c r="D213" s="1"/>
       <c r="E213" s="1" t="s">
-        <v>169</v>
+        <v>223</v>
       </c>
       <c r="F213" s="1" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="214" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C214" s="1" t="s">
+      <c r="G213" s="2" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="214" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B214" s="5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="215" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B215" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="216" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C216" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D216" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E216" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F216" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G216" s="2" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="217" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C217" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="D214" s="1" t="s">
+      <c r="D217" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="E214" s="1" t="s">
+      <c r="E217" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F217" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="218" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C218" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="D218" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="E218" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="F214" s="1" t="s">
+      <c r="F218" s="1" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="215" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C215" s="1" t="s">
+    <row r="219" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C219" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="D215" s="1" t="s">
+      <c r="D219" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="E215" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="F215" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="G215" s="2" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="216" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C216" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="D216" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="E216" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="F216" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="G216" s="2" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="217" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B217" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="C217" s="3"/>
-      <c r="D217" s="3"/>
-      <c r="E217" s="3"/>
-      <c r="F217" s="3"/>
-    </row>
-    <row r="218" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B218" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C218" s="1"/>
-      <c r="D218" s="1"/>
-    </row>
-    <row r="219" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B219" s="1"/>
-      <c r="C219" s="1"/>
-      <c r="D219" s="1"/>
       <c r="E219" s="1" t="s">
         <v>169</v>
       </c>
       <c r="F219" s="1" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="220" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B220" s="1"/>
-      <c r="C220" s="1"/>
-      <c r="D220" s="1"/>
+      <c r="G219" s="2" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="220" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C220" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="D220" s="1" t="s">
+        <v>226</v>
+      </c>
       <c r="E220" s="1" t="s">
         <v>223</v>
       </c>
       <c r="F220" s="1" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E221" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="F221" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="G221" s="2" t="s">
+      <c r="G220" s="2" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="222" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="221" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B221" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="C221" s="3"/>
+      <c r="D221" s="3"/>
+      <c r="E221" s="3"/>
+      <c r="F221" s="3"/>
+    </row>
+    <row r="222" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B222" s="1" t="s">
+        <v>197</v>
+      </c>
       <c r="C222" s="1"/>
       <c r="D222" s="1"/>
-      <c r="E222" s="1" t="s">
+    </row>
+    <row r="223" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B223" s="1"/>
+      <c r="C223" s="1"/>
+      <c r="D223" s="1"/>
+      <c r="E223" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F223" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="224" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B224" s="1"/>
+      <c r="C224" s="1"/>
+      <c r="D224" s="1"/>
+      <c r="E224" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="F222" s="1" t="s">
+      <c r="F224" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="G222" s="2" t="s">
+    </row>
+    <row r="225" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E225" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F225" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="G225" s="2" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="223" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B223" s="5" t="s">
+    <row r="226" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C226" s="1"/>
+      <c r="D226" s="1"/>
+      <c r="E226" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="F226" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="G226" s="2" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="227" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B227" s="5" t="s">
         <v>119</v>
-      </c>
-    </row>
-    <row r="224" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A224" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="225" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A225" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="B225" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="226" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A226" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="B226" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="227" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A227" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="B227" s="4" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="228" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A228" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="229" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A229" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B229" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="230" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A230" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B230" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="231" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A231" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B231" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="232" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A232" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B228" s="1" t="s">
+      <c r="B232" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C228" s="2" t="s">
+      <c r="C232" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D228" s="2" t="s">
+      <c r="D232" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E228" s="2" t="s">
+      <c r="E232" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="F228" s="2" t="s">
+      <c r="F232" s="2" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="229" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C229" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="D229" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="E229" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="F229" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="G229" s="1"/>
-    </row>
-    <row r="230" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D230" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="E230" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="F230" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="G230" s="1"/>
-    </row>
-    <row r="231" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C231" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="D231" s="1"/>
-      <c r="E231" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="F231" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="G231" s="1"/>
-    </row>
-    <row r="232" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C232" s="1"/>
-      <c r="D232" s="1"/>
-      <c r="E232" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="F232" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="G232" s="1"/>
     </row>
     <row r="233" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C233" s="1" t="s">
@@ -14381,9 +14430,11 @@
         <v>268</v>
       </c>
       <c r="E233" s="1" t="s">
-        <v>478</v>
-      </c>
-      <c r="F233" s="1"/>
+        <v>234</v>
+      </c>
+      <c r="F233" s="1" t="s">
+        <v>265</v>
+      </c>
       <c r="G233" s="1"/>
     </row>
     <row r="234" spans="1:7" x14ac:dyDescent="0.2">
@@ -14391,9 +14442,11 @@
         <v>268</v>
       </c>
       <c r="E234" s="1" t="s">
-        <v>478</v>
-      </c>
-      <c r="F234" s="1"/>
+        <v>234</v>
+      </c>
+      <c r="F234" s="1" t="s">
+        <v>265</v>
+      </c>
       <c r="G234" s="1"/>
     </row>
     <row r="235" spans="1:7" x14ac:dyDescent="0.2">
@@ -14402,207 +14455,179 @@
       </c>
       <c r="D235" s="1"/>
       <c r="E235" s="1" t="s">
-        <v>478</v>
-      </c>
-      <c r="F235" s="1"/>
+        <v>234</v>
+      </c>
+      <c r="F235" s="1" t="s">
+        <v>265</v>
+      </c>
       <c r="G235" s="1"/>
     </row>
     <row r="236" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C236" s="1"/>
       <c r="D236" s="1"/>
       <c r="E236" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="F236" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="G236" s="1"/>
+    </row>
+    <row r="237" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C237" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="D237" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="E237" s="1" t="s">
         <v>478</v>
       </c>
-      <c r="F236" s="1"/>
-      <c r="G236" s="1"/>
-    </row>
-    <row r="237" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A237" s="2" t="s">
+      <c r="F237" s="1"/>
+      <c r="G237" s="1"/>
+    </row>
+    <row r="238" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D238" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="E238" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="F238" s="1"/>
+      <c r="G238" s="1"/>
+    </row>
+    <row r="239" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C239" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="D239" s="1"/>
+      <c r="E239" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="F239" s="1"/>
+      <c r="G239" s="1"/>
+    </row>
+    <row r="240" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C240" s="1"/>
+      <c r="D240" s="1"/>
+      <c r="E240" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="F240" s="1"/>
+      <c r="G240" s="1"/>
+    </row>
+    <row r="241" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A241" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="B237" s="1" t="s">
+      <c r="B241" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="G237" s="1"/>
-    </row>
-    <row r="238" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C238" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="D238" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="F238" s="1" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="239" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D239" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="F239" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="G239" s="1"/>
-    </row>
-    <row r="240" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B240" s="1"/>
-      <c r="C240" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="D240" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="F240" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="G240" s="1"/>
-    </row>
-    <row r="241" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D241" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="F241" s="1" t="s">
-        <v>265</v>
-      </c>
+      <c r="G241" s="1"/>
     </row>
     <row r="242" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C242" s="1" t="s">
         <v>264</v>
       </c>
       <c r="D242" s="1" t="s">
-        <v>478</v>
-      </c>
-      <c r="F242" s="1"/>
+        <v>234</v>
+      </c>
+      <c r="F242" s="1" t="s">
+        <v>265</v>
+      </c>
     </row>
     <row r="243" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D243" s="1" t="s">
-        <v>478</v>
-      </c>
-      <c r="F243" s="1"/>
+        <v>234</v>
+      </c>
+      <c r="F243" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="G243" s="1"/>
     </row>
     <row r="244" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B244" s="1"/>
       <c r="C244" s="1" t="s">
         <v>264</v>
       </c>
       <c r="D244" s="2" t="s">
-        <v>479</v>
-      </c>
-      <c r="F244" s="1"/>
+        <v>174</v>
+      </c>
+      <c r="F244" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="G244" s="1"/>
     </row>
     <row r="245" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D245" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="F245" s="1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="246" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C246" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="D246" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="F246" s="1"/>
+    </row>
+    <row r="247" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D247" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="F247" s="1"/>
+    </row>
+    <row r="248" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C248" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="D248" s="2" t="s">
         <v>479</v>
       </c>
-      <c r="G245" s="1"/>
-    </row>
-    <row r="246" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B246" s="5" t="s">
+      <c r="F248" s="1"/>
+    </row>
+    <row r="249" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D249" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="G249" s="1"/>
+    </row>
+    <row r="250" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B250" s="5" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="247" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A247" s="2" t="s">
+    <row r="251" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A251" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="B247" s="1" t="s">
+      <c r="B251" s="1" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="248" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A248" s="2" t="s">
+    <row r="252" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A252" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="B248" s="1"/>
-      <c r="C248" s="2" t="s">
+      <c r="B252" s="1"/>
+      <c r="C252" s="2" t="s">
         <v>503</v>
       </c>
-      <c r="F248" s="2" t="s">
+      <c r="F252" s="2" t="s">
         <v>504</v>
       </c>
-      <c r="H248" s="2" t="s">
+      <c r="H252" s="2" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="249" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B249" s="1"/>
-      <c r="C249" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="D249" s="2" t="s">
-        <v>415</v>
-      </c>
-      <c r="E249" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="F249" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="G249" s="2" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="250" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B250" s="1"/>
-      <c r="C250" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="D250" s="2" t="s">
-        <v>415</v>
-      </c>
-      <c r="E250" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="F250" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="G250" s="2" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="251" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B251" s="1"/>
-      <c r="C251" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="D251" s="2" t="s">
-        <v>415</v>
-      </c>
-      <c r="E251" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="F251" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="G251" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="H251" s="2" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="252" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B252" s="1"/>
-      <c r="C252" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="D252" s="2" t="s">
-        <v>415</v>
-      </c>
-      <c r="E252" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="F252" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="G252" s="2" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="253" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B253" s="1"/>
       <c r="C253" s="1" t="s">
-        <v>169</v>
+        <v>223</v>
       </c>
       <c r="D253" s="2" t="s">
         <v>415</v>
@@ -14611,15 +14636,16 @@
         <v>235</v>
       </c>
       <c r="F253" s="1" t="s">
-        <v>223</v>
+        <v>169</v>
       </c>
       <c r="G253" s="2" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="254" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B254" s="1"/>
       <c r="C254" s="1" t="s">
-        <v>169</v>
+        <v>223</v>
       </c>
       <c r="D254" s="2" t="s">
         <v>415</v>
@@ -14633,191 +14659,205 @@
       <c r="G254" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="H254" s="2" t="s">
+    </row>
+    <row r="255" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B255" s="1"/>
+      <c r="C255" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="D255" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="E255" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="F255" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="G255" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="H255" s="2" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="255" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B255" s="5" t="s">
+    <row r="256" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B256" s="1"/>
+      <c r="C256" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D256" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="E256" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="F256" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="G256" s="2" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="257" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B257" s="1"/>
+      <c r="C257" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D257" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="E257" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="F257" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="G257" s="2" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="258" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C258" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D258" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="E258" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="F258" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="G258" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="H258" s="2" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="259" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B259" s="5" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="256" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A256" s="2" t="s">
+    <row r="260" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A260" s="2" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="257" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A257" s="2" t="s">
+    <row r="261" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A261" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B257" s="1" t="s">
+      <c r="B261" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="C257" s="2" t="s">
+      <c r="C261" s="2" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="258" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A258" s="2" t="s">
+    <row r="262" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A262" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="B258" s="1" t="s">
+      <c r="B262" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="C258" s="1" t="s">
+      <c r="C262" s="1" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="259" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A259" s="2" t="s">
+    <row r="263" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A263" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="C259" s="2" t="s">
+      <c r="C263" s="2" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="260" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B260" s="5" t="s">
+    <row r="264" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B264" s="5" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="261" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A261" s="2" t="s">
+    <row r="265" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A265" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B261" s="1" t="s">
+      <c r="B265" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="262" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C262" s="2" t="s">
+    <row r="266" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C266" s="2" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="263" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B263" s="5" t="s">
+    <row r="267" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B267" s="5" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="264" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A264" s="2" t="s">
+    <row r="268" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A268" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="265" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A265" s="2" t="s">
+    <row r="269" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A269" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B265" s="1" t="s">
+      <c r="B269" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C265" s="2" t="s">
+      <c r="C269" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D265" s="2" t="s">
+      <c r="D269" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E265" s="2" t="s">
+      <c r="E269" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F265" s="2" t="s">
+      <c r="F269" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="G265" s="2" t="s">
+      <c r="G269" s="2" t="s">
         <v>496</v>
       </c>
     </row>
-    <row r="266" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C266" s="1" t="s">
+    <row r="270" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C270" s="1" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="267" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A267" s="2" t="s">
+    <row r="271" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A271" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B267" s="1" t="s">
+      <c r="B271" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="268" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C268" s="1" t="s">
+    <row r="272" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C272" s="1" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="269" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A269" s="2" t="s">
+    <row r="273" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A273" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="B269" s="1" t="s">
+      <c r="B273" s="1" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="270" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A270" s="2" t="s">
+    <row r="274" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A274" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B270" s="1"/>
-      <c r="C270" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="D270" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="E270" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="271" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A271" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B271" s="1"/>
-      <c r="C271" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="D271" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="E271" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="F271" s="1" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="272" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B272" s="1"/>
-      <c r="C272" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="D272" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="E272" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="F272" s="1" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="273" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B273" s="1"/>
-      <c r="C273" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="D273" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="E273" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="F273" s="1" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="274" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B274" s="1"/>
       <c r="C274" s="1" t="s">
         <v>271</v>
@@ -14826,13 +14866,14 @@
         <v>273</v>
       </c>
       <c r="E274" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="F274" s="1" t="s">
-        <v>282</v>
+        <v>495</v>
       </c>
     </row>
     <row r="275" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A275" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B275" s="1"/>
       <c r="C275" s="1" t="s">
         <v>271</v>
       </c>
@@ -14840,13 +14881,14 @@
         <v>273</v>
       </c>
       <c r="E275" s="1" t="s">
-        <v>495</v>
-      </c>
-      <c r="G275" s="2" t="s">
-        <v>501</v>
+        <v>275</v>
+      </c>
+      <c r="F275" s="1" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="276" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B276" s="1"/>
       <c r="C276" s="1" t="s">
         <v>271</v>
       </c>
@@ -14854,16 +14896,14 @@
         <v>273</v>
       </c>
       <c r="E276" s="1" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="F276" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="G276" s="2" t="s">
-        <v>501</v>
+        <v>280</v>
       </c>
     </row>
     <row r="277" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B277" s="1"/>
       <c r="C277" s="1" t="s">
         <v>271</v>
       </c>
@@ -14871,16 +14911,14 @@
         <v>273</v>
       </c>
       <c r="E277" s="1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="F277" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="G277" s="2" t="s">
-        <v>501</v>
+        <v>281</v>
       </c>
     </row>
     <row r="278" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B278" s="1"/>
       <c r="C278" s="1" t="s">
         <v>271</v>
       </c>
@@ -14888,13 +14926,10 @@
         <v>273</v>
       </c>
       <c r="E278" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="F278" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="G278" s="2" t="s">
-        <v>501</v>
+        <v>282</v>
       </c>
     </row>
     <row r="279" spans="1:7" x14ac:dyDescent="0.2">
@@ -14905,87 +14940,92 @@
         <v>273</v>
       </c>
       <c r="E279" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="F279" s="1" t="s">
-        <v>282</v>
+        <v>495</v>
       </c>
       <c r="G279" s="2" t="s">
         <v>501</v>
       </c>
     </row>
     <row r="280" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A280" s="2" t="s">
+      <c r="C280" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="D280" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="E280" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="F280" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="G280" s="2" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="281" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C281" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="D281" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="E281" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="F281" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="G281" s="2" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="282" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C282" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="D282" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="E282" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="F282" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="G282" s="2" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="283" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C283" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="D283" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="E283" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="F283" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="G283" s="2" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="284" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A284" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="B280" s="1" t="s">
+      <c r="B284" s="1" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="281" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A281" s="2" t="s">
+    <row r="285" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A285" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="B281" s="1"/>
-      <c r="C281" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="D281" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="E281" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="282" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A282" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="B282" s="1"/>
-      <c r="C282" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="D282" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="E282" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="F282" s="1" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="283" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B283" s="1"/>
-      <c r="C283" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="D283" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="E283" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="F283" s="1" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="284" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B284" s="1"/>
-      <c r="C284" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="D284" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="E284" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="F284" s="1" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="285" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B285" s="1"/>
       <c r="C285" s="1" t="s">
         <v>272</v>
@@ -14994,13 +15034,14 @@
         <v>274</v>
       </c>
       <c r="E285" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="F285" s="1" t="s">
-        <v>282</v>
+        <v>495</v>
       </c>
     </row>
     <row r="286" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A286" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B286" s="1"/>
       <c r="C286" s="1" t="s">
         <v>272</v>
       </c>
@@ -15008,13 +15049,14 @@
         <v>274</v>
       </c>
       <c r="E286" s="1" t="s">
-        <v>495</v>
-      </c>
-      <c r="G286" s="2" t="s">
-        <v>501</v>
+        <v>275</v>
+      </c>
+      <c r="F286" s="1" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="287" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B287" s="1"/>
       <c r="C287" s="1" t="s">
         <v>272</v>
       </c>
@@ -15022,16 +15064,14 @@
         <v>274</v>
       </c>
       <c r="E287" s="1" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="F287" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="G287" s="2" t="s">
-        <v>501</v>
+        <v>280</v>
       </c>
     </row>
     <row r="288" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B288" s="1"/>
       <c r="C288" s="1" t="s">
         <v>272</v>
       </c>
@@ -15039,16 +15079,14 @@
         <v>274</v>
       </c>
       <c r="E288" s="1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="F288" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="G288" s="2" t="s">
-        <v>501</v>
+        <v>281</v>
       </c>
     </row>
     <row r="289" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B289" s="1"/>
       <c r="C289" s="1" t="s">
         <v>272</v>
       </c>
@@ -15056,13 +15094,10 @@
         <v>274</v>
       </c>
       <c r="E289" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="F289" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="G289" s="2" t="s">
-        <v>501</v>
+        <v>282</v>
       </c>
     </row>
     <row r="290" spans="1:7" x14ac:dyDescent="0.2">
@@ -15073,50 +15108,115 @@
         <v>274</v>
       </c>
       <c r="E290" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="F290" s="1" t="s">
-        <v>282</v>
+        <v>495</v>
       </c>
       <c r="G290" s="2" t="s">
         <v>501</v>
       </c>
     </row>
-    <row r="291" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B291" s="5" t="s">
+    <row r="291" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C291" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="D291" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="E291" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="F291" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="G291" s="2" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="292" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C292" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="D292" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="E292" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="F292" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="G292" s="2" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="293" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C293" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="D293" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="E293" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="F293" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="G293" s="2" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="294" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C294" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="D294" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="E294" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="F294" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="G294" s="2" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="295" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B295" s="5" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="292" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A292" s="2" t="s">
+    <row r="296" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A296" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="B292" s="1" t="s">
+      <c r="B296" s="1" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="293" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B293" s="1"/>
-      <c r="C293" s="2" t="s">
+    <row r="297" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B297" s="1"/>
+      <c r="C297" s="2" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="294" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B294" s="5" t="s">
+    <row r="298" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B298" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="C294" s="3"/>
-    </row>
-    <row r="295" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A295" s="2" t="s">
+      <c r="C298" s="3"/>
+    </row>
+    <row r="299" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A299" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B295" s="1" t="s">
+      <c r="B299" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="296" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C296" s="2" t="s">
+    <row r="300" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C300" s="2" t="s">
         <v>172</v>
       </c>
     </row>

</xml_diff>